<commit_message>
Update automatico via Actualizar 12-16-2021 14-08-30
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11084" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11132" uniqueCount="367">
   <si>
     <t>Región</t>
   </si>
@@ -1113,13 +1113,16 @@
   <si>
     <t>2021-12-12</t>
   </si>
+  <si>
+    <t>2021-12-13</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -1189,7 +1192,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1473,17 +1476,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5557"/>
+  <dimension ref="A1:D5573"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5530" workbookViewId="0">
-      <selection activeCell="D5557" sqref="A5542:D5557"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="51.28515625" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -78836,8 +78833,8 @@
       </c>
     </row>
     <row r="5526" spans="1:4">
-      <c r="A5526" t="s">
-        <v>4</v>
+      <c r="A5526">
+        <v>1</v>
       </c>
       <c r="B5526" s="2">
         <v>44542</v>
@@ -78850,8 +78847,8 @@
       </c>
     </row>
     <row r="5527" spans="1:4">
-      <c r="A5527" t="s">
-        <v>5</v>
+      <c r="A5527">
+        <v>2</v>
       </c>
       <c r="B5527" s="2">
         <v>44542</v>
@@ -78864,8 +78861,8 @@
       </c>
     </row>
     <row r="5528" spans="1:4">
-      <c r="A5528" t="s">
-        <v>6</v>
+      <c r="A5528">
+        <v>3</v>
       </c>
       <c r="B5528" s="2">
         <v>44542</v>
@@ -78878,8 +78875,8 @@
       </c>
     </row>
     <row r="5529" spans="1:4">
-      <c r="A5529" t="s">
-        <v>7</v>
+      <c r="A5529">
+        <v>4</v>
       </c>
       <c r="B5529" s="2">
         <v>44542</v>
@@ -78892,8 +78889,8 @@
       </c>
     </row>
     <row r="5530" spans="1:4">
-      <c r="A5530" t="s">
-        <v>8</v>
+      <c r="A5530">
+        <v>5</v>
       </c>
       <c r="B5530" s="2">
         <v>44542</v>
@@ -78906,8 +78903,8 @@
       </c>
     </row>
     <row r="5531" spans="1:4">
-      <c r="A5531" t="s">
-        <v>9</v>
+      <c r="A5531">
+        <v>6</v>
       </c>
       <c r="B5531" s="2">
         <v>44542</v>
@@ -78920,8 +78917,8 @@
       </c>
     </row>
     <row r="5532" spans="1:4">
-      <c r="A5532" t="s">
-        <v>10</v>
+      <c r="A5532">
+        <v>7</v>
       </c>
       <c r="B5532" s="2">
         <v>44542</v>
@@ -78934,8 +78931,8 @@
       </c>
     </row>
     <row r="5533" spans="1:4">
-      <c r="A5533" t="s">
-        <v>11</v>
+      <c r="A5533">
+        <v>8</v>
       </c>
       <c r="B5533" s="2">
         <v>44542</v>
@@ -78948,8 +78945,8 @@
       </c>
     </row>
     <row r="5534" spans="1:4">
-      <c r="A5534" t="s">
-        <v>12</v>
+      <c r="A5534">
+        <v>9</v>
       </c>
       <c r="B5534" s="2">
         <v>44542</v>
@@ -78962,8 +78959,8 @@
       </c>
     </row>
     <row r="5535" spans="1:4">
-      <c r="A5535" t="s">
-        <v>13</v>
+      <c r="A5535">
+        <v>10</v>
       </c>
       <c r="B5535" s="2">
         <v>44542</v>
@@ -78976,8 +78973,8 @@
       </c>
     </row>
     <row r="5536" spans="1:4">
-      <c r="A5536" t="s">
-        <v>14</v>
+      <c r="A5536">
+        <v>11</v>
       </c>
       <c r="B5536" s="2">
         <v>44542</v>
@@ -78990,8 +78987,8 @@
       </c>
     </row>
     <row r="5537" spans="1:4">
-      <c r="A5537" t="s">
-        <v>15</v>
+      <c r="A5537">
+        <v>12</v>
       </c>
       <c r="B5537" s="2">
         <v>44542</v>
@@ -79004,8 +79001,8 @@
       </c>
     </row>
     <row r="5538" spans="1:4">
-      <c r="A5538" t="s">
-        <v>16</v>
+      <c r="A5538">
+        <v>13</v>
       </c>
       <c r="B5538" s="2">
         <v>44542</v>
@@ -79018,8 +79015,8 @@
       </c>
     </row>
     <row r="5539" spans="1:4">
-      <c r="A5539" t="s">
-        <v>17</v>
+      <c r="A5539">
+        <v>14</v>
       </c>
       <c r="B5539" s="2">
         <v>44542</v>
@@ -79032,8 +79029,8 @@
       </c>
     </row>
     <row r="5540" spans="1:4">
-      <c r="A5540" t="s">
-        <v>18</v>
+      <c r="A5540">
+        <v>15</v>
       </c>
       <c r="B5540" s="2">
         <v>44542</v>
@@ -79046,8 +79043,8 @@
       </c>
     </row>
     <row r="5541" spans="1:4">
-      <c r="A5541" t="s">
-        <v>19</v>
+      <c r="A5541">
+        <v>16</v>
       </c>
       <c r="B5541" s="2">
         <v>44542</v>
@@ -79060,52 +79057,452 @@
       </c>
     </row>
     <row r="5542" spans="1:4">
-      <c r="B5542" s="2"/>
+      <c r="A5542" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5542" s="2">
+        <v>44542</v>
+      </c>
+      <c r="C5542" t="s">
+        <v>365</v>
+      </c>
+      <c r="D5542">
+        <v>0</v>
+      </c>
     </row>
     <row r="5543" spans="1:4">
-      <c r="B5543" s="2"/>
+      <c r="A5543" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5543" s="2">
+        <v>44542</v>
+      </c>
+      <c r="C5543" t="s">
+        <v>365</v>
+      </c>
+      <c r="D5543">
+        <v>1</v>
+      </c>
     </row>
     <row r="5544" spans="1:4">
-      <c r="B5544" s="2"/>
+      <c r="A5544" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5544" s="2">
+        <v>44542</v>
+      </c>
+      <c r="C5544" t="s">
+        <v>365</v>
+      </c>
+      <c r="D5544">
+        <v>1</v>
+      </c>
     </row>
     <row r="5545" spans="1:4">
-      <c r="B5545" s="2"/>
+      <c r="A5545" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5545" s="2">
+        <v>44542</v>
+      </c>
+      <c r="C5545" t="s">
+        <v>365</v>
+      </c>
+      <c r="D5545">
+        <v>0</v>
+      </c>
     </row>
     <row r="5546" spans="1:4">
-      <c r="B5546" s="2"/>
+      <c r="A5546" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5546" s="2">
+        <v>44542</v>
+      </c>
+      <c r="C5546" t="s">
+        <v>365</v>
+      </c>
+      <c r="D5546">
+        <v>1</v>
+      </c>
     </row>
     <row r="5547" spans="1:4">
-      <c r="B5547" s="2"/>
+      <c r="A5547" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5547" s="2">
+        <v>44542</v>
+      </c>
+      <c r="C5547" t="s">
+        <v>365</v>
+      </c>
+      <c r="D5547">
+        <v>1</v>
+      </c>
     </row>
     <row r="5548" spans="1:4">
-      <c r="B5548" s="2"/>
+      <c r="A5548" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5548" s="2">
+        <v>44542</v>
+      </c>
+      <c r="C5548" t="s">
+        <v>365</v>
+      </c>
+      <c r="D5548">
+        <v>0</v>
+      </c>
     </row>
     <row r="5549" spans="1:4">
-      <c r="B5549" s="2"/>
+      <c r="A5549" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5549" s="2">
+        <v>44542</v>
+      </c>
+      <c r="C5549" t="s">
+        <v>365</v>
+      </c>
+      <c r="D5549">
+        <v>0</v>
+      </c>
     </row>
     <row r="5550" spans="1:4">
-      <c r="B5550" s="2"/>
+      <c r="A5550" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5550" s="2">
+        <v>44542</v>
+      </c>
+      <c r="C5550" t="s">
+        <v>365</v>
+      </c>
+      <c r="D5550">
+        <v>0</v>
+      </c>
     </row>
     <row r="5551" spans="1:4">
-      <c r="B5551" s="2"/>
+      <c r="A5551" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5551" s="2">
+        <v>44542</v>
+      </c>
+      <c r="C5551" t="s">
+        <v>365</v>
+      </c>
+      <c r="D5551">
+        <v>0</v>
+      </c>
     </row>
     <row r="5552" spans="1:4">
-      <c r="B5552" s="2"/>
-    </row>
-    <row r="5553" spans="2:2">
-      <c r="B5553" s="2"/>
-    </row>
-    <row r="5554" spans="2:2">
-      <c r="B5554" s="2"/>
-    </row>
-    <row r="5555" spans="2:2">
-      <c r="B5555" s="2"/>
-    </row>
-    <row r="5556" spans="2:2">
-      <c r="B5556" s="2"/>
-    </row>
-    <row r="5557" spans="2:2">
-      <c r="B5557" s="2"/>
+      <c r="A5552" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5552" s="2">
+        <v>44542</v>
+      </c>
+      <c r="C5552" t="s">
+        <v>365</v>
+      </c>
+      <c r="D5552">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5553" spans="1:4">
+      <c r="A5553" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5553" s="2">
+        <v>44542</v>
+      </c>
+      <c r="C5553" t="s">
+        <v>365</v>
+      </c>
+      <c r="D5553">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5554" spans="1:4">
+      <c r="A5554" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5554" s="2">
+        <v>44542</v>
+      </c>
+      <c r="C5554" t="s">
+        <v>365</v>
+      </c>
+      <c r="D5554">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5555" spans="1:4">
+      <c r="A5555" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5555" s="2">
+        <v>44542</v>
+      </c>
+      <c r="C5555" t="s">
+        <v>365</v>
+      </c>
+      <c r="D5555">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5556" spans="1:4">
+      <c r="A5556" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5556" s="2">
+        <v>44542</v>
+      </c>
+      <c r="C5556" t="s">
+        <v>365</v>
+      </c>
+      <c r="D5556">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5557" spans="1:4">
+      <c r="A5557" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5557" s="2">
+        <v>44542</v>
+      </c>
+      <c r="C5557" t="s">
+        <v>365</v>
+      </c>
+      <c r="D5557">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5558" spans="1:4">
+      <c r="A5558" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5558" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5558" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5558">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5559" spans="1:4">
+      <c r="A5559" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5559" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5559" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5559">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5560" spans="1:4">
+      <c r="A5560" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5560" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5560" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5560">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5561" spans="1:4">
+      <c r="A5561" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5561" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5561" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5561">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5562" spans="1:4">
+      <c r="A5562" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5562" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5562" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5562">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5563" spans="1:4">
+      <c r="A5563" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5563" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5563" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5563">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5564" spans="1:4">
+      <c r="A5564" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5564" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5564" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5564">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5565" spans="1:4">
+      <c r="A5565" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5565" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5565" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5565">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5566" spans="1:4">
+      <c r="A5566" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5566" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5566" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5566">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5567" spans="1:4">
+      <c r="A5567" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5567" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5567" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5567">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5568" spans="1:4">
+      <c r="A5568" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5568" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5568" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5568">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5569" spans="1:4">
+      <c r="A5569" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5569" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5569" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5569">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5570" spans="1:4">
+      <c r="A5570" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5570" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5570" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5570">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5571" spans="1:4">
+      <c r="A5571" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5571" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5571" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5571">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5572" spans="1:4">
+      <c r="A5572" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5572" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5572" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5572">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5573" spans="1:4">
+      <c r="A5573" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5573" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5573" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5573">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-17-2021 15-02-55
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11132" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11196" uniqueCount="369">
   <si>
     <t>Región</t>
   </si>
@@ -1116,6 +1116,12 @@
   <si>
     <t>2021-12-13</t>
   </si>
+  <si>
+    <t>2021-12-14</t>
+  </si>
+  <si>
+    <t>2021-12-15</t>
+  </si>
 </sst>
 </file>
 
@@ -1476,7 +1482,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5573"/>
+  <dimension ref="A1:D5621"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -79057,8 +79063,8 @@
       </c>
     </row>
     <row r="5542" spans="1:4">
-      <c r="A5542" t="s">
-        <v>4</v>
+      <c r="A5542">
+        <v>1</v>
       </c>
       <c r="B5542" s="2">
         <v>44542</v>
@@ -79071,8 +79077,8 @@
       </c>
     </row>
     <row r="5543" spans="1:4">
-      <c r="A5543" t="s">
-        <v>5</v>
+      <c r="A5543">
+        <v>2</v>
       </c>
       <c r="B5543" s="2">
         <v>44542</v>
@@ -79085,8 +79091,8 @@
       </c>
     </row>
     <row r="5544" spans="1:4">
-      <c r="A5544" t="s">
-        <v>6</v>
+      <c r="A5544">
+        <v>3</v>
       </c>
       <c r="B5544" s="2">
         <v>44542</v>
@@ -79099,8 +79105,8 @@
       </c>
     </row>
     <row r="5545" spans="1:4">
-      <c r="A5545" t="s">
-        <v>7</v>
+      <c r="A5545">
+        <v>4</v>
       </c>
       <c r="B5545" s="2">
         <v>44542</v>
@@ -79113,8 +79119,8 @@
       </c>
     </row>
     <row r="5546" spans="1:4">
-      <c r="A5546" t="s">
-        <v>8</v>
+      <c r="A5546">
+        <v>5</v>
       </c>
       <c r="B5546" s="2">
         <v>44542</v>
@@ -79127,8 +79133,8 @@
       </c>
     </row>
     <row r="5547" spans="1:4">
-      <c r="A5547" t="s">
-        <v>9</v>
+      <c r="A5547">
+        <v>6</v>
       </c>
       <c r="B5547" s="2">
         <v>44542</v>
@@ -79141,8 +79147,8 @@
       </c>
     </row>
     <row r="5548" spans="1:4">
-      <c r="A5548" t="s">
-        <v>10</v>
+      <c r="A5548">
+        <v>7</v>
       </c>
       <c r="B5548" s="2">
         <v>44542</v>
@@ -79155,8 +79161,8 @@
       </c>
     </row>
     <row r="5549" spans="1:4">
-      <c r="A5549" t="s">
-        <v>11</v>
+      <c r="A5549">
+        <v>8</v>
       </c>
       <c r="B5549" s="2">
         <v>44542</v>
@@ -79169,8 +79175,8 @@
       </c>
     </row>
     <row r="5550" spans="1:4">
-      <c r="A5550" t="s">
-        <v>12</v>
+      <c r="A5550">
+        <v>9</v>
       </c>
       <c r="B5550" s="2">
         <v>44542</v>
@@ -79183,8 +79189,8 @@
       </c>
     </row>
     <row r="5551" spans="1:4">
-      <c r="A5551" t="s">
-        <v>13</v>
+      <c r="A5551">
+        <v>10</v>
       </c>
       <c r="B5551" s="2">
         <v>44542</v>
@@ -79197,8 +79203,8 @@
       </c>
     </row>
     <row r="5552" spans="1:4">
-      <c r="A5552" t="s">
-        <v>14</v>
+      <c r="A5552">
+        <v>11</v>
       </c>
       <c r="B5552" s="2">
         <v>44542</v>
@@ -79211,8 +79217,8 @@
       </c>
     </row>
     <row r="5553" spans="1:4">
-      <c r="A5553" t="s">
-        <v>15</v>
+      <c r="A5553">
+        <v>12</v>
       </c>
       <c r="B5553" s="2">
         <v>44542</v>
@@ -79225,8 +79231,8 @@
       </c>
     </row>
     <row r="5554" spans="1:4">
-      <c r="A5554" t="s">
-        <v>16</v>
+      <c r="A5554">
+        <v>13</v>
       </c>
       <c r="B5554" s="2">
         <v>44542</v>
@@ -79239,8 +79245,8 @@
       </c>
     </row>
     <row r="5555" spans="1:4">
-      <c r="A5555" t="s">
-        <v>17</v>
+      <c r="A5555">
+        <v>14</v>
       </c>
       <c r="B5555" s="2">
         <v>44542</v>
@@ -79253,8 +79259,8 @@
       </c>
     </row>
     <row r="5556" spans="1:4">
-      <c r="A5556" t="s">
-        <v>18</v>
+      <c r="A5556">
+        <v>15</v>
       </c>
       <c r="B5556" s="2">
         <v>44542</v>
@@ -79267,8 +79273,8 @@
       </c>
     </row>
     <row r="5557" spans="1:4">
-      <c r="A5557" t="s">
-        <v>19</v>
+      <c r="A5557">
+        <v>16</v>
       </c>
       <c r="B5557" s="2">
         <v>44542</v>
@@ -79281,8 +79287,8 @@
       </c>
     </row>
     <row r="5558" spans="1:4">
-      <c r="A5558" t="s">
-        <v>4</v>
+      <c r="A5558">
+        <v>1</v>
       </c>
       <c r="B5558" s="2">
         <v>44543</v>
@@ -79295,8 +79301,8 @@
       </c>
     </row>
     <row r="5559" spans="1:4">
-      <c r="A5559" t="s">
-        <v>5</v>
+      <c r="A5559">
+        <v>2</v>
       </c>
       <c r="B5559" s="2">
         <v>44543</v>
@@ -79309,8 +79315,8 @@
       </c>
     </row>
     <row r="5560" spans="1:4">
-      <c r="A5560" t="s">
-        <v>6</v>
+      <c r="A5560">
+        <v>3</v>
       </c>
       <c r="B5560" s="2">
         <v>44543</v>
@@ -79323,8 +79329,8 @@
       </c>
     </row>
     <row r="5561" spans="1:4">
-      <c r="A5561" t="s">
-        <v>7</v>
+      <c r="A5561">
+        <v>4</v>
       </c>
       <c r="B5561" s="2">
         <v>44543</v>
@@ -79337,8 +79343,8 @@
       </c>
     </row>
     <row r="5562" spans="1:4">
-      <c r="A5562" t="s">
-        <v>8</v>
+      <c r="A5562">
+        <v>5</v>
       </c>
       <c r="B5562" s="2">
         <v>44543</v>
@@ -79351,8 +79357,8 @@
       </c>
     </row>
     <row r="5563" spans="1:4">
-      <c r="A5563" t="s">
-        <v>9</v>
+      <c r="A5563">
+        <v>6</v>
       </c>
       <c r="B5563" s="2">
         <v>44543</v>
@@ -79365,8 +79371,8 @@
       </c>
     </row>
     <row r="5564" spans="1:4">
-      <c r="A5564" t="s">
-        <v>10</v>
+      <c r="A5564">
+        <v>7</v>
       </c>
       <c r="B5564" s="2">
         <v>44543</v>
@@ -79379,8 +79385,8 @@
       </c>
     </row>
     <row r="5565" spans="1:4">
-      <c r="A5565" t="s">
-        <v>11</v>
+      <c r="A5565">
+        <v>8</v>
       </c>
       <c r="B5565" s="2">
         <v>44543</v>
@@ -79393,8 +79399,8 @@
       </c>
     </row>
     <row r="5566" spans="1:4">
-      <c r="A5566" t="s">
-        <v>12</v>
+      <c r="A5566">
+        <v>9</v>
       </c>
       <c r="B5566" s="2">
         <v>44543</v>
@@ -79407,8 +79413,8 @@
       </c>
     </row>
     <row r="5567" spans="1:4">
-      <c r="A5567" t="s">
-        <v>13</v>
+      <c r="A5567">
+        <v>10</v>
       </c>
       <c r="B5567" s="2">
         <v>44543</v>
@@ -79421,8 +79427,8 @@
       </c>
     </row>
     <row r="5568" spans="1:4">
-      <c r="A5568" t="s">
-        <v>14</v>
+      <c r="A5568">
+        <v>11</v>
       </c>
       <c r="B5568" s="2">
         <v>44543</v>
@@ -79435,8 +79441,8 @@
       </c>
     </row>
     <row r="5569" spans="1:4">
-      <c r="A5569" t="s">
-        <v>15</v>
+      <c r="A5569">
+        <v>12</v>
       </c>
       <c r="B5569" s="2">
         <v>44543</v>
@@ -79449,8 +79455,8 @@
       </c>
     </row>
     <row r="5570" spans="1:4">
-      <c r="A5570" t="s">
-        <v>16</v>
+      <c r="A5570">
+        <v>13</v>
       </c>
       <c r="B5570" s="2">
         <v>44543</v>
@@ -79463,8 +79469,8 @@
       </c>
     </row>
     <row r="5571" spans="1:4">
-      <c r="A5571" t="s">
-        <v>17</v>
+      <c r="A5571">
+        <v>14</v>
       </c>
       <c r="B5571" s="2">
         <v>44543</v>
@@ -79477,8 +79483,8 @@
       </c>
     </row>
     <row r="5572" spans="1:4">
-      <c r="A5572" t="s">
-        <v>18</v>
+      <c r="A5572">
+        <v>15</v>
       </c>
       <c r="B5572" s="2">
         <v>44543</v>
@@ -79491,8 +79497,8 @@
       </c>
     </row>
     <row r="5573" spans="1:4">
-      <c r="A5573" t="s">
-        <v>19</v>
+      <c r="A5573">
+        <v>16</v>
       </c>
       <c r="B5573" s="2">
         <v>44543</v>
@@ -79501,6 +79507,678 @@
         <v>366</v>
       </c>
       <c r="D5573">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5574" spans="1:4">
+      <c r="A5574" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5574" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5574" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5574">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5575" spans="1:4">
+      <c r="A5575" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5575" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5575" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5575">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5576" spans="1:4">
+      <c r="A5576" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5576" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5576" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5576">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5577" spans="1:4">
+      <c r="A5577" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5577" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5577" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5577">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5578" spans="1:4">
+      <c r="A5578" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5578" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5578" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5578">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5579" spans="1:4">
+      <c r="A5579" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5579" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5579" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5579">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5580" spans="1:4">
+      <c r="A5580" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5580" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5580" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5580">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5581" spans="1:4">
+      <c r="A5581" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5581" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5581" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5581">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5582" spans="1:4">
+      <c r="A5582" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5582" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5582" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5582">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5583" spans="1:4">
+      <c r="A5583" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5583" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5583" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5583">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5584" spans="1:4">
+      <c r="A5584" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5584" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5584" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5584">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5585" spans="1:4">
+      <c r="A5585" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5585" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5585" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5585">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5586" spans="1:4">
+      <c r="A5586" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5586" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5586" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5586">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5587" spans="1:4">
+      <c r="A5587" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5587" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5587" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5587">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5588" spans="1:4">
+      <c r="A5588" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5588" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5588" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5588">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5589" spans="1:4">
+      <c r="A5589" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5589" s="2">
+        <v>44543</v>
+      </c>
+      <c r="C5589" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5589">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5590" spans="1:4">
+      <c r="A5590" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5590" s="2">
+        <v>44544</v>
+      </c>
+      <c r="C5590" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5590">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5591" spans="1:4">
+      <c r="A5591" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5591" s="2">
+        <v>44544</v>
+      </c>
+      <c r="C5591" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5591">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5592" spans="1:4">
+      <c r="A5592" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5592" s="2">
+        <v>44544</v>
+      </c>
+      <c r="C5592" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5592">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5593" spans="1:4">
+      <c r="A5593" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5593" s="2">
+        <v>44544</v>
+      </c>
+      <c r="C5593" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5593">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5594" spans="1:4">
+      <c r="A5594" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5594" s="2">
+        <v>44544</v>
+      </c>
+      <c r="C5594" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5594">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5595" spans="1:4">
+      <c r="A5595" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5595" s="2">
+        <v>44544</v>
+      </c>
+      <c r="C5595" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5595">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5596" spans="1:4">
+      <c r="A5596" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5596" s="2">
+        <v>44544</v>
+      </c>
+      <c r="C5596" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5596">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5597" spans="1:4">
+      <c r="A5597" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5597" s="2">
+        <v>44544</v>
+      </c>
+      <c r="C5597" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5597">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5598" spans="1:4">
+      <c r="A5598" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5598" s="2">
+        <v>44544</v>
+      </c>
+      <c r="C5598" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5598">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5599" spans="1:4">
+      <c r="A5599" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5599" s="2">
+        <v>44544</v>
+      </c>
+      <c r="C5599" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5599">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5600" spans="1:4">
+      <c r="A5600" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5600" s="2">
+        <v>44544</v>
+      </c>
+      <c r="C5600" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5600">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5601" spans="1:4">
+      <c r="A5601" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5601" s="2">
+        <v>44544</v>
+      </c>
+      <c r="C5601" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5601">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5602" spans="1:4">
+      <c r="A5602" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5602" s="2">
+        <v>44544</v>
+      </c>
+      <c r="C5602" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5602">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5603" spans="1:4">
+      <c r="A5603" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5603" s="2">
+        <v>44544</v>
+      </c>
+      <c r="C5603" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5603">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5604" spans="1:4">
+      <c r="A5604" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5604" s="2">
+        <v>44544</v>
+      </c>
+      <c r="C5604" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5604">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5605" spans="1:4">
+      <c r="A5605" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5605" s="2">
+        <v>44544</v>
+      </c>
+      <c r="C5605" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5605">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5606" spans="1:4">
+      <c r="A5606" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5606" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5606" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5606">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5607" spans="1:4">
+      <c r="A5607" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5607" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5607" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5607">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5608" spans="1:4">
+      <c r="A5608" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5608" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5608" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5608">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5609" spans="1:4">
+      <c r="A5609" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5609" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5609" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5609">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5610" spans="1:4">
+      <c r="A5610" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5610" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5610" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5610">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5611" spans="1:4">
+      <c r="A5611" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5611" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5611" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5611">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5612" spans="1:4">
+      <c r="A5612" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5612" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5612" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5612">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5613" spans="1:4">
+      <c r="A5613" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5613" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5613" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5613">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5614" spans="1:4">
+      <c r="A5614" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5614" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5614" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5614">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5615" spans="1:4">
+      <c r="A5615" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5615" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5615" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5615">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5616" spans="1:4">
+      <c r="A5616" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5616" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5616" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5616">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5617" spans="1:4">
+      <c r="A5617" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5617" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5617" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5617">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5618" spans="1:4">
+      <c r="A5618" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5618" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5618" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5618">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5619" spans="1:4">
+      <c r="A5619" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5619" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5619" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5619">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5620" spans="1:4">
+      <c r="A5620" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5620" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5620" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5620">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5621" spans="1:4">
+      <c r="A5621" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5621" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5621" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5621">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-18-2021 15-34-36
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11196" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11212" uniqueCount="370">
   <si>
     <t>Región</t>
   </si>
@@ -1122,6 +1122,9 @@
   <si>
     <t>2021-12-15</t>
   </si>
+  <si>
+    <t>2021-12-16</t>
+  </si>
 </sst>
 </file>
 
@@ -1482,7 +1485,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5621"/>
+  <dimension ref="A1:D5653"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -79511,8 +79514,8 @@
       </c>
     </row>
     <row r="5574" spans="1:4">
-      <c r="A5574" t="s">
-        <v>4</v>
+      <c r="A5574">
+        <v>1</v>
       </c>
       <c r="B5574" s="2">
         <v>44543</v>
@@ -79525,8 +79528,8 @@
       </c>
     </row>
     <row r="5575" spans="1:4">
-      <c r="A5575" t="s">
-        <v>5</v>
+      <c r="A5575">
+        <v>2</v>
       </c>
       <c r="B5575" s="2">
         <v>44543</v>
@@ -79539,8 +79542,8 @@
       </c>
     </row>
     <row r="5576" spans="1:4">
-      <c r="A5576" t="s">
-        <v>6</v>
+      <c r="A5576">
+        <v>3</v>
       </c>
       <c r="B5576" s="2">
         <v>44543</v>
@@ -79553,8 +79556,8 @@
       </c>
     </row>
     <row r="5577" spans="1:4">
-      <c r="A5577" t="s">
-        <v>7</v>
+      <c r="A5577">
+        <v>4</v>
       </c>
       <c r="B5577" s="2">
         <v>44543</v>
@@ -79567,8 +79570,8 @@
       </c>
     </row>
     <row r="5578" spans="1:4">
-      <c r="A5578" t="s">
-        <v>8</v>
+      <c r="A5578">
+        <v>5</v>
       </c>
       <c r="B5578" s="2">
         <v>44543</v>
@@ -79581,8 +79584,8 @@
       </c>
     </row>
     <row r="5579" spans="1:4">
-      <c r="A5579" t="s">
-        <v>9</v>
+      <c r="A5579">
+        <v>6</v>
       </c>
       <c r="B5579" s="2">
         <v>44543</v>
@@ -79595,8 +79598,8 @@
       </c>
     </row>
     <row r="5580" spans="1:4">
-      <c r="A5580" t="s">
-        <v>10</v>
+      <c r="A5580">
+        <v>7</v>
       </c>
       <c r="B5580" s="2">
         <v>44543</v>
@@ -79609,8 +79612,8 @@
       </c>
     </row>
     <row r="5581" spans="1:4">
-      <c r="A5581" t="s">
-        <v>11</v>
+      <c r="A5581">
+        <v>8</v>
       </c>
       <c r="B5581" s="2">
         <v>44543</v>
@@ -79623,8 +79626,8 @@
       </c>
     </row>
     <row r="5582" spans="1:4">
-      <c r="A5582" t="s">
-        <v>12</v>
+      <c r="A5582">
+        <v>9</v>
       </c>
       <c r="B5582" s="2">
         <v>44543</v>
@@ -79637,8 +79640,8 @@
       </c>
     </row>
     <row r="5583" spans="1:4">
-      <c r="A5583" t="s">
-        <v>13</v>
+      <c r="A5583">
+        <v>10</v>
       </c>
       <c r="B5583" s="2">
         <v>44543</v>
@@ -79651,8 +79654,8 @@
       </c>
     </row>
     <row r="5584" spans="1:4">
-      <c r="A5584" t="s">
-        <v>14</v>
+      <c r="A5584">
+        <v>11</v>
       </c>
       <c r="B5584" s="2">
         <v>44543</v>
@@ -79665,8 +79668,8 @@
       </c>
     </row>
     <row r="5585" spans="1:4">
-      <c r="A5585" t="s">
-        <v>15</v>
+      <c r="A5585">
+        <v>12</v>
       </c>
       <c r="B5585" s="2">
         <v>44543</v>
@@ -79679,8 +79682,8 @@
       </c>
     </row>
     <row r="5586" spans="1:4">
-      <c r="A5586" t="s">
-        <v>16</v>
+      <c r="A5586">
+        <v>13</v>
       </c>
       <c r="B5586" s="2">
         <v>44543</v>
@@ -79693,8 +79696,8 @@
       </c>
     </row>
     <row r="5587" spans="1:4">
-      <c r="A5587" t="s">
-        <v>17</v>
+      <c r="A5587">
+        <v>14</v>
       </c>
       <c r="B5587" s="2">
         <v>44543</v>
@@ -79707,8 +79710,8 @@
       </c>
     </row>
     <row r="5588" spans="1:4">
-      <c r="A5588" t="s">
-        <v>18</v>
+      <c r="A5588">
+        <v>15</v>
       </c>
       <c r="B5588" s="2">
         <v>44543</v>
@@ -79721,8 +79724,8 @@
       </c>
     </row>
     <row r="5589" spans="1:4">
-      <c r="A5589" t="s">
-        <v>19</v>
+      <c r="A5589">
+        <v>16</v>
       </c>
       <c r="B5589" s="2">
         <v>44543</v>
@@ -79735,8 +79738,8 @@
       </c>
     </row>
     <row r="5590" spans="1:4">
-      <c r="A5590" t="s">
-        <v>4</v>
+      <c r="A5590">
+        <v>1</v>
       </c>
       <c r="B5590" s="2">
         <v>44544</v>
@@ -79749,8 +79752,8 @@
       </c>
     </row>
     <row r="5591" spans="1:4">
-      <c r="A5591" t="s">
-        <v>5</v>
+      <c r="A5591">
+        <v>2</v>
       </c>
       <c r="B5591" s="2">
         <v>44544</v>
@@ -79763,8 +79766,8 @@
       </c>
     </row>
     <row r="5592" spans="1:4">
-      <c r="A5592" t="s">
-        <v>6</v>
+      <c r="A5592">
+        <v>3</v>
       </c>
       <c r="B5592" s="2">
         <v>44544</v>
@@ -79777,8 +79780,8 @@
       </c>
     </row>
     <row r="5593" spans="1:4">
-      <c r="A5593" t="s">
-        <v>7</v>
+      <c r="A5593">
+        <v>4</v>
       </c>
       <c r="B5593" s="2">
         <v>44544</v>
@@ -79791,8 +79794,8 @@
       </c>
     </row>
     <row r="5594" spans="1:4">
-      <c r="A5594" t="s">
-        <v>8</v>
+      <c r="A5594">
+        <v>5</v>
       </c>
       <c r="B5594" s="2">
         <v>44544</v>
@@ -79805,8 +79808,8 @@
       </c>
     </row>
     <row r="5595" spans="1:4">
-      <c r="A5595" t="s">
-        <v>9</v>
+      <c r="A5595">
+        <v>6</v>
       </c>
       <c r="B5595" s="2">
         <v>44544</v>
@@ -79819,8 +79822,8 @@
       </c>
     </row>
     <row r="5596" spans="1:4">
-      <c r="A5596" t="s">
-        <v>10</v>
+      <c r="A5596">
+        <v>7</v>
       </c>
       <c r="B5596" s="2">
         <v>44544</v>
@@ -79833,8 +79836,8 @@
       </c>
     </row>
     <row r="5597" spans="1:4">
-      <c r="A5597" t="s">
-        <v>11</v>
+      <c r="A5597">
+        <v>8</v>
       </c>
       <c r="B5597" s="2">
         <v>44544</v>
@@ -79847,8 +79850,8 @@
       </c>
     </row>
     <row r="5598" spans="1:4">
-      <c r="A5598" t="s">
-        <v>12</v>
+      <c r="A5598">
+        <v>9</v>
       </c>
       <c r="B5598" s="2">
         <v>44544</v>
@@ -79861,8 +79864,8 @@
       </c>
     </row>
     <row r="5599" spans="1:4">
-      <c r="A5599" t="s">
-        <v>13</v>
+      <c r="A5599">
+        <v>10</v>
       </c>
       <c r="B5599" s="2">
         <v>44544</v>
@@ -79875,8 +79878,8 @@
       </c>
     </row>
     <row r="5600" spans="1:4">
-      <c r="A5600" t="s">
-        <v>14</v>
+      <c r="A5600">
+        <v>11</v>
       </c>
       <c r="B5600" s="2">
         <v>44544</v>
@@ -79889,8 +79892,8 @@
       </c>
     </row>
     <row r="5601" spans="1:4">
-      <c r="A5601" t="s">
-        <v>15</v>
+      <c r="A5601">
+        <v>12</v>
       </c>
       <c r="B5601" s="2">
         <v>44544</v>
@@ -79903,8 +79906,8 @@
       </c>
     </row>
     <row r="5602" spans="1:4">
-      <c r="A5602" t="s">
-        <v>16</v>
+      <c r="A5602">
+        <v>13</v>
       </c>
       <c r="B5602" s="2">
         <v>44544</v>
@@ -79917,8 +79920,8 @@
       </c>
     </row>
     <row r="5603" spans="1:4">
-      <c r="A5603" t="s">
-        <v>17</v>
+      <c r="A5603">
+        <v>14</v>
       </c>
       <c r="B5603" s="2">
         <v>44544</v>
@@ -79931,8 +79934,8 @@
       </c>
     </row>
     <row r="5604" spans="1:4">
-      <c r="A5604" t="s">
-        <v>18</v>
+      <c r="A5604">
+        <v>15</v>
       </c>
       <c r="B5604" s="2">
         <v>44544</v>
@@ -79945,8 +79948,8 @@
       </c>
     </row>
     <row r="5605" spans="1:4">
-      <c r="A5605" t="s">
-        <v>19</v>
+      <c r="A5605">
+        <v>16</v>
       </c>
       <c r="B5605" s="2">
         <v>44544</v>
@@ -79959,8 +79962,8 @@
       </c>
     </row>
     <row r="5606" spans="1:4">
-      <c r="A5606" t="s">
-        <v>4</v>
+      <c r="A5606">
+        <v>1</v>
       </c>
       <c r="B5606" s="2">
         <v>44545</v>
@@ -79973,8 +79976,8 @@
       </c>
     </row>
     <row r="5607" spans="1:4">
-      <c r="A5607" t="s">
-        <v>5</v>
+      <c r="A5607">
+        <v>2</v>
       </c>
       <c r="B5607" s="2">
         <v>44545</v>
@@ -79987,8 +79990,8 @@
       </c>
     </row>
     <row r="5608" spans="1:4">
-      <c r="A5608" t="s">
-        <v>6</v>
+      <c r="A5608">
+        <v>3</v>
       </c>
       <c r="B5608" s="2">
         <v>44545</v>
@@ -80001,8 +80004,8 @@
       </c>
     </row>
     <row r="5609" spans="1:4">
-      <c r="A5609" t="s">
-        <v>7</v>
+      <c r="A5609">
+        <v>4</v>
       </c>
       <c r="B5609" s="2">
         <v>44545</v>
@@ -80015,8 +80018,8 @@
       </c>
     </row>
     <row r="5610" spans="1:4">
-      <c r="A5610" t="s">
-        <v>8</v>
+      <c r="A5610">
+        <v>5</v>
       </c>
       <c r="B5610" s="2">
         <v>44545</v>
@@ -80029,8 +80032,8 @@
       </c>
     </row>
     <row r="5611" spans="1:4">
-      <c r="A5611" t="s">
-        <v>9</v>
+      <c r="A5611">
+        <v>6</v>
       </c>
       <c r="B5611" s="2">
         <v>44545</v>
@@ -80043,8 +80046,8 @@
       </c>
     </row>
     <row r="5612" spans="1:4">
-      <c r="A5612" t="s">
-        <v>10</v>
+      <c r="A5612">
+        <v>7</v>
       </c>
       <c r="B5612" s="2">
         <v>44545</v>
@@ -80057,8 +80060,8 @@
       </c>
     </row>
     <row r="5613" spans="1:4">
-      <c r="A5613" t="s">
-        <v>11</v>
+      <c r="A5613">
+        <v>8</v>
       </c>
       <c r="B5613" s="2">
         <v>44545</v>
@@ -80071,8 +80074,8 @@
       </c>
     </row>
     <row r="5614" spans="1:4">
-      <c r="A5614" t="s">
-        <v>12</v>
+      <c r="A5614">
+        <v>9</v>
       </c>
       <c r="B5614" s="2">
         <v>44545</v>
@@ -80085,8 +80088,8 @@
       </c>
     </row>
     <row r="5615" spans="1:4">
-      <c r="A5615" t="s">
-        <v>13</v>
+      <c r="A5615">
+        <v>10</v>
       </c>
       <c r="B5615" s="2">
         <v>44545</v>
@@ -80099,8 +80102,8 @@
       </c>
     </row>
     <row r="5616" spans="1:4">
-      <c r="A5616" t="s">
-        <v>14</v>
+      <c r="A5616">
+        <v>11</v>
       </c>
       <c r="B5616" s="2">
         <v>44545</v>
@@ -80113,8 +80116,8 @@
       </c>
     </row>
     <row r="5617" spans="1:4">
-      <c r="A5617" t="s">
-        <v>15</v>
+      <c r="A5617">
+        <v>12</v>
       </c>
       <c r="B5617" s="2">
         <v>44545</v>
@@ -80127,8 +80130,8 @@
       </c>
     </row>
     <row r="5618" spans="1:4">
-      <c r="A5618" t="s">
-        <v>16</v>
+      <c r="A5618">
+        <v>13</v>
       </c>
       <c r="B5618" s="2">
         <v>44545</v>
@@ -80141,8 +80144,8 @@
       </c>
     </row>
     <row r="5619" spans="1:4">
-      <c r="A5619" t="s">
-        <v>17</v>
+      <c r="A5619">
+        <v>14</v>
       </c>
       <c r="B5619" s="2">
         <v>44545</v>
@@ -80155,8 +80158,8 @@
       </c>
     </row>
     <row r="5620" spans="1:4">
-      <c r="A5620" t="s">
-        <v>18</v>
+      <c r="A5620">
+        <v>15</v>
       </c>
       <c r="B5620" s="2">
         <v>44545</v>
@@ -80169,8 +80172,8 @@
       </c>
     </row>
     <row r="5621" spans="1:4">
-      <c r="A5621" t="s">
-        <v>19</v>
+      <c r="A5621">
+        <v>16</v>
       </c>
       <c r="B5621" s="2">
         <v>44545</v>
@@ -80180,6 +80183,454 @@
       </c>
       <c r="D5621">
         <v>0</v>
+      </c>
+    </row>
+    <row r="5622" spans="1:4">
+      <c r="A5622" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5622" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5622" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5622">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5623" spans="1:4">
+      <c r="A5623" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5623" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5623" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5623">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5624" spans="1:4">
+      <c r="A5624" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5624" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5624" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5624">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5625" spans="1:4">
+      <c r="A5625" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5625" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5625" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5625">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5626" spans="1:4">
+      <c r="A5626" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5626" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5626" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5626">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5627" spans="1:4">
+      <c r="A5627" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5627" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5627" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5627">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5628" spans="1:4">
+      <c r="A5628" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5628" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5628" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5628">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5629" spans="1:4">
+      <c r="A5629" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5629" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5629" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5629">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5630" spans="1:4">
+      <c r="A5630" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5630" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5630" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5630">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5631" spans="1:4">
+      <c r="A5631" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5631" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5631" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5631">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5632" spans="1:4">
+      <c r="A5632" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5632" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5632" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5632">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5633" spans="1:4">
+      <c r="A5633" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5633" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5633" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5633">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5634" spans="1:4">
+      <c r="A5634" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5634" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5634" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5634">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5635" spans="1:4">
+      <c r="A5635" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5635" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5635" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5635">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5636" spans="1:4">
+      <c r="A5636" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5636" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5636" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5636">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5637" spans="1:4">
+      <c r="A5637" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5637" s="2">
+        <v>44545</v>
+      </c>
+      <c r="C5637" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5637">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5638" spans="1:4">
+      <c r="A5638" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5638" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5638" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5638">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5639" spans="1:4">
+      <c r="A5639" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5639" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5639" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5639">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5640" spans="1:4">
+      <c r="A5640" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5640" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5640" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5640">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5641" spans="1:4">
+      <c r="A5641" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5641" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5641" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5641">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5642" spans="1:4">
+      <c r="A5642" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5642" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5642" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5642">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5643" spans="1:4">
+      <c r="A5643" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5643" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5643" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5643">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5644" spans="1:4">
+      <c r="A5644" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5644" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5644" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5644">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5645" spans="1:4">
+      <c r="A5645" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5645" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5645" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5645">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5646" spans="1:4">
+      <c r="A5646" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5646" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5646" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5646">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5647" spans="1:4">
+      <c r="A5647" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5647" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5647" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5647">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5648" spans="1:4">
+      <c r="A5648" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5648" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5648" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5648">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5649" spans="1:4">
+      <c r="A5649" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5649" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5649" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5649">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5650" spans="1:4">
+      <c r="A5650" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5650" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5650" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5650">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5651" spans="1:4">
+      <c r="A5651" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5651" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5651" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5651">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5652" spans="1:4">
+      <c r="A5652" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5652" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5652" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5652">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5653" spans="1:4">
+      <c r="A5653" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5653" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5653" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5653">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-19-2021 16-04-00
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11212" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11244" uniqueCount="371">
   <si>
     <t>Región</t>
   </si>
@@ -1125,6 +1125,9 @@
   <si>
     <t>2021-12-16</t>
   </si>
+  <si>
+    <t>2021-12-17</t>
+  </si>
 </sst>
 </file>
 
@@ -1485,7 +1488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5653"/>
+  <dimension ref="A1:D5685"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -80186,8 +80189,8 @@
       </c>
     </row>
     <row r="5622" spans="1:4">
-      <c r="A5622" t="s">
-        <v>4</v>
+      <c r="A5622">
+        <v>1</v>
       </c>
       <c r="B5622" s="2">
         <v>44545</v>
@@ -80200,8 +80203,8 @@
       </c>
     </row>
     <row r="5623" spans="1:4">
-      <c r="A5623" t="s">
-        <v>5</v>
+      <c r="A5623">
+        <v>2</v>
       </c>
       <c r="B5623" s="2">
         <v>44545</v>
@@ -80214,8 +80217,8 @@
       </c>
     </row>
     <row r="5624" spans="1:4">
-      <c r="A5624" t="s">
-        <v>6</v>
+      <c r="A5624">
+        <v>3</v>
       </c>
       <c r="B5624" s="2">
         <v>44545</v>
@@ -80228,8 +80231,8 @@
       </c>
     </row>
     <row r="5625" spans="1:4">
-      <c r="A5625" t="s">
-        <v>7</v>
+      <c r="A5625">
+        <v>4</v>
       </c>
       <c r="B5625" s="2">
         <v>44545</v>
@@ -80242,8 +80245,8 @@
       </c>
     </row>
     <row r="5626" spans="1:4">
-      <c r="A5626" t="s">
-        <v>8</v>
+      <c r="A5626">
+        <v>5</v>
       </c>
       <c r="B5626" s="2">
         <v>44545</v>
@@ -80256,8 +80259,8 @@
       </c>
     </row>
     <row r="5627" spans="1:4">
-      <c r="A5627" t="s">
-        <v>9</v>
+      <c r="A5627">
+        <v>6</v>
       </c>
       <c r="B5627" s="2">
         <v>44545</v>
@@ -80270,8 +80273,8 @@
       </c>
     </row>
     <row r="5628" spans="1:4">
-      <c r="A5628" t="s">
-        <v>10</v>
+      <c r="A5628">
+        <v>7</v>
       </c>
       <c r="B5628" s="2">
         <v>44545</v>
@@ -80284,8 +80287,8 @@
       </c>
     </row>
     <row r="5629" spans="1:4">
-      <c r="A5629" t="s">
-        <v>11</v>
+      <c r="A5629">
+        <v>8</v>
       </c>
       <c r="B5629" s="2">
         <v>44545</v>
@@ -80298,8 +80301,8 @@
       </c>
     </row>
     <row r="5630" spans="1:4">
-      <c r="A5630" t="s">
-        <v>12</v>
+      <c r="A5630">
+        <v>9</v>
       </c>
       <c r="B5630" s="2">
         <v>44545</v>
@@ -80312,8 +80315,8 @@
       </c>
     </row>
     <row r="5631" spans="1:4">
-      <c r="A5631" t="s">
-        <v>13</v>
+      <c r="A5631">
+        <v>10</v>
       </c>
       <c r="B5631" s="2">
         <v>44545</v>
@@ -80326,8 +80329,8 @@
       </c>
     </row>
     <row r="5632" spans="1:4">
-      <c r="A5632" t="s">
-        <v>14</v>
+      <c r="A5632">
+        <v>11</v>
       </c>
       <c r="B5632" s="2">
         <v>44545</v>
@@ -80340,8 +80343,8 @@
       </c>
     </row>
     <row r="5633" spans="1:4">
-      <c r="A5633" t="s">
-        <v>15</v>
+      <c r="A5633">
+        <v>12</v>
       </c>
       <c r="B5633" s="2">
         <v>44545</v>
@@ -80354,8 +80357,8 @@
       </c>
     </row>
     <row r="5634" spans="1:4">
-      <c r="A5634" t="s">
-        <v>16</v>
+      <c r="A5634">
+        <v>13</v>
       </c>
       <c r="B5634" s="2">
         <v>44545</v>
@@ -80368,8 +80371,8 @@
       </c>
     </row>
     <row r="5635" spans="1:4">
-      <c r="A5635" t="s">
-        <v>17</v>
+      <c r="A5635">
+        <v>14</v>
       </c>
       <c r="B5635" s="2">
         <v>44545</v>
@@ -80382,8 +80385,8 @@
       </c>
     </row>
     <row r="5636" spans="1:4">
-      <c r="A5636" t="s">
-        <v>18</v>
+      <c r="A5636">
+        <v>15</v>
       </c>
       <c r="B5636" s="2">
         <v>44545</v>
@@ -80396,8 +80399,8 @@
       </c>
     </row>
     <row r="5637" spans="1:4">
-      <c r="A5637" t="s">
-        <v>19</v>
+      <c r="A5637">
+        <v>16</v>
       </c>
       <c r="B5637" s="2">
         <v>44545</v>
@@ -80410,8 +80413,8 @@
       </c>
     </row>
     <row r="5638" spans="1:4">
-      <c r="A5638" t="s">
-        <v>4</v>
+      <c r="A5638">
+        <v>1</v>
       </c>
       <c r="B5638" s="2">
         <v>44546</v>
@@ -80424,8 +80427,8 @@
       </c>
     </row>
     <row r="5639" spans="1:4">
-      <c r="A5639" t="s">
-        <v>5</v>
+      <c r="A5639">
+        <v>2</v>
       </c>
       <c r="B5639" s="2">
         <v>44546</v>
@@ -80438,8 +80441,8 @@
       </c>
     </row>
     <row r="5640" spans="1:4">
-      <c r="A5640" t="s">
-        <v>6</v>
+      <c r="A5640">
+        <v>3</v>
       </c>
       <c r="B5640" s="2">
         <v>44546</v>
@@ -80452,8 +80455,8 @@
       </c>
     </row>
     <row r="5641" spans="1:4">
-      <c r="A5641" t="s">
-        <v>7</v>
+      <c r="A5641">
+        <v>4</v>
       </c>
       <c r="B5641" s="2">
         <v>44546</v>
@@ -80466,8 +80469,8 @@
       </c>
     </row>
     <row r="5642" spans="1:4">
-      <c r="A5642" t="s">
-        <v>8</v>
+      <c r="A5642">
+        <v>5</v>
       </c>
       <c r="B5642" s="2">
         <v>44546</v>
@@ -80480,8 +80483,8 @@
       </c>
     </row>
     <row r="5643" spans="1:4">
-      <c r="A5643" t="s">
-        <v>9</v>
+      <c r="A5643">
+        <v>6</v>
       </c>
       <c r="B5643" s="2">
         <v>44546</v>
@@ -80494,8 +80497,8 @@
       </c>
     </row>
     <row r="5644" spans="1:4">
-      <c r="A5644" t="s">
-        <v>10</v>
+      <c r="A5644">
+        <v>7</v>
       </c>
       <c r="B5644" s="2">
         <v>44546</v>
@@ -80508,8 +80511,8 @@
       </c>
     </row>
     <row r="5645" spans="1:4">
-      <c r="A5645" t="s">
-        <v>11</v>
+      <c r="A5645">
+        <v>8</v>
       </c>
       <c r="B5645" s="2">
         <v>44546</v>
@@ -80522,8 +80525,8 @@
       </c>
     </row>
     <row r="5646" spans="1:4">
-      <c r="A5646" t="s">
-        <v>12</v>
+      <c r="A5646">
+        <v>9</v>
       </c>
       <c r="B5646" s="2">
         <v>44546</v>
@@ -80536,8 +80539,8 @@
       </c>
     </row>
     <row r="5647" spans="1:4">
-      <c r="A5647" t="s">
-        <v>13</v>
+      <c r="A5647">
+        <v>10</v>
       </c>
       <c r="B5647" s="2">
         <v>44546</v>
@@ -80550,8 +80553,8 @@
       </c>
     </row>
     <row r="5648" spans="1:4">
-      <c r="A5648" t="s">
-        <v>14</v>
+      <c r="A5648">
+        <v>11</v>
       </c>
       <c r="B5648" s="2">
         <v>44546</v>
@@ -80564,8 +80567,8 @@
       </c>
     </row>
     <row r="5649" spans="1:4">
-      <c r="A5649" t="s">
-        <v>15</v>
+      <c r="A5649">
+        <v>12</v>
       </c>
       <c r="B5649" s="2">
         <v>44546</v>
@@ -80578,8 +80581,8 @@
       </c>
     </row>
     <row r="5650" spans="1:4">
-      <c r="A5650" t="s">
-        <v>16</v>
+      <c r="A5650">
+        <v>13</v>
       </c>
       <c r="B5650" s="2">
         <v>44546</v>
@@ -80592,8 +80595,8 @@
       </c>
     </row>
     <row r="5651" spans="1:4">
-      <c r="A5651" t="s">
-        <v>17</v>
+      <c r="A5651">
+        <v>14</v>
       </c>
       <c r="B5651" s="2">
         <v>44546</v>
@@ -80606,8 +80609,8 @@
       </c>
     </row>
     <row r="5652" spans="1:4">
-      <c r="A5652" t="s">
-        <v>18</v>
+      <c r="A5652">
+        <v>15</v>
       </c>
       <c r="B5652" s="2">
         <v>44546</v>
@@ -80620,8 +80623,8 @@
       </c>
     </row>
     <row r="5653" spans="1:4">
-      <c r="A5653" t="s">
-        <v>19</v>
+      <c r="A5653">
+        <v>16</v>
       </c>
       <c r="B5653" s="2">
         <v>44546</v>
@@ -80630,6 +80633,454 @@
         <v>369</v>
       </c>
       <c r="D5653">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5654" spans="1:4">
+      <c r="A5654" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5654" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5654" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5654">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5655" spans="1:4">
+      <c r="A5655" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5655" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5655" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5655">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5656" spans="1:4">
+      <c r="A5656" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5656" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5656" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5656">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5657" spans="1:4">
+      <c r="A5657" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5657" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5657" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5657">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5658" spans="1:4">
+      <c r="A5658" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5658" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5658" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5658">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5659" spans="1:4">
+      <c r="A5659" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5659" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5659" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5659">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5660" spans="1:4">
+      <c r="A5660" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5660" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5660" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5660">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5661" spans="1:4">
+      <c r="A5661" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5661" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5661" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5661">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5662" spans="1:4">
+      <c r="A5662" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5662" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5662" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5662">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5663" spans="1:4">
+      <c r="A5663" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5663" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5663" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5663">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5664" spans="1:4">
+      <c r="A5664" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5664" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5664" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5664">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5665" spans="1:4">
+      <c r="A5665" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5665" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5665" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5665">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5666" spans="1:4">
+      <c r="A5666" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5666" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5666" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5666">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5667" spans="1:4">
+      <c r="A5667" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5667" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5667" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5667">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5668" spans="1:4">
+      <c r="A5668" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5668" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5668" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5668">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5669" spans="1:4">
+      <c r="A5669" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5669" s="2">
+        <v>44546</v>
+      </c>
+      <c r="C5669" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5669">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5670" spans="1:4">
+      <c r="A5670" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5670" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5670" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5670">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5671" spans="1:4">
+      <c r="A5671" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5671" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5671" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5671">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5672" spans="1:4">
+      <c r="A5672" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5672" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5672" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5672">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5673" spans="1:4">
+      <c r="A5673" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5673" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5673" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5673">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5674" spans="1:4">
+      <c r="A5674" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5674" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5674" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5674">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5675" spans="1:4">
+      <c r="A5675" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5675" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5675" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5675">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5676" spans="1:4">
+      <c r="A5676" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5676" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5676" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5676">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5677" spans="1:4">
+      <c r="A5677" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5677" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5677" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5677">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5678" spans="1:4">
+      <c r="A5678" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5678" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5678" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5678">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5679" spans="1:4">
+      <c r="A5679" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5679" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5679" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5679">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5680" spans="1:4">
+      <c r="A5680" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5680" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5680" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5680">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5681" spans="1:4">
+      <c r="A5681" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5681" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5681" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5681">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5682" spans="1:4">
+      <c r="A5682" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5682" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5682" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5682">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5683" spans="1:4">
+      <c r="A5683" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5683" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5683" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5683">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5684" spans="1:4">
+      <c r="A5684" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5684" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5684" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5684">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5685" spans="1:4">
+      <c r="A5685" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5685" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5685" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5685">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-20-2021 16-38-52
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11244" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11276" uniqueCount="372">
   <si>
     <t>Región</t>
   </si>
@@ -1128,6 +1128,9 @@
   <si>
     <t>2021-12-17</t>
   </si>
+  <si>
+    <t>2021-12-18</t>
+  </si>
 </sst>
 </file>
 
@@ -1488,7 +1491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5685"/>
+  <dimension ref="A1:D5717"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -80637,8 +80640,8 @@
       </c>
     </row>
     <row r="5654" spans="1:4">
-      <c r="A5654" t="s">
-        <v>4</v>
+      <c r="A5654">
+        <v>1</v>
       </c>
       <c r="B5654" s="2">
         <v>44546</v>
@@ -80651,8 +80654,8 @@
       </c>
     </row>
     <row r="5655" spans="1:4">
-      <c r="A5655" t="s">
-        <v>5</v>
+      <c r="A5655">
+        <v>2</v>
       </c>
       <c r="B5655" s="2">
         <v>44546</v>
@@ -80665,8 +80668,8 @@
       </c>
     </row>
     <row r="5656" spans="1:4">
-      <c r="A5656" t="s">
-        <v>6</v>
+      <c r="A5656">
+        <v>3</v>
       </c>
       <c r="B5656" s="2">
         <v>44546</v>
@@ -80679,8 +80682,8 @@
       </c>
     </row>
     <row r="5657" spans="1:4">
-      <c r="A5657" t="s">
-        <v>7</v>
+      <c r="A5657">
+        <v>4</v>
       </c>
       <c r="B5657" s="2">
         <v>44546</v>
@@ -80693,8 +80696,8 @@
       </c>
     </row>
     <row r="5658" spans="1:4">
-      <c r="A5658" t="s">
-        <v>8</v>
+      <c r="A5658">
+        <v>5</v>
       </c>
       <c r="B5658" s="2">
         <v>44546</v>
@@ -80707,8 +80710,8 @@
       </c>
     </row>
     <row r="5659" spans="1:4">
-      <c r="A5659" t="s">
-        <v>9</v>
+      <c r="A5659">
+        <v>6</v>
       </c>
       <c r="B5659" s="2">
         <v>44546</v>
@@ -80721,8 +80724,8 @@
       </c>
     </row>
     <row r="5660" spans="1:4">
-      <c r="A5660" t="s">
-        <v>10</v>
+      <c r="A5660">
+        <v>7</v>
       </c>
       <c r="B5660" s="2">
         <v>44546</v>
@@ -80735,8 +80738,8 @@
       </c>
     </row>
     <row r="5661" spans="1:4">
-      <c r="A5661" t="s">
-        <v>11</v>
+      <c r="A5661">
+        <v>8</v>
       </c>
       <c r="B5661" s="2">
         <v>44546</v>
@@ -80749,8 +80752,8 @@
       </c>
     </row>
     <row r="5662" spans="1:4">
-      <c r="A5662" t="s">
-        <v>12</v>
+      <c r="A5662">
+        <v>9</v>
       </c>
       <c r="B5662" s="2">
         <v>44546</v>
@@ -80763,8 +80766,8 @@
       </c>
     </row>
     <row r="5663" spans="1:4">
-      <c r="A5663" t="s">
-        <v>13</v>
+      <c r="A5663">
+        <v>10</v>
       </c>
       <c r="B5663" s="2">
         <v>44546</v>
@@ -80777,8 +80780,8 @@
       </c>
     </row>
     <row r="5664" spans="1:4">
-      <c r="A5664" t="s">
-        <v>14</v>
+      <c r="A5664">
+        <v>11</v>
       </c>
       <c r="B5664" s="2">
         <v>44546</v>
@@ -80791,8 +80794,8 @@
       </c>
     </row>
     <row r="5665" spans="1:4">
-      <c r="A5665" t="s">
-        <v>15</v>
+      <c r="A5665">
+        <v>12</v>
       </c>
       <c r="B5665" s="2">
         <v>44546</v>
@@ -80805,8 +80808,8 @@
       </c>
     </row>
     <row r="5666" spans="1:4">
-      <c r="A5666" t="s">
-        <v>16</v>
+      <c r="A5666">
+        <v>13</v>
       </c>
       <c r="B5666" s="2">
         <v>44546</v>
@@ -80819,8 +80822,8 @@
       </c>
     </row>
     <row r="5667" spans="1:4">
-      <c r="A5667" t="s">
-        <v>17</v>
+      <c r="A5667">
+        <v>14</v>
       </c>
       <c r="B5667" s="2">
         <v>44546</v>
@@ -80833,8 +80836,8 @@
       </c>
     </row>
     <row r="5668" spans="1:4">
-      <c r="A5668" t="s">
-        <v>18</v>
+      <c r="A5668">
+        <v>15</v>
       </c>
       <c r="B5668" s="2">
         <v>44546</v>
@@ -80847,8 +80850,8 @@
       </c>
     </row>
     <row r="5669" spans="1:4">
-      <c r="A5669" t="s">
-        <v>19</v>
+      <c r="A5669">
+        <v>16</v>
       </c>
       <c r="B5669" s="2">
         <v>44546</v>
@@ -80861,8 +80864,8 @@
       </c>
     </row>
     <row r="5670" spans="1:4">
-      <c r="A5670" t="s">
-        <v>4</v>
+      <c r="A5670">
+        <v>1</v>
       </c>
       <c r="B5670" s="2">
         <v>44547</v>
@@ -80875,8 +80878,8 @@
       </c>
     </row>
     <row r="5671" spans="1:4">
-      <c r="A5671" t="s">
-        <v>5</v>
+      <c r="A5671">
+        <v>2</v>
       </c>
       <c r="B5671" s="2">
         <v>44547</v>
@@ -80889,8 +80892,8 @@
       </c>
     </row>
     <row r="5672" spans="1:4">
-      <c r="A5672" t="s">
-        <v>6</v>
+      <c r="A5672">
+        <v>3</v>
       </c>
       <c r="B5672" s="2">
         <v>44547</v>
@@ -80903,8 +80906,8 @@
       </c>
     </row>
     <row r="5673" spans="1:4">
-      <c r="A5673" t="s">
-        <v>7</v>
+      <c r="A5673">
+        <v>4</v>
       </c>
       <c r="B5673" s="2">
         <v>44547</v>
@@ -80917,8 +80920,8 @@
       </c>
     </row>
     <row r="5674" spans="1:4">
-      <c r="A5674" t="s">
-        <v>8</v>
+      <c r="A5674">
+        <v>5</v>
       </c>
       <c r="B5674" s="2">
         <v>44547</v>
@@ -80931,8 +80934,8 @@
       </c>
     </row>
     <row r="5675" spans="1:4">
-      <c r="A5675" t="s">
-        <v>9</v>
+      <c r="A5675">
+        <v>6</v>
       </c>
       <c r="B5675" s="2">
         <v>44547</v>
@@ -80945,8 +80948,8 @@
       </c>
     </row>
     <row r="5676" spans="1:4">
-      <c r="A5676" t="s">
-        <v>10</v>
+      <c r="A5676">
+        <v>7</v>
       </c>
       <c r="B5676" s="2">
         <v>44547</v>
@@ -80959,8 +80962,8 @@
       </c>
     </row>
     <row r="5677" spans="1:4">
-      <c r="A5677" t="s">
-        <v>11</v>
+      <c r="A5677">
+        <v>8</v>
       </c>
       <c r="B5677" s="2">
         <v>44547</v>
@@ -80973,8 +80976,8 @@
       </c>
     </row>
     <row r="5678" spans="1:4">
-      <c r="A5678" t="s">
-        <v>12</v>
+      <c r="A5678">
+        <v>9</v>
       </c>
       <c r="B5678" s="2">
         <v>44547</v>
@@ -80987,8 +80990,8 @@
       </c>
     </row>
     <row r="5679" spans="1:4">
-      <c r="A5679" t="s">
-        <v>13</v>
+      <c r="A5679">
+        <v>10</v>
       </c>
       <c r="B5679" s="2">
         <v>44547</v>
@@ -81001,8 +81004,8 @@
       </c>
     </row>
     <row r="5680" spans="1:4">
-      <c r="A5680" t="s">
-        <v>14</v>
+      <c r="A5680">
+        <v>11</v>
       </c>
       <c r="B5680" s="2">
         <v>44547</v>
@@ -81015,8 +81018,8 @@
       </c>
     </row>
     <row r="5681" spans="1:4">
-      <c r="A5681" t="s">
-        <v>15</v>
+      <c r="A5681">
+        <v>12</v>
       </c>
       <c r="B5681" s="2">
         <v>44547</v>
@@ -81029,8 +81032,8 @@
       </c>
     </row>
     <row r="5682" spans="1:4">
-      <c r="A5682" t="s">
-        <v>16</v>
+      <c r="A5682">
+        <v>13</v>
       </c>
       <c r="B5682" s="2">
         <v>44547</v>
@@ -81043,8 +81046,8 @@
       </c>
     </row>
     <row r="5683" spans="1:4">
-      <c r="A5683" t="s">
-        <v>17</v>
+      <c r="A5683">
+        <v>14</v>
       </c>
       <c r="B5683" s="2">
         <v>44547</v>
@@ -81057,8 +81060,8 @@
       </c>
     </row>
     <row r="5684" spans="1:4">
-      <c r="A5684" t="s">
-        <v>18</v>
+      <c r="A5684">
+        <v>15</v>
       </c>
       <c r="B5684" s="2">
         <v>44547</v>
@@ -81071,8 +81074,8 @@
       </c>
     </row>
     <row r="5685" spans="1:4">
-      <c r="A5685" t="s">
-        <v>19</v>
+      <c r="A5685">
+        <v>16</v>
       </c>
       <c r="B5685" s="2">
         <v>44547</v>
@@ -81081,6 +81084,454 @@
         <v>370</v>
       </c>
       <c r="D5685">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5686" spans="1:4">
+      <c r="A5686" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5686" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5686" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5686">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5687" spans="1:4">
+      <c r="A5687" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5687" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5687" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5687">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5688" spans="1:4">
+      <c r="A5688" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5688" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5688" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5688">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5689" spans="1:4">
+      <c r="A5689" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5689" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5689" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5689">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5690" spans="1:4">
+      <c r="A5690" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5690" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5690" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5690">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5691" spans="1:4">
+      <c r="A5691" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5691" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5691" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5691">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5692" spans="1:4">
+      <c r="A5692" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5692" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5692" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5692">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5693" spans="1:4">
+      <c r="A5693" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5693" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5693" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5693">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5694" spans="1:4">
+      <c r="A5694" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5694" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5694" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5694">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5695" spans="1:4">
+      <c r="A5695" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5695" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5695" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5695">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5696" spans="1:4">
+      <c r="A5696" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5696" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5696" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5696">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5697" spans="1:4">
+      <c r="A5697" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5697" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5697" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5697">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5698" spans="1:4">
+      <c r="A5698" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5698" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5698" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5698">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5699" spans="1:4">
+      <c r="A5699" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5699" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5699" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5699">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5700" spans="1:4">
+      <c r="A5700" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5700" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5700" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5700">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5701" spans="1:4">
+      <c r="A5701" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5701" s="2">
+        <v>44547</v>
+      </c>
+      <c r="C5701" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5701">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5702" spans="1:4">
+      <c r="A5702" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5702" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5702" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5702">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5703" spans="1:4">
+      <c r="A5703" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5703" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5703" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5703">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5704" spans="1:4">
+      <c r="A5704" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5704" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5704" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5704">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5705" spans="1:4">
+      <c r="A5705" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5705" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5705" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5705">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5706" spans="1:4">
+      <c r="A5706" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5706" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5706" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5706">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5707" spans="1:4">
+      <c r="A5707" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5707" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5707" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5707">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5708" spans="1:4">
+      <c r="A5708" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5708" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5708" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5708">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5709" spans="1:4">
+      <c r="A5709" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5709" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5709" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5709">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5710" spans="1:4">
+      <c r="A5710" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5710" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5710" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5710">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5711" spans="1:4">
+      <c r="A5711" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5711" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5711" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5711">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5712" spans="1:4">
+      <c r="A5712" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5712" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5712" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5712">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5713" spans="1:4">
+      <c r="A5713" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5713" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5713" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5713">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5714" spans="1:4">
+      <c r="A5714" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5714" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5714" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5714">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5715" spans="1:4">
+      <c r="A5715" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5715" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5715" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5715">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5716" spans="1:4">
+      <c r="A5716" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5716" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5716" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5716">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5717" spans="1:4">
+      <c r="A5717" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5717" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5717" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5717">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-21-2021 17-10-35
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11276" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11308" uniqueCount="373">
   <si>
     <t>Región</t>
   </si>
@@ -1131,6 +1131,9 @@
   <si>
     <t>2021-12-18</t>
   </si>
+  <si>
+    <t>2021-12-19</t>
+  </si>
 </sst>
 </file>
 
@@ -1491,7 +1494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5717"/>
+  <dimension ref="A1:D5749"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -81088,8 +81091,8 @@
       </c>
     </row>
     <row r="5686" spans="1:4">
-      <c r="A5686" t="s">
-        <v>4</v>
+      <c r="A5686">
+        <v>1</v>
       </c>
       <c r="B5686" s="2">
         <v>44547</v>
@@ -81102,8 +81105,8 @@
       </c>
     </row>
     <row r="5687" spans="1:4">
-      <c r="A5687" t="s">
-        <v>5</v>
+      <c r="A5687">
+        <v>2</v>
       </c>
       <c r="B5687" s="2">
         <v>44547</v>
@@ -81116,8 +81119,8 @@
       </c>
     </row>
     <row r="5688" spans="1:4">
-      <c r="A5688" t="s">
-        <v>6</v>
+      <c r="A5688">
+        <v>3</v>
       </c>
       <c r="B5688" s="2">
         <v>44547</v>
@@ -81130,8 +81133,8 @@
       </c>
     </row>
     <row r="5689" spans="1:4">
-      <c r="A5689" t="s">
-        <v>7</v>
+      <c r="A5689">
+        <v>4</v>
       </c>
       <c r="B5689" s="2">
         <v>44547</v>
@@ -81144,8 +81147,8 @@
       </c>
     </row>
     <row r="5690" spans="1:4">
-      <c r="A5690" t="s">
-        <v>8</v>
+      <c r="A5690">
+        <v>5</v>
       </c>
       <c r="B5690" s="2">
         <v>44547</v>
@@ -81158,8 +81161,8 @@
       </c>
     </row>
     <row r="5691" spans="1:4">
-      <c r="A5691" t="s">
-        <v>9</v>
+      <c r="A5691">
+        <v>6</v>
       </c>
       <c r="B5691" s="2">
         <v>44547</v>
@@ -81172,8 +81175,8 @@
       </c>
     </row>
     <row r="5692" spans="1:4">
-      <c r="A5692" t="s">
-        <v>10</v>
+      <c r="A5692">
+        <v>7</v>
       </c>
       <c r="B5692" s="2">
         <v>44547</v>
@@ -81186,8 +81189,8 @@
       </c>
     </row>
     <row r="5693" spans="1:4">
-      <c r="A5693" t="s">
-        <v>11</v>
+      <c r="A5693">
+        <v>8</v>
       </c>
       <c r="B5693" s="2">
         <v>44547</v>
@@ -81200,8 +81203,8 @@
       </c>
     </row>
     <row r="5694" spans="1:4">
-      <c r="A5694" t="s">
-        <v>12</v>
+      <c r="A5694">
+        <v>9</v>
       </c>
       <c r="B5694" s="2">
         <v>44547</v>
@@ -81214,8 +81217,8 @@
       </c>
     </row>
     <row r="5695" spans="1:4">
-      <c r="A5695" t="s">
-        <v>13</v>
+      <c r="A5695">
+        <v>10</v>
       </c>
       <c r="B5695" s="2">
         <v>44547</v>
@@ -81228,8 +81231,8 @@
       </c>
     </row>
     <row r="5696" spans="1:4">
-      <c r="A5696" t="s">
-        <v>14</v>
+      <c r="A5696">
+        <v>11</v>
       </c>
       <c r="B5696" s="2">
         <v>44547</v>
@@ -81242,8 +81245,8 @@
       </c>
     </row>
     <row r="5697" spans="1:4">
-      <c r="A5697" t="s">
-        <v>15</v>
+      <c r="A5697">
+        <v>12</v>
       </c>
       <c r="B5697" s="2">
         <v>44547</v>
@@ -81256,8 +81259,8 @@
       </c>
     </row>
     <row r="5698" spans="1:4">
-      <c r="A5698" t="s">
-        <v>16</v>
+      <c r="A5698">
+        <v>13</v>
       </c>
       <c r="B5698" s="2">
         <v>44547</v>
@@ -81270,8 +81273,8 @@
       </c>
     </row>
     <row r="5699" spans="1:4">
-      <c r="A5699" t="s">
-        <v>17</v>
+      <c r="A5699">
+        <v>14</v>
       </c>
       <c r="B5699" s="2">
         <v>44547</v>
@@ -81284,8 +81287,8 @@
       </c>
     </row>
     <row r="5700" spans="1:4">
-      <c r="A5700" t="s">
-        <v>18</v>
+      <c r="A5700">
+        <v>15</v>
       </c>
       <c r="B5700" s="2">
         <v>44547</v>
@@ -81298,8 +81301,8 @@
       </c>
     </row>
     <row r="5701" spans="1:4">
-      <c r="A5701" t="s">
-        <v>19</v>
+      <c r="A5701">
+        <v>16</v>
       </c>
       <c r="B5701" s="2">
         <v>44547</v>
@@ -81312,8 +81315,8 @@
       </c>
     </row>
     <row r="5702" spans="1:4">
-      <c r="A5702" t="s">
-        <v>4</v>
+      <c r="A5702">
+        <v>1</v>
       </c>
       <c r="B5702" s="2">
         <v>44548</v>
@@ -81326,8 +81329,8 @@
       </c>
     </row>
     <row r="5703" spans="1:4">
-      <c r="A5703" t="s">
-        <v>5</v>
+      <c r="A5703">
+        <v>2</v>
       </c>
       <c r="B5703" s="2">
         <v>44548</v>
@@ -81340,8 +81343,8 @@
       </c>
     </row>
     <row r="5704" spans="1:4">
-      <c r="A5704" t="s">
-        <v>6</v>
+      <c r="A5704">
+        <v>3</v>
       </c>
       <c r="B5704" s="2">
         <v>44548</v>
@@ -81354,8 +81357,8 @@
       </c>
     </row>
     <row r="5705" spans="1:4">
-      <c r="A5705" t="s">
-        <v>7</v>
+      <c r="A5705">
+        <v>4</v>
       </c>
       <c r="B5705" s="2">
         <v>44548</v>
@@ -81368,8 +81371,8 @@
       </c>
     </row>
     <row r="5706" spans="1:4">
-      <c r="A5706" t="s">
-        <v>8</v>
+      <c r="A5706">
+        <v>5</v>
       </c>
       <c r="B5706" s="2">
         <v>44548</v>
@@ -81382,8 +81385,8 @@
       </c>
     </row>
     <row r="5707" spans="1:4">
-      <c r="A5707" t="s">
-        <v>9</v>
+      <c r="A5707">
+        <v>6</v>
       </c>
       <c r="B5707" s="2">
         <v>44548</v>
@@ -81396,8 +81399,8 @@
       </c>
     </row>
     <row r="5708" spans="1:4">
-      <c r="A5708" t="s">
-        <v>10</v>
+      <c r="A5708">
+        <v>7</v>
       </c>
       <c r="B5708" s="2">
         <v>44548</v>
@@ -81410,8 +81413,8 @@
       </c>
     </row>
     <row r="5709" spans="1:4">
-      <c r="A5709" t="s">
-        <v>11</v>
+      <c r="A5709">
+        <v>8</v>
       </c>
       <c r="B5709" s="2">
         <v>44548</v>
@@ -81424,8 +81427,8 @@
       </c>
     </row>
     <row r="5710" spans="1:4">
-      <c r="A5710" t="s">
-        <v>12</v>
+      <c r="A5710">
+        <v>9</v>
       </c>
       <c r="B5710" s="2">
         <v>44548</v>
@@ -81438,8 +81441,8 @@
       </c>
     </row>
     <row r="5711" spans="1:4">
-      <c r="A5711" t="s">
-        <v>13</v>
+      <c r="A5711">
+        <v>10</v>
       </c>
       <c r="B5711" s="2">
         <v>44548</v>
@@ -81452,8 +81455,8 @@
       </c>
     </row>
     <row r="5712" spans="1:4">
-      <c r="A5712" t="s">
-        <v>14</v>
+      <c r="A5712">
+        <v>11</v>
       </c>
       <c r="B5712" s="2">
         <v>44548</v>
@@ -81466,8 +81469,8 @@
       </c>
     </row>
     <row r="5713" spans="1:4">
-      <c r="A5713" t="s">
-        <v>15</v>
+      <c r="A5713">
+        <v>12</v>
       </c>
       <c r="B5713" s="2">
         <v>44548</v>
@@ -81480,8 +81483,8 @@
       </c>
     </row>
     <row r="5714" spans="1:4">
-      <c r="A5714" t="s">
-        <v>16</v>
+      <c r="A5714">
+        <v>13</v>
       </c>
       <c r="B5714" s="2">
         <v>44548</v>
@@ -81494,8 +81497,8 @@
       </c>
     </row>
     <row r="5715" spans="1:4">
-      <c r="A5715" t="s">
-        <v>17</v>
+      <c r="A5715">
+        <v>14</v>
       </c>
       <c r="B5715" s="2">
         <v>44548</v>
@@ -81508,8 +81511,8 @@
       </c>
     </row>
     <row r="5716" spans="1:4">
-      <c r="A5716" t="s">
-        <v>18</v>
+      <c r="A5716">
+        <v>15</v>
       </c>
       <c r="B5716" s="2">
         <v>44548</v>
@@ -81522,8 +81525,8 @@
       </c>
     </row>
     <row r="5717" spans="1:4">
-      <c r="A5717" t="s">
-        <v>19</v>
+      <c r="A5717">
+        <v>16</v>
       </c>
       <c r="B5717" s="2">
         <v>44548</v>
@@ -81532,6 +81535,454 @@
         <v>371</v>
       </c>
       <c r="D5717">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5718" spans="1:4">
+      <c r="A5718" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5718" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5718" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5718">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5719" spans="1:4">
+      <c r="A5719" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5719" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5719" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5719">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5720" spans="1:4">
+      <c r="A5720" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5720" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5720" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5720">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5721" spans="1:4">
+      <c r="A5721" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5721" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5721" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5721">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5722" spans="1:4">
+      <c r="A5722" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5722" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5722" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5722">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5723" spans="1:4">
+      <c r="A5723" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5723" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5723" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5723">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5724" spans="1:4">
+      <c r="A5724" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5724" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5724" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5724">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5725" spans="1:4">
+      <c r="A5725" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5725" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5725" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5725">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5726" spans="1:4">
+      <c r="A5726" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5726" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5726" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5726">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5727" spans="1:4">
+      <c r="A5727" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5727" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5727" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5727">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5728" spans="1:4">
+      <c r="A5728" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5728" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5728" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5728">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5729" spans="1:4">
+      <c r="A5729" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5729" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5729" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5729">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5730" spans="1:4">
+      <c r="A5730" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5730" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5730" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5730">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5731" spans="1:4">
+      <c r="A5731" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5731" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5731" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5731">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5732" spans="1:4">
+      <c r="A5732" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5732" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5732" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5732">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5733" spans="1:4">
+      <c r="A5733" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5733" s="2">
+        <v>44548</v>
+      </c>
+      <c r="C5733" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5733">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5734" spans="1:4">
+      <c r="A5734" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5734" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5734" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5734">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5735" spans="1:4">
+      <c r="A5735" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5735" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5735" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5735">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5736" spans="1:4">
+      <c r="A5736" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5736" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5736" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5736">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5737" spans="1:4">
+      <c r="A5737" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5737" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5737" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5737">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5738" spans="1:4">
+      <c r="A5738" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5738" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5738" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5738">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5739" spans="1:4">
+      <c r="A5739" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5739" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5739" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5739">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5740" spans="1:4">
+      <c r="A5740" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5740" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5740" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5740">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5741" spans="1:4">
+      <c r="A5741" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5741" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5741" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5741">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5742" spans="1:4">
+      <c r="A5742" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5742" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5742" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5742">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5743" spans="1:4">
+      <c r="A5743" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5743" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5743" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5743">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5744" spans="1:4">
+      <c r="A5744" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5744" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5744" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5744">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5745" spans="1:4">
+      <c r="A5745" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5745" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5745" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5745">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5746" spans="1:4">
+      <c r="A5746" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5746" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5746" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5746">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5747" spans="1:4">
+      <c r="A5747" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5747" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5747" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5747">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5748" spans="1:4">
+      <c r="A5748" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5748" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5748" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5748">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5749" spans="1:4">
+      <c r="A5749" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5749" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5749" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5749">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-22-2021 17-43-32
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11308" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11340" uniqueCount="374">
   <si>
     <t>Región</t>
   </si>
@@ -1134,6 +1134,9 @@
   <si>
     <t>2021-12-19</t>
   </si>
+  <si>
+    <t>2021-12-20</t>
+  </si>
 </sst>
 </file>
 
@@ -1494,7 +1497,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5749"/>
+  <dimension ref="A1:D5781"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -81539,8 +81542,8 @@
       </c>
     </row>
     <row r="5718" spans="1:4">
-      <c r="A5718" t="s">
-        <v>4</v>
+      <c r="A5718">
+        <v>1</v>
       </c>
       <c r="B5718" s="2">
         <v>44548</v>
@@ -81553,8 +81556,8 @@
       </c>
     </row>
     <row r="5719" spans="1:4">
-      <c r="A5719" t="s">
-        <v>5</v>
+      <c r="A5719">
+        <v>2</v>
       </c>
       <c r="B5719" s="2">
         <v>44548</v>
@@ -81567,8 +81570,8 @@
       </c>
     </row>
     <row r="5720" spans="1:4">
-      <c r="A5720" t="s">
-        <v>6</v>
+      <c r="A5720">
+        <v>3</v>
       </c>
       <c r="B5720" s="2">
         <v>44548</v>
@@ -81581,8 +81584,8 @@
       </c>
     </row>
     <row r="5721" spans="1:4">
-      <c r="A5721" t="s">
-        <v>7</v>
+      <c r="A5721">
+        <v>4</v>
       </c>
       <c r="B5721" s="2">
         <v>44548</v>
@@ -81595,8 +81598,8 @@
       </c>
     </row>
     <row r="5722" spans="1:4">
-      <c r="A5722" t="s">
-        <v>8</v>
+      <c r="A5722">
+        <v>5</v>
       </c>
       <c r="B5722" s="2">
         <v>44548</v>
@@ -81609,8 +81612,8 @@
       </c>
     </row>
     <row r="5723" spans="1:4">
-      <c r="A5723" t="s">
-        <v>9</v>
+      <c r="A5723">
+        <v>6</v>
       </c>
       <c r="B5723" s="2">
         <v>44548</v>
@@ -81623,8 +81626,8 @@
       </c>
     </row>
     <row r="5724" spans="1:4">
-      <c r="A5724" t="s">
-        <v>10</v>
+      <c r="A5724">
+        <v>7</v>
       </c>
       <c r="B5724" s="2">
         <v>44548</v>
@@ -81637,8 +81640,8 @@
       </c>
     </row>
     <row r="5725" spans="1:4">
-      <c r="A5725" t="s">
-        <v>11</v>
+      <c r="A5725">
+        <v>8</v>
       </c>
       <c r="B5725" s="2">
         <v>44548</v>
@@ -81651,8 +81654,8 @@
       </c>
     </row>
     <row r="5726" spans="1:4">
-      <c r="A5726" t="s">
-        <v>12</v>
+      <c r="A5726">
+        <v>9</v>
       </c>
       <c r="B5726" s="2">
         <v>44548</v>
@@ -81665,8 +81668,8 @@
       </c>
     </row>
     <row r="5727" spans="1:4">
-      <c r="A5727" t="s">
-        <v>13</v>
+      <c r="A5727">
+        <v>10</v>
       </c>
       <c r="B5727" s="2">
         <v>44548</v>
@@ -81679,8 +81682,8 @@
       </c>
     </row>
     <row r="5728" spans="1:4">
-      <c r="A5728" t="s">
-        <v>14</v>
+      <c r="A5728">
+        <v>11</v>
       </c>
       <c r="B5728" s="2">
         <v>44548</v>
@@ -81693,8 +81696,8 @@
       </c>
     </row>
     <row r="5729" spans="1:4">
-      <c r="A5729" t="s">
-        <v>15</v>
+      <c r="A5729">
+        <v>12</v>
       </c>
       <c r="B5729" s="2">
         <v>44548</v>
@@ -81707,8 +81710,8 @@
       </c>
     </row>
     <row r="5730" spans="1:4">
-      <c r="A5730" t="s">
-        <v>16</v>
+      <c r="A5730">
+        <v>13</v>
       </c>
       <c r="B5730" s="2">
         <v>44548</v>
@@ -81721,8 +81724,8 @@
       </c>
     </row>
     <row r="5731" spans="1:4">
-      <c r="A5731" t="s">
-        <v>17</v>
+      <c r="A5731">
+        <v>14</v>
       </c>
       <c r="B5731" s="2">
         <v>44548</v>
@@ -81735,8 +81738,8 @@
       </c>
     </row>
     <row r="5732" spans="1:4">
-      <c r="A5732" t="s">
-        <v>18</v>
+      <c r="A5732">
+        <v>15</v>
       </c>
       <c r="B5732" s="2">
         <v>44548</v>
@@ -81749,8 +81752,8 @@
       </c>
     </row>
     <row r="5733" spans="1:4">
-      <c r="A5733" t="s">
-        <v>19</v>
+      <c r="A5733">
+        <v>16</v>
       </c>
       <c r="B5733" s="2">
         <v>44548</v>
@@ -81763,8 +81766,8 @@
       </c>
     </row>
     <row r="5734" spans="1:4">
-      <c r="A5734" t="s">
-        <v>4</v>
+      <c r="A5734">
+        <v>1</v>
       </c>
       <c r="B5734" s="2">
         <v>44549</v>
@@ -81777,8 +81780,8 @@
       </c>
     </row>
     <row r="5735" spans="1:4">
-      <c r="A5735" t="s">
-        <v>5</v>
+      <c r="A5735">
+        <v>2</v>
       </c>
       <c r="B5735" s="2">
         <v>44549</v>
@@ -81791,8 +81794,8 @@
       </c>
     </row>
     <row r="5736" spans="1:4">
-      <c r="A5736" t="s">
-        <v>6</v>
+      <c r="A5736">
+        <v>3</v>
       </c>
       <c r="B5736" s="2">
         <v>44549</v>
@@ -81805,8 +81808,8 @@
       </c>
     </row>
     <row r="5737" spans="1:4">
-      <c r="A5737" t="s">
-        <v>7</v>
+      <c r="A5737">
+        <v>4</v>
       </c>
       <c r="B5737" s="2">
         <v>44549</v>
@@ -81819,8 +81822,8 @@
       </c>
     </row>
     <row r="5738" spans="1:4">
-      <c r="A5738" t="s">
-        <v>8</v>
+      <c r="A5738">
+        <v>5</v>
       </c>
       <c r="B5738" s="2">
         <v>44549</v>
@@ -81833,8 +81836,8 @@
       </c>
     </row>
     <row r="5739" spans="1:4">
-      <c r="A5739" t="s">
-        <v>9</v>
+      <c r="A5739">
+        <v>6</v>
       </c>
       <c r="B5739" s="2">
         <v>44549</v>
@@ -81847,8 +81850,8 @@
       </c>
     </row>
     <row r="5740" spans="1:4">
-      <c r="A5740" t="s">
-        <v>10</v>
+      <c r="A5740">
+        <v>7</v>
       </c>
       <c r="B5740" s="2">
         <v>44549</v>
@@ -81861,8 +81864,8 @@
       </c>
     </row>
     <row r="5741" spans="1:4">
-      <c r="A5741" t="s">
-        <v>11</v>
+      <c r="A5741">
+        <v>8</v>
       </c>
       <c r="B5741" s="2">
         <v>44549</v>
@@ -81875,8 +81878,8 @@
       </c>
     </row>
     <row r="5742" spans="1:4">
-      <c r="A5742" t="s">
-        <v>12</v>
+      <c r="A5742">
+        <v>9</v>
       </c>
       <c r="B5742" s="2">
         <v>44549</v>
@@ -81889,8 +81892,8 @@
       </c>
     </row>
     <row r="5743" spans="1:4">
-      <c r="A5743" t="s">
-        <v>13</v>
+      <c r="A5743">
+        <v>10</v>
       </c>
       <c r="B5743" s="2">
         <v>44549</v>
@@ -81903,8 +81906,8 @@
       </c>
     </row>
     <row r="5744" spans="1:4">
-      <c r="A5744" t="s">
-        <v>14</v>
+      <c r="A5744">
+        <v>11</v>
       </c>
       <c r="B5744" s="2">
         <v>44549</v>
@@ -81917,8 +81920,8 @@
       </c>
     </row>
     <row r="5745" spans="1:4">
-      <c r="A5745" t="s">
-        <v>15</v>
+      <c r="A5745">
+        <v>12</v>
       </c>
       <c r="B5745" s="2">
         <v>44549</v>
@@ -81931,8 +81934,8 @@
       </c>
     </row>
     <row r="5746" spans="1:4">
-      <c r="A5746" t="s">
-        <v>16</v>
+      <c r="A5746">
+        <v>13</v>
       </c>
       <c r="B5746" s="2">
         <v>44549</v>
@@ -81945,8 +81948,8 @@
       </c>
     </row>
     <row r="5747" spans="1:4">
-      <c r="A5747" t="s">
-        <v>17</v>
+      <c r="A5747">
+        <v>14</v>
       </c>
       <c r="B5747" s="2">
         <v>44549</v>
@@ -81959,8 +81962,8 @@
       </c>
     </row>
     <row r="5748" spans="1:4">
-      <c r="A5748" t="s">
-        <v>18</v>
+      <c r="A5748">
+        <v>15</v>
       </c>
       <c r="B5748" s="2">
         <v>44549</v>
@@ -81973,8 +81976,8 @@
       </c>
     </row>
     <row r="5749" spans="1:4">
-      <c r="A5749" t="s">
-        <v>19</v>
+      <c r="A5749">
+        <v>16</v>
       </c>
       <c r="B5749" s="2">
         <v>44549</v>
@@ -81983,6 +81986,454 @@
         <v>372</v>
       </c>
       <c r="D5749">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5750" spans="1:4">
+      <c r="A5750" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5750" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5750" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5750">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5751" spans="1:4">
+      <c r="A5751" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5751" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5751" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5751">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5752" spans="1:4">
+      <c r="A5752" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5752" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5752" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5752">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5753" spans="1:4">
+      <c r="A5753" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5753" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5753" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5753">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5754" spans="1:4">
+      <c r="A5754" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5754" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5754" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5754">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5755" spans="1:4">
+      <c r="A5755" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5755" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5755" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5755">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5756" spans="1:4">
+      <c r="A5756" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5756" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5756" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5756">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5757" spans="1:4">
+      <c r="A5757" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5757" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5757" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5757">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5758" spans="1:4">
+      <c r="A5758" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5758" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5758" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5758">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5759" spans="1:4">
+      <c r="A5759" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5759" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5759" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5759">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5760" spans="1:4">
+      <c r="A5760" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5760" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5760" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5760">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5761" spans="1:4">
+      <c r="A5761" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5761" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5761" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5761">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5762" spans="1:4">
+      <c r="A5762" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5762" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5762" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5762">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5763" spans="1:4">
+      <c r="A5763" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5763" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5763" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5763">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5764" spans="1:4">
+      <c r="A5764" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5764" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5764" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5764">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5765" spans="1:4">
+      <c r="A5765" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5765" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5765" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5765">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5766" spans="1:4">
+      <c r="A5766" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5766" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5766" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5766">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5767" spans="1:4">
+      <c r="A5767" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5767" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5767" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5767">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5768" spans="1:4">
+      <c r="A5768" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5768" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5768" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5768">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5769" spans="1:4">
+      <c r="A5769" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5769" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5769" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5769">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5770" spans="1:4">
+      <c r="A5770" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5770" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5770" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5770">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5771" spans="1:4">
+      <c r="A5771" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5771" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5771" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5771">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5772" spans="1:4">
+      <c r="A5772" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5772" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5772" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5772">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5773" spans="1:4">
+      <c r="A5773" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5773" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5773" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5773">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5774" spans="1:4">
+      <c r="A5774" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5774" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5774" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5774">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5775" spans="1:4">
+      <c r="A5775" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5775" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5775" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5775">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5776" spans="1:4">
+      <c r="A5776" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5776" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5776" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5776">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5777" spans="1:4">
+      <c r="A5777" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5777" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5777" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5777">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5778" spans="1:4">
+      <c r="A5778" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5778" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5778" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5778">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5779" spans="1:4">
+      <c r="A5779" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5779" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5779" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5779">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5780" spans="1:4">
+      <c r="A5780" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5780" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5780" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5780">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5781" spans="1:4">
+      <c r="A5781" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5781" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5781" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5781">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-23-2021 18-18-26
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11340" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11372" uniqueCount="375">
   <si>
     <t>Región</t>
   </si>
@@ -1137,6 +1137,9 @@
   <si>
     <t>2021-12-20</t>
   </si>
+  <si>
+    <t>2021-12-21</t>
+  </si>
 </sst>
 </file>
 
@@ -1497,7 +1500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5781"/>
+  <dimension ref="A1:D5813"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -81990,8 +81993,8 @@
       </c>
     </row>
     <row r="5750" spans="1:4">
-      <c r="A5750" t="s">
-        <v>4</v>
+      <c r="A5750">
+        <v>1</v>
       </c>
       <c r="B5750" s="2">
         <v>44549</v>
@@ -82004,8 +82007,8 @@
       </c>
     </row>
     <row r="5751" spans="1:4">
-      <c r="A5751" t="s">
-        <v>5</v>
+      <c r="A5751">
+        <v>2</v>
       </c>
       <c r="B5751" s="2">
         <v>44549</v>
@@ -82018,8 +82021,8 @@
       </c>
     </row>
     <row r="5752" spans="1:4">
-      <c r="A5752" t="s">
-        <v>6</v>
+      <c r="A5752">
+        <v>3</v>
       </c>
       <c r="B5752" s="2">
         <v>44549</v>
@@ -82032,8 +82035,8 @@
       </c>
     </row>
     <row r="5753" spans="1:4">
-      <c r="A5753" t="s">
-        <v>7</v>
+      <c r="A5753">
+        <v>4</v>
       </c>
       <c r="B5753" s="2">
         <v>44549</v>
@@ -82046,8 +82049,8 @@
       </c>
     </row>
     <row r="5754" spans="1:4">
-      <c r="A5754" t="s">
-        <v>8</v>
+      <c r="A5754">
+        <v>5</v>
       </c>
       <c r="B5754" s="2">
         <v>44549</v>
@@ -82060,8 +82063,8 @@
       </c>
     </row>
     <row r="5755" spans="1:4">
-      <c r="A5755" t="s">
-        <v>9</v>
+      <c r="A5755">
+        <v>6</v>
       </c>
       <c r="B5755" s="2">
         <v>44549</v>
@@ -82074,8 +82077,8 @@
       </c>
     </row>
     <row r="5756" spans="1:4">
-      <c r="A5756" t="s">
-        <v>10</v>
+      <c r="A5756">
+        <v>7</v>
       </c>
       <c r="B5756" s="2">
         <v>44549</v>
@@ -82088,8 +82091,8 @@
       </c>
     </row>
     <row r="5757" spans="1:4">
-      <c r="A5757" t="s">
-        <v>11</v>
+      <c r="A5757">
+        <v>8</v>
       </c>
       <c r="B5757" s="2">
         <v>44549</v>
@@ -82102,8 +82105,8 @@
       </c>
     </row>
     <row r="5758" spans="1:4">
-      <c r="A5758" t="s">
-        <v>12</v>
+      <c r="A5758">
+        <v>9</v>
       </c>
       <c r="B5758" s="2">
         <v>44549</v>
@@ -82116,8 +82119,8 @@
       </c>
     </row>
     <row r="5759" spans="1:4">
-      <c r="A5759" t="s">
-        <v>13</v>
+      <c r="A5759">
+        <v>10</v>
       </c>
       <c r="B5759" s="2">
         <v>44549</v>
@@ -82130,8 +82133,8 @@
       </c>
     </row>
     <row r="5760" spans="1:4">
-      <c r="A5760" t="s">
-        <v>14</v>
+      <c r="A5760">
+        <v>11</v>
       </c>
       <c r="B5760" s="2">
         <v>44549</v>
@@ -82144,8 +82147,8 @@
       </c>
     </row>
     <row r="5761" spans="1:4">
-      <c r="A5761" t="s">
-        <v>15</v>
+      <c r="A5761">
+        <v>12</v>
       </c>
       <c r="B5761" s="2">
         <v>44549</v>
@@ -82158,8 +82161,8 @@
       </c>
     </row>
     <row r="5762" spans="1:4">
-      <c r="A5762" t="s">
-        <v>16</v>
+      <c r="A5762">
+        <v>13</v>
       </c>
       <c r="B5762" s="2">
         <v>44549</v>
@@ -82172,8 +82175,8 @@
       </c>
     </row>
     <row r="5763" spans="1:4">
-      <c r="A5763" t="s">
-        <v>17</v>
+      <c r="A5763">
+        <v>14</v>
       </c>
       <c r="B5763" s="2">
         <v>44549</v>
@@ -82186,8 +82189,8 @@
       </c>
     </row>
     <row r="5764" spans="1:4">
-      <c r="A5764" t="s">
-        <v>18</v>
+      <c r="A5764">
+        <v>15</v>
       </c>
       <c r="B5764" s="2">
         <v>44549</v>
@@ -82200,8 +82203,8 @@
       </c>
     </row>
     <row r="5765" spans="1:4">
-      <c r="A5765" t="s">
-        <v>19</v>
+      <c r="A5765">
+        <v>16</v>
       </c>
       <c r="B5765" s="2">
         <v>44549</v>
@@ -82214,8 +82217,8 @@
       </c>
     </row>
     <row r="5766" spans="1:4">
-      <c r="A5766" t="s">
-        <v>4</v>
+      <c r="A5766">
+        <v>1</v>
       </c>
       <c r="B5766" s="2">
         <v>44550</v>
@@ -82228,8 +82231,8 @@
       </c>
     </row>
     <row r="5767" spans="1:4">
-      <c r="A5767" t="s">
-        <v>5</v>
+      <c r="A5767">
+        <v>2</v>
       </c>
       <c r="B5767" s="2">
         <v>44550</v>
@@ -82242,8 +82245,8 @@
       </c>
     </row>
     <row r="5768" spans="1:4">
-      <c r="A5768" t="s">
-        <v>6</v>
+      <c r="A5768">
+        <v>3</v>
       </c>
       <c r="B5768" s="2">
         <v>44550</v>
@@ -82256,8 +82259,8 @@
       </c>
     </row>
     <row r="5769" spans="1:4">
-      <c r="A5769" t="s">
-        <v>7</v>
+      <c r="A5769">
+        <v>4</v>
       </c>
       <c r="B5769" s="2">
         <v>44550</v>
@@ -82270,8 +82273,8 @@
       </c>
     </row>
     <row r="5770" spans="1:4">
-      <c r="A5770" t="s">
-        <v>8</v>
+      <c r="A5770">
+        <v>5</v>
       </c>
       <c r="B5770" s="2">
         <v>44550</v>
@@ -82284,8 +82287,8 @@
       </c>
     </row>
     <row r="5771" spans="1:4">
-      <c r="A5771" t="s">
-        <v>9</v>
+      <c r="A5771">
+        <v>6</v>
       </c>
       <c r="B5771" s="2">
         <v>44550</v>
@@ -82298,8 +82301,8 @@
       </c>
     </row>
     <row r="5772" spans="1:4">
-      <c r="A5772" t="s">
-        <v>10</v>
+      <c r="A5772">
+        <v>7</v>
       </c>
       <c r="B5772" s="2">
         <v>44550</v>
@@ -82312,8 +82315,8 @@
       </c>
     </row>
     <row r="5773" spans="1:4">
-      <c r="A5773" t="s">
-        <v>11</v>
+      <c r="A5773">
+        <v>8</v>
       </c>
       <c r="B5773" s="2">
         <v>44550</v>
@@ -82326,8 +82329,8 @@
       </c>
     </row>
     <row r="5774" spans="1:4">
-      <c r="A5774" t="s">
-        <v>12</v>
+      <c r="A5774">
+        <v>9</v>
       </c>
       <c r="B5774" s="2">
         <v>44550</v>
@@ -82340,8 +82343,8 @@
       </c>
     </row>
     <row r="5775" spans="1:4">
-      <c r="A5775" t="s">
-        <v>13</v>
+      <c r="A5775">
+        <v>10</v>
       </c>
       <c r="B5775" s="2">
         <v>44550</v>
@@ -82354,8 +82357,8 @@
       </c>
     </row>
     <row r="5776" spans="1:4">
-      <c r="A5776" t="s">
-        <v>14</v>
+      <c r="A5776">
+        <v>11</v>
       </c>
       <c r="B5776" s="2">
         <v>44550</v>
@@ -82368,8 +82371,8 @@
       </c>
     </row>
     <row r="5777" spans="1:4">
-      <c r="A5777" t="s">
-        <v>15</v>
+      <c r="A5777">
+        <v>12</v>
       </c>
       <c r="B5777" s="2">
         <v>44550</v>
@@ -82382,8 +82385,8 @@
       </c>
     </row>
     <row r="5778" spans="1:4">
-      <c r="A5778" t="s">
-        <v>16</v>
+      <c r="A5778">
+        <v>13</v>
       </c>
       <c r="B5778" s="2">
         <v>44550</v>
@@ -82396,8 +82399,8 @@
       </c>
     </row>
     <row r="5779" spans="1:4">
-      <c r="A5779" t="s">
-        <v>17</v>
+      <c r="A5779">
+        <v>14</v>
       </c>
       <c r="B5779" s="2">
         <v>44550</v>
@@ -82410,8 +82413,8 @@
       </c>
     </row>
     <row r="5780" spans="1:4">
-      <c r="A5780" t="s">
-        <v>18</v>
+      <c r="A5780">
+        <v>15</v>
       </c>
       <c r="B5780" s="2">
         <v>44550</v>
@@ -82424,8 +82427,8 @@
       </c>
     </row>
     <row r="5781" spans="1:4">
-      <c r="A5781" t="s">
-        <v>19</v>
+      <c r="A5781">
+        <v>16</v>
       </c>
       <c r="B5781" s="2">
         <v>44550</v>
@@ -82434,6 +82437,454 @@
         <v>373</v>
       </c>
       <c r="D5781">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5782" spans="1:4">
+      <c r="A5782" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5782" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5782" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5782">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5783" spans="1:4">
+      <c r="A5783" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5783" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5783" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5783">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5784" spans="1:4">
+      <c r="A5784" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5784" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5784" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5784">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5785" spans="1:4">
+      <c r="A5785" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5785" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5785" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5785">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5786" spans="1:4">
+      <c r="A5786" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5786" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5786" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5786">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5787" spans="1:4">
+      <c r="A5787" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5787" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5787" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5787">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5788" spans="1:4">
+      <c r="A5788" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5788" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5788" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5788">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5789" spans="1:4">
+      <c r="A5789" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5789" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5789" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5789">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5790" spans="1:4">
+      <c r="A5790" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5790" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5790" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5790">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5791" spans="1:4">
+      <c r="A5791" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5791" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5791" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5791">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5792" spans="1:4">
+      <c r="A5792" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5792" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5792" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5792">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5793" spans="1:4">
+      <c r="A5793" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5793" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5793" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5793">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5794" spans="1:4">
+      <c r="A5794" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5794" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5794" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5794">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5795" spans="1:4">
+      <c r="A5795" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5795" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5795" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5795">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5796" spans="1:4">
+      <c r="A5796" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5796" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5796" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5796">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5797" spans="1:4">
+      <c r="A5797" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5797" s="2">
+        <v>44550</v>
+      </c>
+      <c r="C5797" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5797">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5798" spans="1:4">
+      <c r="A5798" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5798" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5798" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5798">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5799" spans="1:4">
+      <c r="A5799" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5799" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5799" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5799">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5800" spans="1:4">
+      <c r="A5800" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5800" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5800" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5800">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5801" spans="1:4">
+      <c r="A5801" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5801" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5801" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5801">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5802" spans="1:4">
+      <c r="A5802" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5802" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5802" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5802">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5803" spans="1:4">
+      <c r="A5803" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5803" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5803" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5803">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5804" spans="1:4">
+      <c r="A5804" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5804" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5804" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5804">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5805" spans="1:4">
+      <c r="A5805" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5805" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5805" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5805">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5806" spans="1:4">
+      <c r="A5806" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5806" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5806" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5806">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5807" spans="1:4">
+      <c r="A5807" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5807" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5807" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5807">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5808" spans="1:4">
+      <c r="A5808" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5808" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5808" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5808">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5809" spans="1:4">
+      <c r="A5809" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5809" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5809" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5809">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5810" spans="1:4">
+      <c r="A5810" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5810" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5810" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5810">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5811" spans="1:4">
+      <c r="A5811" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5811" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5811" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5811">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5812" spans="1:4">
+      <c r="A5812" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5812" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5812" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5812">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5813" spans="1:4">
+      <c r="A5813" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5813" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5813" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5813">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-24-2021 18-49-29
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11372" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11404" uniqueCount="376">
   <si>
     <t>Región</t>
   </si>
@@ -1140,6 +1140,9 @@
   <si>
     <t>2021-12-21</t>
   </si>
+  <si>
+    <t>2021-12-22</t>
+  </si>
 </sst>
 </file>
 
@@ -1500,7 +1503,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5813"/>
+  <dimension ref="A1:D5845"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -82441,8 +82444,8 @@
       </c>
     </row>
     <row r="5782" spans="1:4">
-      <c r="A5782" t="s">
-        <v>4</v>
+      <c r="A5782">
+        <v>1</v>
       </c>
       <c r="B5782" s="2">
         <v>44550</v>
@@ -82455,8 +82458,8 @@
       </c>
     </row>
     <row r="5783" spans="1:4">
-      <c r="A5783" t="s">
-        <v>5</v>
+      <c r="A5783">
+        <v>2</v>
       </c>
       <c r="B5783" s="2">
         <v>44550</v>
@@ -82469,8 +82472,8 @@
       </c>
     </row>
     <row r="5784" spans="1:4">
-      <c r="A5784" t="s">
-        <v>6</v>
+      <c r="A5784">
+        <v>3</v>
       </c>
       <c r="B5784" s="2">
         <v>44550</v>
@@ -82483,8 +82486,8 @@
       </c>
     </row>
     <row r="5785" spans="1:4">
-      <c r="A5785" t="s">
-        <v>7</v>
+      <c r="A5785">
+        <v>4</v>
       </c>
       <c r="B5785" s="2">
         <v>44550</v>
@@ -82497,8 +82500,8 @@
       </c>
     </row>
     <row r="5786" spans="1:4">
-      <c r="A5786" t="s">
-        <v>8</v>
+      <c r="A5786">
+        <v>5</v>
       </c>
       <c r="B5786" s="2">
         <v>44550</v>
@@ -82511,8 +82514,8 @@
       </c>
     </row>
     <row r="5787" spans="1:4">
-      <c r="A5787" t="s">
-        <v>9</v>
+      <c r="A5787">
+        <v>6</v>
       </c>
       <c r="B5787" s="2">
         <v>44550</v>
@@ -82525,8 +82528,8 @@
       </c>
     </row>
     <row r="5788" spans="1:4">
-      <c r="A5788" t="s">
-        <v>10</v>
+      <c r="A5788">
+        <v>7</v>
       </c>
       <c r="B5788" s="2">
         <v>44550</v>
@@ -82539,8 +82542,8 @@
       </c>
     </row>
     <row r="5789" spans="1:4">
-      <c r="A5789" t="s">
-        <v>11</v>
+      <c r="A5789">
+        <v>8</v>
       </c>
       <c r="B5789" s="2">
         <v>44550</v>
@@ -82553,8 +82556,8 @@
       </c>
     </row>
     <row r="5790" spans="1:4">
-      <c r="A5790" t="s">
-        <v>12</v>
+      <c r="A5790">
+        <v>9</v>
       </c>
       <c r="B5790" s="2">
         <v>44550</v>
@@ -82567,8 +82570,8 @@
       </c>
     </row>
     <row r="5791" spans="1:4">
-      <c r="A5791" t="s">
-        <v>13</v>
+      <c r="A5791">
+        <v>10</v>
       </c>
       <c r="B5791" s="2">
         <v>44550</v>
@@ -82581,8 +82584,8 @@
       </c>
     </row>
     <row r="5792" spans="1:4">
-      <c r="A5792" t="s">
-        <v>14</v>
+      <c r="A5792">
+        <v>11</v>
       </c>
       <c r="B5792" s="2">
         <v>44550</v>
@@ -82595,8 +82598,8 @@
       </c>
     </row>
     <row r="5793" spans="1:4">
-      <c r="A5793" t="s">
-        <v>15</v>
+      <c r="A5793">
+        <v>12</v>
       </c>
       <c r="B5793" s="2">
         <v>44550</v>
@@ -82609,8 +82612,8 @@
       </c>
     </row>
     <row r="5794" spans="1:4">
-      <c r="A5794" t="s">
-        <v>16</v>
+      <c r="A5794">
+        <v>13</v>
       </c>
       <c r="B5794" s="2">
         <v>44550</v>
@@ -82623,8 +82626,8 @@
       </c>
     </row>
     <row r="5795" spans="1:4">
-      <c r="A5795" t="s">
-        <v>17</v>
+      <c r="A5795">
+        <v>14</v>
       </c>
       <c r="B5795" s="2">
         <v>44550</v>
@@ -82637,8 +82640,8 @@
       </c>
     </row>
     <row r="5796" spans="1:4">
-      <c r="A5796" t="s">
-        <v>18</v>
+      <c r="A5796">
+        <v>15</v>
       </c>
       <c r="B5796" s="2">
         <v>44550</v>
@@ -82651,8 +82654,8 @@
       </c>
     </row>
     <row r="5797" spans="1:4">
-      <c r="A5797" t="s">
-        <v>19</v>
+      <c r="A5797">
+        <v>16</v>
       </c>
       <c r="B5797" s="2">
         <v>44550</v>
@@ -82665,8 +82668,8 @@
       </c>
     </row>
     <row r="5798" spans="1:4">
-      <c r="A5798" t="s">
-        <v>4</v>
+      <c r="A5798">
+        <v>1</v>
       </c>
       <c r="B5798" s="2">
         <v>44551</v>
@@ -82679,8 +82682,8 @@
       </c>
     </row>
     <row r="5799" spans="1:4">
-      <c r="A5799" t="s">
-        <v>5</v>
+      <c r="A5799">
+        <v>2</v>
       </c>
       <c r="B5799" s="2">
         <v>44551</v>
@@ -82693,8 +82696,8 @@
       </c>
     </row>
     <row r="5800" spans="1:4">
-      <c r="A5800" t="s">
-        <v>6</v>
+      <c r="A5800">
+        <v>3</v>
       </c>
       <c r="B5800" s="2">
         <v>44551</v>
@@ -82707,8 +82710,8 @@
       </c>
     </row>
     <row r="5801" spans="1:4">
-      <c r="A5801" t="s">
-        <v>7</v>
+      <c r="A5801">
+        <v>4</v>
       </c>
       <c r="B5801" s="2">
         <v>44551</v>
@@ -82721,8 +82724,8 @@
       </c>
     </row>
     <row r="5802" spans="1:4">
-      <c r="A5802" t="s">
-        <v>8</v>
+      <c r="A5802">
+        <v>5</v>
       </c>
       <c r="B5802" s="2">
         <v>44551</v>
@@ -82735,8 +82738,8 @@
       </c>
     </row>
     <row r="5803" spans="1:4">
-      <c r="A5803" t="s">
-        <v>9</v>
+      <c r="A5803">
+        <v>6</v>
       </c>
       <c r="B5803" s="2">
         <v>44551</v>
@@ -82749,8 +82752,8 @@
       </c>
     </row>
     <row r="5804" spans="1:4">
-      <c r="A5804" t="s">
-        <v>10</v>
+      <c r="A5804">
+        <v>7</v>
       </c>
       <c r="B5804" s="2">
         <v>44551</v>
@@ -82763,8 +82766,8 @@
       </c>
     </row>
     <row r="5805" spans="1:4">
-      <c r="A5805" t="s">
-        <v>11</v>
+      <c r="A5805">
+        <v>8</v>
       </c>
       <c r="B5805" s="2">
         <v>44551</v>
@@ -82777,8 +82780,8 @@
       </c>
     </row>
     <row r="5806" spans="1:4">
-      <c r="A5806" t="s">
-        <v>12</v>
+      <c r="A5806">
+        <v>9</v>
       </c>
       <c r="B5806" s="2">
         <v>44551</v>
@@ -82791,8 +82794,8 @@
       </c>
     </row>
     <row r="5807" spans="1:4">
-      <c r="A5807" t="s">
-        <v>13</v>
+      <c r="A5807">
+        <v>10</v>
       </c>
       <c r="B5807" s="2">
         <v>44551</v>
@@ -82805,8 +82808,8 @@
       </c>
     </row>
     <row r="5808" spans="1:4">
-      <c r="A5808" t="s">
-        <v>14</v>
+      <c r="A5808">
+        <v>11</v>
       </c>
       <c r="B5808" s="2">
         <v>44551</v>
@@ -82819,8 +82822,8 @@
       </c>
     </row>
     <row r="5809" spans="1:4">
-      <c r="A5809" t="s">
-        <v>15</v>
+      <c r="A5809">
+        <v>12</v>
       </c>
       <c r="B5809" s="2">
         <v>44551</v>
@@ -82833,8 +82836,8 @@
       </c>
     </row>
     <row r="5810" spans="1:4">
-      <c r="A5810" t="s">
-        <v>16</v>
+      <c r="A5810">
+        <v>13</v>
       </c>
       <c r="B5810" s="2">
         <v>44551</v>
@@ -82847,8 +82850,8 @@
       </c>
     </row>
     <row r="5811" spans="1:4">
-      <c r="A5811" t="s">
-        <v>17</v>
+      <c r="A5811">
+        <v>14</v>
       </c>
       <c r="B5811" s="2">
         <v>44551</v>
@@ -82861,8 +82864,8 @@
       </c>
     </row>
     <row r="5812" spans="1:4">
-      <c r="A5812" t="s">
-        <v>18</v>
+      <c r="A5812">
+        <v>15</v>
       </c>
       <c r="B5812" s="2">
         <v>44551</v>
@@ -82875,8 +82878,8 @@
       </c>
     </row>
     <row r="5813" spans="1:4">
-      <c r="A5813" t="s">
-        <v>19</v>
+      <c r="A5813">
+        <v>16</v>
       </c>
       <c r="B5813" s="2">
         <v>44551</v>
@@ -82886,6 +82889,454 @@
       </c>
       <c r="D5813">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5814" spans="1:4">
+      <c r="A5814" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5814" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5814" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5814">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5815" spans="1:4">
+      <c r="A5815" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5815" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5815" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5815">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5816" spans="1:4">
+      <c r="A5816" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5816" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5816" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5816">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5817" spans="1:4">
+      <c r="A5817" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5817" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5817" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5817">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5818" spans="1:4">
+      <c r="A5818" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5818" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5818" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5818">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5819" spans="1:4">
+      <c r="A5819" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5819" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5819" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5819">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5820" spans="1:4">
+      <c r="A5820" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5820" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5820" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5820">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5821" spans="1:4">
+      <c r="A5821" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5821" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5821" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5821">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5822" spans="1:4">
+      <c r="A5822" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5822" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5822" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5822">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5823" spans="1:4">
+      <c r="A5823" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5823" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5823" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5823">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5824" spans="1:4">
+      <c r="A5824" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5824" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5824" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5824">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5825" spans="1:4">
+      <c r="A5825" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5825" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5825" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5825">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5826" spans="1:4">
+      <c r="A5826" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5826" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5826" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5826">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5827" spans="1:4">
+      <c r="A5827" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5827" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5827" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5827">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5828" spans="1:4">
+      <c r="A5828" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5828" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5828" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5828">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5829" spans="1:4">
+      <c r="A5829" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5829" s="2">
+        <v>44551</v>
+      </c>
+      <c r="C5829" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5829">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5830" spans="1:4">
+      <c r="A5830" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5830" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5830" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5830">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5831" spans="1:4">
+      <c r="A5831" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5831" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5831" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5831">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5832" spans="1:4">
+      <c r="A5832" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5832" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5832" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5832">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5833" spans="1:4">
+      <c r="A5833" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5833" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5833" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5833">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5834" spans="1:4">
+      <c r="A5834" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5834" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5834" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5834">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5835" spans="1:4">
+      <c r="A5835" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5835" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5835" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5835">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5836" spans="1:4">
+      <c r="A5836" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5836" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5836" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5836">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5837" spans="1:4">
+      <c r="A5837" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5837" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5837" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5837">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5838" spans="1:4">
+      <c r="A5838" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5838" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5838" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5838">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5839" spans="1:4">
+      <c r="A5839" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5839" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5839" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5839">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5840" spans="1:4">
+      <c r="A5840" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5840" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5840" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5840">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5841" spans="1:4">
+      <c r="A5841" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5841" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5841" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5841">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5842" spans="1:4">
+      <c r="A5842" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5842" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5842" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5842">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5843" spans="1:4">
+      <c r="A5843" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5843" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5843" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5843">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5844" spans="1:4">
+      <c r="A5844" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5844" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5844" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5844">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5845" spans="1:4">
+      <c r="A5845" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5845" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5845" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5845">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-25-2021 19-19-05
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11404" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11436" uniqueCount="377">
   <si>
     <t>Región</t>
   </si>
@@ -1143,6 +1143,9 @@
   <si>
     <t>2021-12-22</t>
   </si>
+  <si>
+    <t>2021-12-23</t>
+  </si>
 </sst>
 </file>
 
@@ -1503,7 +1506,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5845"/>
+  <dimension ref="A1:D5877"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -82892,8 +82895,8 @@
       </c>
     </row>
     <row r="5814" spans="1:4">
-      <c r="A5814" t="s">
-        <v>4</v>
+      <c r="A5814">
+        <v>1</v>
       </c>
       <c r="B5814" s="2">
         <v>44551</v>
@@ -82906,8 +82909,8 @@
       </c>
     </row>
     <row r="5815" spans="1:4">
-      <c r="A5815" t="s">
-        <v>5</v>
+      <c r="A5815">
+        <v>2</v>
       </c>
       <c r="B5815" s="2">
         <v>44551</v>
@@ -82920,8 +82923,8 @@
       </c>
     </row>
     <row r="5816" spans="1:4">
-      <c r="A5816" t="s">
-        <v>6</v>
+      <c r="A5816">
+        <v>3</v>
       </c>
       <c r="B5816" s="2">
         <v>44551</v>
@@ -82934,8 +82937,8 @@
       </c>
     </row>
     <row r="5817" spans="1:4">
-      <c r="A5817" t="s">
-        <v>7</v>
+      <c r="A5817">
+        <v>4</v>
       </c>
       <c r="B5817" s="2">
         <v>44551</v>
@@ -82948,8 +82951,8 @@
       </c>
     </row>
     <row r="5818" spans="1:4">
-      <c r="A5818" t="s">
-        <v>8</v>
+      <c r="A5818">
+        <v>5</v>
       </c>
       <c r="B5818" s="2">
         <v>44551</v>
@@ -82962,8 +82965,8 @@
       </c>
     </row>
     <row r="5819" spans="1:4">
-      <c r="A5819" t="s">
-        <v>9</v>
+      <c r="A5819">
+        <v>6</v>
       </c>
       <c r="B5819" s="2">
         <v>44551</v>
@@ -82976,8 +82979,8 @@
       </c>
     </row>
     <row r="5820" spans="1:4">
-      <c r="A5820" t="s">
-        <v>10</v>
+      <c r="A5820">
+        <v>7</v>
       </c>
       <c r="B5820" s="2">
         <v>44551</v>
@@ -82990,8 +82993,8 @@
       </c>
     </row>
     <row r="5821" spans="1:4">
-      <c r="A5821" t="s">
-        <v>11</v>
+      <c r="A5821">
+        <v>8</v>
       </c>
       <c r="B5821" s="2">
         <v>44551</v>
@@ -83004,8 +83007,8 @@
       </c>
     </row>
     <row r="5822" spans="1:4">
-      <c r="A5822" t="s">
-        <v>12</v>
+      <c r="A5822">
+        <v>9</v>
       </c>
       <c r="B5822" s="2">
         <v>44551</v>
@@ -83018,8 +83021,8 @@
       </c>
     </row>
     <row r="5823" spans="1:4">
-      <c r="A5823" t="s">
-        <v>13</v>
+      <c r="A5823">
+        <v>10</v>
       </c>
       <c r="B5823" s="2">
         <v>44551</v>
@@ -83032,8 +83035,8 @@
       </c>
     </row>
     <row r="5824" spans="1:4">
-      <c r="A5824" t="s">
-        <v>14</v>
+      <c r="A5824">
+        <v>11</v>
       </c>
       <c r="B5824" s="2">
         <v>44551</v>
@@ -83046,8 +83049,8 @@
       </c>
     </row>
     <row r="5825" spans="1:4">
-      <c r="A5825" t="s">
-        <v>15</v>
+      <c r="A5825">
+        <v>12</v>
       </c>
       <c r="B5825" s="2">
         <v>44551</v>
@@ -83060,8 +83063,8 @@
       </c>
     </row>
     <row r="5826" spans="1:4">
-      <c r="A5826" t="s">
-        <v>16</v>
+      <c r="A5826">
+        <v>13</v>
       </c>
       <c r="B5826" s="2">
         <v>44551</v>
@@ -83074,8 +83077,8 @@
       </c>
     </row>
     <row r="5827" spans="1:4">
-      <c r="A5827" t="s">
-        <v>17</v>
+      <c r="A5827">
+        <v>14</v>
       </c>
       <c r="B5827" s="2">
         <v>44551</v>
@@ -83088,8 +83091,8 @@
       </c>
     </row>
     <row r="5828" spans="1:4">
-      <c r="A5828" t="s">
-        <v>18</v>
+      <c r="A5828">
+        <v>15</v>
       </c>
       <c r="B5828" s="2">
         <v>44551</v>
@@ -83102,8 +83105,8 @@
       </c>
     </row>
     <row r="5829" spans="1:4">
-      <c r="A5829" t="s">
-        <v>19</v>
+      <c r="A5829">
+        <v>16</v>
       </c>
       <c r="B5829" s="2">
         <v>44551</v>
@@ -83116,8 +83119,8 @@
       </c>
     </row>
     <row r="5830" spans="1:4">
-      <c r="A5830" t="s">
-        <v>4</v>
+      <c r="A5830">
+        <v>1</v>
       </c>
       <c r="B5830" s="2">
         <v>44552</v>
@@ -83130,8 +83133,8 @@
       </c>
     </row>
     <row r="5831" spans="1:4">
-      <c r="A5831" t="s">
-        <v>5</v>
+      <c r="A5831">
+        <v>2</v>
       </c>
       <c r="B5831" s="2">
         <v>44552</v>
@@ -83144,8 +83147,8 @@
       </c>
     </row>
     <row r="5832" spans="1:4">
-      <c r="A5832" t="s">
-        <v>6</v>
+      <c r="A5832">
+        <v>3</v>
       </c>
       <c r="B5832" s="2">
         <v>44552</v>
@@ -83158,8 +83161,8 @@
       </c>
     </row>
     <row r="5833" spans="1:4">
-      <c r="A5833" t="s">
-        <v>7</v>
+      <c r="A5833">
+        <v>4</v>
       </c>
       <c r="B5833" s="2">
         <v>44552</v>
@@ -83172,8 +83175,8 @@
       </c>
     </row>
     <row r="5834" spans="1:4">
-      <c r="A5834" t="s">
-        <v>8</v>
+      <c r="A5834">
+        <v>5</v>
       </c>
       <c r="B5834" s="2">
         <v>44552</v>
@@ -83186,8 +83189,8 @@
       </c>
     </row>
     <row r="5835" spans="1:4">
-      <c r="A5835" t="s">
-        <v>9</v>
+      <c r="A5835">
+        <v>6</v>
       </c>
       <c r="B5835" s="2">
         <v>44552</v>
@@ -83200,8 +83203,8 @@
       </c>
     </row>
     <row r="5836" spans="1:4">
-      <c r="A5836" t="s">
-        <v>10</v>
+      <c r="A5836">
+        <v>7</v>
       </c>
       <c r="B5836" s="2">
         <v>44552</v>
@@ -83214,8 +83217,8 @@
       </c>
     </row>
     <row r="5837" spans="1:4">
-      <c r="A5837" t="s">
-        <v>11</v>
+      <c r="A5837">
+        <v>8</v>
       </c>
       <c r="B5837" s="2">
         <v>44552</v>
@@ -83228,8 +83231,8 @@
       </c>
     </row>
     <row r="5838" spans="1:4">
-      <c r="A5838" t="s">
-        <v>12</v>
+      <c r="A5838">
+        <v>9</v>
       </c>
       <c r="B5838" s="2">
         <v>44552</v>
@@ -83242,8 +83245,8 @@
       </c>
     </row>
     <row r="5839" spans="1:4">
-      <c r="A5839" t="s">
-        <v>13</v>
+      <c r="A5839">
+        <v>10</v>
       </c>
       <c r="B5839" s="2">
         <v>44552</v>
@@ -83256,8 +83259,8 @@
       </c>
     </row>
     <row r="5840" spans="1:4">
-      <c r="A5840" t="s">
-        <v>14</v>
+      <c r="A5840">
+        <v>11</v>
       </c>
       <c r="B5840" s="2">
         <v>44552</v>
@@ -83270,8 +83273,8 @@
       </c>
     </row>
     <row r="5841" spans="1:4">
-      <c r="A5841" t="s">
-        <v>15</v>
+      <c r="A5841">
+        <v>12</v>
       </c>
       <c r="B5841" s="2">
         <v>44552</v>
@@ -83284,8 +83287,8 @@
       </c>
     </row>
     <row r="5842" spans="1:4">
-      <c r="A5842" t="s">
-        <v>16</v>
+      <c r="A5842">
+        <v>13</v>
       </c>
       <c r="B5842" s="2">
         <v>44552</v>
@@ -83298,8 +83301,8 @@
       </c>
     </row>
     <row r="5843" spans="1:4">
-      <c r="A5843" t="s">
-        <v>17</v>
+      <c r="A5843">
+        <v>14</v>
       </c>
       <c r="B5843" s="2">
         <v>44552</v>
@@ -83312,8 +83315,8 @@
       </c>
     </row>
     <row r="5844" spans="1:4">
-      <c r="A5844" t="s">
-        <v>18</v>
+      <c r="A5844">
+        <v>15</v>
       </c>
       <c r="B5844" s="2">
         <v>44552</v>
@@ -83326,8 +83329,8 @@
       </c>
     </row>
     <row r="5845" spans="1:4">
-      <c r="A5845" t="s">
-        <v>19</v>
+      <c r="A5845">
+        <v>16</v>
       </c>
       <c r="B5845" s="2">
         <v>44552</v>
@@ -83337,6 +83340,454 @@
       </c>
       <c r="D5845">
         <v>0</v>
+      </c>
+    </row>
+    <row r="5846" spans="1:4">
+      <c r="A5846" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5846" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5846" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5846">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5847" spans="1:4">
+      <c r="A5847" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5847" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5847" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5847">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5848" spans="1:4">
+      <c r="A5848" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5848" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5848" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5848">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5849" spans="1:4">
+      <c r="A5849" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5849" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5849" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5849">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5850" spans="1:4">
+      <c r="A5850" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5850" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5850" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5850">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5851" spans="1:4">
+      <c r="A5851" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5851" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5851" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5851">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5852" spans="1:4">
+      <c r="A5852" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5852" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5852" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5852">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5853" spans="1:4">
+      <c r="A5853" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5853" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5853" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5853">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5854" spans="1:4">
+      <c r="A5854" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5854" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5854" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5854">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5855" spans="1:4">
+      <c r="A5855" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5855" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5855" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5855">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5856" spans="1:4">
+      <c r="A5856" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5856" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5856" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5856">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5857" spans="1:4">
+      <c r="A5857" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5857" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5857" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5857">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5858" spans="1:4">
+      <c r="A5858" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5858" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5858" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5858">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5859" spans="1:4">
+      <c r="A5859" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5859" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5859" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5859">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5860" spans="1:4">
+      <c r="A5860" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5860" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5860" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5860">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5861" spans="1:4">
+      <c r="A5861" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5861" s="2">
+        <v>44552</v>
+      </c>
+      <c r="C5861" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5861">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5862" spans="1:4">
+      <c r="A5862" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5862" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5862" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5862">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5863" spans="1:4">
+      <c r="A5863" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5863" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5863" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5863">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5864" spans="1:4">
+      <c r="A5864" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5864" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5864" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5864">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5865" spans="1:4">
+      <c r="A5865" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5865" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5865" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5865">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5866" spans="1:4">
+      <c r="A5866" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5866" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5866" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5866">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5867" spans="1:4">
+      <c r="A5867" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5867" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5867" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5867">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5868" spans="1:4">
+      <c r="A5868" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5868" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5868" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5868">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5869" spans="1:4">
+      <c r="A5869" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5869" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5869" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5869">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5870" spans="1:4">
+      <c r="A5870" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5870" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5870" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5870">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5871" spans="1:4">
+      <c r="A5871" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5871" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5871" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5871">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5872" spans="1:4">
+      <c r="A5872" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5872" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5872" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5872">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5873" spans="1:4">
+      <c r="A5873" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5873" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5873" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5873">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5874" spans="1:4">
+      <c r="A5874" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5874" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5874" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5874">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5875" spans="1:4">
+      <c r="A5875" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5875" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5875" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5875">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5876" spans="1:4">
+      <c r="A5876" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5876" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5876" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5876">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5877" spans="1:4">
+      <c r="A5877" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5877" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5877" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5877">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-26-2021 19-48-30
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11436" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11468" uniqueCount="378">
   <si>
     <t>Región</t>
   </si>
@@ -1146,6 +1146,9 @@
   <si>
     <t>2021-12-23</t>
   </si>
+  <si>
+    <t>2021-12-24</t>
+  </si>
 </sst>
 </file>
 
@@ -1506,7 +1509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5877"/>
+  <dimension ref="A1:D5909"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -83343,8 +83346,8 @@
       </c>
     </row>
     <row r="5846" spans="1:4">
-      <c r="A5846" t="s">
-        <v>4</v>
+      <c r="A5846">
+        <v>1</v>
       </c>
       <c r="B5846" s="2">
         <v>44552</v>
@@ -83357,8 +83360,8 @@
       </c>
     </row>
     <row r="5847" spans="1:4">
-      <c r="A5847" t="s">
-        <v>5</v>
+      <c r="A5847">
+        <v>2</v>
       </c>
       <c r="B5847" s="2">
         <v>44552</v>
@@ -83371,8 +83374,8 @@
       </c>
     </row>
     <row r="5848" spans="1:4">
-      <c r="A5848" t="s">
-        <v>6</v>
+      <c r="A5848">
+        <v>3</v>
       </c>
       <c r="B5848" s="2">
         <v>44552</v>
@@ -83385,8 +83388,8 @@
       </c>
     </row>
     <row r="5849" spans="1:4">
-      <c r="A5849" t="s">
-        <v>7</v>
+      <c r="A5849">
+        <v>4</v>
       </c>
       <c r="B5849" s="2">
         <v>44552</v>
@@ -83399,8 +83402,8 @@
       </c>
     </row>
     <row r="5850" spans="1:4">
-      <c r="A5850" t="s">
-        <v>8</v>
+      <c r="A5850">
+        <v>5</v>
       </c>
       <c r="B5850" s="2">
         <v>44552</v>
@@ -83413,8 +83416,8 @@
       </c>
     </row>
     <row r="5851" spans="1:4">
-      <c r="A5851" t="s">
-        <v>9</v>
+      <c r="A5851">
+        <v>6</v>
       </c>
       <c r="B5851" s="2">
         <v>44552</v>
@@ -83427,8 +83430,8 @@
       </c>
     </row>
     <row r="5852" spans="1:4">
-      <c r="A5852" t="s">
-        <v>10</v>
+      <c r="A5852">
+        <v>7</v>
       </c>
       <c r="B5852" s="2">
         <v>44552</v>
@@ -83441,8 +83444,8 @@
       </c>
     </row>
     <row r="5853" spans="1:4">
-      <c r="A5853" t="s">
-        <v>11</v>
+      <c r="A5853">
+        <v>8</v>
       </c>
       <c r="B5853" s="2">
         <v>44552</v>
@@ -83455,8 +83458,8 @@
       </c>
     </row>
     <row r="5854" spans="1:4">
-      <c r="A5854" t="s">
-        <v>12</v>
+      <c r="A5854">
+        <v>9</v>
       </c>
       <c r="B5854" s="2">
         <v>44552</v>
@@ -83469,8 +83472,8 @@
       </c>
     </row>
     <row r="5855" spans="1:4">
-      <c r="A5855" t="s">
-        <v>13</v>
+      <c r="A5855">
+        <v>10</v>
       </c>
       <c r="B5855" s="2">
         <v>44552</v>
@@ -83483,8 +83486,8 @@
       </c>
     </row>
     <row r="5856" spans="1:4">
-      <c r="A5856" t="s">
-        <v>14</v>
+      <c r="A5856">
+        <v>11</v>
       </c>
       <c r="B5856" s="2">
         <v>44552</v>
@@ -83497,8 +83500,8 @@
       </c>
     </row>
     <row r="5857" spans="1:4">
-      <c r="A5857" t="s">
-        <v>15</v>
+      <c r="A5857">
+        <v>12</v>
       </c>
       <c r="B5857" s="2">
         <v>44552</v>
@@ -83511,8 +83514,8 @@
       </c>
     </row>
     <row r="5858" spans="1:4">
-      <c r="A5858" t="s">
-        <v>16</v>
+      <c r="A5858">
+        <v>13</v>
       </c>
       <c r="B5858" s="2">
         <v>44552</v>
@@ -83525,8 +83528,8 @@
       </c>
     </row>
     <row r="5859" spans="1:4">
-      <c r="A5859" t="s">
-        <v>17</v>
+      <c r="A5859">
+        <v>14</v>
       </c>
       <c r="B5859" s="2">
         <v>44552</v>
@@ -83539,8 +83542,8 @@
       </c>
     </row>
     <row r="5860" spans="1:4">
-      <c r="A5860" t="s">
-        <v>18</v>
+      <c r="A5860">
+        <v>15</v>
       </c>
       <c r="B5860" s="2">
         <v>44552</v>
@@ -83553,8 +83556,8 @@
       </c>
     </row>
     <row r="5861" spans="1:4">
-      <c r="A5861" t="s">
-        <v>19</v>
+      <c r="A5861">
+        <v>16</v>
       </c>
       <c r="B5861" s="2">
         <v>44552</v>
@@ -83567,8 +83570,8 @@
       </c>
     </row>
     <row r="5862" spans="1:4">
-      <c r="A5862" t="s">
-        <v>4</v>
+      <c r="A5862">
+        <v>1</v>
       </c>
       <c r="B5862" s="2">
         <v>44553</v>
@@ -83581,8 +83584,8 @@
       </c>
     </row>
     <row r="5863" spans="1:4">
-      <c r="A5863" t="s">
-        <v>5</v>
+      <c r="A5863">
+        <v>2</v>
       </c>
       <c r="B5863" s="2">
         <v>44553</v>
@@ -83595,8 +83598,8 @@
       </c>
     </row>
     <row r="5864" spans="1:4">
-      <c r="A5864" t="s">
-        <v>6</v>
+      <c r="A5864">
+        <v>3</v>
       </c>
       <c r="B5864" s="2">
         <v>44553</v>
@@ -83609,8 +83612,8 @@
       </c>
     </row>
     <row r="5865" spans="1:4">
-      <c r="A5865" t="s">
-        <v>7</v>
+      <c r="A5865">
+        <v>4</v>
       </c>
       <c r="B5865" s="2">
         <v>44553</v>
@@ -83623,8 +83626,8 @@
       </c>
     </row>
     <row r="5866" spans="1:4">
-      <c r="A5866" t="s">
-        <v>8</v>
+      <c r="A5866">
+        <v>5</v>
       </c>
       <c r="B5866" s="2">
         <v>44553</v>
@@ -83637,8 +83640,8 @@
       </c>
     </row>
     <row r="5867" spans="1:4">
-      <c r="A5867" t="s">
-        <v>9</v>
+      <c r="A5867">
+        <v>6</v>
       </c>
       <c r="B5867" s="2">
         <v>44553</v>
@@ -83651,8 +83654,8 @@
       </c>
     </row>
     <row r="5868" spans="1:4">
-      <c r="A5868" t="s">
-        <v>10</v>
+      <c r="A5868">
+        <v>7</v>
       </c>
       <c r="B5868" s="2">
         <v>44553</v>
@@ -83665,8 +83668,8 @@
       </c>
     </row>
     <row r="5869" spans="1:4">
-      <c r="A5869" t="s">
-        <v>11</v>
+      <c r="A5869">
+        <v>8</v>
       </c>
       <c r="B5869" s="2">
         <v>44553</v>
@@ -83679,8 +83682,8 @@
       </c>
     </row>
     <row r="5870" spans="1:4">
-      <c r="A5870" t="s">
-        <v>12</v>
+      <c r="A5870">
+        <v>9</v>
       </c>
       <c r="B5870" s="2">
         <v>44553</v>
@@ -83693,8 +83696,8 @@
       </c>
     </row>
     <row r="5871" spans="1:4">
-      <c r="A5871" t="s">
-        <v>13</v>
+      <c r="A5871">
+        <v>10</v>
       </c>
       <c r="B5871" s="2">
         <v>44553</v>
@@ -83707,8 +83710,8 @@
       </c>
     </row>
     <row r="5872" spans="1:4">
-      <c r="A5872" t="s">
-        <v>14</v>
+      <c r="A5872">
+        <v>11</v>
       </c>
       <c r="B5872" s="2">
         <v>44553</v>
@@ -83721,8 +83724,8 @@
       </c>
     </row>
     <row r="5873" spans="1:4">
-      <c r="A5873" t="s">
-        <v>15</v>
+      <c r="A5873">
+        <v>12</v>
       </c>
       <c r="B5873" s="2">
         <v>44553</v>
@@ -83735,8 +83738,8 @@
       </c>
     </row>
     <row r="5874" spans="1:4">
-      <c r="A5874" t="s">
-        <v>16</v>
+      <c r="A5874">
+        <v>13</v>
       </c>
       <c r="B5874" s="2">
         <v>44553</v>
@@ -83749,8 +83752,8 @@
       </c>
     </row>
     <row r="5875" spans="1:4">
-      <c r="A5875" t="s">
-        <v>17</v>
+      <c r="A5875">
+        <v>14</v>
       </c>
       <c r="B5875" s="2">
         <v>44553</v>
@@ -83763,8 +83766,8 @@
       </c>
     </row>
     <row r="5876" spans="1:4">
-      <c r="A5876" t="s">
-        <v>18</v>
+      <c r="A5876">
+        <v>15</v>
       </c>
       <c r="B5876" s="2">
         <v>44553</v>
@@ -83777,8 +83780,8 @@
       </c>
     </row>
     <row r="5877" spans="1:4">
-      <c r="A5877" t="s">
-        <v>19</v>
+      <c r="A5877">
+        <v>16</v>
       </c>
       <c r="B5877" s="2">
         <v>44553</v>
@@ -83788,6 +83791,454 @@
       </c>
       <c r="D5877">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5878" spans="1:4">
+      <c r="A5878" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5878" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5878" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5878">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5879" spans="1:4">
+      <c r="A5879" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5879" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5879" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5879">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5880" spans="1:4">
+      <c r="A5880" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5880" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5880" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5880">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5881" spans="1:4">
+      <c r="A5881" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5881" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5881" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5881">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5882" spans="1:4">
+      <c r="A5882" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5882" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5882" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5882">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5883" spans="1:4">
+      <c r="A5883" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5883" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5883" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5883">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5884" spans="1:4">
+      <c r="A5884" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5884" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5884" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5884">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5885" spans="1:4">
+      <c r="A5885" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5885" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5885" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5885">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5886" spans="1:4">
+      <c r="A5886" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5886" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5886" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5886">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5887" spans="1:4">
+      <c r="A5887" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5887" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5887" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5887">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5888" spans="1:4">
+      <c r="A5888" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5888" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5888" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5888">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5889" spans="1:4">
+      <c r="A5889" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5889" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5889" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5889">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5890" spans="1:4">
+      <c r="A5890" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5890" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5890" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5890">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5891" spans="1:4">
+      <c r="A5891" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5891" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5891" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5891">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5892" spans="1:4">
+      <c r="A5892" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5892" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5892" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5892">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5893" spans="1:4">
+      <c r="A5893" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5893" s="2">
+        <v>44553</v>
+      </c>
+      <c r="C5893" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5893">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5894" spans="1:4">
+      <c r="A5894" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5894" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5894" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5894">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5895" spans="1:4">
+      <c r="A5895" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5895" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5895" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5895">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5896" spans="1:4">
+      <c r="A5896" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5896" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5896" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5896">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5897" spans="1:4">
+      <c r="A5897" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5897" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5897" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5897">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5898" spans="1:4">
+      <c r="A5898" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5898" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5898" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5898">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5899" spans="1:4">
+      <c r="A5899" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5899" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5899" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5899">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5900" spans="1:4">
+      <c r="A5900" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5900" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5900" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5900">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5901" spans="1:4">
+      <c r="A5901" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5901" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5901" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5901">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5902" spans="1:4">
+      <c r="A5902" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5902" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5902" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5902">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5903" spans="1:4">
+      <c r="A5903" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5903" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5903" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5903">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5904" spans="1:4">
+      <c r="A5904" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5904" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5904" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5904">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5905" spans="1:4">
+      <c r="A5905" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5905" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5905" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5905">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5906" spans="1:4">
+      <c r="A5906" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5906" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5906" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5906">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5907" spans="1:4">
+      <c r="A5907" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5907" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5907" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5907">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5908" spans="1:4">
+      <c r="A5908" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5908" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5908" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5908">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5909" spans="1:4">
+      <c r="A5909" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5909" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5909" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5909">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-27-2021 13-59-12
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -4,20 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$5717</definedName>
-  </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11260" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11308" uniqueCount="379">
   <si>
     <t>Región</t>
   </si>
@@ -1152,13 +1149,16 @@
   <si>
     <t>2021-12-24</t>
   </si>
+  <si>
+    <t>2021-12-25</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -1228,7 +1228,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1512,16 +1512,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5717"/>
+  <dimension ref="A1:D5749"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4985" workbookViewId="0">
-      <selection activeCell="C4985" sqref="C4985"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="3" max="3" width="39.6640625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -81338,8 +81333,8 @@
       </c>
     </row>
     <row r="5702" spans="1:4">
-      <c r="A5702" t="s">
-        <v>4</v>
+      <c r="A5702">
+        <v>1</v>
       </c>
       <c r="B5702" s="2">
         <v>44554</v>
@@ -81352,8 +81347,8 @@
       </c>
     </row>
     <row r="5703" spans="1:4">
-      <c r="A5703" t="s">
-        <v>5</v>
+      <c r="A5703">
+        <v>2</v>
       </c>
       <c r="B5703" s="2">
         <v>44554</v>
@@ -81366,8 +81361,8 @@
       </c>
     </row>
     <row r="5704" spans="1:4">
-      <c r="A5704" t="s">
-        <v>6</v>
+      <c r="A5704">
+        <v>3</v>
       </c>
       <c r="B5704" s="2">
         <v>44554</v>
@@ -81380,8 +81375,8 @@
       </c>
     </row>
     <row r="5705" spans="1:4">
-      <c r="A5705" t="s">
-        <v>7</v>
+      <c r="A5705">
+        <v>4</v>
       </c>
       <c r="B5705" s="2">
         <v>44554</v>
@@ -81394,8 +81389,8 @@
       </c>
     </row>
     <row r="5706" spans="1:4">
-      <c r="A5706" t="s">
-        <v>8</v>
+      <c r="A5706">
+        <v>5</v>
       </c>
       <c r="B5706" s="2">
         <v>44554</v>
@@ -81408,8 +81403,8 @@
       </c>
     </row>
     <row r="5707" spans="1:4">
-      <c r="A5707" t="s">
-        <v>9</v>
+      <c r="A5707">
+        <v>6</v>
       </c>
       <c r="B5707" s="2">
         <v>44554</v>
@@ -81422,8 +81417,8 @@
       </c>
     </row>
     <row r="5708" spans="1:4">
-      <c r="A5708" t="s">
-        <v>10</v>
+      <c r="A5708">
+        <v>7</v>
       </c>
       <c r="B5708" s="2">
         <v>44554</v>
@@ -81436,8 +81431,8 @@
       </c>
     </row>
     <row r="5709" spans="1:4">
-      <c r="A5709" t="s">
-        <v>11</v>
+      <c r="A5709">
+        <v>8</v>
       </c>
       <c r="B5709" s="2">
         <v>44554</v>
@@ -81450,8 +81445,8 @@
       </c>
     </row>
     <row r="5710" spans="1:4">
-      <c r="A5710" t="s">
-        <v>12</v>
+      <c r="A5710">
+        <v>9</v>
       </c>
       <c r="B5710" s="2">
         <v>44554</v>
@@ -81464,8 +81459,8 @@
       </c>
     </row>
     <row r="5711" spans="1:4">
-      <c r="A5711" t="s">
-        <v>13</v>
+      <c r="A5711">
+        <v>10</v>
       </c>
       <c r="B5711" s="2">
         <v>44554</v>
@@ -81478,8 +81473,8 @@
       </c>
     </row>
     <row r="5712" spans="1:4">
-      <c r="A5712" t="s">
-        <v>14</v>
+      <c r="A5712">
+        <v>11</v>
       </c>
       <c r="B5712" s="2">
         <v>44554</v>
@@ -81492,8 +81487,8 @@
       </c>
     </row>
     <row r="5713" spans="1:4">
-      <c r="A5713" t="s">
-        <v>15</v>
+      <c r="A5713">
+        <v>12</v>
       </c>
       <c r="B5713" s="2">
         <v>44554</v>
@@ -81506,8 +81501,8 @@
       </c>
     </row>
     <row r="5714" spans="1:4">
-      <c r="A5714" t="s">
-        <v>16</v>
+      <c r="A5714">
+        <v>13</v>
       </c>
       <c r="B5714" s="2">
         <v>44554</v>
@@ -81520,8 +81515,8 @@
       </c>
     </row>
     <row r="5715" spans="1:4">
-      <c r="A5715" t="s">
-        <v>17</v>
+      <c r="A5715">
+        <v>14</v>
       </c>
       <c r="B5715" s="2">
         <v>44554</v>
@@ -81534,8 +81529,8 @@
       </c>
     </row>
     <row r="5716" spans="1:4">
-      <c r="A5716" t="s">
-        <v>18</v>
+      <c r="A5716">
+        <v>15</v>
       </c>
       <c r="B5716" s="2">
         <v>44554</v>
@@ -81548,8 +81543,8 @@
       </c>
     </row>
     <row r="5717" spans="1:4">
-      <c r="A5717" t="s">
-        <v>19</v>
+      <c r="A5717">
+        <v>16</v>
       </c>
       <c r="B5717" s="2">
         <v>44554</v>
@@ -81561,8 +81556,455 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5718" spans="1:4">
+      <c r="A5718" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5718" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5718" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5718">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5719" spans="1:4">
+      <c r="A5719" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5719" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5719" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5719">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5720" spans="1:4">
+      <c r="A5720" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5720" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5720" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5720">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5721" spans="1:4">
+      <c r="A5721" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5721" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5721" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5721">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5722" spans="1:4">
+      <c r="A5722" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5722" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5722" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5722">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5723" spans="1:4">
+      <c r="A5723" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5723" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5723" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5723">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5724" spans="1:4">
+      <c r="A5724" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5724" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5724" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5724">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5725" spans="1:4">
+      <c r="A5725" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5725" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5725" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5725">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5726" spans="1:4">
+      <c r="A5726" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5726" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5726" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5726">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5727" spans="1:4">
+      <c r="A5727" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5727" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5727" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5727">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5728" spans="1:4">
+      <c r="A5728" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5728" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5728" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5728">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5729" spans="1:4">
+      <c r="A5729" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5729" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5729" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5729">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5730" spans="1:4">
+      <c r="A5730" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5730" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5730" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5730">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5731" spans="1:4">
+      <c r="A5731" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5731" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5731" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5731">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5732" spans="1:4">
+      <c r="A5732" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5732" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5732" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5732">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5733" spans="1:4">
+      <c r="A5733" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5733" s="2">
+        <v>44554</v>
+      </c>
+      <c r="C5733" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5733">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5734" spans="1:4">
+      <c r="A5734" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5734" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5734" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5734">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5735" spans="1:4">
+      <c r="A5735" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5735" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5735" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5735">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5736" spans="1:4">
+      <c r="A5736" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5736" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5736" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5736">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5737" spans="1:4">
+      <c r="A5737" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5737" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5737" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5737">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5738" spans="1:4">
+      <c r="A5738" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5738" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5738" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5738">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5739" spans="1:4">
+      <c r="A5739" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5739" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5739" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5739">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5740" spans="1:4">
+      <c r="A5740" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5740" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5740" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5740">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5741" spans="1:4">
+      <c r="A5741" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5741" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5741" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5741">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5742" spans="1:4">
+      <c r="A5742" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5742" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5742" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5742">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5743" spans="1:4">
+      <c r="A5743" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5743" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5743" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5743">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5744" spans="1:4">
+      <c r="A5744" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5744" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5744" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5744">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5745" spans="1:4">
+      <c r="A5745" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5745" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5745" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5745">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5746" spans="1:4">
+      <c r="A5746" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5746" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5746" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5746">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5747" spans="1:4">
+      <c r="A5747" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5747" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5747" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5747">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5748" spans="1:4">
+      <c r="A5748" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5748" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5748" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5748">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5749" spans="1:4">
+      <c r="A5749" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5749" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5749" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5749">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D5717"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 12-28-2021 14-30-13
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11308" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11340" uniqueCount="380">
   <si>
     <t>Región</t>
   </si>
@@ -1152,6 +1152,9 @@
   <si>
     <t>2021-12-25</t>
   </si>
+  <si>
+    <t>2021-12-26</t>
+  </si>
 </sst>
 </file>
 
@@ -1512,7 +1515,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5749"/>
+  <dimension ref="A1:D5781"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -81557,8 +81560,8 @@
       </c>
     </row>
     <row r="5718" spans="1:4">
-      <c r="A5718" t="s">
-        <v>4</v>
+      <c r="A5718">
+        <v>1</v>
       </c>
       <c r="B5718" s="2">
         <v>44554</v>
@@ -81571,8 +81574,8 @@
       </c>
     </row>
     <row r="5719" spans="1:4">
-      <c r="A5719" t="s">
-        <v>5</v>
+      <c r="A5719">
+        <v>2</v>
       </c>
       <c r="B5719" s="2">
         <v>44554</v>
@@ -81585,8 +81588,8 @@
       </c>
     </row>
     <row r="5720" spans="1:4">
-      <c r="A5720" t="s">
-        <v>6</v>
+      <c r="A5720">
+        <v>3</v>
       </c>
       <c r="B5720" s="2">
         <v>44554</v>
@@ -81599,8 +81602,8 @@
       </c>
     </row>
     <row r="5721" spans="1:4">
-      <c r="A5721" t="s">
-        <v>7</v>
+      <c r="A5721">
+        <v>4</v>
       </c>
       <c r="B5721" s="2">
         <v>44554</v>
@@ -81613,8 +81616,8 @@
       </c>
     </row>
     <row r="5722" spans="1:4">
-      <c r="A5722" t="s">
-        <v>8</v>
+      <c r="A5722">
+        <v>5</v>
       </c>
       <c r="B5722" s="2">
         <v>44554</v>
@@ -81627,8 +81630,8 @@
       </c>
     </row>
     <row r="5723" spans="1:4">
-      <c r="A5723" t="s">
-        <v>9</v>
+      <c r="A5723">
+        <v>6</v>
       </c>
       <c r="B5723" s="2">
         <v>44554</v>
@@ -81641,8 +81644,8 @@
       </c>
     </row>
     <row r="5724" spans="1:4">
-      <c r="A5724" t="s">
-        <v>10</v>
+      <c r="A5724">
+        <v>7</v>
       </c>
       <c r="B5724" s="2">
         <v>44554</v>
@@ -81655,8 +81658,8 @@
       </c>
     </row>
     <row r="5725" spans="1:4">
-      <c r="A5725" t="s">
-        <v>11</v>
+      <c r="A5725">
+        <v>8</v>
       </c>
       <c r="B5725" s="2">
         <v>44554</v>
@@ -81669,8 +81672,8 @@
       </c>
     </row>
     <row r="5726" spans="1:4">
-      <c r="A5726" t="s">
-        <v>12</v>
+      <c r="A5726">
+        <v>9</v>
       </c>
       <c r="B5726" s="2">
         <v>44554</v>
@@ -81683,8 +81686,8 @@
       </c>
     </row>
     <row r="5727" spans="1:4">
-      <c r="A5727" t="s">
-        <v>13</v>
+      <c r="A5727">
+        <v>10</v>
       </c>
       <c r="B5727" s="2">
         <v>44554</v>
@@ -81697,8 +81700,8 @@
       </c>
     </row>
     <row r="5728" spans="1:4">
-      <c r="A5728" t="s">
-        <v>14</v>
+      <c r="A5728">
+        <v>11</v>
       </c>
       <c r="B5728" s="2">
         <v>44554</v>
@@ -81711,8 +81714,8 @@
       </c>
     </row>
     <row r="5729" spans="1:4">
-      <c r="A5729" t="s">
-        <v>15</v>
+      <c r="A5729">
+        <v>12</v>
       </c>
       <c r="B5729" s="2">
         <v>44554</v>
@@ -81725,8 +81728,8 @@
       </c>
     </row>
     <row r="5730" spans="1:4">
-      <c r="A5730" t="s">
-        <v>16</v>
+      <c r="A5730">
+        <v>13</v>
       </c>
       <c r="B5730" s="2">
         <v>44554</v>
@@ -81739,8 +81742,8 @@
       </c>
     </row>
     <row r="5731" spans="1:4">
-      <c r="A5731" t="s">
-        <v>17</v>
+      <c r="A5731">
+        <v>14</v>
       </c>
       <c r="B5731" s="2">
         <v>44554</v>
@@ -81753,8 +81756,8 @@
       </c>
     </row>
     <row r="5732" spans="1:4">
-      <c r="A5732" t="s">
-        <v>18</v>
+      <c r="A5732">
+        <v>15</v>
       </c>
       <c r="B5732" s="2">
         <v>44554</v>
@@ -81767,8 +81770,8 @@
       </c>
     </row>
     <row r="5733" spans="1:4">
-      <c r="A5733" t="s">
-        <v>19</v>
+      <c r="A5733">
+        <v>16</v>
       </c>
       <c r="B5733" s="2">
         <v>44554</v>
@@ -81781,8 +81784,8 @@
       </c>
     </row>
     <row r="5734" spans="1:4">
-      <c r="A5734" t="s">
-        <v>4</v>
+      <c r="A5734">
+        <v>1</v>
       </c>
       <c r="B5734" s="2">
         <v>44555</v>
@@ -81795,8 +81798,8 @@
       </c>
     </row>
     <row r="5735" spans="1:4">
-      <c r="A5735" t="s">
-        <v>5</v>
+      <c r="A5735">
+        <v>2</v>
       </c>
       <c r="B5735" s="2">
         <v>44555</v>
@@ -81809,8 +81812,8 @@
       </c>
     </row>
     <row r="5736" spans="1:4">
-      <c r="A5736" t="s">
-        <v>6</v>
+      <c r="A5736">
+        <v>3</v>
       </c>
       <c r="B5736" s="2">
         <v>44555</v>
@@ -81823,8 +81826,8 @@
       </c>
     </row>
     <row r="5737" spans="1:4">
-      <c r="A5737" t="s">
-        <v>7</v>
+      <c r="A5737">
+        <v>4</v>
       </c>
       <c r="B5737" s="2">
         <v>44555</v>
@@ -81837,8 +81840,8 @@
       </c>
     </row>
     <row r="5738" spans="1:4">
-      <c r="A5738" t="s">
-        <v>8</v>
+      <c r="A5738">
+        <v>5</v>
       </c>
       <c r="B5738" s="2">
         <v>44555</v>
@@ -81851,8 +81854,8 @@
       </c>
     </row>
     <row r="5739" spans="1:4">
-      <c r="A5739" t="s">
-        <v>9</v>
+      <c r="A5739">
+        <v>6</v>
       </c>
       <c r="B5739" s="2">
         <v>44555</v>
@@ -81865,8 +81868,8 @@
       </c>
     </row>
     <row r="5740" spans="1:4">
-      <c r="A5740" t="s">
-        <v>10</v>
+      <c r="A5740">
+        <v>7</v>
       </c>
       <c r="B5740" s="2">
         <v>44555</v>
@@ -81879,8 +81882,8 @@
       </c>
     </row>
     <row r="5741" spans="1:4">
-      <c r="A5741" t="s">
-        <v>11</v>
+      <c r="A5741">
+        <v>8</v>
       </c>
       <c r="B5741" s="2">
         <v>44555</v>
@@ -81893,8 +81896,8 @@
       </c>
     </row>
     <row r="5742" spans="1:4">
-      <c r="A5742" t="s">
-        <v>12</v>
+      <c r="A5742">
+        <v>9</v>
       </c>
       <c r="B5742" s="2">
         <v>44555</v>
@@ -81907,8 +81910,8 @@
       </c>
     </row>
     <row r="5743" spans="1:4">
-      <c r="A5743" t="s">
-        <v>13</v>
+      <c r="A5743">
+        <v>10</v>
       </c>
       <c r="B5743" s="2">
         <v>44555</v>
@@ -81921,8 +81924,8 @@
       </c>
     </row>
     <row r="5744" spans="1:4">
-      <c r="A5744" t="s">
-        <v>14</v>
+      <c r="A5744">
+        <v>11</v>
       </c>
       <c r="B5744" s="2">
         <v>44555</v>
@@ -81935,8 +81938,8 @@
       </c>
     </row>
     <row r="5745" spans="1:4">
-      <c r="A5745" t="s">
-        <v>15</v>
+      <c r="A5745">
+        <v>12</v>
       </c>
       <c r="B5745" s="2">
         <v>44555</v>
@@ -81949,8 +81952,8 @@
       </c>
     </row>
     <row r="5746" spans="1:4">
-      <c r="A5746" t="s">
-        <v>16</v>
+      <c r="A5746">
+        <v>13</v>
       </c>
       <c r="B5746" s="2">
         <v>44555</v>
@@ -81963,8 +81966,8 @@
       </c>
     </row>
     <row r="5747" spans="1:4">
-      <c r="A5747" t="s">
-        <v>17</v>
+      <c r="A5747">
+        <v>14</v>
       </c>
       <c r="B5747" s="2">
         <v>44555</v>
@@ -81977,8 +81980,8 @@
       </c>
     </row>
     <row r="5748" spans="1:4">
-      <c r="A5748" t="s">
-        <v>18</v>
+      <c r="A5748">
+        <v>15</v>
       </c>
       <c r="B5748" s="2">
         <v>44555</v>
@@ -81991,8 +81994,8 @@
       </c>
     </row>
     <row r="5749" spans="1:4">
-      <c r="A5749" t="s">
-        <v>19</v>
+      <c r="A5749">
+        <v>16</v>
       </c>
       <c r="B5749" s="2">
         <v>44555</v>
@@ -82001,6 +82004,454 @@
         <v>378</v>
       </c>
       <c r="D5749">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5750" spans="1:4">
+      <c r="A5750" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5750" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5750" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5750">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5751" spans="1:4">
+      <c r="A5751" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5751" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5751" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5751">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5752" spans="1:4">
+      <c r="A5752" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5752" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5752" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5752">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5753" spans="1:4">
+      <c r="A5753" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5753" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5753" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5753">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5754" spans="1:4">
+      <c r="A5754" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5754" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5754" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5754">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5755" spans="1:4">
+      <c r="A5755" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5755" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5755" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5755">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5756" spans="1:4">
+      <c r="A5756" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5756" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5756" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5756">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5757" spans="1:4">
+      <c r="A5757" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5757" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5757" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5757">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5758" spans="1:4">
+      <c r="A5758" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5758" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5758" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5758">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5759" spans="1:4">
+      <c r="A5759" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5759" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5759" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5759">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5760" spans="1:4">
+      <c r="A5760" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5760" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5760" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5760">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5761" spans="1:4">
+      <c r="A5761" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5761" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5761" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5761">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5762" spans="1:4">
+      <c r="A5762" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5762" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5762" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5762">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5763" spans="1:4">
+      <c r="A5763" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5763" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5763" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5763">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5764" spans="1:4">
+      <c r="A5764" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5764" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5764" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5764">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5765" spans="1:4">
+      <c r="A5765" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5765" s="2">
+        <v>44555</v>
+      </c>
+      <c r="C5765" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5765">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5766" spans="1:4">
+      <c r="A5766" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5766" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5766" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5766">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5767" spans="1:4">
+      <c r="A5767" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5767" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5767" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5767">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5768" spans="1:4">
+      <c r="A5768" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5768" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5768" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5768">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5769" spans="1:4">
+      <c r="A5769" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5769" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5769" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5769">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5770" spans="1:4">
+      <c r="A5770" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5770" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5770" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5770">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5771" spans="1:4">
+      <c r="A5771" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5771" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5771" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5771">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5772" spans="1:4">
+      <c r="A5772" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5772" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5772" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5772">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5773" spans="1:4">
+      <c r="A5773" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5773" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5773" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5773">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5774" spans="1:4">
+      <c r="A5774" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5774" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5774" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5774">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5775" spans="1:4">
+      <c r="A5775" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5775" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5775" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5775">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5776" spans="1:4">
+      <c r="A5776" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5776" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5776" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5776">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5777" spans="1:4">
+      <c r="A5777" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5777" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5777" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5777">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5778" spans="1:4">
+      <c r="A5778" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5778" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5778" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5778">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5779" spans="1:4">
+      <c r="A5779" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5779" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5779" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5779">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5780" spans="1:4">
+      <c r="A5780" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5780" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5780" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5780">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5781" spans="1:4">
+      <c r="A5781" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5781" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5781" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5781">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-29-2021 15-02-24
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11340" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11372" uniqueCount="381">
   <si>
     <t>Región</t>
   </si>
@@ -1155,6 +1155,9 @@
   <si>
     <t>2021-12-26</t>
   </si>
+  <si>
+    <t>2021-12-27</t>
+  </si>
 </sst>
 </file>
 
@@ -1515,7 +1518,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5781"/>
+  <dimension ref="A1:D5813"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -82008,8 +82011,8 @@
       </c>
     </row>
     <row r="5750" spans="1:4">
-      <c r="A5750" t="s">
-        <v>4</v>
+      <c r="A5750">
+        <v>1</v>
       </c>
       <c r="B5750" s="2">
         <v>44555</v>
@@ -82022,8 +82025,8 @@
       </c>
     </row>
     <row r="5751" spans="1:4">
-      <c r="A5751" t="s">
-        <v>5</v>
+      <c r="A5751">
+        <v>2</v>
       </c>
       <c r="B5751" s="2">
         <v>44555</v>
@@ -82036,8 +82039,8 @@
       </c>
     </row>
     <row r="5752" spans="1:4">
-      <c r="A5752" t="s">
-        <v>6</v>
+      <c r="A5752">
+        <v>3</v>
       </c>
       <c r="B5752" s="2">
         <v>44555</v>
@@ -82050,8 +82053,8 @@
       </c>
     </row>
     <row r="5753" spans="1:4">
-      <c r="A5753" t="s">
-        <v>7</v>
+      <c r="A5753">
+        <v>4</v>
       </c>
       <c r="B5753" s="2">
         <v>44555</v>
@@ -82064,8 +82067,8 @@
       </c>
     </row>
     <row r="5754" spans="1:4">
-      <c r="A5754" t="s">
-        <v>8</v>
+      <c r="A5754">
+        <v>5</v>
       </c>
       <c r="B5754" s="2">
         <v>44555</v>
@@ -82078,8 +82081,8 @@
       </c>
     </row>
     <row r="5755" spans="1:4">
-      <c r="A5755" t="s">
-        <v>9</v>
+      <c r="A5755">
+        <v>6</v>
       </c>
       <c r="B5755" s="2">
         <v>44555</v>
@@ -82092,8 +82095,8 @@
       </c>
     </row>
     <row r="5756" spans="1:4">
-      <c r="A5756" t="s">
-        <v>10</v>
+      <c r="A5756">
+        <v>7</v>
       </c>
       <c r="B5756" s="2">
         <v>44555</v>
@@ -82106,8 +82109,8 @@
       </c>
     </row>
     <row r="5757" spans="1:4">
-      <c r="A5757" t="s">
-        <v>11</v>
+      <c r="A5757">
+        <v>8</v>
       </c>
       <c r="B5757" s="2">
         <v>44555</v>
@@ -82120,8 +82123,8 @@
       </c>
     </row>
     <row r="5758" spans="1:4">
-      <c r="A5758" t="s">
-        <v>12</v>
+      <c r="A5758">
+        <v>9</v>
       </c>
       <c r="B5758" s="2">
         <v>44555</v>
@@ -82134,8 +82137,8 @@
       </c>
     </row>
     <row r="5759" spans="1:4">
-      <c r="A5759" t="s">
-        <v>13</v>
+      <c r="A5759">
+        <v>10</v>
       </c>
       <c r="B5759" s="2">
         <v>44555</v>
@@ -82148,8 +82151,8 @@
       </c>
     </row>
     <row r="5760" spans="1:4">
-      <c r="A5760" t="s">
-        <v>14</v>
+      <c r="A5760">
+        <v>11</v>
       </c>
       <c r="B5760" s="2">
         <v>44555</v>
@@ -82162,8 +82165,8 @@
       </c>
     </row>
     <row r="5761" spans="1:4">
-      <c r="A5761" t="s">
-        <v>15</v>
+      <c r="A5761">
+        <v>12</v>
       </c>
       <c r="B5761" s="2">
         <v>44555</v>
@@ -82176,8 +82179,8 @@
       </c>
     </row>
     <row r="5762" spans="1:4">
-      <c r="A5762" t="s">
-        <v>16</v>
+      <c r="A5762">
+        <v>13</v>
       </c>
       <c r="B5762" s="2">
         <v>44555</v>
@@ -82190,8 +82193,8 @@
       </c>
     </row>
     <row r="5763" spans="1:4">
-      <c r="A5763" t="s">
-        <v>17</v>
+      <c r="A5763">
+        <v>14</v>
       </c>
       <c r="B5763" s="2">
         <v>44555</v>
@@ -82204,8 +82207,8 @@
       </c>
     </row>
     <row r="5764" spans="1:4">
-      <c r="A5764" t="s">
-        <v>18</v>
+      <c r="A5764">
+        <v>15</v>
       </c>
       <c r="B5764" s="2">
         <v>44555</v>
@@ -82218,8 +82221,8 @@
       </c>
     </row>
     <row r="5765" spans="1:4">
-      <c r="A5765" t="s">
-        <v>19</v>
+      <c r="A5765">
+        <v>16</v>
       </c>
       <c r="B5765" s="2">
         <v>44555</v>
@@ -82232,8 +82235,8 @@
       </c>
     </row>
     <row r="5766" spans="1:4">
-      <c r="A5766" t="s">
-        <v>4</v>
+      <c r="A5766">
+        <v>1</v>
       </c>
       <c r="B5766" s="2">
         <v>44556</v>
@@ -82246,8 +82249,8 @@
       </c>
     </row>
     <row r="5767" spans="1:4">
-      <c r="A5767" t="s">
-        <v>5</v>
+      <c r="A5767">
+        <v>2</v>
       </c>
       <c r="B5767" s="2">
         <v>44556</v>
@@ -82260,8 +82263,8 @@
       </c>
     </row>
     <row r="5768" spans="1:4">
-      <c r="A5768" t="s">
-        <v>6</v>
+      <c r="A5768">
+        <v>3</v>
       </c>
       <c r="B5768" s="2">
         <v>44556</v>
@@ -82274,8 +82277,8 @@
       </c>
     </row>
     <row r="5769" spans="1:4">
-      <c r="A5769" t="s">
-        <v>7</v>
+      <c r="A5769">
+        <v>4</v>
       </c>
       <c r="B5769" s="2">
         <v>44556</v>
@@ -82288,8 +82291,8 @@
       </c>
     </row>
     <row r="5770" spans="1:4">
-      <c r="A5770" t="s">
-        <v>8</v>
+      <c r="A5770">
+        <v>5</v>
       </c>
       <c r="B5770" s="2">
         <v>44556</v>
@@ -82302,8 +82305,8 @@
       </c>
     </row>
     <row r="5771" spans="1:4">
-      <c r="A5771" t="s">
-        <v>9</v>
+      <c r="A5771">
+        <v>6</v>
       </c>
       <c r="B5771" s="2">
         <v>44556</v>
@@ -82316,8 +82319,8 @@
       </c>
     </row>
     <row r="5772" spans="1:4">
-      <c r="A5772" t="s">
-        <v>10</v>
+      <c r="A5772">
+        <v>7</v>
       </c>
       <c r="B5772" s="2">
         <v>44556</v>
@@ -82330,8 +82333,8 @@
       </c>
     </row>
     <row r="5773" spans="1:4">
-      <c r="A5773" t="s">
-        <v>11</v>
+      <c r="A5773">
+        <v>8</v>
       </c>
       <c r="B5773" s="2">
         <v>44556</v>
@@ -82344,8 +82347,8 @@
       </c>
     </row>
     <row r="5774" spans="1:4">
-      <c r="A5774" t="s">
-        <v>12</v>
+      <c r="A5774">
+        <v>9</v>
       </c>
       <c r="B5774" s="2">
         <v>44556</v>
@@ -82358,8 +82361,8 @@
       </c>
     </row>
     <row r="5775" spans="1:4">
-      <c r="A5775" t="s">
-        <v>13</v>
+      <c r="A5775">
+        <v>10</v>
       </c>
       <c r="B5775" s="2">
         <v>44556</v>
@@ -82372,8 +82375,8 @@
       </c>
     </row>
     <row r="5776" spans="1:4">
-      <c r="A5776" t="s">
-        <v>14</v>
+      <c r="A5776">
+        <v>11</v>
       </c>
       <c r="B5776" s="2">
         <v>44556</v>
@@ -82386,8 +82389,8 @@
       </c>
     </row>
     <row r="5777" spans="1:4">
-      <c r="A5777" t="s">
-        <v>15</v>
+      <c r="A5777">
+        <v>12</v>
       </c>
       <c r="B5777" s="2">
         <v>44556</v>
@@ -82400,8 +82403,8 @@
       </c>
     </row>
     <row r="5778" spans="1:4">
-      <c r="A5778" t="s">
-        <v>16</v>
+      <c r="A5778">
+        <v>13</v>
       </c>
       <c r="B5778" s="2">
         <v>44556</v>
@@ -82414,8 +82417,8 @@
       </c>
     </row>
     <row r="5779" spans="1:4">
-      <c r="A5779" t="s">
-        <v>17</v>
+      <c r="A5779">
+        <v>14</v>
       </c>
       <c r="B5779" s="2">
         <v>44556</v>
@@ -82428,8 +82431,8 @@
       </c>
     </row>
     <row r="5780" spans="1:4">
-      <c r="A5780" t="s">
-        <v>18</v>
+      <c r="A5780">
+        <v>15</v>
       </c>
       <c r="B5780" s="2">
         <v>44556</v>
@@ -82442,8 +82445,8 @@
       </c>
     </row>
     <row r="5781" spans="1:4">
-      <c r="A5781" t="s">
-        <v>19</v>
+      <c r="A5781">
+        <v>16</v>
       </c>
       <c r="B5781" s="2">
         <v>44556</v>
@@ -82452,6 +82455,454 @@
         <v>379</v>
       </c>
       <c r="D5781">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5782" spans="1:4">
+      <c r="A5782" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5782" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5782" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5782">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5783" spans="1:4">
+      <c r="A5783" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5783" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5783" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5783">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5784" spans="1:4">
+      <c r="A5784" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5784" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5784" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5784">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5785" spans="1:4">
+      <c r="A5785" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5785" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5785" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5785">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5786" spans="1:4">
+      <c r="A5786" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5786" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5786" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5786">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5787" spans="1:4">
+      <c r="A5787" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5787" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5787" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5787">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5788" spans="1:4">
+      <c r="A5788" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5788" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5788" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5788">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5789" spans="1:4">
+      <c r="A5789" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5789" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5789" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5789">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5790" spans="1:4">
+      <c r="A5790" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5790" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5790" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5790">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5791" spans="1:4">
+      <c r="A5791" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5791" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5791" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5791">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5792" spans="1:4">
+      <c r="A5792" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5792" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5792" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5792">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5793" spans="1:4">
+      <c r="A5793" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5793" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5793" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5793">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5794" spans="1:4">
+      <c r="A5794" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5794" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5794" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5794">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5795" spans="1:4">
+      <c r="A5795" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5795" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5795" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5795">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5796" spans="1:4">
+      <c r="A5796" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5796" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5796" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5796">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5797" spans="1:4">
+      <c r="A5797" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5797" s="2">
+        <v>44556</v>
+      </c>
+      <c r="C5797" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5797">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5798" spans="1:4">
+      <c r="A5798" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5798" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5798" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5798">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5799" spans="1:4">
+      <c r="A5799" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5799" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5799" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5799">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5800" spans="1:4">
+      <c r="A5800" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5800" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5800" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5800">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5801" spans="1:4">
+      <c r="A5801" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5801" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5801" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5801">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5802" spans="1:4">
+      <c r="A5802" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5802" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5802" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5802">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5803" spans="1:4">
+      <c r="A5803" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5803" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5803" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5803">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5804" spans="1:4">
+      <c r="A5804" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5804" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5804" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5804">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5805" spans="1:4">
+      <c r="A5805" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5805" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5805" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5805">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5806" spans="1:4">
+      <c r="A5806" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5806" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5806" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5806">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5807" spans="1:4">
+      <c r="A5807" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5807" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5807" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5807">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5808" spans="1:4">
+      <c r="A5808" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5808" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5808" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5808">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5809" spans="1:4">
+      <c r="A5809" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5809" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5809" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5809">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5810" spans="1:4">
+      <c r="A5810" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5810" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5810" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5810">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5811" spans="1:4">
+      <c r="A5811" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5811" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5811" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5811">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5812" spans="1:4">
+      <c r="A5812" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5812" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5812" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5812">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5813" spans="1:4">
+      <c r="A5813" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5813" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5813" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5813">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-30-2021 15-34-06
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11372" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11404" uniqueCount="382">
   <si>
     <t>Región</t>
   </si>
@@ -1158,6 +1158,9 @@
   <si>
     <t>2021-12-27</t>
   </si>
+  <si>
+    <t>2021-12-28</t>
+  </si>
 </sst>
 </file>
 
@@ -1518,7 +1521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5813"/>
+  <dimension ref="A1:D5845"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -82459,8 +82462,8 @@
       </c>
     </row>
     <row r="5782" spans="1:4">
-      <c r="A5782" t="s">
-        <v>4</v>
+      <c r="A5782">
+        <v>1</v>
       </c>
       <c r="B5782" s="2">
         <v>44556</v>
@@ -82473,8 +82476,8 @@
       </c>
     </row>
     <row r="5783" spans="1:4">
-      <c r="A5783" t="s">
-        <v>5</v>
+      <c r="A5783">
+        <v>2</v>
       </c>
       <c r="B5783" s="2">
         <v>44556</v>
@@ -82487,8 +82490,8 @@
       </c>
     </row>
     <row r="5784" spans="1:4">
-      <c r="A5784" t="s">
-        <v>6</v>
+      <c r="A5784">
+        <v>3</v>
       </c>
       <c r="B5784" s="2">
         <v>44556</v>
@@ -82501,8 +82504,8 @@
       </c>
     </row>
     <row r="5785" spans="1:4">
-      <c r="A5785" t="s">
-        <v>7</v>
+      <c r="A5785">
+        <v>4</v>
       </c>
       <c r="B5785" s="2">
         <v>44556</v>
@@ -82515,8 +82518,8 @@
       </c>
     </row>
     <row r="5786" spans="1:4">
-      <c r="A5786" t="s">
-        <v>8</v>
+      <c r="A5786">
+        <v>5</v>
       </c>
       <c r="B5786" s="2">
         <v>44556</v>
@@ -82529,8 +82532,8 @@
       </c>
     </row>
     <row r="5787" spans="1:4">
-      <c r="A5787" t="s">
-        <v>9</v>
+      <c r="A5787">
+        <v>6</v>
       </c>
       <c r="B5787" s="2">
         <v>44556</v>
@@ -82543,8 +82546,8 @@
       </c>
     </row>
     <row r="5788" spans="1:4">
-      <c r="A5788" t="s">
-        <v>10</v>
+      <c r="A5788">
+        <v>7</v>
       </c>
       <c r="B5788" s="2">
         <v>44556</v>
@@ -82557,8 +82560,8 @@
       </c>
     </row>
     <row r="5789" spans="1:4">
-      <c r="A5789" t="s">
-        <v>11</v>
+      <c r="A5789">
+        <v>8</v>
       </c>
       <c r="B5789" s="2">
         <v>44556</v>
@@ -82571,8 +82574,8 @@
       </c>
     </row>
     <row r="5790" spans="1:4">
-      <c r="A5790" t="s">
-        <v>12</v>
+      <c r="A5790">
+        <v>9</v>
       </c>
       <c r="B5790" s="2">
         <v>44556</v>
@@ -82585,8 +82588,8 @@
       </c>
     </row>
     <row r="5791" spans="1:4">
-      <c r="A5791" t="s">
-        <v>13</v>
+      <c r="A5791">
+        <v>10</v>
       </c>
       <c r="B5791" s="2">
         <v>44556</v>
@@ -82599,8 +82602,8 @@
       </c>
     </row>
     <row r="5792" spans="1:4">
-      <c r="A5792" t="s">
-        <v>14</v>
+      <c r="A5792">
+        <v>11</v>
       </c>
       <c r="B5792" s="2">
         <v>44556</v>
@@ -82613,8 +82616,8 @@
       </c>
     </row>
     <row r="5793" spans="1:4">
-      <c r="A5793" t="s">
-        <v>15</v>
+      <c r="A5793">
+        <v>12</v>
       </c>
       <c r="B5793" s="2">
         <v>44556</v>
@@ -82627,8 +82630,8 @@
       </c>
     </row>
     <row r="5794" spans="1:4">
-      <c r="A5794" t="s">
-        <v>16</v>
+      <c r="A5794">
+        <v>13</v>
       </c>
       <c r="B5794" s="2">
         <v>44556</v>
@@ -82641,8 +82644,8 @@
       </c>
     </row>
     <row r="5795" spans="1:4">
-      <c r="A5795" t="s">
-        <v>17</v>
+      <c r="A5795">
+        <v>14</v>
       </c>
       <c r="B5795" s="2">
         <v>44556</v>
@@ -82655,8 +82658,8 @@
       </c>
     </row>
     <row r="5796" spans="1:4">
-      <c r="A5796" t="s">
-        <v>18</v>
+      <c r="A5796">
+        <v>15</v>
       </c>
       <c r="B5796" s="2">
         <v>44556</v>
@@ -82669,8 +82672,8 @@
       </c>
     </row>
     <row r="5797" spans="1:4">
-      <c r="A5797" t="s">
-        <v>19</v>
+      <c r="A5797">
+        <v>16</v>
       </c>
       <c r="B5797" s="2">
         <v>44556</v>
@@ -82683,8 +82686,8 @@
       </c>
     </row>
     <row r="5798" spans="1:4">
-      <c r="A5798" t="s">
-        <v>4</v>
+      <c r="A5798">
+        <v>1</v>
       </c>
       <c r="B5798" s="2">
         <v>44557</v>
@@ -82697,8 +82700,8 @@
       </c>
     </row>
     <row r="5799" spans="1:4">
-      <c r="A5799" t="s">
-        <v>5</v>
+      <c r="A5799">
+        <v>2</v>
       </c>
       <c r="B5799" s="2">
         <v>44557</v>
@@ -82711,8 +82714,8 @@
       </c>
     </row>
     <row r="5800" spans="1:4">
-      <c r="A5800" t="s">
-        <v>6</v>
+      <c r="A5800">
+        <v>3</v>
       </c>
       <c r="B5800" s="2">
         <v>44557</v>
@@ -82725,8 +82728,8 @@
       </c>
     </row>
     <row r="5801" spans="1:4">
-      <c r="A5801" t="s">
-        <v>7</v>
+      <c r="A5801">
+        <v>4</v>
       </c>
       <c r="B5801" s="2">
         <v>44557</v>
@@ -82739,8 +82742,8 @@
       </c>
     </row>
     <row r="5802" spans="1:4">
-      <c r="A5802" t="s">
-        <v>8</v>
+      <c r="A5802">
+        <v>5</v>
       </c>
       <c r="B5802" s="2">
         <v>44557</v>
@@ -82753,8 +82756,8 @@
       </c>
     </row>
     <row r="5803" spans="1:4">
-      <c r="A5803" t="s">
-        <v>9</v>
+      <c r="A5803">
+        <v>6</v>
       </c>
       <c r="B5803" s="2">
         <v>44557</v>
@@ -82767,8 +82770,8 @@
       </c>
     </row>
     <row r="5804" spans="1:4">
-      <c r="A5804" t="s">
-        <v>10</v>
+      <c r="A5804">
+        <v>7</v>
       </c>
       <c r="B5804" s="2">
         <v>44557</v>
@@ -82781,8 +82784,8 @@
       </c>
     </row>
     <row r="5805" spans="1:4">
-      <c r="A5805" t="s">
-        <v>11</v>
+      <c r="A5805">
+        <v>8</v>
       </c>
       <c r="B5805" s="2">
         <v>44557</v>
@@ -82795,8 +82798,8 @@
       </c>
     </row>
     <row r="5806" spans="1:4">
-      <c r="A5806" t="s">
-        <v>12</v>
+      <c r="A5806">
+        <v>9</v>
       </c>
       <c r="B5806" s="2">
         <v>44557</v>
@@ -82809,8 +82812,8 @@
       </c>
     </row>
     <row r="5807" spans="1:4">
-      <c r="A5807" t="s">
-        <v>13</v>
+      <c r="A5807">
+        <v>10</v>
       </c>
       <c r="B5807" s="2">
         <v>44557</v>
@@ -82823,8 +82826,8 @@
       </c>
     </row>
     <row r="5808" spans="1:4">
-      <c r="A5808" t="s">
-        <v>14</v>
+      <c r="A5808">
+        <v>11</v>
       </c>
       <c r="B5808" s="2">
         <v>44557</v>
@@ -82837,8 +82840,8 @@
       </c>
     </row>
     <row r="5809" spans="1:4">
-      <c r="A5809" t="s">
-        <v>15</v>
+      <c r="A5809">
+        <v>12</v>
       </c>
       <c r="B5809" s="2">
         <v>44557</v>
@@ -82851,8 +82854,8 @@
       </c>
     </row>
     <row r="5810" spans="1:4">
-      <c r="A5810" t="s">
-        <v>16</v>
+      <c r="A5810">
+        <v>13</v>
       </c>
       <c r="B5810" s="2">
         <v>44557</v>
@@ -82865,8 +82868,8 @@
       </c>
     </row>
     <row r="5811" spans="1:4">
-      <c r="A5811" t="s">
-        <v>17</v>
+      <c r="A5811">
+        <v>14</v>
       </c>
       <c r="B5811" s="2">
         <v>44557</v>
@@ -82879,8 +82882,8 @@
       </c>
     </row>
     <row r="5812" spans="1:4">
-      <c r="A5812" t="s">
-        <v>18</v>
+      <c r="A5812">
+        <v>15</v>
       </c>
       <c r="B5812" s="2">
         <v>44557</v>
@@ -82893,8 +82896,8 @@
       </c>
     </row>
     <row r="5813" spans="1:4">
-      <c r="A5813" t="s">
-        <v>19</v>
+      <c r="A5813">
+        <v>16</v>
       </c>
       <c r="B5813" s="2">
         <v>44557</v>
@@ -82904,6 +82907,454 @@
       </c>
       <c r="D5813">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5814" spans="1:4">
+      <c r="A5814" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5814" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5814" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5814">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5815" spans="1:4">
+      <c r="A5815" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5815" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5815" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5815">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5816" spans="1:4">
+      <c r="A5816" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5816" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5816" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5816">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5817" spans="1:4">
+      <c r="A5817" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5817" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5817" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5817">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5818" spans="1:4">
+      <c r="A5818" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5818" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5818" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5818">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5819" spans="1:4">
+      <c r="A5819" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5819" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5819" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5819">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5820" spans="1:4">
+      <c r="A5820" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5820" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5820" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5820">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5821" spans="1:4">
+      <c r="A5821" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5821" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5821" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5821">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5822" spans="1:4">
+      <c r="A5822" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5822" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5822" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5822">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5823" spans="1:4">
+      <c r="A5823" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5823" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5823" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5823">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5824" spans="1:4">
+      <c r="A5824" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5824" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5824" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5824">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5825" spans="1:4">
+      <c r="A5825" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5825" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5825" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5825">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5826" spans="1:4">
+      <c r="A5826" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5826" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5826" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5826">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5827" spans="1:4">
+      <c r="A5827" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5827" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5827" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5827">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5828" spans="1:4">
+      <c r="A5828" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5828" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5828" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5828">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5829" spans="1:4">
+      <c r="A5829" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5829" s="2">
+        <v>44557</v>
+      </c>
+      <c r="C5829" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5829">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5830" spans="1:4">
+      <c r="A5830" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5830" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5830" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5830">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5831" spans="1:4">
+      <c r="A5831" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5831" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5831" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5831">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5832" spans="1:4">
+      <c r="A5832" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5832" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5832" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5832">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5833" spans="1:4">
+      <c r="A5833" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5833" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5833" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5833">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5834" spans="1:4">
+      <c r="A5834" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5834" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5834" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5834">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5835" spans="1:4">
+      <c r="A5835" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5835" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5835" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5835">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5836" spans="1:4">
+      <c r="A5836" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5836" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5836" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5836">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5837" spans="1:4">
+      <c r="A5837" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5837" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5837" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5837">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5838" spans="1:4">
+      <c r="A5838" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5838" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5838" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5838">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5839" spans="1:4">
+      <c r="A5839" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5839" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5839" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5839">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5840" spans="1:4">
+      <c r="A5840" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5840" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5840" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5840">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5841" spans="1:4">
+      <c r="A5841" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5841" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5841" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5841">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5842" spans="1:4">
+      <c r="A5842" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5842" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5842" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5842">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5843" spans="1:4">
+      <c r="A5843" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5843" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5843" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5843">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5844" spans="1:4">
+      <c r="A5844" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5844" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5844" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5844">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5845" spans="1:4">
+      <c r="A5845" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5845" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5845" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5845">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-31-2021 16-05-39
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11404" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11436" uniqueCount="383">
   <si>
     <t>Región</t>
   </si>
@@ -1161,6 +1161,9 @@
   <si>
     <t>2021-12-28</t>
   </si>
+  <si>
+    <t>2021-12-29</t>
+  </si>
 </sst>
 </file>
 
@@ -1521,7 +1524,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5845"/>
+  <dimension ref="A1:D5877"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -82910,8 +82913,8 @@
       </c>
     </row>
     <row r="5814" spans="1:4">
-      <c r="A5814" t="s">
-        <v>4</v>
+      <c r="A5814">
+        <v>1</v>
       </c>
       <c r="B5814" s="2">
         <v>44557</v>
@@ -82924,8 +82927,8 @@
       </c>
     </row>
     <row r="5815" spans="1:4">
-      <c r="A5815" t="s">
-        <v>5</v>
+      <c r="A5815">
+        <v>2</v>
       </c>
       <c r="B5815" s="2">
         <v>44557</v>
@@ -82938,8 +82941,8 @@
       </c>
     </row>
     <row r="5816" spans="1:4">
-      <c r="A5816" t="s">
-        <v>6</v>
+      <c r="A5816">
+        <v>3</v>
       </c>
       <c r="B5816" s="2">
         <v>44557</v>
@@ -82952,8 +82955,8 @@
       </c>
     </row>
     <row r="5817" spans="1:4">
-      <c r="A5817" t="s">
-        <v>7</v>
+      <c r="A5817">
+        <v>4</v>
       </c>
       <c r="B5817" s="2">
         <v>44557</v>
@@ -82966,8 +82969,8 @@
       </c>
     </row>
     <row r="5818" spans="1:4">
-      <c r="A5818" t="s">
-        <v>8</v>
+      <c r="A5818">
+        <v>5</v>
       </c>
       <c r="B5818" s="2">
         <v>44557</v>
@@ -82980,8 +82983,8 @@
       </c>
     </row>
     <row r="5819" spans="1:4">
-      <c r="A5819" t="s">
-        <v>9</v>
+      <c r="A5819">
+        <v>6</v>
       </c>
       <c r="B5819" s="2">
         <v>44557</v>
@@ -82994,8 +82997,8 @@
       </c>
     </row>
     <row r="5820" spans="1:4">
-      <c r="A5820" t="s">
-        <v>10</v>
+      <c r="A5820">
+        <v>7</v>
       </c>
       <c r="B5820" s="2">
         <v>44557</v>
@@ -83008,8 +83011,8 @@
       </c>
     </row>
     <row r="5821" spans="1:4">
-      <c r="A5821" t="s">
-        <v>11</v>
+      <c r="A5821">
+        <v>8</v>
       </c>
       <c r="B5821" s="2">
         <v>44557</v>
@@ -83022,8 +83025,8 @@
       </c>
     </row>
     <row r="5822" spans="1:4">
-      <c r="A5822" t="s">
-        <v>12</v>
+      <c r="A5822">
+        <v>9</v>
       </c>
       <c r="B5822" s="2">
         <v>44557</v>
@@ -83036,8 +83039,8 @@
       </c>
     </row>
     <row r="5823" spans="1:4">
-      <c r="A5823" t="s">
-        <v>13</v>
+      <c r="A5823">
+        <v>10</v>
       </c>
       <c r="B5823" s="2">
         <v>44557</v>
@@ -83050,8 +83053,8 @@
       </c>
     </row>
     <row r="5824" spans="1:4">
-      <c r="A5824" t="s">
-        <v>14</v>
+      <c r="A5824">
+        <v>11</v>
       </c>
       <c r="B5824" s="2">
         <v>44557</v>
@@ -83064,8 +83067,8 @@
       </c>
     </row>
     <row r="5825" spans="1:4">
-      <c r="A5825" t="s">
-        <v>15</v>
+      <c r="A5825">
+        <v>12</v>
       </c>
       <c r="B5825" s="2">
         <v>44557</v>
@@ -83078,8 +83081,8 @@
       </c>
     </row>
     <row r="5826" spans="1:4">
-      <c r="A5826" t="s">
-        <v>16</v>
+      <c r="A5826">
+        <v>13</v>
       </c>
       <c r="B5826" s="2">
         <v>44557</v>
@@ -83092,8 +83095,8 @@
       </c>
     </row>
     <row r="5827" spans="1:4">
-      <c r="A5827" t="s">
-        <v>17</v>
+      <c r="A5827">
+        <v>14</v>
       </c>
       <c r="B5827" s="2">
         <v>44557</v>
@@ -83106,8 +83109,8 @@
       </c>
     </row>
     <row r="5828" spans="1:4">
-      <c r="A5828" t="s">
-        <v>18</v>
+      <c r="A5828">
+        <v>15</v>
       </c>
       <c r="B5828" s="2">
         <v>44557</v>
@@ -83120,8 +83123,8 @@
       </c>
     </row>
     <row r="5829" spans="1:4">
-      <c r="A5829" t="s">
-        <v>19</v>
+      <c r="A5829">
+        <v>16</v>
       </c>
       <c r="B5829" s="2">
         <v>44557</v>
@@ -83134,8 +83137,8 @@
       </c>
     </row>
     <row r="5830" spans="1:4">
-      <c r="A5830" t="s">
-        <v>4</v>
+      <c r="A5830">
+        <v>1</v>
       </c>
       <c r="B5830" s="2">
         <v>44558</v>
@@ -83148,8 +83151,8 @@
       </c>
     </row>
     <row r="5831" spans="1:4">
-      <c r="A5831" t="s">
-        <v>5</v>
+      <c r="A5831">
+        <v>2</v>
       </c>
       <c r="B5831" s="2">
         <v>44558</v>
@@ -83162,8 +83165,8 @@
       </c>
     </row>
     <row r="5832" spans="1:4">
-      <c r="A5832" t="s">
-        <v>6</v>
+      <c r="A5832">
+        <v>3</v>
       </c>
       <c r="B5832" s="2">
         <v>44558</v>
@@ -83176,8 +83179,8 @@
       </c>
     </row>
     <row r="5833" spans="1:4">
-      <c r="A5833" t="s">
-        <v>7</v>
+      <c r="A5833">
+        <v>4</v>
       </c>
       <c r="B5833" s="2">
         <v>44558</v>
@@ -83190,8 +83193,8 @@
       </c>
     </row>
     <row r="5834" spans="1:4">
-      <c r="A5834" t="s">
-        <v>8</v>
+      <c r="A5834">
+        <v>5</v>
       </c>
       <c r="B5834" s="2">
         <v>44558</v>
@@ -83204,8 +83207,8 @@
       </c>
     </row>
     <row r="5835" spans="1:4">
-      <c r="A5835" t="s">
-        <v>9</v>
+      <c r="A5835">
+        <v>6</v>
       </c>
       <c r="B5835" s="2">
         <v>44558</v>
@@ -83218,8 +83221,8 @@
       </c>
     </row>
     <row r="5836" spans="1:4">
-      <c r="A5836" t="s">
-        <v>10</v>
+      <c r="A5836">
+        <v>7</v>
       </c>
       <c r="B5836" s="2">
         <v>44558</v>
@@ -83232,8 +83235,8 @@
       </c>
     </row>
     <row r="5837" spans="1:4">
-      <c r="A5837" t="s">
-        <v>11</v>
+      <c r="A5837">
+        <v>8</v>
       </c>
       <c r="B5837" s="2">
         <v>44558</v>
@@ -83246,8 +83249,8 @@
       </c>
     </row>
     <row r="5838" spans="1:4">
-      <c r="A5838" t="s">
-        <v>12</v>
+      <c r="A5838">
+        <v>9</v>
       </c>
       <c r="B5838" s="2">
         <v>44558</v>
@@ -83260,8 +83263,8 @@
       </c>
     </row>
     <row r="5839" spans="1:4">
-      <c r="A5839" t="s">
-        <v>13</v>
+      <c r="A5839">
+        <v>10</v>
       </c>
       <c r="B5839" s="2">
         <v>44558</v>
@@ -83274,8 +83277,8 @@
       </c>
     </row>
     <row r="5840" spans="1:4">
-      <c r="A5840" t="s">
-        <v>14</v>
+      <c r="A5840">
+        <v>11</v>
       </c>
       <c r="B5840" s="2">
         <v>44558</v>
@@ -83288,8 +83291,8 @@
       </c>
     </row>
     <row r="5841" spans="1:4">
-      <c r="A5841" t="s">
-        <v>15</v>
+      <c r="A5841">
+        <v>12</v>
       </c>
       <c r="B5841" s="2">
         <v>44558</v>
@@ -83302,8 +83305,8 @@
       </c>
     </row>
     <row r="5842" spans="1:4">
-      <c r="A5842" t="s">
-        <v>16</v>
+      <c r="A5842">
+        <v>13</v>
       </c>
       <c r="B5842" s="2">
         <v>44558</v>
@@ -83316,8 +83319,8 @@
       </c>
     </row>
     <row r="5843" spans="1:4">
-      <c r="A5843" t="s">
-        <v>17</v>
+      <c r="A5843">
+        <v>14</v>
       </c>
       <c r="B5843" s="2">
         <v>44558</v>
@@ -83330,8 +83333,8 @@
       </c>
     </row>
     <row r="5844" spans="1:4">
-      <c r="A5844" t="s">
-        <v>18</v>
+      <c r="A5844">
+        <v>15</v>
       </c>
       <c r="B5844" s="2">
         <v>44558</v>
@@ -83344,8 +83347,8 @@
       </c>
     </row>
     <row r="5845" spans="1:4">
-      <c r="A5845" t="s">
-        <v>19</v>
+      <c r="A5845">
+        <v>16</v>
       </c>
       <c r="B5845" s="2">
         <v>44558</v>
@@ -83354,6 +83357,454 @@
         <v>381</v>
       </c>
       <c r="D5845">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5846" spans="1:4">
+      <c r="A5846" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5846" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5846" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5846">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5847" spans="1:4">
+      <c r="A5847" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5847" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5847" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5847">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5848" spans="1:4">
+      <c r="A5848" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5848" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5848" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5848">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5849" spans="1:4">
+      <c r="A5849" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5849" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5849" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5849">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5850" spans="1:4">
+      <c r="A5850" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5850" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5850" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5850">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5851" spans="1:4">
+      <c r="A5851" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5851" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5851" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5851">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5852" spans="1:4">
+      <c r="A5852" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5852" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5852" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5852">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5853" spans="1:4">
+      <c r="A5853" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5853" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5853" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5853">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5854" spans="1:4">
+      <c r="A5854" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5854" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5854" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5854">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5855" spans="1:4">
+      <c r="A5855" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5855" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5855" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5855">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5856" spans="1:4">
+      <c r="A5856" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5856" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5856" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5856">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5857" spans="1:4">
+      <c r="A5857" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5857" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5857" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5857">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5858" spans="1:4">
+      <c r="A5858" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5858" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5858" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5858">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5859" spans="1:4">
+      <c r="A5859" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5859" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5859" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5859">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5860" spans="1:4">
+      <c r="A5860" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5860" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5860" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5860">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5861" spans="1:4">
+      <c r="A5861" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5861" s="2">
+        <v>44558</v>
+      </c>
+      <c r="C5861" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5861">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5862" spans="1:4">
+      <c r="A5862" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5862" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5862" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5862">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5863" spans="1:4">
+      <c r="A5863" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5863" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5863" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5863">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5864" spans="1:4">
+      <c r="A5864" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5864" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5864" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5864">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5865" spans="1:4">
+      <c r="A5865" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5865" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5865" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5865">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5866" spans="1:4">
+      <c r="A5866" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5866" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5866" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5866">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5867" spans="1:4">
+      <c r="A5867" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5867" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5867" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5867">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5868" spans="1:4">
+      <c r="A5868" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5868" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5868" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5868">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5869" spans="1:4">
+      <c r="A5869" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5869" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5869" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5869">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5870" spans="1:4">
+      <c r="A5870" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5870" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5870" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5870">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5871" spans="1:4">
+      <c r="A5871" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5871" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5871" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5871">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5872" spans="1:4">
+      <c r="A5872" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5872" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5872" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5872">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5873" spans="1:4">
+      <c r="A5873" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5873" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5873" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5873">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5874" spans="1:4">
+      <c r="A5874" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5874" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5874" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5874">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5875" spans="1:4">
+      <c r="A5875" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5875" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5875" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5875">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5876" spans="1:4">
+      <c r="A5876" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5876" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5876" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5876">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5877" spans="1:4">
+      <c r="A5877" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5877" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5877" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5877">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-01-2022 16-36-36
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11436" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11468" uniqueCount="384">
   <si>
     <t>Región</t>
   </si>
@@ -1164,6 +1164,9 @@
   <si>
     <t>2021-12-29</t>
   </si>
+  <si>
+    <t>2021-12-30</t>
+  </si>
 </sst>
 </file>
 
@@ -1524,7 +1527,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5877"/>
+  <dimension ref="A1:D5909"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -83361,8 +83364,8 @@
       </c>
     </row>
     <row r="5846" spans="1:4">
-      <c r="A5846" t="s">
-        <v>4</v>
+      <c r="A5846">
+        <v>1</v>
       </c>
       <c r="B5846" s="2">
         <v>44558</v>
@@ -83375,8 +83378,8 @@
       </c>
     </row>
     <row r="5847" spans="1:4">
-      <c r="A5847" t="s">
-        <v>5</v>
+      <c r="A5847">
+        <v>2</v>
       </c>
       <c r="B5847" s="2">
         <v>44558</v>
@@ -83389,8 +83392,8 @@
       </c>
     </row>
     <row r="5848" spans="1:4">
-      <c r="A5848" t="s">
-        <v>6</v>
+      <c r="A5848">
+        <v>3</v>
       </c>
       <c r="B5848" s="2">
         <v>44558</v>
@@ -83403,8 +83406,8 @@
       </c>
     </row>
     <row r="5849" spans="1:4">
-      <c r="A5849" t="s">
-        <v>7</v>
+      <c r="A5849">
+        <v>4</v>
       </c>
       <c r="B5849" s="2">
         <v>44558</v>
@@ -83417,8 +83420,8 @@
       </c>
     </row>
     <row r="5850" spans="1:4">
-      <c r="A5850" t="s">
-        <v>8</v>
+      <c r="A5850">
+        <v>5</v>
       </c>
       <c r="B5850" s="2">
         <v>44558</v>
@@ -83431,8 +83434,8 @@
       </c>
     </row>
     <row r="5851" spans="1:4">
-      <c r="A5851" t="s">
-        <v>9</v>
+      <c r="A5851">
+        <v>6</v>
       </c>
       <c r="B5851" s="2">
         <v>44558</v>
@@ -83445,8 +83448,8 @@
       </c>
     </row>
     <row r="5852" spans="1:4">
-      <c r="A5852" t="s">
-        <v>10</v>
+      <c r="A5852">
+        <v>7</v>
       </c>
       <c r="B5852" s="2">
         <v>44558</v>
@@ -83459,8 +83462,8 @@
       </c>
     </row>
     <row r="5853" spans="1:4">
-      <c r="A5853" t="s">
-        <v>11</v>
+      <c r="A5853">
+        <v>8</v>
       </c>
       <c r="B5853" s="2">
         <v>44558</v>
@@ -83473,8 +83476,8 @@
       </c>
     </row>
     <row r="5854" spans="1:4">
-      <c r="A5854" t="s">
-        <v>12</v>
+      <c r="A5854">
+        <v>9</v>
       </c>
       <c r="B5854" s="2">
         <v>44558</v>
@@ -83487,8 +83490,8 @@
       </c>
     </row>
     <row r="5855" spans="1:4">
-      <c r="A5855" t="s">
-        <v>13</v>
+      <c r="A5855">
+        <v>10</v>
       </c>
       <c r="B5855" s="2">
         <v>44558</v>
@@ -83501,8 +83504,8 @@
       </c>
     </row>
     <row r="5856" spans="1:4">
-      <c r="A5856" t="s">
-        <v>14</v>
+      <c r="A5856">
+        <v>11</v>
       </c>
       <c r="B5856" s="2">
         <v>44558</v>
@@ -83515,8 +83518,8 @@
       </c>
     </row>
     <row r="5857" spans="1:4">
-      <c r="A5857" t="s">
-        <v>15</v>
+      <c r="A5857">
+        <v>12</v>
       </c>
       <c r="B5857" s="2">
         <v>44558</v>
@@ -83529,8 +83532,8 @@
       </c>
     </row>
     <row r="5858" spans="1:4">
-      <c r="A5858" t="s">
-        <v>16</v>
+      <c r="A5858">
+        <v>13</v>
       </c>
       <c r="B5858" s="2">
         <v>44558</v>
@@ -83543,8 +83546,8 @@
       </c>
     </row>
     <row r="5859" spans="1:4">
-      <c r="A5859" t="s">
-        <v>17</v>
+      <c r="A5859">
+        <v>14</v>
       </c>
       <c r="B5859" s="2">
         <v>44558</v>
@@ -83557,8 +83560,8 @@
       </c>
     </row>
     <row r="5860" spans="1:4">
-      <c r="A5860" t="s">
-        <v>18</v>
+      <c r="A5860">
+        <v>15</v>
       </c>
       <c r="B5860" s="2">
         <v>44558</v>
@@ -83571,8 +83574,8 @@
       </c>
     </row>
     <row r="5861" spans="1:4">
-      <c r="A5861" t="s">
-        <v>19</v>
+      <c r="A5861">
+        <v>16</v>
       </c>
       <c r="B5861" s="2">
         <v>44558</v>
@@ -83585,8 +83588,8 @@
       </c>
     </row>
     <row r="5862" spans="1:4">
-      <c r="A5862" t="s">
-        <v>4</v>
+      <c r="A5862">
+        <v>1</v>
       </c>
       <c r="B5862" s="2">
         <v>44559</v>
@@ -83599,8 +83602,8 @@
       </c>
     </row>
     <row r="5863" spans="1:4">
-      <c r="A5863" t="s">
-        <v>5</v>
+      <c r="A5863">
+        <v>2</v>
       </c>
       <c r="B5863" s="2">
         <v>44559</v>
@@ -83613,8 +83616,8 @@
       </c>
     </row>
     <row r="5864" spans="1:4">
-      <c r="A5864" t="s">
-        <v>6</v>
+      <c r="A5864">
+        <v>3</v>
       </c>
       <c r="B5864" s="2">
         <v>44559</v>
@@ -83627,8 +83630,8 @@
       </c>
     </row>
     <row r="5865" spans="1:4">
-      <c r="A5865" t="s">
-        <v>7</v>
+      <c r="A5865">
+        <v>4</v>
       </c>
       <c r="B5865" s="2">
         <v>44559</v>
@@ -83641,8 +83644,8 @@
       </c>
     </row>
     <row r="5866" spans="1:4">
-      <c r="A5866" t="s">
-        <v>8</v>
+      <c r="A5866">
+        <v>5</v>
       </c>
       <c r="B5866" s="2">
         <v>44559</v>
@@ -83655,8 +83658,8 @@
       </c>
     </row>
     <row r="5867" spans="1:4">
-      <c r="A5867" t="s">
-        <v>9</v>
+      <c r="A5867">
+        <v>6</v>
       </c>
       <c r="B5867" s="2">
         <v>44559</v>
@@ -83669,8 +83672,8 @@
       </c>
     </row>
     <row r="5868" spans="1:4">
-      <c r="A5868" t="s">
-        <v>10</v>
+      <c r="A5868">
+        <v>7</v>
       </c>
       <c r="B5868" s="2">
         <v>44559</v>
@@ -83683,8 +83686,8 @@
       </c>
     </row>
     <row r="5869" spans="1:4">
-      <c r="A5869" t="s">
-        <v>11</v>
+      <c r="A5869">
+        <v>8</v>
       </c>
       <c r="B5869" s="2">
         <v>44559</v>
@@ -83697,8 +83700,8 @@
       </c>
     </row>
     <row r="5870" spans="1:4">
-      <c r="A5870" t="s">
-        <v>12</v>
+      <c r="A5870">
+        <v>9</v>
       </c>
       <c r="B5870" s="2">
         <v>44559</v>
@@ -83711,8 +83714,8 @@
       </c>
     </row>
     <row r="5871" spans="1:4">
-      <c r="A5871" t="s">
-        <v>13</v>
+      <c r="A5871">
+        <v>10</v>
       </c>
       <c r="B5871" s="2">
         <v>44559</v>
@@ -83725,8 +83728,8 @@
       </c>
     </row>
     <row r="5872" spans="1:4">
-      <c r="A5872" t="s">
-        <v>14</v>
+      <c r="A5872">
+        <v>11</v>
       </c>
       <c r="B5872" s="2">
         <v>44559</v>
@@ -83739,8 +83742,8 @@
       </c>
     </row>
     <row r="5873" spans="1:4">
-      <c r="A5873" t="s">
-        <v>15</v>
+      <c r="A5873">
+        <v>12</v>
       </c>
       <c r="B5873" s="2">
         <v>44559</v>
@@ -83753,8 +83756,8 @@
       </c>
     </row>
     <row r="5874" spans="1:4">
-      <c r="A5874" t="s">
-        <v>16</v>
+      <c r="A5874">
+        <v>13</v>
       </c>
       <c r="B5874" s="2">
         <v>44559</v>
@@ -83767,8 +83770,8 @@
       </c>
     </row>
     <row r="5875" spans="1:4">
-      <c r="A5875" t="s">
-        <v>17</v>
+      <c r="A5875">
+        <v>14</v>
       </c>
       <c r="B5875" s="2">
         <v>44559</v>
@@ -83781,8 +83784,8 @@
       </c>
     </row>
     <row r="5876" spans="1:4">
-      <c r="A5876" t="s">
-        <v>18</v>
+      <c r="A5876">
+        <v>15</v>
       </c>
       <c r="B5876" s="2">
         <v>44559</v>
@@ -83795,8 +83798,8 @@
       </c>
     </row>
     <row r="5877" spans="1:4">
-      <c r="A5877" t="s">
-        <v>19</v>
+      <c r="A5877">
+        <v>16</v>
       </c>
       <c r="B5877" s="2">
         <v>44559</v>
@@ -83806,6 +83809,454 @@
       </c>
       <c r="D5877">
         <v>0</v>
+      </c>
+    </row>
+    <row r="5878" spans="1:4">
+      <c r="A5878" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5878" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5878" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5878">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5879" spans="1:4">
+      <c r="A5879" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5879" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5879" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5879">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5880" spans="1:4">
+      <c r="A5880" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5880" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5880" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5880">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5881" spans="1:4">
+      <c r="A5881" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5881" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5881" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5881">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5882" spans="1:4">
+      <c r="A5882" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5882" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5882" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5882">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5883" spans="1:4">
+      <c r="A5883" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5883" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5883" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5883">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5884" spans="1:4">
+      <c r="A5884" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5884" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5884" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5884">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5885" spans="1:4">
+      <c r="A5885" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5885" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5885" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5885">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5886" spans="1:4">
+      <c r="A5886" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5886" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5886" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5886">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5887" spans="1:4">
+      <c r="A5887" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5887" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5887" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5887">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5888" spans="1:4">
+      <c r="A5888" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5888" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5888" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5888">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5889" spans="1:4">
+      <c r="A5889" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5889" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5889" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5889">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5890" spans="1:4">
+      <c r="A5890" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5890" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5890" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5890">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5891" spans="1:4">
+      <c r="A5891" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5891" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5891" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5891">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5892" spans="1:4">
+      <c r="A5892" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5892" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5892" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5892">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5893" spans="1:4">
+      <c r="A5893" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5893" s="2">
+        <v>44559</v>
+      </c>
+      <c r="C5893" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5893">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5894" spans="1:4">
+      <c r="A5894" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5894" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5894" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5894">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5895" spans="1:4">
+      <c r="A5895" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5895" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5895" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5895">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5896" spans="1:4">
+      <c r="A5896" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5896" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5896" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5896">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5897" spans="1:4">
+      <c r="A5897" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5897" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5897" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5897">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5898" spans="1:4">
+      <c r="A5898" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5898" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5898" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5898">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5899" spans="1:4">
+      <c r="A5899" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5899" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5899" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5899">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5900" spans="1:4">
+      <c r="A5900" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5900" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5900" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5900">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5901" spans="1:4">
+      <c r="A5901" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5901" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5901" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5901">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5902" spans="1:4">
+      <c r="A5902" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5902" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5902" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5902">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5903" spans="1:4">
+      <c r="A5903" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5903" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5903" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5903">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5904" spans="1:4">
+      <c r="A5904" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5904" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5904" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5904">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5905" spans="1:4">
+      <c r="A5905" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5905" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5905" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5905">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5906" spans="1:4">
+      <c r="A5906" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5906" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5906" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5906">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5907" spans="1:4">
+      <c r="A5907" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5907" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5907" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5907">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5908" spans="1:4">
+      <c r="A5908" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5908" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5908" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5908">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5909" spans="1:4">
+      <c r="A5909" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5909" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5909" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5909">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-02-2022 17-08-14
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11468" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11500" uniqueCount="385">
   <si>
     <t>Región</t>
   </si>
@@ -1167,6 +1167,9 @@
   <si>
     <t>2021-12-30</t>
   </si>
+  <si>
+    <t>2021-12-31</t>
+  </si>
 </sst>
 </file>
 
@@ -1527,7 +1530,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5909"/>
+  <dimension ref="A1:D5941"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -83812,8 +83815,8 @@
       </c>
     </row>
     <row r="5878" spans="1:4">
-      <c r="A5878" t="s">
-        <v>4</v>
+      <c r="A5878">
+        <v>1</v>
       </c>
       <c r="B5878" s="2">
         <v>44559</v>
@@ -83826,8 +83829,8 @@
       </c>
     </row>
     <row r="5879" spans="1:4">
-      <c r="A5879" t="s">
-        <v>5</v>
+      <c r="A5879">
+        <v>2</v>
       </c>
       <c r="B5879" s="2">
         <v>44559</v>
@@ -83840,8 +83843,8 @@
       </c>
     </row>
     <row r="5880" spans="1:4">
-      <c r="A5880" t="s">
-        <v>6</v>
+      <c r="A5880">
+        <v>3</v>
       </c>
       <c r="B5880" s="2">
         <v>44559</v>
@@ -83854,8 +83857,8 @@
       </c>
     </row>
     <row r="5881" spans="1:4">
-      <c r="A5881" t="s">
-        <v>7</v>
+      <c r="A5881">
+        <v>4</v>
       </c>
       <c r="B5881" s="2">
         <v>44559</v>
@@ -83868,8 +83871,8 @@
       </c>
     </row>
     <row r="5882" spans="1:4">
-      <c r="A5882" t="s">
-        <v>8</v>
+      <c r="A5882">
+        <v>5</v>
       </c>
       <c r="B5882" s="2">
         <v>44559</v>
@@ -83882,8 +83885,8 @@
       </c>
     </row>
     <row r="5883" spans="1:4">
-      <c r="A5883" t="s">
-        <v>9</v>
+      <c r="A5883">
+        <v>6</v>
       </c>
       <c r="B5883" s="2">
         <v>44559</v>
@@ -83896,8 +83899,8 @@
       </c>
     </row>
     <row r="5884" spans="1:4">
-      <c r="A5884" t="s">
-        <v>10</v>
+      <c r="A5884">
+        <v>7</v>
       </c>
       <c r="B5884" s="2">
         <v>44559</v>
@@ -83910,8 +83913,8 @@
       </c>
     </row>
     <row r="5885" spans="1:4">
-      <c r="A5885" t="s">
-        <v>11</v>
+      <c r="A5885">
+        <v>8</v>
       </c>
       <c r="B5885" s="2">
         <v>44559</v>
@@ -83924,8 +83927,8 @@
       </c>
     </row>
     <row r="5886" spans="1:4">
-      <c r="A5886" t="s">
-        <v>12</v>
+      <c r="A5886">
+        <v>9</v>
       </c>
       <c r="B5886" s="2">
         <v>44559</v>
@@ -83938,8 +83941,8 @@
       </c>
     </row>
     <row r="5887" spans="1:4">
-      <c r="A5887" t="s">
-        <v>13</v>
+      <c r="A5887">
+        <v>10</v>
       </c>
       <c r="B5887" s="2">
         <v>44559</v>
@@ -83952,8 +83955,8 @@
       </c>
     </row>
     <row r="5888" spans="1:4">
-      <c r="A5888" t="s">
-        <v>14</v>
+      <c r="A5888">
+        <v>11</v>
       </c>
       <c r="B5888" s="2">
         <v>44559</v>
@@ -83966,8 +83969,8 @@
       </c>
     </row>
     <row r="5889" spans="1:4">
-      <c r="A5889" t="s">
-        <v>15</v>
+      <c r="A5889">
+        <v>12</v>
       </c>
       <c r="B5889" s="2">
         <v>44559</v>
@@ -83980,8 +83983,8 @@
       </c>
     </row>
     <row r="5890" spans="1:4">
-      <c r="A5890" t="s">
-        <v>16</v>
+      <c r="A5890">
+        <v>13</v>
       </c>
       <c r="B5890" s="2">
         <v>44559</v>
@@ -83994,8 +83997,8 @@
       </c>
     </row>
     <row r="5891" spans="1:4">
-      <c r="A5891" t="s">
-        <v>17</v>
+      <c r="A5891">
+        <v>14</v>
       </c>
       <c r="B5891" s="2">
         <v>44559</v>
@@ -84008,8 +84011,8 @@
       </c>
     </row>
     <row r="5892" spans="1:4">
-      <c r="A5892" t="s">
-        <v>18</v>
+      <c r="A5892">
+        <v>15</v>
       </c>
       <c r="B5892" s="2">
         <v>44559</v>
@@ -84022,8 +84025,8 @@
       </c>
     </row>
     <row r="5893" spans="1:4">
-      <c r="A5893" t="s">
-        <v>19</v>
+      <c r="A5893">
+        <v>16</v>
       </c>
       <c r="B5893" s="2">
         <v>44559</v>
@@ -84036,8 +84039,8 @@
       </c>
     </row>
     <row r="5894" spans="1:4">
-      <c r="A5894" t="s">
-        <v>4</v>
+      <c r="A5894">
+        <v>1</v>
       </c>
       <c r="B5894" s="2">
         <v>44560</v>
@@ -84050,8 +84053,8 @@
       </c>
     </row>
     <row r="5895" spans="1:4">
-      <c r="A5895" t="s">
-        <v>5</v>
+      <c r="A5895">
+        <v>2</v>
       </c>
       <c r="B5895" s="2">
         <v>44560</v>
@@ -84064,8 +84067,8 @@
       </c>
     </row>
     <row r="5896" spans="1:4">
-      <c r="A5896" t="s">
-        <v>6</v>
+      <c r="A5896">
+        <v>3</v>
       </c>
       <c r="B5896" s="2">
         <v>44560</v>
@@ -84078,8 +84081,8 @@
       </c>
     </row>
     <row r="5897" spans="1:4">
-      <c r="A5897" t="s">
-        <v>7</v>
+      <c r="A5897">
+        <v>4</v>
       </c>
       <c r="B5897" s="2">
         <v>44560</v>
@@ -84092,8 +84095,8 @@
       </c>
     </row>
     <row r="5898" spans="1:4">
-      <c r="A5898" t="s">
-        <v>8</v>
+      <c r="A5898">
+        <v>5</v>
       </c>
       <c r="B5898" s="2">
         <v>44560</v>
@@ -84106,8 +84109,8 @@
       </c>
     </row>
     <row r="5899" spans="1:4">
-      <c r="A5899" t="s">
-        <v>9</v>
+      <c r="A5899">
+        <v>6</v>
       </c>
       <c r="B5899" s="2">
         <v>44560</v>
@@ -84120,8 +84123,8 @@
       </c>
     </row>
     <row r="5900" spans="1:4">
-      <c r="A5900" t="s">
-        <v>10</v>
+      <c r="A5900">
+        <v>7</v>
       </c>
       <c r="B5900" s="2">
         <v>44560</v>
@@ -84134,8 +84137,8 @@
       </c>
     </row>
     <row r="5901" spans="1:4">
-      <c r="A5901" t="s">
-        <v>11</v>
+      <c r="A5901">
+        <v>8</v>
       </c>
       <c r="B5901" s="2">
         <v>44560</v>
@@ -84148,8 +84151,8 @@
       </c>
     </row>
     <row r="5902" spans="1:4">
-      <c r="A5902" t="s">
-        <v>12</v>
+      <c r="A5902">
+        <v>9</v>
       </c>
       <c r="B5902" s="2">
         <v>44560</v>
@@ -84162,8 +84165,8 @@
       </c>
     </row>
     <row r="5903" spans="1:4">
-      <c r="A5903" t="s">
-        <v>13</v>
+      <c r="A5903">
+        <v>10</v>
       </c>
       <c r="B5903" s="2">
         <v>44560</v>
@@ -84176,8 +84179,8 @@
       </c>
     </row>
     <row r="5904" spans="1:4">
-      <c r="A5904" t="s">
-        <v>14</v>
+      <c r="A5904">
+        <v>11</v>
       </c>
       <c r="B5904" s="2">
         <v>44560</v>
@@ -84190,8 +84193,8 @@
       </c>
     </row>
     <row r="5905" spans="1:4">
-      <c r="A5905" t="s">
-        <v>15</v>
+      <c r="A5905">
+        <v>12</v>
       </c>
       <c r="B5905" s="2">
         <v>44560</v>
@@ -84204,8 +84207,8 @@
       </c>
     </row>
     <row r="5906" spans="1:4">
-      <c r="A5906" t="s">
-        <v>16</v>
+      <c r="A5906">
+        <v>13</v>
       </c>
       <c r="B5906" s="2">
         <v>44560</v>
@@ -84218,8 +84221,8 @@
       </c>
     </row>
     <row r="5907" spans="1:4">
-      <c r="A5907" t="s">
-        <v>17</v>
+      <c r="A5907">
+        <v>14</v>
       </c>
       <c r="B5907" s="2">
         <v>44560</v>
@@ -84232,8 +84235,8 @@
       </c>
     </row>
     <row r="5908" spans="1:4">
-      <c r="A5908" t="s">
-        <v>18</v>
+      <c r="A5908">
+        <v>15</v>
       </c>
       <c r="B5908" s="2">
         <v>44560</v>
@@ -84246,8 +84249,8 @@
       </c>
     </row>
     <row r="5909" spans="1:4">
-      <c r="A5909" t="s">
-        <v>19</v>
+      <c r="A5909">
+        <v>16</v>
       </c>
       <c r="B5909" s="2">
         <v>44560</v>
@@ -84256,6 +84259,454 @@
         <v>383</v>
       </c>
       <c r="D5909">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5910" spans="1:4">
+      <c r="A5910" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5910" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5910" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5910">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5911" spans="1:4">
+      <c r="A5911" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5911" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5911" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5911">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5912" spans="1:4">
+      <c r="A5912" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5912" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5912" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5912">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5913" spans="1:4">
+      <c r="A5913" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5913" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5913" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5913">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5914" spans="1:4">
+      <c r="A5914" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5914" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5914" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5914">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5915" spans="1:4">
+      <c r="A5915" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5915" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5915" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5915">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5916" spans="1:4">
+      <c r="A5916" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5916" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5916" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5916">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5917" spans="1:4">
+      <c r="A5917" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5917" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5917" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5917">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5918" spans="1:4">
+      <c r="A5918" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5918" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5918" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5918">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5919" spans="1:4">
+      <c r="A5919" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5919" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5919" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5919">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5920" spans="1:4">
+      <c r="A5920" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5920" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5920" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5920">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5921" spans="1:4">
+      <c r="A5921" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5921" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5921" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5921">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5922" spans="1:4">
+      <c r="A5922" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5922" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5922" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5922">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5923" spans="1:4">
+      <c r="A5923" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5923" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5923" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5923">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5924" spans="1:4">
+      <c r="A5924" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5924" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5924" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5924">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5925" spans="1:4">
+      <c r="A5925" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5925" s="2">
+        <v>44560</v>
+      </c>
+      <c r="C5925" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5925">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5926" spans="1:4">
+      <c r="A5926" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5926" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5926" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5926">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5927" spans="1:4">
+      <c r="A5927" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5927" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5927" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5927">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5928" spans="1:4">
+      <c r="A5928" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5928" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5928" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5928">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5929" spans="1:4">
+      <c r="A5929" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5929" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5929" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5929">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5930" spans="1:4">
+      <c r="A5930" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5930" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5930" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5930">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5931" spans="1:4">
+      <c r="A5931" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5931" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5931" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5931">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5932" spans="1:4">
+      <c r="A5932" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5932" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5932" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5932">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5933" spans="1:4">
+      <c r="A5933" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5933" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5933" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5933">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5934" spans="1:4">
+      <c r="A5934" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5934" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5934" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5934">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5935" spans="1:4">
+      <c r="A5935" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5935" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5935" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5935">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5936" spans="1:4">
+      <c r="A5936" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5936" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5936" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5936">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5937" spans="1:4">
+      <c r="A5937" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5937" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5937" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5937">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5938" spans="1:4">
+      <c r="A5938" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5938" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5938" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5938">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5939" spans="1:4">
+      <c r="A5939" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5939" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5939" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5939">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5940" spans="1:4">
+      <c r="A5940" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5940" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5940" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5940">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5941" spans="1:4">
+      <c r="A5941" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5941" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5941" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5941">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-03-2022 17-40-42
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11500" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11532" uniqueCount="386">
   <si>
     <t>Región</t>
   </si>
@@ -1170,6 +1170,9 @@
   <si>
     <t>2021-12-31</t>
   </si>
+  <si>
+    <t>2022-01-01</t>
+  </si>
 </sst>
 </file>
 
@@ -1530,7 +1533,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5941"/>
+  <dimension ref="A1:D5973"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -84263,8 +84266,8 @@
       </c>
     </row>
     <row r="5910" spans="1:4">
-      <c r="A5910" t="s">
-        <v>4</v>
+      <c r="A5910">
+        <v>1</v>
       </c>
       <c r="B5910" s="2">
         <v>44560</v>
@@ -84277,8 +84280,8 @@
       </c>
     </row>
     <row r="5911" spans="1:4">
-      <c r="A5911" t="s">
-        <v>5</v>
+      <c r="A5911">
+        <v>2</v>
       </c>
       <c r="B5911" s="2">
         <v>44560</v>
@@ -84291,8 +84294,8 @@
       </c>
     </row>
     <row r="5912" spans="1:4">
-      <c r="A5912" t="s">
-        <v>6</v>
+      <c r="A5912">
+        <v>3</v>
       </c>
       <c r="B5912" s="2">
         <v>44560</v>
@@ -84305,8 +84308,8 @@
       </c>
     </row>
     <row r="5913" spans="1:4">
-      <c r="A5913" t="s">
-        <v>7</v>
+      <c r="A5913">
+        <v>4</v>
       </c>
       <c r="B5913" s="2">
         <v>44560</v>
@@ -84319,8 +84322,8 @@
       </c>
     </row>
     <row r="5914" spans="1:4">
-      <c r="A5914" t="s">
-        <v>8</v>
+      <c r="A5914">
+        <v>5</v>
       </c>
       <c r="B5914" s="2">
         <v>44560</v>
@@ -84333,8 +84336,8 @@
       </c>
     </row>
     <row r="5915" spans="1:4">
-      <c r="A5915" t="s">
-        <v>9</v>
+      <c r="A5915">
+        <v>6</v>
       </c>
       <c r="B5915" s="2">
         <v>44560</v>
@@ -84347,8 +84350,8 @@
       </c>
     </row>
     <row r="5916" spans="1:4">
-      <c r="A5916" t="s">
-        <v>10</v>
+      <c r="A5916">
+        <v>7</v>
       </c>
       <c r="B5916" s="2">
         <v>44560</v>
@@ -84361,8 +84364,8 @@
       </c>
     </row>
     <row r="5917" spans="1:4">
-      <c r="A5917" t="s">
-        <v>11</v>
+      <c r="A5917">
+        <v>8</v>
       </c>
       <c r="B5917" s="2">
         <v>44560</v>
@@ -84375,8 +84378,8 @@
       </c>
     </row>
     <row r="5918" spans="1:4">
-      <c r="A5918" t="s">
-        <v>12</v>
+      <c r="A5918">
+        <v>9</v>
       </c>
       <c r="B5918" s="2">
         <v>44560</v>
@@ -84389,8 +84392,8 @@
       </c>
     </row>
     <row r="5919" spans="1:4">
-      <c r="A5919" t="s">
-        <v>13</v>
+      <c r="A5919">
+        <v>10</v>
       </c>
       <c r="B5919" s="2">
         <v>44560</v>
@@ -84403,8 +84406,8 @@
       </c>
     </row>
     <row r="5920" spans="1:4">
-      <c r="A5920" t="s">
-        <v>14</v>
+      <c r="A5920">
+        <v>11</v>
       </c>
       <c r="B5920" s="2">
         <v>44560</v>
@@ -84417,8 +84420,8 @@
       </c>
     </row>
     <row r="5921" spans="1:4">
-      <c r="A5921" t="s">
-        <v>15</v>
+      <c r="A5921">
+        <v>12</v>
       </c>
       <c r="B5921" s="2">
         <v>44560</v>
@@ -84431,8 +84434,8 @@
       </c>
     </row>
     <row r="5922" spans="1:4">
-      <c r="A5922" t="s">
-        <v>16</v>
+      <c r="A5922">
+        <v>13</v>
       </c>
       <c r="B5922" s="2">
         <v>44560</v>
@@ -84445,8 +84448,8 @@
       </c>
     </row>
     <row r="5923" spans="1:4">
-      <c r="A5923" t="s">
-        <v>17</v>
+      <c r="A5923">
+        <v>14</v>
       </c>
       <c r="B5923" s="2">
         <v>44560</v>
@@ -84459,8 +84462,8 @@
       </c>
     </row>
     <row r="5924" spans="1:4">
-      <c r="A5924" t="s">
-        <v>18</v>
+      <c r="A5924">
+        <v>15</v>
       </c>
       <c r="B5924" s="2">
         <v>44560</v>
@@ -84473,8 +84476,8 @@
       </c>
     </row>
     <row r="5925" spans="1:4">
-      <c r="A5925" t="s">
-        <v>19</v>
+      <c r="A5925">
+        <v>16</v>
       </c>
       <c r="B5925" s="2">
         <v>44560</v>
@@ -84487,8 +84490,8 @@
       </c>
     </row>
     <row r="5926" spans="1:4">
-      <c r="A5926" t="s">
-        <v>4</v>
+      <c r="A5926">
+        <v>1</v>
       </c>
       <c r="B5926" s="2">
         <v>44561</v>
@@ -84501,8 +84504,8 @@
       </c>
     </row>
     <row r="5927" spans="1:4">
-      <c r="A5927" t="s">
-        <v>5</v>
+      <c r="A5927">
+        <v>2</v>
       </c>
       <c r="B5927" s="2">
         <v>44561</v>
@@ -84515,8 +84518,8 @@
       </c>
     </row>
     <row r="5928" spans="1:4">
-      <c r="A5928" t="s">
-        <v>6</v>
+      <c r="A5928">
+        <v>3</v>
       </c>
       <c r="B5928" s="2">
         <v>44561</v>
@@ -84529,8 +84532,8 @@
       </c>
     </row>
     <row r="5929" spans="1:4">
-      <c r="A5929" t="s">
-        <v>7</v>
+      <c r="A5929">
+        <v>4</v>
       </c>
       <c r="B5929" s="2">
         <v>44561</v>
@@ -84543,8 +84546,8 @@
       </c>
     </row>
     <row r="5930" spans="1:4">
-      <c r="A5930" t="s">
-        <v>8</v>
+      <c r="A5930">
+        <v>5</v>
       </c>
       <c r="B5930" s="2">
         <v>44561</v>
@@ -84557,8 +84560,8 @@
       </c>
     </row>
     <row r="5931" spans="1:4">
-      <c r="A5931" t="s">
-        <v>9</v>
+      <c r="A5931">
+        <v>6</v>
       </c>
       <c r="B5931" s="2">
         <v>44561</v>
@@ -84571,8 +84574,8 @@
       </c>
     </row>
     <row r="5932" spans="1:4">
-      <c r="A5932" t="s">
-        <v>10</v>
+      <c r="A5932">
+        <v>7</v>
       </c>
       <c r="B5932" s="2">
         <v>44561</v>
@@ -84585,8 +84588,8 @@
       </c>
     </row>
     <row r="5933" spans="1:4">
-      <c r="A5933" t="s">
-        <v>11</v>
+      <c r="A5933">
+        <v>8</v>
       </c>
       <c r="B5933" s="2">
         <v>44561</v>
@@ -84599,8 +84602,8 @@
       </c>
     </row>
     <row r="5934" spans="1:4">
-      <c r="A5934" t="s">
-        <v>12</v>
+      <c r="A5934">
+        <v>9</v>
       </c>
       <c r="B5934" s="2">
         <v>44561</v>
@@ -84613,8 +84616,8 @@
       </c>
     </row>
     <row r="5935" spans="1:4">
-      <c r="A5935" t="s">
-        <v>13</v>
+      <c r="A5935">
+        <v>10</v>
       </c>
       <c r="B5935" s="2">
         <v>44561</v>
@@ -84627,8 +84630,8 @@
       </c>
     </row>
     <row r="5936" spans="1:4">
-      <c r="A5936" t="s">
-        <v>14</v>
+      <c r="A5936">
+        <v>11</v>
       </c>
       <c r="B5936" s="2">
         <v>44561</v>
@@ -84641,8 +84644,8 @@
       </c>
     </row>
     <row r="5937" spans="1:4">
-      <c r="A5937" t="s">
-        <v>15</v>
+      <c r="A5937">
+        <v>12</v>
       </c>
       <c r="B5937" s="2">
         <v>44561</v>
@@ -84655,8 +84658,8 @@
       </c>
     </row>
     <row r="5938" spans="1:4">
-      <c r="A5938" t="s">
-        <v>16</v>
+      <c r="A5938">
+        <v>13</v>
       </c>
       <c r="B5938" s="2">
         <v>44561</v>
@@ -84669,8 +84672,8 @@
       </c>
     </row>
     <row r="5939" spans="1:4">
-      <c r="A5939" t="s">
-        <v>17</v>
+      <c r="A5939">
+        <v>14</v>
       </c>
       <c r="B5939" s="2">
         <v>44561</v>
@@ -84683,8 +84686,8 @@
       </c>
     </row>
     <row r="5940" spans="1:4">
-      <c r="A5940" t="s">
-        <v>18</v>
+      <c r="A5940">
+        <v>15</v>
       </c>
       <c r="B5940" s="2">
         <v>44561</v>
@@ -84697,8 +84700,8 @@
       </c>
     </row>
     <row r="5941" spans="1:4">
-      <c r="A5941" t="s">
-        <v>19</v>
+      <c r="A5941">
+        <v>16</v>
       </c>
       <c r="B5941" s="2">
         <v>44561</v>
@@ -84708,6 +84711,454 @@
       </c>
       <c r="D5941">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5942" spans="1:4">
+      <c r="A5942" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5942" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5942" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5942">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5943" spans="1:4">
+      <c r="A5943" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5943" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5943" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5943">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5944" spans="1:4">
+      <c r="A5944" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5944" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5944" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5944">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5945" spans="1:4">
+      <c r="A5945" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5945" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5945" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5945">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5946" spans="1:4">
+      <c r="A5946" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5946" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5946" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5946">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5947" spans="1:4">
+      <c r="A5947" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5947" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5947" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5947">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5948" spans="1:4">
+      <c r="A5948" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5948" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5948" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5948">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5949" spans="1:4">
+      <c r="A5949" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5949" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5949" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5949">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5950" spans="1:4">
+      <c r="A5950" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5950" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5950" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5950">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5951" spans="1:4">
+      <c r="A5951" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5951" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5951" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5951">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5952" spans="1:4">
+      <c r="A5952" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5952" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5952" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5952">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5953" spans="1:4">
+      <c r="A5953" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5953" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5953" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5953">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5954" spans="1:4">
+      <c r="A5954" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5954" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5954" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5954">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5955" spans="1:4">
+      <c r="A5955" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5955" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5955" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5955">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5956" spans="1:4">
+      <c r="A5956" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5956" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5956" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5956">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5957" spans="1:4">
+      <c r="A5957" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5957" s="2">
+        <v>44561</v>
+      </c>
+      <c r="C5957" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5957">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5958" spans="1:4">
+      <c r="A5958" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5958" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5958" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5958">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5959" spans="1:4">
+      <c r="A5959" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5959" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5959" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5959">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5960" spans="1:4">
+      <c r="A5960" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5960" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5960" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5960">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5961" spans="1:4">
+      <c r="A5961" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5961" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5961" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5961">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5962" spans="1:4">
+      <c r="A5962" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5962" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5962" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5962">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5963" spans="1:4">
+      <c r="A5963" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5963" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5963" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5963">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5964" spans="1:4">
+      <c r="A5964" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5964" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5964" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5964">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5965" spans="1:4">
+      <c r="A5965" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5965" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5965" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5965">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5966" spans="1:4">
+      <c r="A5966" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5966" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5966" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5966">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5967" spans="1:4">
+      <c r="A5967" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5967" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5967" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5967">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5968" spans="1:4">
+      <c r="A5968" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5968" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5968" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5968">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5969" spans="1:4">
+      <c r="A5969" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5969" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5969" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5969">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5970" spans="1:4">
+      <c r="A5970" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5970" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5970" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5970">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5971" spans="1:4">
+      <c r="A5971" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5971" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5971" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5971">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5972" spans="1:4">
+      <c r="A5972" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5972" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5972" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5972">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5973" spans="1:4">
+      <c r="A5973" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5973" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5973" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5973">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-04-2022 18-13-39
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11532" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11564" uniqueCount="387">
   <si>
     <t>Región</t>
   </si>
@@ -1173,6 +1173,9 @@
   <si>
     <t>2022-01-01</t>
   </si>
+  <si>
+    <t>2022-01-02</t>
+  </si>
 </sst>
 </file>
 
@@ -1533,7 +1536,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5973"/>
+  <dimension ref="A1:D6005"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -84714,8 +84717,8 @@
       </c>
     </row>
     <row r="5942" spans="1:4">
-      <c r="A5942" t="s">
-        <v>4</v>
+      <c r="A5942">
+        <v>1</v>
       </c>
       <c r="B5942" s="2">
         <v>44561</v>
@@ -84728,8 +84731,8 @@
       </c>
     </row>
     <row r="5943" spans="1:4">
-      <c r="A5943" t="s">
-        <v>5</v>
+      <c r="A5943">
+        <v>2</v>
       </c>
       <c r="B5943" s="2">
         <v>44561</v>
@@ -84742,8 +84745,8 @@
       </c>
     </row>
     <row r="5944" spans="1:4">
-      <c r="A5944" t="s">
-        <v>6</v>
+      <c r="A5944">
+        <v>3</v>
       </c>
       <c r="B5944" s="2">
         <v>44561</v>
@@ -84756,8 +84759,8 @@
       </c>
     </row>
     <row r="5945" spans="1:4">
-      <c r="A5945" t="s">
-        <v>7</v>
+      <c r="A5945">
+        <v>4</v>
       </c>
       <c r="B5945" s="2">
         <v>44561</v>
@@ -84770,8 +84773,8 @@
       </c>
     </row>
     <row r="5946" spans="1:4">
-      <c r="A5946" t="s">
-        <v>8</v>
+      <c r="A5946">
+        <v>5</v>
       </c>
       <c r="B5946" s="2">
         <v>44561</v>
@@ -84784,8 +84787,8 @@
       </c>
     </row>
     <row r="5947" spans="1:4">
-      <c r="A5947" t="s">
-        <v>9</v>
+      <c r="A5947">
+        <v>6</v>
       </c>
       <c r="B5947" s="2">
         <v>44561</v>
@@ -84798,8 +84801,8 @@
       </c>
     </row>
     <row r="5948" spans="1:4">
-      <c r="A5948" t="s">
-        <v>10</v>
+      <c r="A5948">
+        <v>7</v>
       </c>
       <c r="B5948" s="2">
         <v>44561</v>
@@ -84812,8 +84815,8 @@
       </c>
     </row>
     <row r="5949" spans="1:4">
-      <c r="A5949" t="s">
-        <v>11</v>
+      <c r="A5949">
+        <v>8</v>
       </c>
       <c r="B5949" s="2">
         <v>44561</v>
@@ -84826,8 +84829,8 @@
       </c>
     </row>
     <row r="5950" spans="1:4">
-      <c r="A5950" t="s">
-        <v>12</v>
+      <c r="A5950">
+        <v>9</v>
       </c>
       <c r="B5950" s="2">
         <v>44561</v>
@@ -84840,8 +84843,8 @@
       </c>
     </row>
     <row r="5951" spans="1:4">
-      <c r="A5951" t="s">
-        <v>13</v>
+      <c r="A5951">
+        <v>10</v>
       </c>
       <c r="B5951" s="2">
         <v>44561</v>
@@ -84854,8 +84857,8 @@
       </c>
     </row>
     <row r="5952" spans="1:4">
-      <c r="A5952" t="s">
-        <v>14</v>
+      <c r="A5952">
+        <v>11</v>
       </c>
       <c r="B5952" s="2">
         <v>44561</v>
@@ -84868,8 +84871,8 @@
       </c>
     </row>
     <row r="5953" spans="1:4">
-      <c r="A5953" t="s">
-        <v>15</v>
+      <c r="A5953">
+        <v>12</v>
       </c>
       <c r="B5953" s="2">
         <v>44561</v>
@@ -84882,8 +84885,8 @@
       </c>
     </row>
     <row r="5954" spans="1:4">
-      <c r="A5954" t="s">
-        <v>16</v>
+      <c r="A5954">
+        <v>13</v>
       </c>
       <c r="B5954" s="2">
         <v>44561</v>
@@ -84896,8 +84899,8 @@
       </c>
     </row>
     <row r="5955" spans="1:4">
-      <c r="A5955" t="s">
-        <v>17</v>
+      <c r="A5955">
+        <v>14</v>
       </c>
       <c r="B5955" s="2">
         <v>44561</v>
@@ -84910,8 +84913,8 @@
       </c>
     </row>
     <row r="5956" spans="1:4">
-      <c r="A5956" t="s">
-        <v>18</v>
+      <c r="A5956">
+        <v>15</v>
       </c>
       <c r="B5956" s="2">
         <v>44561</v>
@@ -84924,8 +84927,8 @@
       </c>
     </row>
     <row r="5957" spans="1:4">
-      <c r="A5957" t="s">
-        <v>19</v>
+      <c r="A5957">
+        <v>16</v>
       </c>
       <c r="B5957" s="2">
         <v>44561</v>
@@ -84938,8 +84941,8 @@
       </c>
     </row>
     <row r="5958" spans="1:4">
-      <c r="A5958" t="s">
-        <v>4</v>
+      <c r="A5958">
+        <v>1</v>
       </c>
       <c r="B5958" s="2">
         <v>44562</v>
@@ -84952,8 +84955,8 @@
       </c>
     </row>
     <row r="5959" spans="1:4">
-      <c r="A5959" t="s">
-        <v>5</v>
+      <c r="A5959">
+        <v>2</v>
       </c>
       <c r="B5959" s="2">
         <v>44562</v>
@@ -84966,8 +84969,8 @@
       </c>
     </row>
     <row r="5960" spans="1:4">
-      <c r="A5960" t="s">
-        <v>6</v>
+      <c r="A5960">
+        <v>3</v>
       </c>
       <c r="B5960" s="2">
         <v>44562</v>
@@ -84980,8 +84983,8 @@
       </c>
     </row>
     <row r="5961" spans="1:4">
-      <c r="A5961" t="s">
-        <v>7</v>
+      <c r="A5961">
+        <v>4</v>
       </c>
       <c r="B5961" s="2">
         <v>44562</v>
@@ -84994,8 +84997,8 @@
       </c>
     </row>
     <row r="5962" spans="1:4">
-      <c r="A5962" t="s">
-        <v>8</v>
+      <c r="A5962">
+        <v>5</v>
       </c>
       <c r="B5962" s="2">
         <v>44562</v>
@@ -85008,8 +85011,8 @@
       </c>
     </row>
     <row r="5963" spans="1:4">
-      <c r="A5963" t="s">
-        <v>9</v>
+      <c r="A5963">
+        <v>6</v>
       </c>
       <c r="B5963" s="2">
         <v>44562</v>
@@ -85022,8 +85025,8 @@
       </c>
     </row>
     <row r="5964" spans="1:4">
-      <c r="A5964" t="s">
-        <v>10</v>
+      <c r="A5964">
+        <v>7</v>
       </c>
       <c r="B5964" s="2">
         <v>44562</v>
@@ -85036,8 +85039,8 @@
       </c>
     </row>
     <row r="5965" spans="1:4">
-      <c r="A5965" t="s">
-        <v>11</v>
+      <c r="A5965">
+        <v>8</v>
       </c>
       <c r="B5965" s="2">
         <v>44562</v>
@@ -85050,8 +85053,8 @@
       </c>
     </row>
     <row r="5966" spans="1:4">
-      <c r="A5966" t="s">
-        <v>12</v>
+      <c r="A5966">
+        <v>9</v>
       </c>
       <c r="B5966" s="2">
         <v>44562</v>
@@ -85064,8 +85067,8 @@
       </c>
     </row>
     <row r="5967" spans="1:4">
-      <c r="A5967" t="s">
-        <v>13</v>
+      <c r="A5967">
+        <v>10</v>
       </c>
       <c r="B5967" s="2">
         <v>44562</v>
@@ -85078,8 +85081,8 @@
       </c>
     </row>
     <row r="5968" spans="1:4">
-      <c r="A5968" t="s">
-        <v>14</v>
+      <c r="A5968">
+        <v>11</v>
       </c>
       <c r="B5968" s="2">
         <v>44562</v>
@@ -85092,8 +85095,8 @@
       </c>
     </row>
     <row r="5969" spans="1:4">
-      <c r="A5969" t="s">
-        <v>15</v>
+      <c r="A5969">
+        <v>12</v>
       </c>
       <c r="B5969" s="2">
         <v>44562</v>
@@ -85106,8 +85109,8 @@
       </c>
     </row>
     <row r="5970" spans="1:4">
-      <c r="A5970" t="s">
-        <v>16</v>
+      <c r="A5970">
+        <v>13</v>
       </c>
       <c r="B5970" s="2">
         <v>44562</v>
@@ -85120,8 +85123,8 @@
       </c>
     </row>
     <row r="5971" spans="1:4">
-      <c r="A5971" t="s">
-        <v>17</v>
+      <c r="A5971">
+        <v>14</v>
       </c>
       <c r="B5971" s="2">
         <v>44562</v>
@@ -85134,8 +85137,8 @@
       </c>
     </row>
     <row r="5972" spans="1:4">
-      <c r="A5972" t="s">
-        <v>18</v>
+      <c r="A5972">
+        <v>15</v>
       </c>
       <c r="B5972" s="2">
         <v>44562</v>
@@ -85148,8 +85151,8 @@
       </c>
     </row>
     <row r="5973" spans="1:4">
-      <c r="A5973" t="s">
-        <v>19</v>
+      <c r="A5973">
+        <v>16</v>
       </c>
       <c r="B5973" s="2">
         <v>44562</v>
@@ -85158,6 +85161,454 @@
         <v>385</v>
       </c>
       <c r="D5973">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5974" spans="1:4">
+      <c r="A5974" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5974" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5974" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5974">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5975" spans="1:4">
+      <c r="A5975" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5975" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5975" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5975">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5976" spans="1:4">
+      <c r="A5976" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5976" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5976" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5976">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5977" spans="1:4">
+      <c r="A5977" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5977" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5977" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5977">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5978" spans="1:4">
+      <c r="A5978" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5978" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5978" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5978">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5979" spans="1:4">
+      <c r="A5979" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5979" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5979" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5979">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5980" spans="1:4">
+      <c r="A5980" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5980" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5980" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5980">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5981" spans="1:4">
+      <c r="A5981" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5981" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5981" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5981">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5982" spans="1:4">
+      <c r="A5982" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5982" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5982" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5982">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5983" spans="1:4">
+      <c r="A5983" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5983" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5983" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5983">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5984" spans="1:4">
+      <c r="A5984" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5984" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5984" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5984">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5985" spans="1:4">
+      <c r="A5985" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5985" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5985" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5985">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5986" spans="1:4">
+      <c r="A5986" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5986" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5986" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5986">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5987" spans="1:4">
+      <c r="A5987" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5987" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5987" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5987">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5988" spans="1:4">
+      <c r="A5988" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5988" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5988" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5988">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5989" spans="1:4">
+      <c r="A5989" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5989" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C5989" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5989">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5990" spans="1:4">
+      <c r="A5990" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5990" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C5990" t="s">
+        <v>386</v>
+      </c>
+      <c r="D5990">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5991" spans="1:4">
+      <c r="A5991" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5991" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C5991" t="s">
+        <v>386</v>
+      </c>
+      <c r="D5991">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5992" spans="1:4">
+      <c r="A5992" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5992" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C5992" t="s">
+        <v>386</v>
+      </c>
+      <c r="D5992">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5993" spans="1:4">
+      <c r="A5993" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5993" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C5993" t="s">
+        <v>386</v>
+      </c>
+      <c r="D5993">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5994" spans="1:4">
+      <c r="A5994" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5994" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C5994" t="s">
+        <v>386</v>
+      </c>
+      <c r="D5994">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5995" spans="1:4">
+      <c r="A5995" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5995" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C5995" t="s">
+        <v>386</v>
+      </c>
+      <c r="D5995">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5996" spans="1:4">
+      <c r="A5996" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5996" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C5996" t="s">
+        <v>386</v>
+      </c>
+      <c r="D5996">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5997" spans="1:4">
+      <c r="A5997" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5997" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C5997" t="s">
+        <v>386</v>
+      </c>
+      <c r="D5997">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5998" spans="1:4">
+      <c r="A5998" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5998" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C5998" t="s">
+        <v>386</v>
+      </c>
+      <c r="D5998">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5999" spans="1:4">
+      <c r="A5999" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5999" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C5999" t="s">
+        <v>386</v>
+      </c>
+      <c r="D5999">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6000" spans="1:4">
+      <c r="A6000" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6000" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6000" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6000">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6001" spans="1:4">
+      <c r="A6001" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6001" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6001" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6001">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6002" spans="1:4">
+      <c r="A6002" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6002" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6002" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6002">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6003" spans="1:4">
+      <c r="A6003" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6003" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6003" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6003">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6004" spans="1:4">
+      <c r="A6004" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6004" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6004" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6005" spans="1:4">
+      <c r="A6005" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6005" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6005" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6005">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-05-2022 18-45-08
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11564" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11596" uniqueCount="388">
   <si>
     <t>Región</t>
   </si>
@@ -1176,6 +1176,9 @@
   <si>
     <t>2022-01-02</t>
   </si>
+  <si>
+    <t>2022-01-03</t>
+  </si>
 </sst>
 </file>
 
@@ -1536,7 +1539,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6005"/>
+  <dimension ref="A1:D6037"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -85165,8 +85168,8 @@
       </c>
     </row>
     <row r="5974" spans="1:4">
-      <c r="A5974" t="s">
-        <v>4</v>
+      <c r="A5974">
+        <v>1</v>
       </c>
       <c r="B5974" s="2">
         <v>44562</v>
@@ -85179,8 +85182,8 @@
       </c>
     </row>
     <row r="5975" spans="1:4">
-      <c r="A5975" t="s">
-        <v>5</v>
+      <c r="A5975">
+        <v>2</v>
       </c>
       <c r="B5975" s="2">
         <v>44562</v>
@@ -85193,8 +85196,8 @@
       </c>
     </row>
     <row r="5976" spans="1:4">
-      <c r="A5976" t="s">
-        <v>6</v>
+      <c r="A5976">
+        <v>3</v>
       </c>
       <c r="B5976" s="2">
         <v>44562</v>
@@ -85207,8 +85210,8 @@
       </c>
     </row>
     <row r="5977" spans="1:4">
-      <c r="A5977" t="s">
-        <v>7</v>
+      <c r="A5977">
+        <v>4</v>
       </c>
       <c r="B5977" s="2">
         <v>44562</v>
@@ -85221,8 +85224,8 @@
       </c>
     </row>
     <row r="5978" spans="1:4">
-      <c r="A5978" t="s">
-        <v>8</v>
+      <c r="A5978">
+        <v>5</v>
       </c>
       <c r="B5978" s="2">
         <v>44562</v>
@@ -85235,8 +85238,8 @@
       </c>
     </row>
     <row r="5979" spans="1:4">
-      <c r="A5979" t="s">
-        <v>9</v>
+      <c r="A5979">
+        <v>6</v>
       </c>
       <c r="B5979" s="2">
         <v>44562</v>
@@ -85249,8 +85252,8 @@
       </c>
     </row>
     <row r="5980" spans="1:4">
-      <c r="A5980" t="s">
-        <v>10</v>
+      <c r="A5980">
+        <v>7</v>
       </c>
       <c r="B5980" s="2">
         <v>44562</v>
@@ -85263,8 +85266,8 @@
       </c>
     </row>
     <row r="5981" spans="1:4">
-      <c r="A5981" t="s">
-        <v>11</v>
+      <c r="A5981">
+        <v>8</v>
       </c>
       <c r="B5981" s="2">
         <v>44562</v>
@@ -85277,8 +85280,8 @@
       </c>
     </row>
     <row r="5982" spans="1:4">
-      <c r="A5982" t="s">
-        <v>12</v>
+      <c r="A5982">
+        <v>9</v>
       </c>
       <c r="B5982" s="2">
         <v>44562</v>
@@ -85291,8 +85294,8 @@
       </c>
     </row>
     <row r="5983" spans="1:4">
-      <c r="A5983" t="s">
-        <v>13</v>
+      <c r="A5983">
+        <v>10</v>
       </c>
       <c r="B5983" s="2">
         <v>44562</v>
@@ -85305,8 +85308,8 @@
       </c>
     </row>
     <row r="5984" spans="1:4">
-      <c r="A5984" t="s">
-        <v>14</v>
+      <c r="A5984">
+        <v>11</v>
       </c>
       <c r="B5984" s="2">
         <v>44562</v>
@@ -85319,8 +85322,8 @@
       </c>
     </row>
     <row r="5985" spans="1:4">
-      <c r="A5985" t="s">
-        <v>15</v>
+      <c r="A5985">
+        <v>12</v>
       </c>
       <c r="B5985" s="2">
         <v>44562</v>
@@ -85333,8 +85336,8 @@
       </c>
     </row>
     <row r="5986" spans="1:4">
-      <c r="A5986" t="s">
-        <v>16</v>
+      <c r="A5986">
+        <v>13</v>
       </c>
       <c r="B5986" s="2">
         <v>44562</v>
@@ -85347,8 +85350,8 @@
       </c>
     </row>
     <row r="5987" spans="1:4">
-      <c r="A5987" t="s">
-        <v>17</v>
+      <c r="A5987">
+        <v>14</v>
       </c>
       <c r="B5987" s="2">
         <v>44562</v>
@@ -85361,8 +85364,8 @@
       </c>
     </row>
     <row r="5988" spans="1:4">
-      <c r="A5988" t="s">
-        <v>18</v>
+      <c r="A5988">
+        <v>15</v>
       </c>
       <c r="B5988" s="2">
         <v>44562</v>
@@ -85375,8 +85378,8 @@
       </c>
     </row>
     <row r="5989" spans="1:4">
-      <c r="A5989" t="s">
-        <v>19</v>
+      <c r="A5989">
+        <v>16</v>
       </c>
       <c r="B5989" s="2">
         <v>44562</v>
@@ -85389,8 +85392,8 @@
       </c>
     </row>
     <row r="5990" spans="1:4">
-      <c r="A5990" t="s">
-        <v>4</v>
+      <c r="A5990">
+        <v>1</v>
       </c>
       <c r="B5990" s="2">
         <v>44563</v>
@@ -85403,8 +85406,8 @@
       </c>
     </row>
     <row r="5991" spans="1:4">
-      <c r="A5991" t="s">
-        <v>5</v>
+      <c r="A5991">
+        <v>2</v>
       </c>
       <c r="B5991" s="2">
         <v>44563</v>
@@ -85417,8 +85420,8 @@
       </c>
     </row>
     <row r="5992" spans="1:4">
-      <c r="A5992" t="s">
-        <v>6</v>
+      <c r="A5992">
+        <v>3</v>
       </c>
       <c r="B5992" s="2">
         <v>44563</v>
@@ -85431,8 +85434,8 @@
       </c>
     </row>
     <row r="5993" spans="1:4">
-      <c r="A5993" t="s">
-        <v>7</v>
+      <c r="A5993">
+        <v>4</v>
       </c>
       <c r="B5993" s="2">
         <v>44563</v>
@@ -85445,8 +85448,8 @@
       </c>
     </row>
     <row r="5994" spans="1:4">
-      <c r="A5994" t="s">
-        <v>8</v>
+      <c r="A5994">
+        <v>5</v>
       </c>
       <c r="B5994" s="2">
         <v>44563</v>
@@ -85459,8 +85462,8 @@
       </c>
     </row>
     <row r="5995" spans="1:4">
-      <c r="A5995" t="s">
-        <v>9</v>
+      <c r="A5995">
+        <v>6</v>
       </c>
       <c r="B5995" s="2">
         <v>44563</v>
@@ -85473,8 +85476,8 @@
       </c>
     </row>
     <row r="5996" spans="1:4">
-      <c r="A5996" t="s">
-        <v>10</v>
+      <c r="A5996">
+        <v>7</v>
       </c>
       <c r="B5996" s="2">
         <v>44563</v>
@@ -85487,8 +85490,8 @@
       </c>
     </row>
     <row r="5997" spans="1:4">
-      <c r="A5997" t="s">
-        <v>11</v>
+      <c r="A5997">
+        <v>8</v>
       </c>
       <c r="B5997" s="2">
         <v>44563</v>
@@ -85501,8 +85504,8 @@
       </c>
     </row>
     <row r="5998" spans="1:4">
-      <c r="A5998" t="s">
-        <v>12</v>
+      <c r="A5998">
+        <v>9</v>
       </c>
       <c r="B5998" s="2">
         <v>44563</v>
@@ -85515,8 +85518,8 @@
       </c>
     </row>
     <row r="5999" spans="1:4">
-      <c r="A5999" t="s">
-        <v>13</v>
+      <c r="A5999">
+        <v>10</v>
       </c>
       <c r="B5999" s="2">
         <v>44563</v>
@@ -85529,8 +85532,8 @@
       </c>
     </row>
     <row r="6000" spans="1:4">
-      <c r="A6000" t="s">
-        <v>14</v>
+      <c r="A6000">
+        <v>11</v>
       </c>
       <c r="B6000" s="2">
         <v>44563</v>
@@ -85543,8 +85546,8 @@
       </c>
     </row>
     <row r="6001" spans="1:4">
-      <c r="A6001" t="s">
-        <v>15</v>
+      <c r="A6001">
+        <v>12</v>
       </c>
       <c r="B6001" s="2">
         <v>44563</v>
@@ -85557,8 +85560,8 @@
       </c>
     </row>
     <row r="6002" spans="1:4">
-      <c r="A6002" t="s">
-        <v>16</v>
+      <c r="A6002">
+        <v>13</v>
       </c>
       <c r="B6002" s="2">
         <v>44563</v>
@@ -85571,8 +85574,8 @@
       </c>
     </row>
     <row r="6003" spans="1:4">
-      <c r="A6003" t="s">
-        <v>17</v>
+      <c r="A6003">
+        <v>14</v>
       </c>
       <c r="B6003" s="2">
         <v>44563</v>
@@ -85585,8 +85588,8 @@
       </c>
     </row>
     <row r="6004" spans="1:4">
-      <c r="A6004" t="s">
-        <v>18</v>
+      <c r="A6004">
+        <v>15</v>
       </c>
       <c r="B6004" s="2">
         <v>44563</v>
@@ -85599,8 +85602,8 @@
       </c>
     </row>
     <row r="6005" spans="1:4">
-      <c r="A6005" t="s">
-        <v>19</v>
+      <c r="A6005">
+        <v>16</v>
       </c>
       <c r="B6005" s="2">
         <v>44563</v>
@@ -85609,6 +85612,454 @@
         <v>386</v>
       </c>
       <c r="D6005">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6006" spans="1:4">
+      <c r="A6006" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6006" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6006" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6006">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6007" spans="1:4">
+      <c r="A6007" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6007" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6007" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6007">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6008" spans="1:4">
+      <c r="A6008" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6008" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6008" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6008">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6009" spans="1:4">
+      <c r="A6009" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6009" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6009" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6009">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6010" spans="1:4">
+      <c r="A6010" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6010" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6010" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6010">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6011" spans="1:4">
+      <c r="A6011" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6011" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6011" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6011">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6012" spans="1:4">
+      <c r="A6012" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6012" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6012" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6012">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6013" spans="1:4">
+      <c r="A6013" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6013" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6013" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6013">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6014" spans="1:4">
+      <c r="A6014" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6014" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6014" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6014">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6015" spans="1:4">
+      <c r="A6015" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6015" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6015" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6015">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6016" spans="1:4">
+      <c r="A6016" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6016" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6016" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6016">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6017" spans="1:4">
+      <c r="A6017" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6017" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6017" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6017">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6018" spans="1:4">
+      <c r="A6018" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6018" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6018" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6018">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6019" spans="1:4">
+      <c r="A6019" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6019" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6019" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6019">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6020" spans="1:4">
+      <c r="A6020" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6020" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6020" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6020">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6021" spans="1:4">
+      <c r="A6021" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6021" s="2">
+        <v>44563</v>
+      </c>
+      <c r="C6021" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6021">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6022" spans="1:4">
+      <c r="A6022" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6022" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6022" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6022">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6023" spans="1:4">
+      <c r="A6023" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6023" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6023" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6023">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6024" spans="1:4">
+      <c r="A6024" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6024" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6024" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6024">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6025" spans="1:4">
+      <c r="A6025" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6025" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6025" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6025">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6026" spans="1:4">
+      <c r="A6026" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6026" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6026" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6026">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6027" spans="1:4">
+      <c r="A6027" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6027" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6027" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6027">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6028" spans="1:4">
+      <c r="A6028" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6028" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6028" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6028">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6029" spans="1:4">
+      <c r="A6029" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6029" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6029" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6029">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6030" spans="1:4">
+      <c r="A6030" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6030" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6030" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6030">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6031" spans="1:4">
+      <c r="A6031" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6031" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6031" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6031">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6032" spans="1:4">
+      <c r="A6032" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6032" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6032" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6032">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6033" spans="1:4">
+      <c r="A6033" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6033" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6033" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6033">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6034" spans="1:4">
+      <c r="A6034" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6034" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6034" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6034">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6035" spans="1:4">
+      <c r="A6035" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6035" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6035" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6035">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6036" spans="1:4">
+      <c r="A6036" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6036" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6036" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6036">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6037" spans="1:4">
+      <c r="A6037" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6037" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6037" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6037">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-06-2022 19-19-36
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11596" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11628" uniqueCount="389">
   <si>
     <t>Región</t>
   </si>
@@ -1179,6 +1179,9 @@
   <si>
     <t>2022-01-03</t>
   </si>
+  <si>
+    <t>2022-01-04</t>
+  </si>
 </sst>
 </file>
 
@@ -1539,7 +1542,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6037"/>
+  <dimension ref="A1:D6069"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -85616,8 +85619,8 @@
       </c>
     </row>
     <row r="6006" spans="1:4">
-      <c r="A6006" t="s">
-        <v>4</v>
+      <c r="A6006">
+        <v>1</v>
       </c>
       <c r="B6006" s="2">
         <v>44563</v>
@@ -85630,8 +85633,8 @@
       </c>
     </row>
     <row r="6007" spans="1:4">
-      <c r="A6007" t="s">
-        <v>5</v>
+      <c r="A6007">
+        <v>2</v>
       </c>
       <c r="B6007" s="2">
         <v>44563</v>
@@ -85644,8 +85647,8 @@
       </c>
     </row>
     <row r="6008" spans="1:4">
-      <c r="A6008" t="s">
-        <v>6</v>
+      <c r="A6008">
+        <v>3</v>
       </c>
       <c r="B6008" s="2">
         <v>44563</v>
@@ -85658,8 +85661,8 @@
       </c>
     </row>
     <row r="6009" spans="1:4">
-      <c r="A6009" t="s">
-        <v>7</v>
+      <c r="A6009">
+        <v>4</v>
       </c>
       <c r="B6009" s="2">
         <v>44563</v>
@@ -85672,8 +85675,8 @@
       </c>
     </row>
     <row r="6010" spans="1:4">
-      <c r="A6010" t="s">
-        <v>8</v>
+      <c r="A6010">
+        <v>5</v>
       </c>
       <c r="B6010" s="2">
         <v>44563</v>
@@ -85686,8 +85689,8 @@
       </c>
     </row>
     <row r="6011" spans="1:4">
-      <c r="A6011" t="s">
-        <v>9</v>
+      <c r="A6011">
+        <v>6</v>
       </c>
       <c r="B6011" s="2">
         <v>44563</v>
@@ -85700,8 +85703,8 @@
       </c>
     </row>
     <row r="6012" spans="1:4">
-      <c r="A6012" t="s">
-        <v>10</v>
+      <c r="A6012">
+        <v>7</v>
       </c>
       <c r="B6012" s="2">
         <v>44563</v>
@@ -85714,8 +85717,8 @@
       </c>
     </row>
     <row r="6013" spans="1:4">
-      <c r="A6013" t="s">
-        <v>11</v>
+      <c r="A6013">
+        <v>8</v>
       </c>
       <c r="B6013" s="2">
         <v>44563</v>
@@ -85728,8 +85731,8 @@
       </c>
     </row>
     <row r="6014" spans="1:4">
-      <c r="A6014" t="s">
-        <v>12</v>
+      <c r="A6014">
+        <v>9</v>
       </c>
       <c r="B6014" s="2">
         <v>44563</v>
@@ -85742,8 +85745,8 @@
       </c>
     </row>
     <row r="6015" spans="1:4">
-      <c r="A6015" t="s">
-        <v>13</v>
+      <c r="A6015">
+        <v>10</v>
       </c>
       <c r="B6015" s="2">
         <v>44563</v>
@@ -85756,8 +85759,8 @@
       </c>
     </row>
     <row r="6016" spans="1:4">
-      <c r="A6016" t="s">
-        <v>14</v>
+      <c r="A6016">
+        <v>11</v>
       </c>
       <c r="B6016" s="2">
         <v>44563</v>
@@ -85770,8 +85773,8 @@
       </c>
     </row>
     <row r="6017" spans="1:4">
-      <c r="A6017" t="s">
-        <v>15</v>
+      <c r="A6017">
+        <v>12</v>
       </c>
       <c r="B6017" s="2">
         <v>44563</v>
@@ -85784,8 +85787,8 @@
       </c>
     </row>
     <row r="6018" spans="1:4">
-      <c r="A6018" t="s">
-        <v>16</v>
+      <c r="A6018">
+        <v>13</v>
       </c>
       <c r="B6018" s="2">
         <v>44563</v>
@@ -85798,8 +85801,8 @@
       </c>
     </row>
     <row r="6019" spans="1:4">
-      <c r="A6019" t="s">
-        <v>17</v>
+      <c r="A6019">
+        <v>14</v>
       </c>
       <c r="B6019" s="2">
         <v>44563</v>
@@ -85812,8 +85815,8 @@
       </c>
     </row>
     <row r="6020" spans="1:4">
-      <c r="A6020" t="s">
-        <v>18</v>
+      <c r="A6020">
+        <v>15</v>
       </c>
       <c r="B6020" s="2">
         <v>44563</v>
@@ -85826,8 +85829,8 @@
       </c>
     </row>
     <row r="6021" spans="1:4">
-      <c r="A6021" t="s">
-        <v>19</v>
+      <c r="A6021">
+        <v>16</v>
       </c>
       <c r="B6021" s="2">
         <v>44563</v>
@@ -85840,8 +85843,8 @@
       </c>
     </row>
     <row r="6022" spans="1:4">
-      <c r="A6022" t="s">
-        <v>4</v>
+      <c r="A6022">
+        <v>1</v>
       </c>
       <c r="B6022" s="2">
         <v>44564</v>
@@ -85854,8 +85857,8 @@
       </c>
     </row>
     <row r="6023" spans="1:4">
-      <c r="A6023" t="s">
-        <v>5</v>
+      <c r="A6023">
+        <v>2</v>
       </c>
       <c r="B6023" s="2">
         <v>44564</v>
@@ -85868,8 +85871,8 @@
       </c>
     </row>
     <row r="6024" spans="1:4">
-      <c r="A6024" t="s">
-        <v>6</v>
+      <c r="A6024">
+        <v>3</v>
       </c>
       <c r="B6024" s="2">
         <v>44564</v>
@@ -85882,8 +85885,8 @@
       </c>
     </row>
     <row r="6025" spans="1:4">
-      <c r="A6025" t="s">
-        <v>7</v>
+      <c r="A6025">
+        <v>4</v>
       </c>
       <c r="B6025" s="2">
         <v>44564</v>
@@ -85896,8 +85899,8 @@
       </c>
     </row>
     <row r="6026" spans="1:4">
-      <c r="A6026" t="s">
-        <v>8</v>
+      <c r="A6026">
+        <v>5</v>
       </c>
       <c r="B6026" s="2">
         <v>44564</v>
@@ -85910,8 +85913,8 @@
       </c>
     </row>
     <row r="6027" spans="1:4">
-      <c r="A6027" t="s">
-        <v>9</v>
+      <c r="A6027">
+        <v>6</v>
       </c>
       <c r="B6027" s="2">
         <v>44564</v>
@@ -85924,8 +85927,8 @@
       </c>
     </row>
     <row r="6028" spans="1:4">
-      <c r="A6028" t="s">
-        <v>10</v>
+      <c r="A6028">
+        <v>7</v>
       </c>
       <c r="B6028" s="2">
         <v>44564</v>
@@ -85938,8 +85941,8 @@
       </c>
     </row>
     <row r="6029" spans="1:4">
-      <c r="A6029" t="s">
-        <v>11</v>
+      <c r="A6029">
+        <v>8</v>
       </c>
       <c r="B6029" s="2">
         <v>44564</v>
@@ -85952,8 +85955,8 @@
       </c>
     </row>
     <row r="6030" spans="1:4">
-      <c r="A6030" t="s">
-        <v>12</v>
+      <c r="A6030">
+        <v>9</v>
       </c>
       <c r="B6030" s="2">
         <v>44564</v>
@@ -85966,8 +85969,8 @@
       </c>
     </row>
     <row r="6031" spans="1:4">
-      <c r="A6031" t="s">
-        <v>13</v>
+      <c r="A6031">
+        <v>10</v>
       </c>
       <c r="B6031" s="2">
         <v>44564</v>
@@ -85980,8 +85983,8 @@
       </c>
     </row>
     <row r="6032" spans="1:4">
-      <c r="A6032" t="s">
-        <v>14</v>
+      <c r="A6032">
+        <v>11</v>
       </c>
       <c r="B6032" s="2">
         <v>44564</v>
@@ -85994,8 +85997,8 @@
       </c>
     </row>
     <row r="6033" spans="1:4">
-      <c r="A6033" t="s">
-        <v>15</v>
+      <c r="A6033">
+        <v>12</v>
       </c>
       <c r="B6033" s="2">
         <v>44564</v>
@@ -86008,8 +86011,8 @@
       </c>
     </row>
     <row r="6034" spans="1:4">
-      <c r="A6034" t="s">
-        <v>16</v>
+      <c r="A6034">
+        <v>13</v>
       </c>
       <c r="B6034" s="2">
         <v>44564</v>
@@ -86022,8 +86025,8 @@
       </c>
     </row>
     <row r="6035" spans="1:4">
-      <c r="A6035" t="s">
-        <v>17</v>
+      <c r="A6035">
+        <v>14</v>
       </c>
       <c r="B6035" s="2">
         <v>44564</v>
@@ -86036,8 +86039,8 @@
       </c>
     </row>
     <row r="6036" spans="1:4">
-      <c r="A6036" t="s">
-        <v>18</v>
+      <c r="A6036">
+        <v>15</v>
       </c>
       <c r="B6036" s="2">
         <v>44564</v>
@@ -86050,8 +86053,8 @@
       </c>
     </row>
     <row r="6037" spans="1:4">
-      <c r="A6037" t="s">
-        <v>19</v>
+      <c r="A6037">
+        <v>16</v>
       </c>
       <c r="B6037" s="2">
         <v>44564</v>
@@ -86060,6 +86063,454 @@
         <v>387</v>
       </c>
       <c r="D6037">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6038" spans="1:4">
+      <c r="A6038" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6038" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6038" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6038">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6039" spans="1:4">
+      <c r="A6039" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6039" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6039" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6039">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6040" spans="1:4">
+      <c r="A6040" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6040" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6040" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6040">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6041" spans="1:4">
+      <c r="A6041" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6041" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6041" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6041">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6042" spans="1:4">
+      <c r="A6042" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6042" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6042" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6042">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6043" spans="1:4">
+      <c r="A6043" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6043" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6043" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6043">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6044" spans="1:4">
+      <c r="A6044" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6044" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6044" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6044">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6045" spans="1:4">
+      <c r="A6045" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6045" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6045" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6045">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6046" spans="1:4">
+      <c r="A6046" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6046" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6046" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6046">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6047" spans="1:4">
+      <c r="A6047" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6047" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6047" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6047">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6048" spans="1:4">
+      <c r="A6048" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6048" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6048" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6048">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6049" spans="1:4">
+      <c r="A6049" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6049" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6049" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6049">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6050" spans="1:4">
+      <c r="A6050" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6050" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6050" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6050">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6051" spans="1:4">
+      <c r="A6051" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6051" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6051" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6051">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6052" spans="1:4">
+      <c r="A6052" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6052" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6052" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6052">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6053" spans="1:4">
+      <c r="A6053" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6053" s="2">
+        <v>44564</v>
+      </c>
+      <c r="C6053" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6053">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6054" spans="1:4">
+      <c r="A6054" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6054" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6054" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6054">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6055" spans="1:4">
+      <c r="A6055" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6055" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6055" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6055">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6056" spans="1:4">
+      <c r="A6056" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6056" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6056" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6056">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6057" spans="1:4">
+      <c r="A6057" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6057" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6057" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6057">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6058" spans="1:4">
+      <c r="A6058" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6058" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6058" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6058">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6059" spans="1:4">
+      <c r="A6059" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6059" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6059" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6059">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6060" spans="1:4">
+      <c r="A6060" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6060" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6060" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6060">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6061" spans="1:4">
+      <c r="A6061" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6061" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6061" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6061">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6062" spans="1:4">
+      <c r="A6062" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6062" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6062" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6062">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6063" spans="1:4">
+      <c r="A6063" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6063" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6063" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6063">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6064" spans="1:4">
+      <c r="A6064" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6064" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6064" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6064">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6065" spans="1:4">
+      <c r="A6065" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6065" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6065" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6065">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6066" spans="1:4">
+      <c r="A6066" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6066" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6066" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6066">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6067" spans="1:4">
+      <c r="A6067" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6067" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6067" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6067">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6068" spans="1:4">
+      <c r="A6068" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6068" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6068" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6068">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6069" spans="1:4">
+      <c r="A6069" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6069" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6069" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6069">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-07-2022 19-52-37
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11628" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11660" uniqueCount="390">
   <si>
     <t>Región</t>
   </si>
@@ -1182,6 +1182,9 @@
   <si>
     <t>2022-01-04</t>
   </si>
+  <si>
+    <t>2022-01-05</t>
+  </si>
 </sst>
 </file>
 
@@ -1542,7 +1545,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6069"/>
+  <dimension ref="A1:D6101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -86067,8 +86070,8 @@
       </c>
     </row>
     <row r="6038" spans="1:4">
-      <c r="A6038" t="s">
-        <v>4</v>
+      <c r="A6038">
+        <v>1</v>
       </c>
       <c r="B6038" s="2">
         <v>44564</v>
@@ -86081,8 +86084,8 @@
       </c>
     </row>
     <row r="6039" spans="1:4">
-      <c r="A6039" t="s">
-        <v>5</v>
+      <c r="A6039">
+        <v>2</v>
       </c>
       <c r="B6039" s="2">
         <v>44564</v>
@@ -86095,8 +86098,8 @@
       </c>
     </row>
     <row r="6040" spans="1:4">
-      <c r="A6040" t="s">
-        <v>6</v>
+      <c r="A6040">
+        <v>3</v>
       </c>
       <c r="B6040" s="2">
         <v>44564</v>
@@ -86109,8 +86112,8 @@
       </c>
     </row>
     <row r="6041" spans="1:4">
-      <c r="A6041" t="s">
-        <v>7</v>
+      <c r="A6041">
+        <v>4</v>
       </c>
       <c r="B6041" s="2">
         <v>44564</v>
@@ -86123,8 +86126,8 @@
       </c>
     </row>
     <row r="6042" spans="1:4">
-      <c r="A6042" t="s">
-        <v>8</v>
+      <c r="A6042">
+        <v>5</v>
       </c>
       <c r="B6042" s="2">
         <v>44564</v>
@@ -86137,8 +86140,8 @@
       </c>
     </row>
     <row r="6043" spans="1:4">
-      <c r="A6043" t="s">
-        <v>9</v>
+      <c r="A6043">
+        <v>6</v>
       </c>
       <c r="B6043" s="2">
         <v>44564</v>
@@ -86151,8 +86154,8 @@
       </c>
     </row>
     <row r="6044" spans="1:4">
-      <c r="A6044" t="s">
-        <v>10</v>
+      <c r="A6044">
+        <v>7</v>
       </c>
       <c r="B6044" s="2">
         <v>44564</v>
@@ -86165,8 +86168,8 @@
       </c>
     </row>
     <row r="6045" spans="1:4">
-      <c r="A6045" t="s">
-        <v>11</v>
+      <c r="A6045">
+        <v>8</v>
       </c>
       <c r="B6045" s="2">
         <v>44564</v>
@@ -86179,8 +86182,8 @@
       </c>
     </row>
     <row r="6046" spans="1:4">
-      <c r="A6046" t="s">
-        <v>12</v>
+      <c r="A6046">
+        <v>9</v>
       </c>
       <c r="B6046" s="2">
         <v>44564</v>
@@ -86193,8 +86196,8 @@
       </c>
     </row>
     <row r="6047" spans="1:4">
-      <c r="A6047" t="s">
-        <v>13</v>
+      <c r="A6047">
+        <v>10</v>
       </c>
       <c r="B6047" s="2">
         <v>44564</v>
@@ -86207,8 +86210,8 @@
       </c>
     </row>
     <row r="6048" spans="1:4">
-      <c r="A6048" t="s">
-        <v>14</v>
+      <c r="A6048">
+        <v>11</v>
       </c>
       <c r="B6048" s="2">
         <v>44564</v>
@@ -86221,8 +86224,8 @@
       </c>
     </row>
     <row r="6049" spans="1:4">
-      <c r="A6049" t="s">
-        <v>15</v>
+      <c r="A6049">
+        <v>12</v>
       </c>
       <c r="B6049" s="2">
         <v>44564</v>
@@ -86235,8 +86238,8 @@
       </c>
     </row>
     <row r="6050" spans="1:4">
-      <c r="A6050" t="s">
-        <v>16</v>
+      <c r="A6050">
+        <v>13</v>
       </c>
       <c r="B6050" s="2">
         <v>44564</v>
@@ -86249,8 +86252,8 @@
       </c>
     </row>
     <row r="6051" spans="1:4">
-      <c r="A6051" t="s">
-        <v>17</v>
+      <c r="A6051">
+        <v>14</v>
       </c>
       <c r="B6051" s="2">
         <v>44564</v>
@@ -86263,8 +86266,8 @@
       </c>
     </row>
     <row r="6052" spans="1:4">
-      <c r="A6052" t="s">
-        <v>18</v>
+      <c r="A6052">
+        <v>15</v>
       </c>
       <c r="B6052" s="2">
         <v>44564</v>
@@ -86277,8 +86280,8 @@
       </c>
     </row>
     <row r="6053" spans="1:4">
-      <c r="A6053" t="s">
-        <v>19</v>
+      <c r="A6053">
+        <v>16</v>
       </c>
       <c r="B6053" s="2">
         <v>44564</v>
@@ -86291,8 +86294,8 @@
       </c>
     </row>
     <row r="6054" spans="1:4">
-      <c r="A6054" t="s">
-        <v>4</v>
+      <c r="A6054">
+        <v>1</v>
       </c>
       <c r="B6054" s="2">
         <v>44565</v>
@@ -86305,8 +86308,8 @@
       </c>
     </row>
     <row r="6055" spans="1:4">
-      <c r="A6055" t="s">
-        <v>5</v>
+      <c r="A6055">
+        <v>2</v>
       </c>
       <c r="B6055" s="2">
         <v>44565</v>
@@ -86319,8 +86322,8 @@
       </c>
     </row>
     <row r="6056" spans="1:4">
-      <c r="A6056" t="s">
-        <v>6</v>
+      <c r="A6056">
+        <v>3</v>
       </c>
       <c r="B6056" s="2">
         <v>44565</v>
@@ -86333,8 +86336,8 @@
       </c>
     </row>
     <row r="6057" spans="1:4">
-      <c r="A6057" t="s">
-        <v>7</v>
+      <c r="A6057">
+        <v>4</v>
       </c>
       <c r="B6057" s="2">
         <v>44565</v>
@@ -86347,8 +86350,8 @@
       </c>
     </row>
     <row r="6058" spans="1:4">
-      <c r="A6058" t="s">
-        <v>8</v>
+      <c r="A6058">
+        <v>5</v>
       </c>
       <c r="B6058" s="2">
         <v>44565</v>
@@ -86361,8 +86364,8 @@
       </c>
     </row>
     <row r="6059" spans="1:4">
-      <c r="A6059" t="s">
-        <v>9</v>
+      <c r="A6059">
+        <v>6</v>
       </c>
       <c r="B6059" s="2">
         <v>44565</v>
@@ -86375,8 +86378,8 @@
       </c>
     </row>
     <row r="6060" spans="1:4">
-      <c r="A6060" t="s">
-        <v>10</v>
+      <c r="A6060">
+        <v>7</v>
       </c>
       <c r="B6060" s="2">
         <v>44565</v>
@@ -86389,8 +86392,8 @@
       </c>
     </row>
     <row r="6061" spans="1:4">
-      <c r="A6061" t="s">
-        <v>11</v>
+      <c r="A6061">
+        <v>8</v>
       </c>
       <c r="B6061" s="2">
         <v>44565</v>
@@ -86403,8 +86406,8 @@
       </c>
     </row>
     <row r="6062" spans="1:4">
-      <c r="A6062" t="s">
-        <v>12</v>
+      <c r="A6062">
+        <v>9</v>
       </c>
       <c r="B6062" s="2">
         <v>44565</v>
@@ -86417,8 +86420,8 @@
       </c>
     </row>
     <row r="6063" spans="1:4">
-      <c r="A6063" t="s">
-        <v>13</v>
+      <c r="A6063">
+        <v>10</v>
       </c>
       <c r="B6063" s="2">
         <v>44565</v>
@@ -86431,8 +86434,8 @@
       </c>
     </row>
     <row r="6064" spans="1:4">
-      <c r="A6064" t="s">
-        <v>14</v>
+      <c r="A6064">
+        <v>11</v>
       </c>
       <c r="B6064" s="2">
         <v>44565</v>
@@ -86445,8 +86448,8 @@
       </c>
     </row>
     <row r="6065" spans="1:4">
-      <c r="A6065" t="s">
-        <v>15</v>
+      <c r="A6065">
+        <v>12</v>
       </c>
       <c r="B6065" s="2">
         <v>44565</v>
@@ -86459,8 +86462,8 @@
       </c>
     </row>
     <row r="6066" spans="1:4">
-      <c r="A6066" t="s">
-        <v>16</v>
+      <c r="A6066">
+        <v>13</v>
       </c>
       <c r="B6066" s="2">
         <v>44565</v>
@@ -86473,8 +86476,8 @@
       </c>
     </row>
     <row r="6067" spans="1:4">
-      <c r="A6067" t="s">
-        <v>17</v>
+      <c r="A6067">
+        <v>14</v>
       </c>
       <c r="B6067" s="2">
         <v>44565</v>
@@ -86487,8 +86490,8 @@
       </c>
     </row>
     <row r="6068" spans="1:4">
-      <c r="A6068" t="s">
-        <v>18</v>
+      <c r="A6068">
+        <v>15</v>
       </c>
       <c r="B6068" s="2">
         <v>44565</v>
@@ -86501,8 +86504,8 @@
       </c>
     </row>
     <row r="6069" spans="1:4">
-      <c r="A6069" t="s">
-        <v>19</v>
+      <c r="A6069">
+        <v>16</v>
       </c>
       <c r="B6069" s="2">
         <v>44565</v>
@@ -86512,6 +86515,454 @@
       </c>
       <c r="D6069">
         <v>0</v>
+      </c>
+    </row>
+    <row r="6070" spans="1:4">
+      <c r="A6070" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6070" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6070" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6070">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6071" spans="1:4">
+      <c r="A6071" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6071" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6071" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6071">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6072" spans="1:4">
+      <c r="A6072" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6072" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6072" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6072">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6073" spans="1:4">
+      <c r="A6073" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6073" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6073" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6073">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6074" spans="1:4">
+      <c r="A6074" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6074" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6074" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6074">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6075" spans="1:4">
+      <c r="A6075" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6075" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6075" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6075">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6076" spans="1:4">
+      <c r="A6076" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6076" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6076" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6076">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6077" spans="1:4">
+      <c r="A6077" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6077" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6077" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6077">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6078" spans="1:4">
+      <c r="A6078" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6078" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6078" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6078">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6079" spans="1:4">
+      <c r="A6079" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6079" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6079" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6079">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6080" spans="1:4">
+      <c r="A6080" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6080" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6080" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6080">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6081" spans="1:4">
+      <c r="A6081" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6081" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6081" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6081">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6082" spans="1:4">
+      <c r="A6082" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6082" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6082" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6082">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6083" spans="1:4">
+      <c r="A6083" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6083" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6083" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6083">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6084" spans="1:4">
+      <c r="A6084" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6084" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6084" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6084">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6085" spans="1:4">
+      <c r="A6085" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6085" s="2">
+        <v>44565</v>
+      </c>
+      <c r="C6085" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6085">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6086" spans="1:4">
+      <c r="A6086" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6086" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6086" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6086">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6087" spans="1:4">
+      <c r="A6087" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6087" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6087" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6087">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6088" spans="1:4">
+      <c r="A6088" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6088" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6088" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6088">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6089" spans="1:4">
+      <c r="A6089" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6089" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6089" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6089">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6090" spans="1:4">
+      <c r="A6090" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6090" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6090" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6090">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6091" spans="1:4">
+      <c r="A6091" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6091" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6091" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6091">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6092" spans="1:4">
+      <c r="A6092" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6092" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6092" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6092">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6093" spans="1:4">
+      <c r="A6093" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6093" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6093" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6093">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6094" spans="1:4">
+      <c r="A6094" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6094" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6094" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6094">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6095" spans="1:4">
+      <c r="A6095" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6095" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6095" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6095">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6096" spans="1:4">
+      <c r="A6096" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6096" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6096" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6096">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6097" spans="1:4">
+      <c r="A6097" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6097" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6097" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6097">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6098" spans="1:4">
+      <c r="A6098" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6098" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6098" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6098">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6099" spans="1:4">
+      <c r="A6099" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6099" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6099" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6099">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6100" spans="1:4">
+      <c r="A6100" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6100" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6100" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6101" spans="1:4">
+      <c r="A6101" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6101" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6101" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6101">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-08-2022 20-24-21
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11660" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11692" uniqueCount="391">
   <si>
     <t>Región</t>
   </si>
@@ -1185,6 +1185,9 @@
   <si>
     <t>2022-01-05</t>
   </si>
+  <si>
+    <t>2022-01-06</t>
+  </si>
 </sst>
 </file>
 
@@ -1545,7 +1548,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6101"/>
+  <dimension ref="A1:D6133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -86518,8 +86521,8 @@
       </c>
     </row>
     <row r="6070" spans="1:4">
-      <c r="A6070" t="s">
-        <v>4</v>
+      <c r="A6070">
+        <v>1</v>
       </c>
       <c r="B6070" s="2">
         <v>44565</v>
@@ -86532,8 +86535,8 @@
       </c>
     </row>
     <row r="6071" spans="1:4">
-      <c r="A6071" t="s">
-        <v>5</v>
+      <c r="A6071">
+        <v>2</v>
       </c>
       <c r="B6071" s="2">
         <v>44565</v>
@@ -86546,8 +86549,8 @@
       </c>
     </row>
     <row r="6072" spans="1:4">
-      <c r="A6072" t="s">
-        <v>6</v>
+      <c r="A6072">
+        <v>3</v>
       </c>
       <c r="B6072" s="2">
         <v>44565</v>
@@ -86560,8 +86563,8 @@
       </c>
     </row>
     <row r="6073" spans="1:4">
-      <c r="A6073" t="s">
-        <v>7</v>
+      <c r="A6073">
+        <v>4</v>
       </c>
       <c r="B6073" s="2">
         <v>44565</v>
@@ -86574,8 +86577,8 @@
       </c>
     </row>
     <row r="6074" spans="1:4">
-      <c r="A6074" t="s">
-        <v>8</v>
+      <c r="A6074">
+        <v>5</v>
       </c>
       <c r="B6074" s="2">
         <v>44565</v>
@@ -86588,8 +86591,8 @@
       </c>
     </row>
     <row r="6075" spans="1:4">
-      <c r="A6075" t="s">
-        <v>9</v>
+      <c r="A6075">
+        <v>6</v>
       </c>
       <c r="B6075" s="2">
         <v>44565</v>
@@ -86602,8 +86605,8 @@
       </c>
     </row>
     <row r="6076" spans="1:4">
-      <c r="A6076" t="s">
-        <v>10</v>
+      <c r="A6076">
+        <v>7</v>
       </c>
       <c r="B6076" s="2">
         <v>44565</v>
@@ -86616,8 +86619,8 @@
       </c>
     </row>
     <row r="6077" spans="1:4">
-      <c r="A6077" t="s">
-        <v>11</v>
+      <c r="A6077">
+        <v>8</v>
       </c>
       <c r="B6077" s="2">
         <v>44565</v>
@@ -86630,8 +86633,8 @@
       </c>
     </row>
     <row r="6078" spans="1:4">
-      <c r="A6078" t="s">
-        <v>12</v>
+      <c r="A6078">
+        <v>9</v>
       </c>
       <c r="B6078" s="2">
         <v>44565</v>
@@ -86644,8 +86647,8 @@
       </c>
     </row>
     <row r="6079" spans="1:4">
-      <c r="A6079" t="s">
-        <v>13</v>
+      <c r="A6079">
+        <v>10</v>
       </c>
       <c r="B6079" s="2">
         <v>44565</v>
@@ -86658,8 +86661,8 @@
       </c>
     </row>
     <row r="6080" spans="1:4">
-      <c r="A6080" t="s">
-        <v>14</v>
+      <c r="A6080">
+        <v>11</v>
       </c>
       <c r="B6080" s="2">
         <v>44565</v>
@@ -86672,8 +86675,8 @@
       </c>
     </row>
     <row r="6081" spans="1:4">
-      <c r="A6081" t="s">
-        <v>15</v>
+      <c r="A6081">
+        <v>12</v>
       </c>
       <c r="B6081" s="2">
         <v>44565</v>
@@ -86686,8 +86689,8 @@
       </c>
     </row>
     <row r="6082" spans="1:4">
-      <c r="A6082" t="s">
-        <v>16</v>
+      <c r="A6082">
+        <v>13</v>
       </c>
       <c r="B6082" s="2">
         <v>44565</v>
@@ -86700,8 +86703,8 @@
       </c>
     </row>
     <row r="6083" spans="1:4">
-      <c r="A6083" t="s">
-        <v>17</v>
+      <c r="A6083">
+        <v>14</v>
       </c>
       <c r="B6083" s="2">
         <v>44565</v>
@@ -86714,8 +86717,8 @@
       </c>
     </row>
     <row r="6084" spans="1:4">
-      <c r="A6084" t="s">
-        <v>18</v>
+      <c r="A6084">
+        <v>15</v>
       </c>
       <c r="B6084" s="2">
         <v>44565</v>
@@ -86728,8 +86731,8 @@
       </c>
     </row>
     <row r="6085" spans="1:4">
-      <c r="A6085" t="s">
-        <v>19</v>
+      <c r="A6085">
+        <v>16</v>
       </c>
       <c r="B6085" s="2">
         <v>44565</v>
@@ -86742,8 +86745,8 @@
       </c>
     </row>
     <row r="6086" spans="1:4">
-      <c r="A6086" t="s">
-        <v>4</v>
+      <c r="A6086">
+        <v>1</v>
       </c>
       <c r="B6086" s="2">
         <v>44566</v>
@@ -86756,8 +86759,8 @@
       </c>
     </row>
     <row r="6087" spans="1:4">
-      <c r="A6087" t="s">
-        <v>5</v>
+      <c r="A6087">
+        <v>2</v>
       </c>
       <c r="B6087" s="2">
         <v>44566</v>
@@ -86770,8 +86773,8 @@
       </c>
     </row>
     <row r="6088" spans="1:4">
-      <c r="A6088" t="s">
-        <v>6</v>
+      <c r="A6088">
+        <v>3</v>
       </c>
       <c r="B6088" s="2">
         <v>44566</v>
@@ -86784,8 +86787,8 @@
       </c>
     </row>
     <row r="6089" spans="1:4">
-      <c r="A6089" t="s">
-        <v>7</v>
+      <c r="A6089">
+        <v>4</v>
       </c>
       <c r="B6089" s="2">
         <v>44566</v>
@@ -86798,8 +86801,8 @@
       </c>
     </row>
     <row r="6090" spans="1:4">
-      <c r="A6090" t="s">
-        <v>8</v>
+      <c r="A6090">
+        <v>5</v>
       </c>
       <c r="B6090" s="2">
         <v>44566</v>
@@ -86812,8 +86815,8 @@
       </c>
     </row>
     <row r="6091" spans="1:4">
-      <c r="A6091" t="s">
-        <v>9</v>
+      <c r="A6091">
+        <v>6</v>
       </c>
       <c r="B6091" s="2">
         <v>44566</v>
@@ -86826,8 +86829,8 @@
       </c>
     </row>
     <row r="6092" spans="1:4">
-      <c r="A6092" t="s">
-        <v>10</v>
+      <c r="A6092">
+        <v>7</v>
       </c>
       <c r="B6092" s="2">
         <v>44566</v>
@@ -86840,8 +86843,8 @@
       </c>
     </row>
     <row r="6093" spans="1:4">
-      <c r="A6093" t="s">
-        <v>11</v>
+      <c r="A6093">
+        <v>8</v>
       </c>
       <c r="B6093" s="2">
         <v>44566</v>
@@ -86854,8 +86857,8 @@
       </c>
     </row>
     <row r="6094" spans="1:4">
-      <c r="A6094" t="s">
-        <v>12</v>
+      <c r="A6094">
+        <v>9</v>
       </c>
       <c r="B6094" s="2">
         <v>44566</v>
@@ -86868,8 +86871,8 @@
       </c>
     </row>
     <row r="6095" spans="1:4">
-      <c r="A6095" t="s">
-        <v>13</v>
+      <c r="A6095">
+        <v>10</v>
       </c>
       <c r="B6095" s="2">
         <v>44566</v>
@@ -86882,8 +86885,8 @@
       </c>
     </row>
     <row r="6096" spans="1:4">
-      <c r="A6096" t="s">
-        <v>14</v>
+      <c r="A6096">
+        <v>11</v>
       </c>
       <c r="B6096" s="2">
         <v>44566</v>
@@ -86896,8 +86899,8 @@
       </c>
     </row>
     <row r="6097" spans="1:4">
-      <c r="A6097" t="s">
-        <v>15</v>
+      <c r="A6097">
+        <v>12</v>
       </c>
       <c r="B6097" s="2">
         <v>44566</v>
@@ -86910,8 +86913,8 @@
       </c>
     </row>
     <row r="6098" spans="1:4">
-      <c r="A6098" t="s">
-        <v>16</v>
+      <c r="A6098">
+        <v>13</v>
       </c>
       <c r="B6098" s="2">
         <v>44566</v>
@@ -86924,8 +86927,8 @@
       </c>
     </row>
     <row r="6099" spans="1:4">
-      <c r="A6099" t="s">
-        <v>17</v>
+      <c r="A6099">
+        <v>14</v>
       </c>
       <c r="B6099" s="2">
         <v>44566</v>
@@ -86938,8 +86941,8 @@
       </c>
     </row>
     <row r="6100" spans="1:4">
-      <c r="A6100" t="s">
-        <v>18</v>
+      <c r="A6100">
+        <v>15</v>
       </c>
       <c r="B6100" s="2">
         <v>44566</v>
@@ -86952,8 +86955,8 @@
       </c>
     </row>
     <row r="6101" spans="1:4">
-      <c r="A6101" t="s">
-        <v>19</v>
+      <c r="A6101">
+        <v>16</v>
       </c>
       <c r="B6101" s="2">
         <v>44566</v>
@@ -86963,6 +86966,454 @@
       </c>
       <c r="D6101">
         <v>1</v>
+      </c>
+    </row>
+    <row r="6102" spans="1:4">
+      <c r="A6102" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6102" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6102" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6103" spans="1:4">
+      <c r="A6103" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6103" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6103" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6104" spans="1:4">
+      <c r="A6104" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6104" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6104" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6105" spans="1:4">
+      <c r="A6105" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6105" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6105" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6106" spans="1:4">
+      <c r="A6106" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6106" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6106" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6107" spans="1:4">
+      <c r="A6107" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6107" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6107" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6108" spans="1:4">
+      <c r="A6108" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6108" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6108" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6109" spans="1:4">
+      <c r="A6109" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6109" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6109" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6109">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6110" spans="1:4">
+      <c r="A6110" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6110" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6110" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6110">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6111" spans="1:4">
+      <c r="A6111" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6111" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6111" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6112" spans="1:4">
+      <c r="A6112" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6112" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6112" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6113" spans="1:4">
+      <c r="A6113" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6113" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6113" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6114" spans="1:4">
+      <c r="A6114" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6114" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6114" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6115" spans="1:4">
+      <c r="A6115" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6115" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6115" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6116" spans="1:4">
+      <c r="A6116" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6116" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6116" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6117" spans="1:4">
+      <c r="A6117" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6117" s="2">
+        <v>44566</v>
+      </c>
+      <c r="C6117" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6118" spans="1:4">
+      <c r="A6118" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6118" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6118" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6119" spans="1:4">
+      <c r="A6119" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6119" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6119" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6120" spans="1:4">
+      <c r="A6120" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6120" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6120" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6121" spans="1:4">
+      <c r="A6121" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6121" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6121" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6122" spans="1:4">
+      <c r="A6122" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6122" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6122" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6123" spans="1:4">
+      <c r="A6123" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6123" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6123" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6124" spans="1:4">
+      <c r="A6124" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6124" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6124" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6125" spans="1:4">
+      <c r="A6125" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6125" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6125" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6126" spans="1:4">
+      <c r="A6126" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6126" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6126" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6127" spans="1:4">
+      <c r="A6127" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6127" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6127" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6128" spans="1:4">
+      <c r="A6128" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6128" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6128" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6129" spans="1:4">
+      <c r="A6129" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6129" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6129" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6130" spans="1:4">
+      <c r="A6130" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6130" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6130" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6131" spans="1:4">
+      <c r="A6131" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6131" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6131" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6132" spans="1:4">
+      <c r="A6132" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6132" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6132" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6133" spans="1:4">
+      <c r="A6133" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6133" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6133" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6133">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-09-2022 20-20-40
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -1548,7 +1548,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6133"/>
+  <dimension ref="A1:D6149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -86969,8 +86969,8 @@
       </c>
     </row>
     <row r="6102" spans="1:4">
-      <c r="A6102" t="s">
-        <v>4</v>
+      <c r="A6102">
+        <v>1</v>
       </c>
       <c r="B6102" s="2">
         <v>44566</v>
@@ -86983,8 +86983,8 @@
       </c>
     </row>
     <row r="6103" spans="1:4">
-      <c r="A6103" t="s">
-        <v>5</v>
+      <c r="A6103">
+        <v>2</v>
       </c>
       <c r="B6103" s="2">
         <v>44566</v>
@@ -86997,8 +86997,8 @@
       </c>
     </row>
     <row r="6104" spans="1:4">
-      <c r="A6104" t="s">
-        <v>6</v>
+      <c r="A6104">
+        <v>3</v>
       </c>
       <c r="B6104" s="2">
         <v>44566</v>
@@ -87011,8 +87011,8 @@
       </c>
     </row>
     <row r="6105" spans="1:4">
-      <c r="A6105" t="s">
-        <v>7</v>
+      <c r="A6105">
+        <v>4</v>
       </c>
       <c r="B6105" s="2">
         <v>44566</v>
@@ -87025,8 +87025,8 @@
       </c>
     </row>
     <row r="6106" spans="1:4">
-      <c r="A6106" t="s">
-        <v>8</v>
+      <c r="A6106">
+        <v>5</v>
       </c>
       <c r="B6106" s="2">
         <v>44566</v>
@@ -87039,8 +87039,8 @@
       </c>
     </row>
     <row r="6107" spans="1:4">
-      <c r="A6107" t="s">
-        <v>9</v>
+      <c r="A6107">
+        <v>6</v>
       </c>
       <c r="B6107" s="2">
         <v>44566</v>
@@ -87053,8 +87053,8 @@
       </c>
     </row>
     <row r="6108" spans="1:4">
-      <c r="A6108" t="s">
-        <v>10</v>
+      <c r="A6108">
+        <v>7</v>
       </c>
       <c r="B6108" s="2">
         <v>44566</v>
@@ -87067,8 +87067,8 @@
       </c>
     </row>
     <row r="6109" spans="1:4">
-      <c r="A6109" t="s">
-        <v>11</v>
+      <c r="A6109">
+        <v>8</v>
       </c>
       <c r="B6109" s="2">
         <v>44566</v>
@@ -87081,8 +87081,8 @@
       </c>
     </row>
     <row r="6110" spans="1:4">
-      <c r="A6110" t="s">
-        <v>12</v>
+      <c r="A6110">
+        <v>9</v>
       </c>
       <c r="B6110" s="2">
         <v>44566</v>
@@ -87095,8 +87095,8 @@
       </c>
     </row>
     <row r="6111" spans="1:4">
-      <c r="A6111" t="s">
-        <v>13</v>
+      <c r="A6111">
+        <v>10</v>
       </c>
       <c r="B6111" s="2">
         <v>44566</v>
@@ -87109,8 +87109,8 @@
       </c>
     </row>
     <row r="6112" spans="1:4">
-      <c r="A6112" t="s">
-        <v>14</v>
+      <c r="A6112">
+        <v>11</v>
       </c>
       <c r="B6112" s="2">
         <v>44566</v>
@@ -87123,8 +87123,8 @@
       </c>
     </row>
     <row r="6113" spans="1:4">
-      <c r="A6113" t="s">
-        <v>15</v>
+      <c r="A6113">
+        <v>12</v>
       </c>
       <c r="B6113" s="2">
         <v>44566</v>
@@ -87137,8 +87137,8 @@
       </c>
     </row>
     <row r="6114" spans="1:4">
-      <c r="A6114" t="s">
-        <v>16</v>
+      <c r="A6114">
+        <v>13</v>
       </c>
       <c r="B6114" s="2">
         <v>44566</v>
@@ -87151,8 +87151,8 @@
       </c>
     </row>
     <row r="6115" spans="1:4">
-      <c r="A6115" t="s">
-        <v>17</v>
+      <c r="A6115">
+        <v>14</v>
       </c>
       <c r="B6115" s="2">
         <v>44566</v>
@@ -87165,8 +87165,8 @@
       </c>
     </row>
     <row r="6116" spans="1:4">
-      <c r="A6116" t="s">
-        <v>18</v>
+      <c r="A6116">
+        <v>15</v>
       </c>
       <c r="B6116" s="2">
         <v>44566</v>
@@ -87179,8 +87179,8 @@
       </c>
     </row>
     <row r="6117" spans="1:4">
-      <c r="A6117" t="s">
-        <v>19</v>
+      <c r="A6117">
+        <v>16</v>
       </c>
       <c r="B6117" s="2">
         <v>44566</v>
@@ -87193,8 +87193,8 @@
       </c>
     </row>
     <row r="6118" spans="1:4">
-      <c r="A6118" t="s">
-        <v>4</v>
+      <c r="A6118">
+        <v>1</v>
       </c>
       <c r="B6118" s="2">
         <v>44567</v>
@@ -87207,8 +87207,8 @@
       </c>
     </row>
     <row r="6119" spans="1:4">
-      <c r="A6119" t="s">
-        <v>5</v>
+      <c r="A6119">
+        <v>2</v>
       </c>
       <c r="B6119" s="2">
         <v>44567</v>
@@ -87221,8 +87221,8 @@
       </c>
     </row>
     <row r="6120" spans="1:4">
-      <c r="A6120" t="s">
-        <v>6</v>
+      <c r="A6120">
+        <v>3</v>
       </c>
       <c r="B6120" s="2">
         <v>44567</v>
@@ -87235,8 +87235,8 @@
       </c>
     </row>
     <row r="6121" spans="1:4">
-      <c r="A6121" t="s">
-        <v>7</v>
+      <c r="A6121">
+        <v>4</v>
       </c>
       <c r="B6121" s="2">
         <v>44567</v>
@@ -87249,8 +87249,8 @@
       </c>
     </row>
     <row r="6122" spans="1:4">
-      <c r="A6122" t="s">
-        <v>8</v>
+      <c r="A6122">
+        <v>5</v>
       </c>
       <c r="B6122" s="2">
         <v>44567</v>
@@ -87263,8 +87263,8 @@
       </c>
     </row>
     <row r="6123" spans="1:4">
-      <c r="A6123" t="s">
-        <v>9</v>
+      <c r="A6123">
+        <v>6</v>
       </c>
       <c r="B6123" s="2">
         <v>44567</v>
@@ -87277,8 +87277,8 @@
       </c>
     </row>
     <row r="6124" spans="1:4">
-      <c r="A6124" t="s">
-        <v>10</v>
+      <c r="A6124">
+        <v>7</v>
       </c>
       <c r="B6124" s="2">
         <v>44567</v>
@@ -87291,8 +87291,8 @@
       </c>
     </row>
     <row r="6125" spans="1:4">
-      <c r="A6125" t="s">
-        <v>11</v>
+      <c r="A6125">
+        <v>8</v>
       </c>
       <c r="B6125" s="2">
         <v>44567</v>
@@ -87305,8 +87305,8 @@
       </c>
     </row>
     <row r="6126" spans="1:4">
-      <c r="A6126" t="s">
-        <v>12</v>
+      <c r="A6126">
+        <v>9</v>
       </c>
       <c r="B6126" s="2">
         <v>44567</v>
@@ -87319,8 +87319,8 @@
       </c>
     </row>
     <row r="6127" spans="1:4">
-      <c r="A6127" t="s">
-        <v>13</v>
+      <c r="A6127">
+        <v>10</v>
       </c>
       <c r="B6127" s="2">
         <v>44567</v>
@@ -87333,8 +87333,8 @@
       </c>
     </row>
     <row r="6128" spans="1:4">
-      <c r="A6128" t="s">
-        <v>14</v>
+      <c r="A6128">
+        <v>11</v>
       </c>
       <c r="B6128" s="2">
         <v>44567</v>
@@ -87347,8 +87347,8 @@
       </c>
     </row>
     <row r="6129" spans="1:4">
-      <c r="A6129" t="s">
-        <v>15</v>
+      <c r="A6129">
+        <v>12</v>
       </c>
       <c r="B6129" s="2">
         <v>44567</v>
@@ -87361,8 +87361,8 @@
       </c>
     </row>
     <row r="6130" spans="1:4">
-      <c r="A6130" t="s">
-        <v>16</v>
+      <c r="A6130">
+        <v>13</v>
       </c>
       <c r="B6130" s="2">
         <v>44567</v>
@@ -87375,8 +87375,8 @@
       </c>
     </row>
     <row r="6131" spans="1:4">
-      <c r="A6131" t="s">
-        <v>17</v>
+      <c r="A6131">
+        <v>14</v>
       </c>
       <c r="B6131" s="2">
         <v>44567</v>
@@ -87389,8 +87389,8 @@
       </c>
     </row>
     <row r="6132" spans="1:4">
-      <c r="A6132" t="s">
-        <v>18</v>
+      <c r="A6132">
+        <v>15</v>
       </c>
       <c r="B6132" s="2">
         <v>44567</v>
@@ -87403,8 +87403,8 @@
       </c>
     </row>
     <row r="6133" spans="1:4">
-      <c r="A6133" t="s">
-        <v>19</v>
+      <c r="A6133">
+        <v>16</v>
       </c>
       <c r="B6133" s="2">
         <v>44567</v>
@@ -87413,6 +87413,230 @@
         <v>390</v>
       </c>
       <c r="D6133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6134" spans="1:4">
+      <c r="A6134" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6134" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6134" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6135" spans="1:4">
+      <c r="A6135" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6135" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6135" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6136" spans="1:4">
+      <c r="A6136" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6136" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6136" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6137" spans="1:4">
+      <c r="A6137" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6137" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6137" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6138" spans="1:4">
+      <c r="A6138" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6138" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6138" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6139" spans="1:4">
+      <c r="A6139" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6139" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6139" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6140" spans="1:4">
+      <c r="A6140" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6140" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6140" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6141" spans="1:4">
+      <c r="A6141" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6141" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6141" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6142" spans="1:4">
+      <c r="A6142" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6142" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6142" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6143" spans="1:4">
+      <c r="A6143" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6143" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6143" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6144" spans="1:4">
+      <c r="A6144" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6144" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6144" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6145" spans="1:4">
+      <c r="A6145" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6145" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6145" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6146" spans="1:4">
+      <c r="A6146" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6146" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6146" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6147" spans="1:4">
+      <c r="A6147" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6147" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6147" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6148" spans="1:4">
+      <c r="A6148" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6148" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6148" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6149" spans="1:4">
+      <c r="A6149" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6149" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6149" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6149">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-10-2022 21-14-15
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11692" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11772" uniqueCount="393">
   <si>
     <t>Región</t>
   </si>
@@ -1188,6 +1188,12 @@
   <si>
     <t>2022-01-06</t>
   </si>
+  <si>
+    <t>2022-01-07</t>
+  </si>
+  <si>
+    <t>2022-01-08</t>
+  </si>
 </sst>
 </file>
 
@@ -1548,7 +1554,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6149"/>
+  <dimension ref="A1:D6197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -87417,8 +87423,8 @@
       </c>
     </row>
     <row r="6134" spans="1:4">
-      <c r="A6134" t="s">
-        <v>4</v>
+      <c r="A6134">
+        <v>1</v>
       </c>
       <c r="B6134" s="2">
         <v>44567</v>
@@ -87431,8 +87437,8 @@
       </c>
     </row>
     <row r="6135" spans="1:4">
-      <c r="A6135" t="s">
-        <v>5</v>
+      <c r="A6135">
+        <v>2</v>
       </c>
       <c r="B6135" s="2">
         <v>44567</v>
@@ -87445,8 +87451,8 @@
       </c>
     </row>
     <row r="6136" spans="1:4">
-      <c r="A6136" t="s">
-        <v>6</v>
+      <c r="A6136">
+        <v>3</v>
       </c>
       <c r="B6136" s="2">
         <v>44567</v>
@@ -87459,8 +87465,8 @@
       </c>
     </row>
     <row r="6137" spans="1:4">
-      <c r="A6137" t="s">
-        <v>7</v>
+      <c r="A6137">
+        <v>4</v>
       </c>
       <c r="B6137" s="2">
         <v>44567</v>
@@ -87473,8 +87479,8 @@
       </c>
     </row>
     <row r="6138" spans="1:4">
-      <c r="A6138" t="s">
-        <v>8</v>
+      <c r="A6138">
+        <v>5</v>
       </c>
       <c r="B6138" s="2">
         <v>44567</v>
@@ -87487,8 +87493,8 @@
       </c>
     </row>
     <row r="6139" spans="1:4">
-      <c r="A6139" t="s">
-        <v>9</v>
+      <c r="A6139">
+        <v>6</v>
       </c>
       <c r="B6139" s="2">
         <v>44567</v>
@@ -87501,8 +87507,8 @@
       </c>
     </row>
     <row r="6140" spans="1:4">
-      <c r="A6140" t="s">
-        <v>10</v>
+      <c r="A6140">
+        <v>7</v>
       </c>
       <c r="B6140" s="2">
         <v>44567</v>
@@ -87515,8 +87521,8 @@
       </c>
     </row>
     <row r="6141" spans="1:4">
-      <c r="A6141" t="s">
-        <v>11</v>
+      <c r="A6141">
+        <v>8</v>
       </c>
       <c r="B6141" s="2">
         <v>44567</v>
@@ -87529,8 +87535,8 @@
       </c>
     </row>
     <row r="6142" spans="1:4">
-      <c r="A6142" t="s">
-        <v>12</v>
+      <c r="A6142">
+        <v>9</v>
       </c>
       <c r="B6142" s="2">
         <v>44567</v>
@@ -87543,8 +87549,8 @@
       </c>
     </row>
     <row r="6143" spans="1:4">
-      <c r="A6143" t="s">
-        <v>13</v>
+      <c r="A6143">
+        <v>10</v>
       </c>
       <c r="B6143" s="2">
         <v>44567</v>
@@ -87557,8 +87563,8 @@
       </c>
     </row>
     <row r="6144" spans="1:4">
-      <c r="A6144" t="s">
-        <v>14</v>
+      <c r="A6144">
+        <v>11</v>
       </c>
       <c r="B6144" s="2">
         <v>44567</v>
@@ -87571,8 +87577,8 @@
       </c>
     </row>
     <row r="6145" spans="1:4">
-      <c r="A6145" t="s">
-        <v>15</v>
+      <c r="A6145">
+        <v>12</v>
       </c>
       <c r="B6145" s="2">
         <v>44567</v>
@@ -87585,8 +87591,8 @@
       </c>
     </row>
     <row r="6146" spans="1:4">
-      <c r="A6146" t="s">
-        <v>16</v>
+      <c r="A6146">
+        <v>13</v>
       </c>
       <c r="B6146" s="2">
         <v>44567</v>
@@ -87599,8 +87605,8 @@
       </c>
     </row>
     <row r="6147" spans="1:4">
-      <c r="A6147" t="s">
-        <v>17</v>
+      <c r="A6147">
+        <v>14</v>
       </c>
       <c r="B6147" s="2">
         <v>44567</v>
@@ -87613,8 +87619,8 @@
       </c>
     </row>
     <row r="6148" spans="1:4">
-      <c r="A6148" t="s">
-        <v>18</v>
+      <c r="A6148">
+        <v>15</v>
       </c>
       <c r="B6148" s="2">
         <v>44567</v>
@@ -87627,8 +87633,8 @@
       </c>
     </row>
     <row r="6149" spans="1:4">
-      <c r="A6149" t="s">
-        <v>19</v>
+      <c r="A6149">
+        <v>16</v>
       </c>
       <c r="B6149" s="2">
         <v>44567</v>
@@ -87637,6 +87643,678 @@
         <v>390</v>
       </c>
       <c r="D6149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6150" spans="1:4">
+      <c r="A6150" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6150" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6150" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6151" spans="1:4">
+      <c r="A6151" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6151" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6151" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6152" spans="1:4">
+      <c r="A6152" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6152" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6152" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6153" spans="1:4">
+      <c r="A6153" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6153" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6153" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6154" spans="1:4">
+      <c r="A6154" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6154" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6154" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6155" spans="1:4">
+      <c r="A6155" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6155" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6155" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6156" spans="1:4">
+      <c r="A6156" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6156" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6156" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6157" spans="1:4">
+      <c r="A6157" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6157" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6157" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6158" spans="1:4">
+      <c r="A6158" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6158" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6158" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6159" spans="1:4">
+      <c r="A6159" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6159" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6159" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6160" spans="1:4">
+      <c r="A6160" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6160" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6160" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6161" spans="1:4">
+      <c r="A6161" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6161" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6161" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6162" spans="1:4">
+      <c r="A6162" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6162" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6162" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6163" spans="1:4">
+      <c r="A6163" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6163" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6163" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6164" spans="1:4">
+      <c r="A6164" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6164" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6164" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6165" spans="1:4">
+      <c r="A6165" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6165" s="2">
+        <v>44567</v>
+      </c>
+      <c r="C6165" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6166" spans="1:4">
+      <c r="A6166" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6166" s="2">
+        <v>44568</v>
+      </c>
+      <c r="C6166" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6167" spans="1:4">
+      <c r="A6167" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6167" s="2">
+        <v>44568</v>
+      </c>
+      <c r="C6167" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6168" spans="1:4">
+      <c r="A6168" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6168" s="2">
+        <v>44568</v>
+      </c>
+      <c r="C6168" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6169" spans="1:4">
+      <c r="A6169" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6169" s="2">
+        <v>44568</v>
+      </c>
+      <c r="C6169" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6170" spans="1:4">
+      <c r="A6170" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6170" s="2">
+        <v>44568</v>
+      </c>
+      <c r="C6170" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6171" spans="1:4">
+      <c r="A6171" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6171" s="2">
+        <v>44568</v>
+      </c>
+      <c r="C6171" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6172" spans="1:4">
+      <c r="A6172" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6172" s="2">
+        <v>44568</v>
+      </c>
+      <c r="C6172" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6173" spans="1:4">
+      <c r="A6173" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6173" s="2">
+        <v>44568</v>
+      </c>
+      <c r="C6173" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6173">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6174" spans="1:4">
+      <c r="A6174" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6174" s="2">
+        <v>44568</v>
+      </c>
+      <c r="C6174" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6174">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6175" spans="1:4">
+      <c r="A6175" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6175" s="2">
+        <v>44568</v>
+      </c>
+      <c r="C6175" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6175">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6176" spans="1:4">
+      <c r="A6176" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6176" s="2">
+        <v>44568</v>
+      </c>
+      <c r="C6176" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6177" spans="1:4">
+      <c r="A6177" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6177" s="2">
+        <v>44568</v>
+      </c>
+      <c r="C6177" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6178" spans="1:4">
+      <c r="A6178" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6178" s="2">
+        <v>44568</v>
+      </c>
+      <c r="C6178" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6179" spans="1:4">
+      <c r="A6179" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6179" s="2">
+        <v>44568</v>
+      </c>
+      <c r="C6179" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6179">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6180" spans="1:4">
+      <c r="A6180" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6180" s="2">
+        <v>44568</v>
+      </c>
+      <c r="C6180" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6181" spans="1:4">
+      <c r="A6181" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6181" s="2">
+        <v>44568</v>
+      </c>
+      <c r="C6181" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6182" spans="1:4">
+      <c r="A6182" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6182" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6182" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6183" spans="1:4">
+      <c r="A6183" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6183" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6183" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6184" spans="1:4">
+      <c r="A6184" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6184" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6184" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6185" spans="1:4">
+      <c r="A6185" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6185" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6185" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6186" spans="1:4">
+      <c r="A6186" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6186" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6186" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6187" spans="1:4">
+      <c r="A6187" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6187" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6187" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6188" spans="1:4">
+      <c r="A6188" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6188" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6188" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6189" spans="1:4">
+      <c r="A6189" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6189" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6189" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6190" spans="1:4">
+      <c r="A6190" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6190" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6190" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6191" spans="1:4">
+      <c r="A6191" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6191" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6191" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6192" spans="1:4">
+      <c r="A6192" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6192" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6192" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6193" spans="1:4">
+      <c r="A6193" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6193" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6193" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6194" spans="1:4">
+      <c r="A6194" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6194" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6194" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6195" spans="1:4">
+      <c r="A6195" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6195" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6195" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6196" spans="1:4">
+      <c r="A6196" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6196" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6196" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6197" spans="1:4">
+      <c r="A6197" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6197" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6197" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6197">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-11-2022 21-45-17
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11772" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11788" uniqueCount="394">
   <si>
     <t>Región</t>
   </si>
@@ -1194,6 +1194,9 @@
   <si>
     <t>2022-01-08</t>
   </si>
+  <si>
+    <t>2022-01-09</t>
+  </si>
 </sst>
 </file>
 
@@ -1554,7 +1557,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6197"/>
+  <dimension ref="A1:D6229"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -87647,8 +87650,8 @@
       </c>
     </row>
     <row r="6150" spans="1:4">
-      <c r="A6150" t="s">
-        <v>4</v>
+      <c r="A6150">
+        <v>1</v>
       </c>
       <c r="B6150" s="2">
         <v>44567</v>
@@ -87661,8 +87664,8 @@
       </c>
     </row>
     <row r="6151" spans="1:4">
-      <c r="A6151" t="s">
-        <v>5</v>
+      <c r="A6151">
+        <v>2</v>
       </c>
       <c r="B6151" s="2">
         <v>44567</v>
@@ -87675,8 +87678,8 @@
       </c>
     </row>
     <row r="6152" spans="1:4">
-      <c r="A6152" t="s">
-        <v>6</v>
+      <c r="A6152">
+        <v>3</v>
       </c>
       <c r="B6152" s="2">
         <v>44567</v>
@@ -87689,8 +87692,8 @@
       </c>
     </row>
     <row r="6153" spans="1:4">
-      <c r="A6153" t="s">
-        <v>7</v>
+      <c r="A6153">
+        <v>4</v>
       </c>
       <c r="B6153" s="2">
         <v>44567</v>
@@ -87703,8 +87706,8 @@
       </c>
     </row>
     <row r="6154" spans="1:4">
-      <c r="A6154" t="s">
-        <v>8</v>
+      <c r="A6154">
+        <v>5</v>
       </c>
       <c r="B6154" s="2">
         <v>44567</v>
@@ -87717,8 +87720,8 @@
       </c>
     </row>
     <row r="6155" spans="1:4">
-      <c r="A6155" t="s">
-        <v>9</v>
+      <c r="A6155">
+        <v>6</v>
       </c>
       <c r="B6155" s="2">
         <v>44567</v>
@@ -87731,8 +87734,8 @@
       </c>
     </row>
     <row r="6156" spans="1:4">
-      <c r="A6156" t="s">
-        <v>10</v>
+      <c r="A6156">
+        <v>7</v>
       </c>
       <c r="B6156" s="2">
         <v>44567</v>
@@ -87745,8 +87748,8 @@
       </c>
     </row>
     <row r="6157" spans="1:4">
-      <c r="A6157" t="s">
-        <v>11</v>
+      <c r="A6157">
+        <v>8</v>
       </c>
       <c r="B6157" s="2">
         <v>44567</v>
@@ -87759,8 +87762,8 @@
       </c>
     </row>
     <row r="6158" spans="1:4">
-      <c r="A6158" t="s">
-        <v>12</v>
+      <c r="A6158">
+        <v>9</v>
       </c>
       <c r="B6158" s="2">
         <v>44567</v>
@@ -87773,8 +87776,8 @@
       </c>
     </row>
     <row r="6159" spans="1:4">
-      <c r="A6159" t="s">
-        <v>13</v>
+      <c r="A6159">
+        <v>10</v>
       </c>
       <c r="B6159" s="2">
         <v>44567</v>
@@ -87787,8 +87790,8 @@
       </c>
     </row>
     <row r="6160" spans="1:4">
-      <c r="A6160" t="s">
-        <v>14</v>
+      <c r="A6160">
+        <v>11</v>
       </c>
       <c r="B6160" s="2">
         <v>44567</v>
@@ -87801,8 +87804,8 @@
       </c>
     </row>
     <row r="6161" spans="1:4">
-      <c r="A6161" t="s">
-        <v>15</v>
+      <c r="A6161">
+        <v>12</v>
       </c>
       <c r="B6161" s="2">
         <v>44567</v>
@@ -87815,8 +87818,8 @@
       </c>
     </row>
     <row r="6162" spans="1:4">
-      <c r="A6162" t="s">
-        <v>16</v>
+      <c r="A6162">
+        <v>13</v>
       </c>
       <c r="B6162" s="2">
         <v>44567</v>
@@ -87829,8 +87832,8 @@
       </c>
     </row>
     <row r="6163" spans="1:4">
-      <c r="A6163" t="s">
-        <v>17</v>
+      <c r="A6163">
+        <v>14</v>
       </c>
       <c r="B6163" s="2">
         <v>44567</v>
@@ -87843,8 +87846,8 @@
       </c>
     </row>
     <row r="6164" spans="1:4">
-      <c r="A6164" t="s">
-        <v>18</v>
+      <c r="A6164">
+        <v>15</v>
       </c>
       <c r="B6164" s="2">
         <v>44567</v>
@@ -87857,8 +87860,8 @@
       </c>
     </row>
     <row r="6165" spans="1:4">
-      <c r="A6165" t="s">
-        <v>19</v>
+      <c r="A6165">
+        <v>16</v>
       </c>
       <c r="B6165" s="2">
         <v>44567</v>
@@ -87871,8 +87874,8 @@
       </c>
     </row>
     <row r="6166" spans="1:4">
-      <c r="A6166" t="s">
-        <v>4</v>
+      <c r="A6166">
+        <v>1</v>
       </c>
       <c r="B6166" s="2">
         <v>44568</v>
@@ -87885,8 +87888,8 @@
       </c>
     </row>
     <row r="6167" spans="1:4">
-      <c r="A6167" t="s">
-        <v>5</v>
+      <c r="A6167">
+        <v>2</v>
       </c>
       <c r="B6167" s="2">
         <v>44568</v>
@@ -87899,8 +87902,8 @@
       </c>
     </row>
     <row r="6168" spans="1:4">
-      <c r="A6168" t="s">
-        <v>6</v>
+      <c r="A6168">
+        <v>3</v>
       </c>
       <c r="B6168" s="2">
         <v>44568</v>
@@ -87913,8 +87916,8 @@
       </c>
     </row>
     <row r="6169" spans="1:4">
-      <c r="A6169" t="s">
-        <v>7</v>
+      <c r="A6169">
+        <v>4</v>
       </c>
       <c r="B6169" s="2">
         <v>44568</v>
@@ -87927,8 +87930,8 @@
       </c>
     </row>
     <row r="6170" spans="1:4">
-      <c r="A6170" t="s">
-        <v>8</v>
+      <c r="A6170">
+        <v>5</v>
       </c>
       <c r="B6170" s="2">
         <v>44568</v>
@@ -87941,8 +87944,8 @@
       </c>
     </row>
     <row r="6171" spans="1:4">
-      <c r="A6171" t="s">
-        <v>9</v>
+      <c r="A6171">
+        <v>6</v>
       </c>
       <c r="B6171" s="2">
         <v>44568</v>
@@ -87955,8 +87958,8 @@
       </c>
     </row>
     <row r="6172" spans="1:4">
-      <c r="A6172" t="s">
-        <v>10</v>
+      <c r="A6172">
+        <v>7</v>
       </c>
       <c r="B6172" s="2">
         <v>44568</v>
@@ -87969,8 +87972,8 @@
       </c>
     </row>
     <row r="6173" spans="1:4">
-      <c r="A6173" t="s">
-        <v>11</v>
+      <c r="A6173">
+        <v>8</v>
       </c>
       <c r="B6173" s="2">
         <v>44568</v>
@@ -87983,8 +87986,8 @@
       </c>
     </row>
     <row r="6174" spans="1:4">
-      <c r="A6174" t="s">
-        <v>12</v>
+      <c r="A6174">
+        <v>9</v>
       </c>
       <c r="B6174" s="2">
         <v>44568</v>
@@ -87997,8 +88000,8 @@
       </c>
     </row>
     <row r="6175" spans="1:4">
-      <c r="A6175" t="s">
-        <v>13</v>
+      <c r="A6175">
+        <v>10</v>
       </c>
       <c r="B6175" s="2">
         <v>44568</v>
@@ -88011,8 +88014,8 @@
       </c>
     </row>
     <row r="6176" spans="1:4">
-      <c r="A6176" t="s">
-        <v>14</v>
+      <c r="A6176">
+        <v>11</v>
       </c>
       <c r="B6176" s="2">
         <v>44568</v>
@@ -88025,8 +88028,8 @@
       </c>
     </row>
     <row r="6177" spans="1:4">
-      <c r="A6177" t="s">
-        <v>15</v>
+      <c r="A6177">
+        <v>12</v>
       </c>
       <c r="B6177" s="2">
         <v>44568</v>
@@ -88039,8 +88042,8 @@
       </c>
     </row>
     <row r="6178" spans="1:4">
-      <c r="A6178" t="s">
-        <v>16</v>
+      <c r="A6178">
+        <v>13</v>
       </c>
       <c r="B6178" s="2">
         <v>44568</v>
@@ -88053,8 +88056,8 @@
       </c>
     </row>
     <row r="6179" spans="1:4">
-      <c r="A6179" t="s">
-        <v>17</v>
+      <c r="A6179">
+        <v>14</v>
       </c>
       <c r="B6179" s="2">
         <v>44568</v>
@@ -88067,8 +88070,8 @@
       </c>
     </row>
     <row r="6180" spans="1:4">
-      <c r="A6180" t="s">
-        <v>18</v>
+      <c r="A6180">
+        <v>15</v>
       </c>
       <c r="B6180" s="2">
         <v>44568</v>
@@ -88081,8 +88084,8 @@
       </c>
     </row>
     <row r="6181" spans="1:4">
-      <c r="A6181" t="s">
-        <v>19</v>
+      <c r="A6181">
+        <v>16</v>
       </c>
       <c r="B6181" s="2">
         <v>44568</v>
@@ -88095,8 +88098,8 @@
       </c>
     </row>
     <row r="6182" spans="1:4">
-      <c r="A6182" t="s">
-        <v>4</v>
+      <c r="A6182">
+        <v>1</v>
       </c>
       <c r="B6182" s="2">
         <v>44569</v>
@@ -88109,8 +88112,8 @@
       </c>
     </row>
     <row r="6183" spans="1:4">
-      <c r="A6183" t="s">
-        <v>5</v>
+      <c r="A6183">
+        <v>2</v>
       </c>
       <c r="B6183" s="2">
         <v>44569</v>
@@ -88123,8 +88126,8 @@
       </c>
     </row>
     <row r="6184" spans="1:4">
-      <c r="A6184" t="s">
-        <v>6</v>
+      <c r="A6184">
+        <v>3</v>
       </c>
       <c r="B6184" s="2">
         <v>44569</v>
@@ -88137,8 +88140,8 @@
       </c>
     </row>
     <row r="6185" spans="1:4">
-      <c r="A6185" t="s">
-        <v>7</v>
+      <c r="A6185">
+        <v>4</v>
       </c>
       <c r="B6185" s="2">
         <v>44569</v>
@@ -88151,8 +88154,8 @@
       </c>
     </row>
     <row r="6186" spans="1:4">
-      <c r="A6186" t="s">
-        <v>8</v>
+      <c r="A6186">
+        <v>5</v>
       </c>
       <c r="B6186" s="2">
         <v>44569</v>
@@ -88165,8 +88168,8 @@
       </c>
     </row>
     <row r="6187" spans="1:4">
-      <c r="A6187" t="s">
-        <v>9</v>
+      <c r="A6187">
+        <v>6</v>
       </c>
       <c r="B6187" s="2">
         <v>44569</v>
@@ -88179,8 +88182,8 @@
       </c>
     </row>
     <row r="6188" spans="1:4">
-      <c r="A6188" t="s">
-        <v>10</v>
+      <c r="A6188">
+        <v>7</v>
       </c>
       <c r="B6188" s="2">
         <v>44569</v>
@@ -88193,8 +88196,8 @@
       </c>
     </row>
     <row r="6189" spans="1:4">
-      <c r="A6189" t="s">
-        <v>11</v>
+      <c r="A6189">
+        <v>8</v>
       </c>
       <c r="B6189" s="2">
         <v>44569</v>
@@ -88207,8 +88210,8 @@
       </c>
     </row>
     <row r="6190" spans="1:4">
-      <c r="A6190" t="s">
-        <v>12</v>
+      <c r="A6190">
+        <v>9</v>
       </c>
       <c r="B6190" s="2">
         <v>44569</v>
@@ -88221,8 +88224,8 @@
       </c>
     </row>
     <row r="6191" spans="1:4">
-      <c r="A6191" t="s">
-        <v>13</v>
+      <c r="A6191">
+        <v>10</v>
       </c>
       <c r="B6191" s="2">
         <v>44569</v>
@@ -88235,8 +88238,8 @@
       </c>
     </row>
     <row r="6192" spans="1:4">
-      <c r="A6192" t="s">
-        <v>14</v>
+      <c r="A6192">
+        <v>11</v>
       </c>
       <c r="B6192" s="2">
         <v>44569</v>
@@ -88249,8 +88252,8 @@
       </c>
     </row>
     <row r="6193" spans="1:4">
-      <c r="A6193" t="s">
-        <v>15</v>
+      <c r="A6193">
+        <v>12</v>
       </c>
       <c r="B6193" s="2">
         <v>44569</v>
@@ -88263,8 +88266,8 @@
       </c>
     </row>
     <row r="6194" spans="1:4">
-      <c r="A6194" t="s">
-        <v>16</v>
+      <c r="A6194">
+        <v>13</v>
       </c>
       <c r="B6194" s="2">
         <v>44569</v>
@@ -88277,8 +88280,8 @@
       </c>
     </row>
     <row r="6195" spans="1:4">
-      <c r="A6195" t="s">
-        <v>17</v>
+      <c r="A6195">
+        <v>14</v>
       </c>
       <c r="B6195" s="2">
         <v>44569</v>
@@ -88291,8 +88294,8 @@
       </c>
     </row>
     <row r="6196" spans="1:4">
-      <c r="A6196" t="s">
-        <v>18</v>
+      <c r="A6196">
+        <v>15</v>
       </c>
       <c r="B6196" s="2">
         <v>44569</v>
@@ -88305,8 +88308,8 @@
       </c>
     </row>
     <row r="6197" spans="1:4">
-      <c r="A6197" t="s">
-        <v>19</v>
+      <c r="A6197">
+        <v>16</v>
       </c>
       <c r="B6197" s="2">
         <v>44569</v>
@@ -88315,6 +88318,454 @@
         <v>392</v>
       </c>
       <c r="D6197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6198" spans="1:4">
+      <c r="A6198" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6198" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6198" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6199" spans="1:4">
+      <c r="A6199" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6199" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6199" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6200" spans="1:4">
+      <c r="A6200" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6200" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6200" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6201" spans="1:4">
+      <c r="A6201" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6201" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6201" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6202" spans="1:4">
+      <c r="A6202" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6202" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6202" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6203" spans="1:4">
+      <c r="A6203" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6203" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6203" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6204" spans="1:4">
+      <c r="A6204" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6204" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6204" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6204">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6205" spans="1:4">
+      <c r="A6205" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6205" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6205" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6206" spans="1:4">
+      <c r="A6206" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6206" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6206" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6207" spans="1:4">
+      <c r="A6207" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6207" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6207" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6208" spans="1:4">
+      <c r="A6208" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6208" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6208" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6209" spans="1:4">
+      <c r="A6209" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6209" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6209" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6210" spans="1:4">
+      <c r="A6210" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6210" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6210" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6211" spans="1:4">
+      <c r="A6211" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6211" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6211" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6212" spans="1:4">
+      <c r="A6212" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6212" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6212" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6213" spans="1:4">
+      <c r="A6213" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6213" s="2">
+        <v>44569</v>
+      </c>
+      <c r="C6213" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6214" spans="1:4">
+      <c r="A6214" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6214" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6214" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6215" spans="1:4">
+      <c r="A6215" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6215" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6215" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6215">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6216" spans="1:4">
+      <c r="A6216" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6216" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6216" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6217" spans="1:4">
+      <c r="A6217" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6217" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6217" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6218" spans="1:4">
+      <c r="A6218" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6218" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6218" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6219" spans="1:4">
+      <c r="A6219" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6219" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6219" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6220" spans="1:4">
+      <c r="A6220" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6220" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6220" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6221" spans="1:4">
+      <c r="A6221" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6221" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6221" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6222" spans="1:4">
+      <c r="A6222" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6222" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6222" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6223" spans="1:4">
+      <c r="A6223" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6223" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6223" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6224" spans="1:4">
+      <c r="A6224" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6224" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6224" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6225" spans="1:4">
+      <c r="A6225" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6225" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6225" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6226" spans="1:4">
+      <c r="A6226" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6226" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6226" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6227" spans="1:4">
+      <c r="A6227" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6227" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6227" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6228" spans="1:4">
+      <c r="A6228" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6228" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6228" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6229" spans="1:4">
+      <c r="A6229" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6229" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6229" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6229">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-17-2022 16-55-40
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11788" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11980" uniqueCount="400">
   <si>
     <t>Región</t>
   </si>
@@ -1197,6 +1197,24 @@
   <si>
     <t>2022-01-09</t>
   </si>
+  <si>
+    <t>2022-01-10</t>
+  </si>
+  <si>
+    <t>2022-01-11</t>
+  </si>
+  <si>
+    <t>2022-01-12</t>
+  </si>
+  <si>
+    <t>2022-01-13</t>
+  </si>
+  <si>
+    <t>2022-01-14</t>
+  </si>
+  <si>
+    <t>2022-01-15</t>
+  </si>
 </sst>
 </file>
 
@@ -1557,7 +1575,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6229"/>
+  <dimension ref="A1:D6341"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -88322,8 +88340,8 @@
       </c>
     </row>
     <row r="6198" spans="1:4">
-      <c r="A6198" t="s">
-        <v>4</v>
+      <c r="A6198">
+        <v>1</v>
       </c>
       <c r="B6198" s="2">
         <v>44569</v>
@@ -88336,8 +88354,8 @@
       </c>
     </row>
     <row r="6199" spans="1:4">
-      <c r="A6199" t="s">
-        <v>5</v>
+      <c r="A6199">
+        <v>2</v>
       </c>
       <c r="B6199" s="2">
         <v>44569</v>
@@ -88350,8 +88368,8 @@
       </c>
     </row>
     <row r="6200" spans="1:4">
-      <c r="A6200" t="s">
-        <v>6</v>
+      <c r="A6200">
+        <v>3</v>
       </c>
       <c r="B6200" s="2">
         <v>44569</v>
@@ -88364,8 +88382,8 @@
       </c>
     </row>
     <row r="6201" spans="1:4">
-      <c r="A6201" t="s">
-        <v>7</v>
+      <c r="A6201">
+        <v>4</v>
       </c>
       <c r="B6201" s="2">
         <v>44569</v>
@@ -88378,8 +88396,8 @@
       </c>
     </row>
     <row r="6202" spans="1:4">
-      <c r="A6202" t="s">
-        <v>8</v>
+      <c r="A6202">
+        <v>5</v>
       </c>
       <c r="B6202" s="2">
         <v>44569</v>
@@ -88392,8 +88410,8 @@
       </c>
     </row>
     <row r="6203" spans="1:4">
-      <c r="A6203" t="s">
-        <v>9</v>
+      <c r="A6203">
+        <v>6</v>
       </c>
       <c r="B6203" s="2">
         <v>44569</v>
@@ -88406,8 +88424,8 @@
       </c>
     </row>
     <row r="6204" spans="1:4">
-      <c r="A6204" t="s">
-        <v>10</v>
+      <c r="A6204">
+        <v>7</v>
       </c>
       <c r="B6204" s="2">
         <v>44569</v>
@@ -88420,8 +88438,8 @@
       </c>
     </row>
     <row r="6205" spans="1:4">
-      <c r="A6205" t="s">
-        <v>11</v>
+      <c r="A6205">
+        <v>8</v>
       </c>
       <c r="B6205" s="2">
         <v>44569</v>
@@ -88434,8 +88452,8 @@
       </c>
     </row>
     <row r="6206" spans="1:4">
-      <c r="A6206" t="s">
-        <v>12</v>
+      <c r="A6206">
+        <v>9</v>
       </c>
       <c r="B6206" s="2">
         <v>44569</v>
@@ -88448,8 +88466,8 @@
       </c>
     </row>
     <row r="6207" spans="1:4">
-      <c r="A6207" t="s">
-        <v>13</v>
+      <c r="A6207">
+        <v>10</v>
       </c>
       <c r="B6207" s="2">
         <v>44569</v>
@@ -88462,8 +88480,8 @@
       </c>
     </row>
     <row r="6208" spans="1:4">
-      <c r="A6208" t="s">
-        <v>14</v>
+      <c r="A6208">
+        <v>11</v>
       </c>
       <c r="B6208" s="2">
         <v>44569</v>
@@ -88476,8 +88494,8 @@
       </c>
     </row>
     <row r="6209" spans="1:4">
-      <c r="A6209" t="s">
-        <v>15</v>
+      <c r="A6209">
+        <v>12</v>
       </c>
       <c r="B6209" s="2">
         <v>44569</v>
@@ -88490,8 +88508,8 @@
       </c>
     </row>
     <row r="6210" spans="1:4">
-      <c r="A6210" t="s">
-        <v>16</v>
+      <c r="A6210">
+        <v>13</v>
       </c>
       <c r="B6210" s="2">
         <v>44569</v>
@@ -88504,8 +88522,8 @@
       </c>
     </row>
     <row r="6211" spans="1:4">
-      <c r="A6211" t="s">
-        <v>17</v>
+      <c r="A6211">
+        <v>14</v>
       </c>
       <c r="B6211" s="2">
         <v>44569</v>
@@ -88518,8 +88536,8 @@
       </c>
     </row>
     <row r="6212" spans="1:4">
-      <c r="A6212" t="s">
-        <v>18</v>
+      <c r="A6212">
+        <v>15</v>
       </c>
       <c r="B6212" s="2">
         <v>44569</v>
@@ -88532,8 +88550,8 @@
       </c>
     </row>
     <row r="6213" spans="1:4">
-      <c r="A6213" t="s">
-        <v>19</v>
+      <c r="A6213">
+        <v>16</v>
       </c>
       <c r="B6213" s="2">
         <v>44569</v>
@@ -88546,8 +88564,8 @@
       </c>
     </row>
     <row r="6214" spans="1:4">
-      <c r="A6214" t="s">
-        <v>4</v>
+      <c r="A6214">
+        <v>1</v>
       </c>
       <c r="B6214" s="2">
         <v>44570</v>
@@ -88560,8 +88578,8 @@
       </c>
     </row>
     <row r="6215" spans="1:4">
-      <c r="A6215" t="s">
-        <v>5</v>
+      <c r="A6215">
+        <v>2</v>
       </c>
       <c r="B6215" s="2">
         <v>44570</v>
@@ -88574,8 +88592,8 @@
       </c>
     </row>
     <row r="6216" spans="1:4">
-      <c r="A6216" t="s">
-        <v>6</v>
+      <c r="A6216">
+        <v>3</v>
       </c>
       <c r="B6216" s="2">
         <v>44570</v>
@@ -88588,8 +88606,8 @@
       </c>
     </row>
     <row r="6217" spans="1:4">
-      <c r="A6217" t="s">
-        <v>7</v>
+      <c r="A6217">
+        <v>4</v>
       </c>
       <c r="B6217" s="2">
         <v>44570</v>
@@ -88602,8 +88620,8 @@
       </c>
     </row>
     <row r="6218" spans="1:4">
-      <c r="A6218" t="s">
-        <v>8</v>
+      <c r="A6218">
+        <v>5</v>
       </c>
       <c r="B6218" s="2">
         <v>44570</v>
@@ -88616,8 +88634,8 @@
       </c>
     </row>
     <row r="6219" spans="1:4">
-      <c r="A6219" t="s">
-        <v>9</v>
+      <c r="A6219">
+        <v>6</v>
       </c>
       <c r="B6219" s="2">
         <v>44570</v>
@@ -88630,8 +88648,8 @@
       </c>
     </row>
     <row r="6220" spans="1:4">
-      <c r="A6220" t="s">
-        <v>10</v>
+      <c r="A6220">
+        <v>7</v>
       </c>
       <c r="B6220" s="2">
         <v>44570</v>
@@ -88644,8 +88662,8 @@
       </c>
     </row>
     <row r="6221" spans="1:4">
-      <c r="A6221" t="s">
-        <v>11</v>
+      <c r="A6221">
+        <v>8</v>
       </c>
       <c r="B6221" s="2">
         <v>44570</v>
@@ -88658,8 +88676,8 @@
       </c>
     </row>
     <row r="6222" spans="1:4">
-      <c r="A6222" t="s">
-        <v>12</v>
+      <c r="A6222">
+        <v>9</v>
       </c>
       <c r="B6222" s="2">
         <v>44570</v>
@@ -88672,8 +88690,8 @@
       </c>
     </row>
     <row r="6223" spans="1:4">
-      <c r="A6223" t="s">
-        <v>13</v>
+      <c r="A6223">
+        <v>10</v>
       </c>
       <c r="B6223" s="2">
         <v>44570</v>
@@ -88686,8 +88704,8 @@
       </c>
     </row>
     <row r="6224" spans="1:4">
-      <c r="A6224" t="s">
-        <v>14</v>
+      <c r="A6224">
+        <v>11</v>
       </c>
       <c r="B6224" s="2">
         <v>44570</v>
@@ -88700,8 +88718,8 @@
       </c>
     </row>
     <row r="6225" spans="1:4">
-      <c r="A6225" t="s">
-        <v>15</v>
+      <c r="A6225">
+        <v>12</v>
       </c>
       <c r="B6225" s="2">
         <v>44570</v>
@@ -88714,8 +88732,8 @@
       </c>
     </row>
     <row r="6226" spans="1:4">
-      <c r="A6226" t="s">
-        <v>16</v>
+      <c r="A6226">
+        <v>13</v>
       </c>
       <c r="B6226" s="2">
         <v>44570</v>
@@ -88728,8 +88746,8 @@
       </c>
     </row>
     <row r="6227" spans="1:4">
-      <c r="A6227" t="s">
-        <v>17</v>
+      <c r="A6227">
+        <v>14</v>
       </c>
       <c r="B6227" s="2">
         <v>44570</v>
@@ -88742,8 +88760,8 @@
       </c>
     </row>
     <row r="6228" spans="1:4">
-      <c r="A6228" t="s">
-        <v>18</v>
+      <c r="A6228">
+        <v>15</v>
       </c>
       <c r="B6228" s="2">
         <v>44570</v>
@@ -88756,8 +88774,8 @@
       </c>
     </row>
     <row r="6229" spans="1:4">
-      <c r="A6229" t="s">
-        <v>19</v>
+      <c r="A6229">
+        <v>16</v>
       </c>
       <c r="B6229" s="2">
         <v>44570</v>
@@ -88766,6 +88784,1574 @@
         <v>393</v>
       </c>
       <c r="D6229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6230" spans="1:4">
+      <c r="A6230" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6230" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6230" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6231" spans="1:4">
+      <c r="A6231" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6231" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6231" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6231">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6232" spans="1:4">
+      <c r="A6232" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6232" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6232" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6233" spans="1:4">
+      <c r="A6233" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6233" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6233" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6233">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6234" spans="1:4">
+      <c r="A6234" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6234" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6234" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6235" spans="1:4">
+      <c r="A6235" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6235" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6235" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6236" spans="1:4">
+      <c r="A6236" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6236" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6236" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6236">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6237" spans="1:4">
+      <c r="A6237" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6237" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6237" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6237">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6238" spans="1:4">
+      <c r="A6238" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6238" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6238" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6239" spans="1:4">
+      <c r="A6239" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6239" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6239" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6240" spans="1:4">
+      <c r="A6240" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6240" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6240" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6241" spans="1:4">
+      <c r="A6241" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6241" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6241" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6242" spans="1:4">
+      <c r="A6242" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6242" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6242" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6243" spans="1:4">
+      <c r="A6243" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6243" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6243" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6243">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6244" spans="1:4">
+      <c r="A6244" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6244" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6244" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6244">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6245" spans="1:4">
+      <c r="A6245" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6245" s="2">
+        <v>44570</v>
+      </c>
+      <c r="C6245" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6246" spans="1:4">
+      <c r="A6246" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6246" s="2">
+        <v>44571</v>
+      </c>
+      <c r="C6246" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6247" spans="1:4">
+      <c r="A6247" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6247" s="2">
+        <v>44571</v>
+      </c>
+      <c r="C6247" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6248" spans="1:4">
+      <c r="A6248" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6248" s="2">
+        <v>44571</v>
+      </c>
+      <c r="C6248" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6248">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6249" spans="1:4">
+      <c r="A6249" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6249" s="2">
+        <v>44571</v>
+      </c>
+      <c r="C6249" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6250" spans="1:4">
+      <c r="A6250" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6250" s="2">
+        <v>44571</v>
+      </c>
+      <c r="C6250" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6251" spans="1:4">
+      <c r="A6251" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6251" s="2">
+        <v>44571</v>
+      </c>
+      <c r="C6251" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6252" spans="1:4">
+      <c r="A6252" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6252" s="2">
+        <v>44571</v>
+      </c>
+      <c r="C6252" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6253" spans="1:4">
+      <c r="A6253" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6253" s="2">
+        <v>44571</v>
+      </c>
+      <c r="C6253" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6253">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6254" spans="1:4">
+      <c r="A6254" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6254" s="2">
+        <v>44571</v>
+      </c>
+      <c r="C6254" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6255" spans="1:4">
+      <c r="A6255" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6255" s="2">
+        <v>44571</v>
+      </c>
+      <c r="C6255" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6256" spans="1:4">
+      <c r="A6256" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6256" s="2">
+        <v>44571</v>
+      </c>
+      <c r="C6256" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6256">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6257" spans="1:4">
+      <c r="A6257" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6257" s="2">
+        <v>44571</v>
+      </c>
+      <c r="C6257" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6258" spans="1:4">
+      <c r="A6258" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6258" s="2">
+        <v>44571</v>
+      </c>
+      <c r="C6258" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6259" spans="1:4">
+      <c r="A6259" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6259" s="2">
+        <v>44571</v>
+      </c>
+      <c r="C6259" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6259">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6260" spans="1:4">
+      <c r="A6260" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6260" s="2">
+        <v>44571</v>
+      </c>
+      <c r="C6260" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6260">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6261" spans="1:4">
+      <c r="A6261" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6261" s="2">
+        <v>44571</v>
+      </c>
+      <c r="C6261" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6261">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6262" spans="1:4">
+      <c r="A6262" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6262" s="2">
+        <v>44572</v>
+      </c>
+      <c r="C6262" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6262">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6263" spans="1:4">
+      <c r="A6263" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6263" s="2">
+        <v>44572</v>
+      </c>
+      <c r="C6263" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6263">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6264" spans="1:4">
+      <c r="A6264" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6264" s="2">
+        <v>44572</v>
+      </c>
+      <c r="C6264" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6264">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6265" spans="1:4">
+      <c r="A6265" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6265" s="2">
+        <v>44572</v>
+      </c>
+      <c r="C6265" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6266" spans="1:4">
+      <c r="A6266" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6266" s="2">
+        <v>44572</v>
+      </c>
+      <c r="C6266" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6266">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6267" spans="1:4">
+      <c r="A6267" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6267" s="2">
+        <v>44572</v>
+      </c>
+      <c r="C6267" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6267">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6268" spans="1:4">
+      <c r="A6268" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6268" s="2">
+        <v>44572</v>
+      </c>
+      <c r="C6268" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6268">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6269" spans="1:4">
+      <c r="A6269" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6269" s="2">
+        <v>44572</v>
+      </c>
+      <c r="C6269" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6269">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6270" spans="1:4">
+      <c r="A6270" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6270" s="2">
+        <v>44572</v>
+      </c>
+      <c r="C6270" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6270">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6271" spans="1:4">
+      <c r="A6271" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6271" s="2">
+        <v>44572</v>
+      </c>
+      <c r="C6271" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6271">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6272" spans="1:4">
+      <c r="A6272" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6272" s="2">
+        <v>44572</v>
+      </c>
+      <c r="C6272" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6272">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6273" spans="1:4">
+      <c r="A6273" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6273" s="2">
+        <v>44572</v>
+      </c>
+      <c r="C6273" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6273">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6274" spans="1:4">
+      <c r="A6274" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6274" s="2">
+        <v>44572</v>
+      </c>
+      <c r="C6274" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6274">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6275" spans="1:4">
+      <c r="A6275" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6275" s="2">
+        <v>44572</v>
+      </c>
+      <c r="C6275" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6275">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6276" spans="1:4">
+      <c r="A6276" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6276" s="2">
+        <v>44572</v>
+      </c>
+      <c r="C6276" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6276">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6277" spans="1:4">
+      <c r="A6277" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6277" s="2">
+        <v>44572</v>
+      </c>
+      <c r="C6277" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6277">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6278" spans="1:4">
+      <c r="A6278" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6278" s="2">
+        <v>44573</v>
+      </c>
+      <c r="C6278" t="s">
+        <v>396</v>
+      </c>
+      <c r="D6278">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6279" spans="1:4">
+      <c r="A6279" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6279" s="2">
+        <v>44573</v>
+      </c>
+      <c r="C6279" t="s">
+        <v>396</v>
+      </c>
+      <c r="D6279">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6280" spans="1:4">
+      <c r="A6280" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6280" s="2">
+        <v>44573</v>
+      </c>
+      <c r="C6280" t="s">
+        <v>396</v>
+      </c>
+      <c r="D6280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6281" spans="1:4">
+      <c r="A6281" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6281" s="2">
+        <v>44573</v>
+      </c>
+      <c r="C6281" t="s">
+        <v>396</v>
+      </c>
+      <c r="D6281">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6282" spans="1:4">
+      <c r="A6282" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6282" s="2">
+        <v>44573</v>
+      </c>
+      <c r="C6282" t="s">
+        <v>396</v>
+      </c>
+      <c r="D6282">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6283" spans="1:4">
+      <c r="A6283" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6283" s="2">
+        <v>44573</v>
+      </c>
+      <c r="C6283" t="s">
+        <v>396</v>
+      </c>
+      <c r="D6283">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6284" spans="1:4">
+      <c r="A6284" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6284" s="2">
+        <v>44573</v>
+      </c>
+      <c r="C6284" t="s">
+        <v>396</v>
+      </c>
+      <c r="D6284">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6285" spans="1:4">
+      <c r="A6285" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6285" s="2">
+        <v>44573</v>
+      </c>
+      <c r="C6285" t="s">
+        <v>396</v>
+      </c>
+      <c r="D6285">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6286" spans="1:4">
+      <c r="A6286" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6286" s="2">
+        <v>44573</v>
+      </c>
+      <c r="C6286" t="s">
+        <v>396</v>
+      </c>
+      <c r="D6286">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6287" spans="1:4">
+      <c r="A6287" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6287" s="2">
+        <v>44573</v>
+      </c>
+      <c r="C6287" t="s">
+        <v>396</v>
+      </c>
+      <c r="D6287">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6288" spans="1:4">
+      <c r="A6288" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6288" s="2">
+        <v>44573</v>
+      </c>
+      <c r="C6288" t="s">
+        <v>396</v>
+      </c>
+      <c r="D6288">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6289" spans="1:4">
+      <c r="A6289" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6289" s="2">
+        <v>44573</v>
+      </c>
+      <c r="C6289" t="s">
+        <v>396</v>
+      </c>
+      <c r="D6289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6290" spans="1:4">
+      <c r="A6290" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6290" s="2">
+        <v>44573</v>
+      </c>
+      <c r="C6290" t="s">
+        <v>396</v>
+      </c>
+      <c r="D6290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6291" spans="1:4">
+      <c r="A6291" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6291" s="2">
+        <v>44573</v>
+      </c>
+      <c r="C6291" t="s">
+        <v>396</v>
+      </c>
+      <c r="D6291">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6292" spans="1:4">
+      <c r="A6292" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6292" s="2">
+        <v>44573</v>
+      </c>
+      <c r="C6292" t="s">
+        <v>396</v>
+      </c>
+      <c r="D6292">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6293" spans="1:4">
+      <c r="A6293" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6293" s="2">
+        <v>44573</v>
+      </c>
+      <c r="C6293" t="s">
+        <v>396</v>
+      </c>
+      <c r="D6293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6294" spans="1:4">
+      <c r="A6294" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6294" s="2">
+        <v>44574</v>
+      </c>
+      <c r="C6294" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6295" spans="1:4">
+      <c r="A6295" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6295" s="2">
+        <v>44574</v>
+      </c>
+      <c r="C6295" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6295">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6296" spans="1:4">
+      <c r="A6296" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6296" s="2">
+        <v>44574</v>
+      </c>
+      <c r="C6296" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6296">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6297" spans="1:4">
+      <c r="A6297" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6297" s="2">
+        <v>44574</v>
+      </c>
+      <c r="C6297" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6298" spans="1:4">
+      <c r="A6298" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6298" s="2">
+        <v>44574</v>
+      </c>
+      <c r="C6298" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6299" spans="1:4">
+      <c r="A6299" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6299" s="2">
+        <v>44574</v>
+      </c>
+      <c r="C6299" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6299">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6300" spans="1:4">
+      <c r="A6300" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6300" s="2">
+        <v>44574</v>
+      </c>
+      <c r="C6300" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6300">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6301" spans="1:4">
+      <c r="A6301" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6301" s="2">
+        <v>44574</v>
+      </c>
+      <c r="C6301" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6301">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6302" spans="1:4">
+      <c r="A6302" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6302" s="2">
+        <v>44574</v>
+      </c>
+      <c r="C6302" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6302">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6303" spans="1:4">
+      <c r="A6303" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6303" s="2">
+        <v>44574</v>
+      </c>
+      <c r="C6303" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6303">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6304" spans="1:4">
+      <c r="A6304" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6304" s="2">
+        <v>44574</v>
+      </c>
+      <c r="C6304" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6304">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6305" spans="1:4">
+      <c r="A6305" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6305" s="2">
+        <v>44574</v>
+      </c>
+      <c r="C6305" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6305">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6306" spans="1:4">
+      <c r="A6306" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6306" s="2">
+        <v>44574</v>
+      </c>
+      <c r="C6306" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6306">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6307" spans="1:4">
+      <c r="A6307" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6307" s="2">
+        <v>44574</v>
+      </c>
+      <c r="C6307" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6307">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6308" spans="1:4">
+      <c r="A6308" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6308" s="2">
+        <v>44574</v>
+      </c>
+      <c r="C6308" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6308">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6309" spans="1:4">
+      <c r="A6309" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6309" s="2">
+        <v>44574</v>
+      </c>
+      <c r="C6309" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6309">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6310" spans="1:4">
+      <c r="A6310" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6310" s="2">
+        <v>44575</v>
+      </c>
+      <c r="C6310" t="s">
+        <v>398</v>
+      </c>
+      <c r="D6310">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6311" spans="1:4">
+      <c r="A6311" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6311" s="2">
+        <v>44575</v>
+      </c>
+      <c r="C6311" t="s">
+        <v>398</v>
+      </c>
+      <c r="D6311">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6312" spans="1:4">
+      <c r="A6312" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6312" s="2">
+        <v>44575</v>
+      </c>
+      <c r="C6312" t="s">
+        <v>398</v>
+      </c>
+      <c r="D6312">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6313" spans="1:4">
+      <c r="A6313" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6313" s="2">
+        <v>44575</v>
+      </c>
+      <c r="C6313" t="s">
+        <v>398</v>
+      </c>
+      <c r="D6313">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6314" spans="1:4">
+      <c r="A6314" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6314" s="2">
+        <v>44575</v>
+      </c>
+      <c r="C6314" t="s">
+        <v>398</v>
+      </c>
+      <c r="D6314">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6315" spans="1:4">
+      <c r="A6315" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6315" s="2">
+        <v>44575</v>
+      </c>
+      <c r="C6315" t="s">
+        <v>398</v>
+      </c>
+      <c r="D6315">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6316" spans="1:4">
+      <c r="A6316" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6316" s="2">
+        <v>44575</v>
+      </c>
+      <c r="C6316" t="s">
+        <v>398</v>
+      </c>
+      <c r="D6316">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6317" spans="1:4">
+      <c r="A6317" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6317" s="2">
+        <v>44575</v>
+      </c>
+      <c r="C6317" t="s">
+        <v>398</v>
+      </c>
+      <c r="D6317">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6318" spans="1:4">
+      <c r="A6318" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6318" s="2">
+        <v>44575</v>
+      </c>
+      <c r="C6318" t="s">
+        <v>398</v>
+      </c>
+      <c r="D6318">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6319" spans="1:4">
+      <c r="A6319" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6319" s="2">
+        <v>44575</v>
+      </c>
+      <c r="C6319" t="s">
+        <v>398</v>
+      </c>
+      <c r="D6319">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6320" spans="1:4">
+      <c r="A6320" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6320" s="2">
+        <v>44575</v>
+      </c>
+      <c r="C6320" t="s">
+        <v>398</v>
+      </c>
+      <c r="D6320">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6321" spans="1:4">
+      <c r="A6321" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6321" s="2">
+        <v>44575</v>
+      </c>
+      <c r="C6321" t="s">
+        <v>398</v>
+      </c>
+      <c r="D6321">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6322" spans="1:4">
+      <c r="A6322" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6322" s="2">
+        <v>44575</v>
+      </c>
+      <c r="C6322" t="s">
+        <v>398</v>
+      </c>
+      <c r="D6322">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6323" spans="1:4">
+      <c r="A6323" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6323" s="2">
+        <v>44575</v>
+      </c>
+      <c r="C6323" t="s">
+        <v>398</v>
+      </c>
+      <c r="D6323">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6324" spans="1:4">
+      <c r="A6324" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6324" s="2">
+        <v>44575</v>
+      </c>
+      <c r="C6324" t="s">
+        <v>398</v>
+      </c>
+      <c r="D6324">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6325" spans="1:4">
+      <c r="A6325" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6325" s="2">
+        <v>44575</v>
+      </c>
+      <c r="C6325" t="s">
+        <v>398</v>
+      </c>
+      <c r="D6325">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6326" spans="1:4">
+      <c r="A6326" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6326" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6326" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6327" spans="1:4">
+      <c r="A6327" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6327" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6327" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6328" spans="1:4">
+      <c r="A6328" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6328" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6328" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6328">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6329" spans="1:4">
+      <c r="A6329" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6329" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6329" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6329">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6330" spans="1:4">
+      <c r="A6330" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6330" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6330" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6330">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6331" spans="1:4">
+      <c r="A6331" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6331" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6331" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6331">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6332" spans="1:4">
+      <c r="A6332" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6332" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6332" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6332">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6333" spans="1:4">
+      <c r="A6333" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6333" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6333" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6333">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6334" spans="1:4">
+      <c r="A6334" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6334" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6334" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6334">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6335" spans="1:4">
+      <c r="A6335" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6335" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6335" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6335">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6336" spans="1:4">
+      <c r="A6336" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6336" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6336" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6336">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6337" spans="1:4">
+      <c r="A6337" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6337" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6337" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6337">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6338" spans="1:4">
+      <c r="A6338" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6338" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6338" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6338">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6339" spans="1:4">
+      <c r="A6339" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6339" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6339" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6339">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6340" spans="1:4">
+      <c r="A6340" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6340" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6340" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6340">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6341" spans="1:4">
+      <c r="A6341" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6341" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6341" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6341">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-18-2022 17-32-20
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11980" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11932" uniqueCount="401">
   <si>
     <t>Región</t>
   </si>
@@ -1215,6 +1215,9 @@
   <si>
     <t>2022-01-15</t>
   </si>
+  <si>
+    <t>2022-01-16</t>
+  </si>
 </sst>
 </file>
 
@@ -1575,7 +1578,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6341"/>
+  <dimension ref="A1:D6373"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -88788,8 +88791,8 @@
       </c>
     </row>
     <row r="6230" spans="1:4">
-      <c r="A6230" t="s">
-        <v>4</v>
+      <c r="A6230">
+        <v>1</v>
       </c>
       <c r="B6230" s="2">
         <v>44570</v>
@@ -88802,8 +88805,8 @@
       </c>
     </row>
     <row r="6231" spans="1:4">
-      <c r="A6231" t="s">
-        <v>5</v>
+      <c r="A6231">
+        <v>2</v>
       </c>
       <c r="B6231" s="2">
         <v>44570</v>
@@ -88816,8 +88819,8 @@
       </c>
     </row>
     <row r="6232" spans="1:4">
-      <c r="A6232" t="s">
-        <v>6</v>
+      <c r="A6232">
+        <v>3</v>
       </c>
       <c r="B6232" s="2">
         <v>44570</v>
@@ -88830,8 +88833,8 @@
       </c>
     </row>
     <row r="6233" spans="1:4">
-      <c r="A6233" t="s">
-        <v>7</v>
+      <c r="A6233">
+        <v>4</v>
       </c>
       <c r="B6233" s="2">
         <v>44570</v>
@@ -88844,8 +88847,8 @@
       </c>
     </row>
     <row r="6234" spans="1:4">
-      <c r="A6234" t="s">
-        <v>8</v>
+      <c r="A6234">
+        <v>5</v>
       </c>
       <c r="B6234" s="2">
         <v>44570</v>
@@ -88858,8 +88861,8 @@
       </c>
     </row>
     <row r="6235" spans="1:4">
-      <c r="A6235" t="s">
-        <v>9</v>
+      <c r="A6235">
+        <v>6</v>
       </c>
       <c r="B6235" s="2">
         <v>44570</v>
@@ -88872,8 +88875,8 @@
       </c>
     </row>
     <row r="6236" spans="1:4">
-      <c r="A6236" t="s">
-        <v>10</v>
+      <c r="A6236">
+        <v>7</v>
       </c>
       <c r="B6236" s="2">
         <v>44570</v>
@@ -88886,8 +88889,8 @@
       </c>
     </row>
     <row r="6237" spans="1:4">
-      <c r="A6237" t="s">
-        <v>11</v>
+      <c r="A6237">
+        <v>8</v>
       </c>
       <c r="B6237" s="2">
         <v>44570</v>
@@ -88900,8 +88903,8 @@
       </c>
     </row>
     <row r="6238" spans="1:4">
-      <c r="A6238" t="s">
-        <v>12</v>
+      <c r="A6238">
+        <v>9</v>
       </c>
       <c r="B6238" s="2">
         <v>44570</v>
@@ -88914,8 +88917,8 @@
       </c>
     </row>
     <row r="6239" spans="1:4">
-      <c r="A6239" t="s">
-        <v>13</v>
+      <c r="A6239">
+        <v>10</v>
       </c>
       <c r="B6239" s="2">
         <v>44570</v>
@@ -88928,8 +88931,8 @@
       </c>
     </row>
     <row r="6240" spans="1:4">
-      <c r="A6240" t="s">
-        <v>14</v>
+      <c r="A6240">
+        <v>11</v>
       </c>
       <c r="B6240" s="2">
         <v>44570</v>
@@ -88942,8 +88945,8 @@
       </c>
     </row>
     <row r="6241" spans="1:4">
-      <c r="A6241" t="s">
-        <v>15</v>
+      <c r="A6241">
+        <v>12</v>
       </c>
       <c r="B6241" s="2">
         <v>44570</v>
@@ -88956,8 +88959,8 @@
       </c>
     </row>
     <row r="6242" spans="1:4">
-      <c r="A6242" t="s">
-        <v>16</v>
+      <c r="A6242">
+        <v>13</v>
       </c>
       <c r="B6242" s="2">
         <v>44570</v>
@@ -88970,8 +88973,8 @@
       </c>
     </row>
     <row r="6243" spans="1:4">
-      <c r="A6243" t="s">
-        <v>17</v>
+      <c r="A6243">
+        <v>14</v>
       </c>
       <c r="B6243" s="2">
         <v>44570</v>
@@ -88984,8 +88987,8 @@
       </c>
     </row>
     <row r="6244" spans="1:4">
-      <c r="A6244" t="s">
-        <v>18</v>
+      <c r="A6244">
+        <v>15</v>
       </c>
       <c r="B6244" s="2">
         <v>44570</v>
@@ -88998,8 +89001,8 @@
       </c>
     </row>
     <row r="6245" spans="1:4">
-      <c r="A6245" t="s">
-        <v>19</v>
+      <c r="A6245">
+        <v>16</v>
       </c>
       <c r="B6245" s="2">
         <v>44570</v>
@@ -89012,8 +89015,8 @@
       </c>
     </row>
     <row r="6246" spans="1:4">
-      <c r="A6246" t="s">
-        <v>4</v>
+      <c r="A6246">
+        <v>1</v>
       </c>
       <c r="B6246" s="2">
         <v>44571</v>
@@ -89026,8 +89029,8 @@
       </c>
     </row>
     <row r="6247" spans="1:4">
-      <c r="A6247" t="s">
-        <v>5</v>
+      <c r="A6247">
+        <v>2</v>
       </c>
       <c r="B6247" s="2">
         <v>44571</v>
@@ -89040,8 +89043,8 @@
       </c>
     </row>
     <row r="6248" spans="1:4">
-      <c r="A6248" t="s">
-        <v>6</v>
+      <c r="A6248">
+        <v>3</v>
       </c>
       <c r="B6248" s="2">
         <v>44571</v>
@@ -89054,8 +89057,8 @@
       </c>
     </row>
     <row r="6249" spans="1:4">
-      <c r="A6249" t="s">
-        <v>7</v>
+      <c r="A6249">
+        <v>4</v>
       </c>
       <c r="B6249" s="2">
         <v>44571</v>
@@ -89068,8 +89071,8 @@
       </c>
     </row>
     <row r="6250" spans="1:4">
-      <c r="A6250" t="s">
-        <v>8</v>
+      <c r="A6250">
+        <v>5</v>
       </c>
       <c r="B6250" s="2">
         <v>44571</v>
@@ -89082,8 +89085,8 @@
       </c>
     </row>
     <row r="6251" spans="1:4">
-      <c r="A6251" t="s">
-        <v>9</v>
+      <c r="A6251">
+        <v>6</v>
       </c>
       <c r="B6251" s="2">
         <v>44571</v>
@@ -89096,8 +89099,8 @@
       </c>
     </row>
     <row r="6252" spans="1:4">
-      <c r="A6252" t="s">
-        <v>10</v>
+      <c r="A6252">
+        <v>7</v>
       </c>
       <c r="B6252" s="2">
         <v>44571</v>
@@ -89110,8 +89113,8 @@
       </c>
     </row>
     <row r="6253" spans="1:4">
-      <c r="A6253" t="s">
-        <v>11</v>
+      <c r="A6253">
+        <v>8</v>
       </c>
       <c r="B6253" s="2">
         <v>44571</v>
@@ -89124,8 +89127,8 @@
       </c>
     </row>
     <row r="6254" spans="1:4">
-      <c r="A6254" t="s">
-        <v>12</v>
+      <c r="A6254">
+        <v>9</v>
       </c>
       <c r="B6254" s="2">
         <v>44571</v>
@@ -89138,8 +89141,8 @@
       </c>
     </row>
     <row r="6255" spans="1:4">
-      <c r="A6255" t="s">
-        <v>13</v>
+      <c r="A6255">
+        <v>10</v>
       </c>
       <c r="B6255" s="2">
         <v>44571</v>
@@ -89152,8 +89155,8 @@
       </c>
     </row>
     <row r="6256" spans="1:4">
-      <c r="A6256" t="s">
-        <v>14</v>
+      <c r="A6256">
+        <v>11</v>
       </c>
       <c r="B6256" s="2">
         <v>44571</v>
@@ -89166,8 +89169,8 @@
       </c>
     </row>
     <row r="6257" spans="1:4">
-      <c r="A6257" t="s">
-        <v>15</v>
+      <c r="A6257">
+        <v>12</v>
       </c>
       <c r="B6257" s="2">
         <v>44571</v>
@@ -89180,8 +89183,8 @@
       </c>
     </row>
     <row r="6258" spans="1:4">
-      <c r="A6258" t="s">
-        <v>16</v>
+      <c r="A6258">
+        <v>13</v>
       </c>
       <c r="B6258" s="2">
         <v>44571</v>
@@ -89194,8 +89197,8 @@
       </c>
     </row>
     <row r="6259" spans="1:4">
-      <c r="A6259" t="s">
-        <v>17</v>
+      <c r="A6259">
+        <v>14</v>
       </c>
       <c r="B6259" s="2">
         <v>44571</v>
@@ -89208,8 +89211,8 @@
       </c>
     </row>
     <row r="6260" spans="1:4">
-      <c r="A6260" t="s">
-        <v>18</v>
+      <c r="A6260">
+        <v>15</v>
       </c>
       <c r="B6260" s="2">
         <v>44571</v>
@@ -89222,8 +89225,8 @@
       </c>
     </row>
     <row r="6261" spans="1:4">
-      <c r="A6261" t="s">
-        <v>19</v>
+      <c r="A6261">
+        <v>16</v>
       </c>
       <c r="B6261" s="2">
         <v>44571</v>
@@ -89236,8 +89239,8 @@
       </c>
     </row>
     <row r="6262" spans="1:4">
-      <c r="A6262" t="s">
-        <v>4</v>
+      <c r="A6262">
+        <v>1</v>
       </c>
       <c r="B6262" s="2">
         <v>44572</v>
@@ -89250,8 +89253,8 @@
       </c>
     </row>
     <row r="6263" spans="1:4">
-      <c r="A6263" t="s">
-        <v>5</v>
+      <c r="A6263">
+        <v>2</v>
       </c>
       <c r="B6263" s="2">
         <v>44572</v>
@@ -89264,8 +89267,8 @@
       </c>
     </row>
     <row r="6264" spans="1:4">
-      <c r="A6264" t="s">
-        <v>6</v>
+      <c r="A6264">
+        <v>3</v>
       </c>
       <c r="B6264" s="2">
         <v>44572</v>
@@ -89278,8 +89281,8 @@
       </c>
     </row>
     <row r="6265" spans="1:4">
-      <c r="A6265" t="s">
-        <v>7</v>
+      <c r="A6265">
+        <v>4</v>
       </c>
       <c r="B6265" s="2">
         <v>44572</v>
@@ -89292,8 +89295,8 @@
       </c>
     </row>
     <row r="6266" spans="1:4">
-      <c r="A6266" t="s">
-        <v>8</v>
+      <c r="A6266">
+        <v>5</v>
       </c>
       <c r="B6266" s="2">
         <v>44572</v>
@@ -89306,8 +89309,8 @@
       </c>
     </row>
     <row r="6267" spans="1:4">
-      <c r="A6267" t="s">
-        <v>9</v>
+      <c r="A6267">
+        <v>6</v>
       </c>
       <c r="B6267" s="2">
         <v>44572</v>
@@ -89320,8 +89323,8 @@
       </c>
     </row>
     <row r="6268" spans="1:4">
-      <c r="A6268" t="s">
-        <v>10</v>
+      <c r="A6268">
+        <v>7</v>
       </c>
       <c r="B6268" s="2">
         <v>44572</v>
@@ -89334,8 +89337,8 @@
       </c>
     </row>
     <row r="6269" spans="1:4">
-      <c r="A6269" t="s">
-        <v>11</v>
+      <c r="A6269">
+        <v>8</v>
       </c>
       <c r="B6269" s="2">
         <v>44572</v>
@@ -89348,8 +89351,8 @@
       </c>
     </row>
     <row r="6270" spans="1:4">
-      <c r="A6270" t="s">
-        <v>12</v>
+      <c r="A6270">
+        <v>9</v>
       </c>
       <c r="B6270" s="2">
         <v>44572</v>
@@ -89362,8 +89365,8 @@
       </c>
     </row>
     <row r="6271" spans="1:4">
-      <c r="A6271" t="s">
-        <v>13</v>
+      <c r="A6271">
+        <v>10</v>
       </c>
       <c r="B6271" s="2">
         <v>44572</v>
@@ -89376,8 +89379,8 @@
       </c>
     </row>
     <row r="6272" spans="1:4">
-      <c r="A6272" t="s">
-        <v>14</v>
+      <c r="A6272">
+        <v>11</v>
       </c>
       <c r="B6272" s="2">
         <v>44572</v>
@@ -89390,8 +89393,8 @@
       </c>
     </row>
     <row r="6273" spans="1:4">
-      <c r="A6273" t="s">
-        <v>15</v>
+      <c r="A6273">
+        <v>12</v>
       </c>
       <c r="B6273" s="2">
         <v>44572</v>
@@ -89404,8 +89407,8 @@
       </c>
     </row>
     <row r="6274" spans="1:4">
-      <c r="A6274" t="s">
-        <v>16</v>
+      <c r="A6274">
+        <v>13</v>
       </c>
       <c r="B6274" s="2">
         <v>44572</v>
@@ -89418,8 +89421,8 @@
       </c>
     </row>
     <row r="6275" spans="1:4">
-      <c r="A6275" t="s">
-        <v>17</v>
+      <c r="A6275">
+        <v>14</v>
       </c>
       <c r="B6275" s="2">
         <v>44572</v>
@@ -89432,8 +89435,8 @@
       </c>
     </row>
     <row r="6276" spans="1:4">
-      <c r="A6276" t="s">
-        <v>18</v>
+      <c r="A6276">
+        <v>15</v>
       </c>
       <c r="B6276" s="2">
         <v>44572</v>
@@ -89446,8 +89449,8 @@
       </c>
     </row>
     <row r="6277" spans="1:4">
-      <c r="A6277" t="s">
-        <v>19</v>
+      <c r="A6277">
+        <v>16</v>
       </c>
       <c r="B6277" s="2">
         <v>44572</v>
@@ -89460,8 +89463,8 @@
       </c>
     </row>
     <row r="6278" spans="1:4">
-      <c r="A6278" t="s">
-        <v>4</v>
+      <c r="A6278">
+        <v>1</v>
       </c>
       <c r="B6278" s="2">
         <v>44573</v>
@@ -89474,8 +89477,8 @@
       </c>
     </row>
     <row r="6279" spans="1:4">
-      <c r="A6279" t="s">
-        <v>5</v>
+      <c r="A6279">
+        <v>2</v>
       </c>
       <c r="B6279" s="2">
         <v>44573</v>
@@ -89488,8 +89491,8 @@
       </c>
     </row>
     <row r="6280" spans="1:4">
-      <c r="A6280" t="s">
-        <v>6</v>
+      <c r="A6280">
+        <v>3</v>
       </c>
       <c r="B6280" s="2">
         <v>44573</v>
@@ -89502,8 +89505,8 @@
       </c>
     </row>
     <row r="6281" spans="1:4">
-      <c r="A6281" t="s">
-        <v>7</v>
+      <c r="A6281">
+        <v>4</v>
       </c>
       <c r="B6281" s="2">
         <v>44573</v>
@@ -89516,8 +89519,8 @@
       </c>
     </row>
     <row r="6282" spans="1:4">
-      <c r="A6282" t="s">
-        <v>8</v>
+      <c r="A6282">
+        <v>5</v>
       </c>
       <c r="B6282" s="2">
         <v>44573</v>
@@ -89530,8 +89533,8 @@
       </c>
     </row>
     <row r="6283" spans="1:4">
-      <c r="A6283" t="s">
-        <v>9</v>
+      <c r="A6283">
+        <v>6</v>
       </c>
       <c r="B6283" s="2">
         <v>44573</v>
@@ -89544,8 +89547,8 @@
       </c>
     </row>
     <row r="6284" spans="1:4">
-      <c r="A6284" t="s">
-        <v>10</v>
+      <c r="A6284">
+        <v>7</v>
       </c>
       <c r="B6284" s="2">
         <v>44573</v>
@@ -89558,8 +89561,8 @@
       </c>
     </row>
     <row r="6285" spans="1:4">
-      <c r="A6285" t="s">
-        <v>11</v>
+      <c r="A6285">
+        <v>8</v>
       </c>
       <c r="B6285" s="2">
         <v>44573</v>
@@ -89572,8 +89575,8 @@
       </c>
     </row>
     <row r="6286" spans="1:4">
-      <c r="A6286" t="s">
-        <v>12</v>
+      <c r="A6286">
+        <v>9</v>
       </c>
       <c r="B6286" s="2">
         <v>44573</v>
@@ -89586,8 +89589,8 @@
       </c>
     </row>
     <row r="6287" spans="1:4">
-      <c r="A6287" t="s">
-        <v>13</v>
+      <c r="A6287">
+        <v>10</v>
       </c>
       <c r="B6287" s="2">
         <v>44573</v>
@@ -89600,8 +89603,8 @@
       </c>
     </row>
     <row r="6288" spans="1:4">
-      <c r="A6288" t="s">
-        <v>14</v>
+      <c r="A6288">
+        <v>11</v>
       </c>
       <c r="B6288" s="2">
         <v>44573</v>
@@ -89614,8 +89617,8 @@
       </c>
     </row>
     <row r="6289" spans="1:4">
-      <c r="A6289" t="s">
-        <v>15</v>
+      <c r="A6289">
+        <v>12</v>
       </c>
       <c r="B6289" s="2">
         <v>44573</v>
@@ -89628,8 +89631,8 @@
       </c>
     </row>
     <row r="6290" spans="1:4">
-      <c r="A6290" t="s">
-        <v>16</v>
+      <c r="A6290">
+        <v>13</v>
       </c>
       <c r="B6290" s="2">
         <v>44573</v>
@@ -89642,8 +89645,8 @@
       </c>
     </row>
     <row r="6291" spans="1:4">
-      <c r="A6291" t="s">
-        <v>17</v>
+      <c r="A6291">
+        <v>14</v>
       </c>
       <c r="B6291" s="2">
         <v>44573</v>
@@ -89656,8 +89659,8 @@
       </c>
     </row>
     <row r="6292" spans="1:4">
-      <c r="A6292" t="s">
-        <v>18</v>
+      <c r="A6292">
+        <v>15</v>
       </c>
       <c r="B6292" s="2">
         <v>44573</v>
@@ -89670,8 +89673,8 @@
       </c>
     </row>
     <row r="6293" spans="1:4">
-      <c r="A6293" t="s">
-        <v>19</v>
+      <c r="A6293">
+        <v>16</v>
       </c>
       <c r="B6293" s="2">
         <v>44573</v>
@@ -89684,8 +89687,8 @@
       </c>
     </row>
     <row r="6294" spans="1:4">
-      <c r="A6294" t="s">
-        <v>4</v>
+      <c r="A6294">
+        <v>1</v>
       </c>
       <c r="B6294" s="2">
         <v>44574</v>
@@ -89698,8 +89701,8 @@
       </c>
     </row>
     <row r="6295" spans="1:4">
-      <c r="A6295" t="s">
-        <v>5</v>
+      <c r="A6295">
+        <v>2</v>
       </c>
       <c r="B6295" s="2">
         <v>44574</v>
@@ -89712,8 +89715,8 @@
       </c>
     </row>
     <row r="6296" spans="1:4">
-      <c r="A6296" t="s">
-        <v>6</v>
+      <c r="A6296">
+        <v>3</v>
       </c>
       <c r="B6296" s="2">
         <v>44574</v>
@@ -89726,8 +89729,8 @@
       </c>
     </row>
     <row r="6297" spans="1:4">
-      <c r="A6297" t="s">
-        <v>7</v>
+      <c r="A6297">
+        <v>4</v>
       </c>
       <c r="B6297" s="2">
         <v>44574</v>
@@ -89740,8 +89743,8 @@
       </c>
     </row>
     <row r="6298" spans="1:4">
-      <c r="A6298" t="s">
-        <v>8</v>
+      <c r="A6298">
+        <v>5</v>
       </c>
       <c r="B6298" s="2">
         <v>44574</v>
@@ -89754,8 +89757,8 @@
       </c>
     </row>
     <row r="6299" spans="1:4">
-      <c r="A6299" t="s">
-        <v>9</v>
+      <c r="A6299">
+        <v>6</v>
       </c>
       <c r="B6299" s="2">
         <v>44574</v>
@@ -89768,8 +89771,8 @@
       </c>
     </row>
     <row r="6300" spans="1:4">
-      <c r="A6300" t="s">
-        <v>10</v>
+      <c r="A6300">
+        <v>7</v>
       </c>
       <c r="B6300" s="2">
         <v>44574</v>
@@ -89782,8 +89785,8 @@
       </c>
     </row>
     <row r="6301" spans="1:4">
-      <c r="A6301" t="s">
-        <v>11</v>
+      <c r="A6301">
+        <v>8</v>
       </c>
       <c r="B6301" s="2">
         <v>44574</v>
@@ -89796,8 +89799,8 @@
       </c>
     </row>
     <row r="6302" spans="1:4">
-      <c r="A6302" t="s">
-        <v>12</v>
+      <c r="A6302">
+        <v>9</v>
       </c>
       <c r="B6302" s="2">
         <v>44574</v>
@@ -89810,8 +89813,8 @@
       </c>
     </row>
     <row r="6303" spans="1:4">
-      <c r="A6303" t="s">
-        <v>13</v>
+      <c r="A6303">
+        <v>10</v>
       </c>
       <c r="B6303" s="2">
         <v>44574</v>
@@ -89824,8 +89827,8 @@
       </c>
     </row>
     <row r="6304" spans="1:4">
-      <c r="A6304" t="s">
-        <v>14</v>
+      <c r="A6304">
+        <v>11</v>
       </c>
       <c r="B6304" s="2">
         <v>44574</v>
@@ -89838,8 +89841,8 @@
       </c>
     </row>
     <row r="6305" spans="1:4">
-      <c r="A6305" t="s">
-        <v>15</v>
+      <c r="A6305">
+        <v>12</v>
       </c>
       <c r="B6305" s="2">
         <v>44574</v>
@@ -89852,8 +89855,8 @@
       </c>
     </row>
     <row r="6306" spans="1:4">
-      <c r="A6306" t="s">
-        <v>16</v>
+      <c r="A6306">
+        <v>13</v>
       </c>
       <c r="B6306" s="2">
         <v>44574</v>
@@ -89866,8 +89869,8 @@
       </c>
     </row>
     <row r="6307" spans="1:4">
-      <c r="A6307" t="s">
-        <v>17</v>
+      <c r="A6307">
+        <v>14</v>
       </c>
       <c r="B6307" s="2">
         <v>44574</v>
@@ -89880,8 +89883,8 @@
       </c>
     </row>
     <row r="6308" spans="1:4">
-      <c r="A6308" t="s">
-        <v>18</v>
+      <c r="A6308">
+        <v>15</v>
       </c>
       <c r="B6308" s="2">
         <v>44574</v>
@@ -89894,8 +89897,8 @@
       </c>
     </row>
     <row r="6309" spans="1:4">
-      <c r="A6309" t="s">
-        <v>19</v>
+      <c r="A6309">
+        <v>16</v>
       </c>
       <c r="B6309" s="2">
         <v>44574</v>
@@ -89908,8 +89911,8 @@
       </c>
     </row>
     <row r="6310" spans="1:4">
-      <c r="A6310" t="s">
-        <v>4</v>
+      <c r="A6310">
+        <v>1</v>
       </c>
       <c r="B6310" s="2">
         <v>44575</v>
@@ -89922,8 +89925,8 @@
       </c>
     </row>
     <row r="6311" spans="1:4">
-      <c r="A6311" t="s">
-        <v>5</v>
+      <c r="A6311">
+        <v>2</v>
       </c>
       <c r="B6311" s="2">
         <v>44575</v>
@@ -89936,8 +89939,8 @@
       </c>
     </row>
     <row r="6312" spans="1:4">
-      <c r="A6312" t="s">
-        <v>6</v>
+      <c r="A6312">
+        <v>3</v>
       </c>
       <c r="B6312" s="2">
         <v>44575</v>
@@ -89950,8 +89953,8 @@
       </c>
     </row>
     <row r="6313" spans="1:4">
-      <c r="A6313" t="s">
-        <v>7</v>
+      <c r="A6313">
+        <v>4</v>
       </c>
       <c r="B6313" s="2">
         <v>44575</v>
@@ -89964,8 +89967,8 @@
       </c>
     </row>
     <row r="6314" spans="1:4">
-      <c r="A6314" t="s">
-        <v>8</v>
+      <c r="A6314">
+        <v>5</v>
       </c>
       <c r="B6314" s="2">
         <v>44575</v>
@@ -89978,8 +89981,8 @@
       </c>
     </row>
     <row r="6315" spans="1:4">
-      <c r="A6315" t="s">
-        <v>9</v>
+      <c r="A6315">
+        <v>6</v>
       </c>
       <c r="B6315" s="2">
         <v>44575</v>
@@ -89992,8 +89995,8 @@
       </c>
     </row>
     <row r="6316" spans="1:4">
-      <c r="A6316" t="s">
-        <v>10</v>
+      <c r="A6316">
+        <v>7</v>
       </c>
       <c r="B6316" s="2">
         <v>44575</v>
@@ -90006,8 +90009,8 @@
       </c>
     </row>
     <row r="6317" spans="1:4">
-      <c r="A6317" t="s">
-        <v>11</v>
+      <c r="A6317">
+        <v>8</v>
       </c>
       <c r="B6317" s="2">
         <v>44575</v>
@@ -90020,8 +90023,8 @@
       </c>
     </row>
     <row r="6318" spans="1:4">
-      <c r="A6318" t="s">
-        <v>12</v>
+      <c r="A6318">
+        <v>9</v>
       </c>
       <c r="B6318" s="2">
         <v>44575</v>
@@ -90034,8 +90037,8 @@
       </c>
     </row>
     <row r="6319" spans="1:4">
-      <c r="A6319" t="s">
-        <v>13</v>
+      <c r="A6319">
+        <v>10</v>
       </c>
       <c r="B6319" s="2">
         <v>44575</v>
@@ -90048,8 +90051,8 @@
       </c>
     </row>
     <row r="6320" spans="1:4">
-      <c r="A6320" t="s">
-        <v>14</v>
+      <c r="A6320">
+        <v>11</v>
       </c>
       <c r="B6320" s="2">
         <v>44575</v>
@@ -90062,8 +90065,8 @@
       </c>
     </row>
     <row r="6321" spans="1:4">
-      <c r="A6321" t="s">
-        <v>15</v>
+      <c r="A6321">
+        <v>12</v>
       </c>
       <c r="B6321" s="2">
         <v>44575</v>
@@ -90076,8 +90079,8 @@
       </c>
     </row>
     <row r="6322" spans="1:4">
-      <c r="A6322" t="s">
-        <v>16</v>
+      <c r="A6322">
+        <v>13</v>
       </c>
       <c r="B6322" s="2">
         <v>44575</v>
@@ -90090,8 +90093,8 @@
       </c>
     </row>
     <row r="6323" spans="1:4">
-      <c r="A6323" t="s">
-        <v>17</v>
+      <c r="A6323">
+        <v>14</v>
       </c>
       <c r="B6323" s="2">
         <v>44575</v>
@@ -90104,8 +90107,8 @@
       </c>
     </row>
     <row r="6324" spans="1:4">
-      <c r="A6324" t="s">
-        <v>18</v>
+      <c r="A6324">
+        <v>15</v>
       </c>
       <c r="B6324" s="2">
         <v>44575</v>
@@ -90118,8 +90121,8 @@
       </c>
     </row>
     <row r="6325" spans="1:4">
-      <c r="A6325" t="s">
-        <v>19</v>
+      <c r="A6325">
+        <v>16</v>
       </c>
       <c r="B6325" s="2">
         <v>44575</v>
@@ -90132,8 +90135,8 @@
       </c>
     </row>
     <row r="6326" spans="1:4">
-      <c r="A6326" t="s">
-        <v>4</v>
+      <c r="A6326">
+        <v>1</v>
       </c>
       <c r="B6326" s="2">
         <v>44576</v>
@@ -90146,8 +90149,8 @@
       </c>
     </row>
     <row r="6327" spans="1:4">
-      <c r="A6327" t="s">
-        <v>5</v>
+      <c r="A6327">
+        <v>2</v>
       </c>
       <c r="B6327" s="2">
         <v>44576</v>
@@ -90160,8 +90163,8 @@
       </c>
     </row>
     <row r="6328" spans="1:4">
-      <c r="A6328" t="s">
-        <v>6</v>
+      <c r="A6328">
+        <v>3</v>
       </c>
       <c r="B6328" s="2">
         <v>44576</v>
@@ -90174,8 +90177,8 @@
       </c>
     </row>
     <row r="6329" spans="1:4">
-      <c r="A6329" t="s">
-        <v>7</v>
+      <c r="A6329">
+        <v>4</v>
       </c>
       <c r="B6329" s="2">
         <v>44576</v>
@@ -90188,8 +90191,8 @@
       </c>
     </row>
     <row r="6330" spans="1:4">
-      <c r="A6330" t="s">
-        <v>8</v>
+      <c r="A6330">
+        <v>5</v>
       </c>
       <c r="B6330" s="2">
         <v>44576</v>
@@ -90202,8 +90205,8 @@
       </c>
     </row>
     <row r="6331" spans="1:4">
-      <c r="A6331" t="s">
-        <v>9</v>
+      <c r="A6331">
+        <v>6</v>
       </c>
       <c r="B6331" s="2">
         <v>44576</v>
@@ -90216,8 +90219,8 @@
       </c>
     </row>
     <row r="6332" spans="1:4">
-      <c r="A6332" t="s">
-        <v>10</v>
+      <c r="A6332">
+        <v>7</v>
       </c>
       <c r="B6332" s="2">
         <v>44576</v>
@@ -90230,8 +90233,8 @@
       </c>
     </row>
     <row r="6333" spans="1:4">
-      <c r="A6333" t="s">
-        <v>11</v>
+      <c r="A6333">
+        <v>8</v>
       </c>
       <c r="B6333" s="2">
         <v>44576</v>
@@ -90244,8 +90247,8 @@
       </c>
     </row>
     <row r="6334" spans="1:4">
-      <c r="A6334" t="s">
-        <v>12</v>
+      <c r="A6334">
+        <v>9</v>
       </c>
       <c r="B6334" s="2">
         <v>44576</v>
@@ -90258,8 +90261,8 @@
       </c>
     </row>
     <row r="6335" spans="1:4">
-      <c r="A6335" t="s">
-        <v>13</v>
+      <c r="A6335">
+        <v>10</v>
       </c>
       <c r="B6335" s="2">
         <v>44576</v>
@@ -90272,8 +90275,8 @@
       </c>
     </row>
     <row r="6336" spans="1:4">
-      <c r="A6336" t="s">
-        <v>14</v>
+      <c r="A6336">
+        <v>11</v>
       </c>
       <c r="B6336" s="2">
         <v>44576</v>
@@ -90286,8 +90289,8 @@
       </c>
     </row>
     <row r="6337" spans="1:4">
-      <c r="A6337" t="s">
-        <v>15</v>
+      <c r="A6337">
+        <v>12</v>
       </c>
       <c r="B6337" s="2">
         <v>44576</v>
@@ -90300,8 +90303,8 @@
       </c>
     </row>
     <row r="6338" spans="1:4">
-      <c r="A6338" t="s">
-        <v>16</v>
+      <c r="A6338">
+        <v>13</v>
       </c>
       <c r="B6338" s="2">
         <v>44576</v>
@@ -90314,8 +90317,8 @@
       </c>
     </row>
     <row r="6339" spans="1:4">
-      <c r="A6339" t="s">
-        <v>17</v>
+      <c r="A6339">
+        <v>14</v>
       </c>
       <c r="B6339" s="2">
         <v>44576</v>
@@ -90328,8 +90331,8 @@
       </c>
     </row>
     <row r="6340" spans="1:4">
-      <c r="A6340" t="s">
-        <v>18</v>
+      <c r="A6340">
+        <v>15</v>
       </c>
       <c r="B6340" s="2">
         <v>44576</v>
@@ -90342,8 +90345,8 @@
       </c>
     </row>
     <row r="6341" spans="1:4">
-      <c r="A6341" t="s">
-        <v>19</v>
+      <c r="A6341">
+        <v>16</v>
       </c>
       <c r="B6341" s="2">
         <v>44576</v>
@@ -90352,6 +90355,454 @@
         <v>399</v>
       </c>
       <c r="D6341">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6342" spans="1:4">
+      <c r="A6342" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6342" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6342" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6342">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6343" spans="1:4">
+      <c r="A6343" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6343" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6343" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6343">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6344" spans="1:4">
+      <c r="A6344" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6344" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6344" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6344">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6345" spans="1:4">
+      <c r="A6345" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6345" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6345" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6345">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6346" spans="1:4">
+      <c r="A6346" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6346" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6346" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6346">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6347" spans="1:4">
+      <c r="A6347" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6347" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6347" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6347">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6348" spans="1:4">
+      <c r="A6348" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6348" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6348" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6348">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6349" spans="1:4">
+      <c r="A6349" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6349" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6349" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6349">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6350" spans="1:4">
+      <c r="A6350" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6350" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6350" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6351" spans="1:4">
+      <c r="A6351" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6351" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6351" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6351">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6352" spans="1:4">
+      <c r="A6352" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6352" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6352" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6352">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6353" spans="1:4">
+      <c r="A6353" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6353" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6353" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6353">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6354" spans="1:4">
+      <c r="A6354" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6354" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6354" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6354">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6355" spans="1:4">
+      <c r="A6355" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6355" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6355" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6355">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6356" spans="1:4">
+      <c r="A6356" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6356" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6356" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6356">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6357" spans="1:4">
+      <c r="A6357" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6357" s="2">
+        <v>44576</v>
+      </c>
+      <c r="C6357" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6357">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6358" spans="1:4">
+      <c r="A6358" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6358" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6358" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6358">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6359" spans="1:4">
+      <c r="A6359" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6359" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6359" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6359">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6360" spans="1:4">
+      <c r="A6360" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6360" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6360" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6360">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6361" spans="1:4">
+      <c r="A6361" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6361" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6361" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6361">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6362" spans="1:4">
+      <c r="A6362" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6362" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6362" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6362">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6363" spans="1:4">
+      <c r="A6363" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6363" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6363" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6363">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6364" spans="1:4">
+      <c r="A6364" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6364" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6364" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6364">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6365" spans="1:4">
+      <c r="A6365" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6365" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6365" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6365">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6366" spans="1:4">
+      <c r="A6366" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6366" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6366" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6366">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6367" spans="1:4">
+      <c r="A6367" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6367" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6367" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6367">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6368" spans="1:4">
+      <c r="A6368" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6368" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6368" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6368">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6369" spans="1:4">
+      <c r="A6369" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6369" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6369" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6369">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6370" spans="1:4">
+      <c r="A6370" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6370" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6370" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6370">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6371" spans="1:4">
+      <c r="A6371" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6371" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6371" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6371">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6372" spans="1:4">
+      <c r="A6372" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6372" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6372" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6372">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6373" spans="1:4">
+      <c r="A6373" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6373" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6373" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6373">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-19-2022 18-05-11
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11932" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11964" uniqueCount="402">
   <si>
     <t>Región</t>
   </si>
@@ -1218,6 +1218,9 @@
   <si>
     <t>2022-01-16</t>
   </si>
+  <si>
+    <t>2022-01-17</t>
+  </si>
 </sst>
 </file>
 
@@ -1578,7 +1581,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6373"/>
+  <dimension ref="A1:D6405"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -90359,8 +90362,8 @@
       </c>
     </row>
     <row r="6342" spans="1:4">
-      <c r="A6342" t="s">
-        <v>4</v>
+      <c r="A6342">
+        <v>1</v>
       </c>
       <c r="B6342" s="2">
         <v>44576</v>
@@ -90373,8 +90376,8 @@
       </c>
     </row>
     <row r="6343" spans="1:4">
-      <c r="A6343" t="s">
-        <v>5</v>
+      <c r="A6343">
+        <v>2</v>
       </c>
       <c r="B6343" s="2">
         <v>44576</v>
@@ -90387,8 +90390,8 @@
       </c>
     </row>
     <row r="6344" spans="1:4">
-      <c r="A6344" t="s">
-        <v>6</v>
+      <c r="A6344">
+        <v>3</v>
       </c>
       <c r="B6344" s="2">
         <v>44576</v>
@@ -90401,8 +90404,8 @@
       </c>
     </row>
     <row r="6345" spans="1:4">
-      <c r="A6345" t="s">
-        <v>7</v>
+      <c r="A6345">
+        <v>4</v>
       </c>
       <c r="B6345" s="2">
         <v>44576</v>
@@ -90415,8 +90418,8 @@
       </c>
     </row>
     <row r="6346" spans="1:4">
-      <c r="A6346" t="s">
-        <v>8</v>
+      <c r="A6346">
+        <v>5</v>
       </c>
       <c r="B6346" s="2">
         <v>44576</v>
@@ -90429,8 +90432,8 @@
       </c>
     </row>
     <row r="6347" spans="1:4">
-      <c r="A6347" t="s">
-        <v>9</v>
+      <c r="A6347">
+        <v>6</v>
       </c>
       <c r="B6347" s="2">
         <v>44576</v>
@@ -90443,8 +90446,8 @@
       </c>
     </row>
     <row r="6348" spans="1:4">
-      <c r="A6348" t="s">
-        <v>10</v>
+      <c r="A6348">
+        <v>7</v>
       </c>
       <c r="B6348" s="2">
         <v>44576</v>
@@ -90457,8 +90460,8 @@
       </c>
     </row>
     <row r="6349" spans="1:4">
-      <c r="A6349" t="s">
-        <v>11</v>
+      <c r="A6349">
+        <v>8</v>
       </c>
       <c r="B6349" s="2">
         <v>44576</v>
@@ -90471,8 +90474,8 @@
       </c>
     </row>
     <row r="6350" spans="1:4">
-      <c r="A6350" t="s">
-        <v>12</v>
+      <c r="A6350">
+        <v>9</v>
       </c>
       <c r="B6350" s="2">
         <v>44576</v>
@@ -90485,8 +90488,8 @@
       </c>
     </row>
     <row r="6351" spans="1:4">
-      <c r="A6351" t="s">
-        <v>13</v>
+      <c r="A6351">
+        <v>10</v>
       </c>
       <c r="B6351" s="2">
         <v>44576</v>
@@ -90499,8 +90502,8 @@
       </c>
     </row>
     <row r="6352" spans="1:4">
-      <c r="A6352" t="s">
-        <v>14</v>
+      <c r="A6352">
+        <v>11</v>
       </c>
       <c r="B6352" s="2">
         <v>44576</v>
@@ -90513,8 +90516,8 @@
       </c>
     </row>
     <row r="6353" spans="1:4">
-      <c r="A6353" t="s">
-        <v>15</v>
+      <c r="A6353">
+        <v>12</v>
       </c>
       <c r="B6353" s="2">
         <v>44576</v>
@@ -90527,8 +90530,8 @@
       </c>
     </row>
     <row r="6354" spans="1:4">
-      <c r="A6354" t="s">
-        <v>16</v>
+      <c r="A6354">
+        <v>13</v>
       </c>
       <c r="B6354" s="2">
         <v>44576</v>
@@ -90541,8 +90544,8 @@
       </c>
     </row>
     <row r="6355" spans="1:4">
-      <c r="A6355" t="s">
-        <v>17</v>
+      <c r="A6355">
+        <v>14</v>
       </c>
       <c r="B6355" s="2">
         <v>44576</v>
@@ -90555,8 +90558,8 @@
       </c>
     </row>
     <row r="6356" spans="1:4">
-      <c r="A6356" t="s">
-        <v>18</v>
+      <c r="A6356">
+        <v>15</v>
       </c>
       <c r="B6356" s="2">
         <v>44576</v>
@@ -90569,8 +90572,8 @@
       </c>
     </row>
     <row r="6357" spans="1:4">
-      <c r="A6357" t="s">
-        <v>19</v>
+      <c r="A6357">
+        <v>16</v>
       </c>
       <c r="B6357" s="2">
         <v>44576</v>
@@ -90583,8 +90586,8 @@
       </c>
     </row>
     <row r="6358" spans="1:4">
-      <c r="A6358" t="s">
-        <v>4</v>
+      <c r="A6358">
+        <v>1</v>
       </c>
       <c r="B6358" s="2">
         <v>44577</v>
@@ -90597,8 +90600,8 @@
       </c>
     </row>
     <row r="6359" spans="1:4">
-      <c r="A6359" t="s">
-        <v>5</v>
+      <c r="A6359">
+        <v>2</v>
       </c>
       <c r="B6359" s="2">
         <v>44577</v>
@@ -90611,8 +90614,8 @@
       </c>
     </row>
     <row r="6360" spans="1:4">
-      <c r="A6360" t="s">
-        <v>6</v>
+      <c r="A6360">
+        <v>3</v>
       </c>
       <c r="B6360" s="2">
         <v>44577</v>
@@ -90625,8 +90628,8 @@
       </c>
     </row>
     <row r="6361" spans="1:4">
-      <c r="A6361" t="s">
-        <v>7</v>
+      <c r="A6361">
+        <v>4</v>
       </c>
       <c r="B6361" s="2">
         <v>44577</v>
@@ -90639,8 +90642,8 @@
       </c>
     </row>
     <row r="6362" spans="1:4">
-      <c r="A6362" t="s">
-        <v>8</v>
+      <c r="A6362">
+        <v>5</v>
       </c>
       <c r="B6362" s="2">
         <v>44577</v>
@@ -90653,8 +90656,8 @@
       </c>
     </row>
     <row r="6363" spans="1:4">
-      <c r="A6363" t="s">
-        <v>9</v>
+      <c r="A6363">
+        <v>6</v>
       </c>
       <c r="B6363" s="2">
         <v>44577</v>
@@ -90667,8 +90670,8 @@
       </c>
     </row>
     <row r="6364" spans="1:4">
-      <c r="A6364" t="s">
-        <v>10</v>
+      <c r="A6364">
+        <v>7</v>
       </c>
       <c r="B6364" s="2">
         <v>44577</v>
@@ -90681,8 +90684,8 @@
       </c>
     </row>
     <row r="6365" spans="1:4">
-      <c r="A6365" t="s">
-        <v>11</v>
+      <c r="A6365">
+        <v>8</v>
       </c>
       <c r="B6365" s="2">
         <v>44577</v>
@@ -90695,8 +90698,8 @@
       </c>
     </row>
     <row r="6366" spans="1:4">
-      <c r="A6366" t="s">
-        <v>12</v>
+      <c r="A6366">
+        <v>9</v>
       </c>
       <c r="B6366" s="2">
         <v>44577</v>
@@ -90709,8 +90712,8 @@
       </c>
     </row>
     <row r="6367" spans="1:4">
-      <c r="A6367" t="s">
-        <v>13</v>
+      <c r="A6367">
+        <v>10</v>
       </c>
       <c r="B6367" s="2">
         <v>44577</v>
@@ -90723,8 +90726,8 @@
       </c>
     </row>
     <row r="6368" spans="1:4">
-      <c r="A6368" t="s">
-        <v>14</v>
+      <c r="A6368">
+        <v>11</v>
       </c>
       <c r="B6368" s="2">
         <v>44577</v>
@@ -90737,8 +90740,8 @@
       </c>
     </row>
     <row r="6369" spans="1:4">
-      <c r="A6369" t="s">
-        <v>15</v>
+      <c r="A6369">
+        <v>12</v>
       </c>
       <c r="B6369" s="2">
         <v>44577</v>
@@ -90751,8 +90754,8 @@
       </c>
     </row>
     <row r="6370" spans="1:4">
-      <c r="A6370" t="s">
-        <v>16</v>
+      <c r="A6370">
+        <v>13</v>
       </c>
       <c r="B6370" s="2">
         <v>44577</v>
@@ -90765,8 +90768,8 @@
       </c>
     </row>
     <row r="6371" spans="1:4">
-      <c r="A6371" t="s">
-        <v>17</v>
+      <c r="A6371">
+        <v>14</v>
       </c>
       <c r="B6371" s="2">
         <v>44577</v>
@@ -90779,8 +90782,8 @@
       </c>
     </row>
     <row r="6372" spans="1:4">
-      <c r="A6372" t="s">
-        <v>18</v>
+      <c r="A6372">
+        <v>15</v>
       </c>
       <c r="B6372" s="2">
         <v>44577</v>
@@ -90793,8 +90796,8 @@
       </c>
     </row>
     <row r="6373" spans="1:4">
-      <c r="A6373" t="s">
-        <v>19</v>
+      <c r="A6373">
+        <v>16</v>
       </c>
       <c r="B6373" s="2">
         <v>44577</v>
@@ -90803,6 +90806,454 @@
         <v>400</v>
       </c>
       <c r="D6373">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6374" spans="1:4">
+      <c r="A6374" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6374" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6374" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6374">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6375" spans="1:4">
+      <c r="A6375" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6375" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6375" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6375">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6376" spans="1:4">
+      <c r="A6376" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6376" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6376" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6376">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6377" spans="1:4">
+      <c r="A6377" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6377" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6377" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6377">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6378" spans="1:4">
+      <c r="A6378" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6378" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6378" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6378">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6379" spans="1:4">
+      <c r="A6379" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6379" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6379" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6379">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6380" spans="1:4">
+      <c r="A6380" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6380" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6380" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6380">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6381" spans="1:4">
+      <c r="A6381" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6381" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6381" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6381">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6382" spans="1:4">
+      <c r="A6382" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6382" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6382" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6382">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6383" spans="1:4">
+      <c r="A6383" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6383" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6383" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6383">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6384" spans="1:4">
+      <c r="A6384" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6384" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6384" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6384">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6385" spans="1:4">
+      <c r="A6385" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6385" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6385" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6385">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6386" spans="1:4">
+      <c r="A6386" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6386" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6386" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6386">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6387" spans="1:4">
+      <c r="A6387" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6387" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6387" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6387">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6388" spans="1:4">
+      <c r="A6388" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6388" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6388" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6388">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6389" spans="1:4">
+      <c r="A6389" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6389" s="2">
+        <v>44577</v>
+      </c>
+      <c r="C6389" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6389">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6390" spans="1:4">
+      <c r="A6390" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6390" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6390" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6390">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6391" spans="1:4">
+      <c r="A6391" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6391" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6391" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6391">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6392" spans="1:4">
+      <c r="A6392" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6392" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6392" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6392">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6393" spans="1:4">
+      <c r="A6393" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6393" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6393" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6393">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6394" spans="1:4">
+      <c r="A6394" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6394" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6394" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6394">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6395" spans="1:4">
+      <c r="A6395" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6395" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6395" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6395">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6396" spans="1:4">
+      <c r="A6396" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6396" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6396" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6396">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6397" spans="1:4">
+      <c r="A6397" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6397" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6397" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6397">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6398" spans="1:4">
+      <c r="A6398" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6398" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6398" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6398">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6399" spans="1:4">
+      <c r="A6399" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6399" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6399" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6399">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6400" spans="1:4">
+      <c r="A6400" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6400" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6400" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6400">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6401" spans="1:4">
+      <c r="A6401" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6401" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6401" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6401">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6402" spans="1:4">
+      <c r="A6402" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6402" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6402" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6402">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6403" spans="1:4">
+      <c r="A6403" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6403" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6403" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6403">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6404" spans="1:4">
+      <c r="A6404" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6404" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6404" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6404">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6405" spans="1:4">
+      <c r="A6405" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6405" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6405" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6405">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-20-2022 18-36-36
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11964" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11996" uniqueCount="403">
   <si>
     <t>Región</t>
   </si>
@@ -1221,6 +1221,9 @@
   <si>
     <t>2022-01-17</t>
   </si>
+  <si>
+    <t>2022-01-18</t>
+  </si>
 </sst>
 </file>
 
@@ -1581,7 +1584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6405"/>
+  <dimension ref="A1:D6437"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -90810,8 +90813,8 @@
       </c>
     </row>
     <row r="6374" spans="1:4">
-      <c r="A6374" t="s">
-        <v>4</v>
+      <c r="A6374">
+        <v>1</v>
       </c>
       <c r="B6374" s="2">
         <v>44577</v>
@@ -90824,8 +90827,8 @@
       </c>
     </row>
     <row r="6375" spans="1:4">
-      <c r="A6375" t="s">
-        <v>5</v>
+      <c r="A6375">
+        <v>2</v>
       </c>
       <c r="B6375" s="2">
         <v>44577</v>
@@ -90838,8 +90841,8 @@
       </c>
     </row>
     <row r="6376" spans="1:4">
-      <c r="A6376" t="s">
-        <v>6</v>
+      <c r="A6376">
+        <v>3</v>
       </c>
       <c r="B6376" s="2">
         <v>44577</v>
@@ -90852,8 +90855,8 @@
       </c>
     </row>
     <row r="6377" spans="1:4">
-      <c r="A6377" t="s">
-        <v>7</v>
+      <c r="A6377">
+        <v>4</v>
       </c>
       <c r="B6377" s="2">
         <v>44577</v>
@@ -90866,8 +90869,8 @@
       </c>
     </row>
     <row r="6378" spans="1:4">
-      <c r="A6378" t="s">
-        <v>8</v>
+      <c r="A6378">
+        <v>5</v>
       </c>
       <c r="B6378" s="2">
         <v>44577</v>
@@ -90880,8 +90883,8 @@
       </c>
     </row>
     <row r="6379" spans="1:4">
-      <c r="A6379" t="s">
-        <v>9</v>
+      <c r="A6379">
+        <v>6</v>
       </c>
       <c r="B6379" s="2">
         <v>44577</v>
@@ -90894,8 +90897,8 @@
       </c>
     </row>
     <row r="6380" spans="1:4">
-      <c r="A6380" t="s">
-        <v>10</v>
+      <c r="A6380">
+        <v>7</v>
       </c>
       <c r="B6380" s="2">
         <v>44577</v>
@@ -90908,8 +90911,8 @@
       </c>
     </row>
     <row r="6381" spans="1:4">
-      <c r="A6381" t="s">
-        <v>11</v>
+      <c r="A6381">
+        <v>8</v>
       </c>
       <c r="B6381" s="2">
         <v>44577</v>
@@ -90922,8 +90925,8 @@
       </c>
     </row>
     <row r="6382" spans="1:4">
-      <c r="A6382" t="s">
-        <v>12</v>
+      <c r="A6382">
+        <v>9</v>
       </c>
       <c r="B6382" s="2">
         <v>44577</v>
@@ -90936,8 +90939,8 @@
       </c>
     </row>
     <row r="6383" spans="1:4">
-      <c r="A6383" t="s">
-        <v>13</v>
+      <c r="A6383">
+        <v>10</v>
       </c>
       <c r="B6383" s="2">
         <v>44577</v>
@@ -90950,8 +90953,8 @@
       </c>
     </row>
     <row r="6384" spans="1:4">
-      <c r="A6384" t="s">
-        <v>14</v>
+      <c r="A6384">
+        <v>11</v>
       </c>
       <c r="B6384" s="2">
         <v>44577</v>
@@ -90964,8 +90967,8 @@
       </c>
     </row>
     <row r="6385" spans="1:4">
-      <c r="A6385" t="s">
-        <v>15</v>
+      <c r="A6385">
+        <v>12</v>
       </c>
       <c r="B6385" s="2">
         <v>44577</v>
@@ -90978,8 +90981,8 @@
       </c>
     </row>
     <row r="6386" spans="1:4">
-      <c r="A6386" t="s">
-        <v>16</v>
+      <c r="A6386">
+        <v>13</v>
       </c>
       <c r="B6386" s="2">
         <v>44577</v>
@@ -90992,8 +90995,8 @@
       </c>
     </row>
     <row r="6387" spans="1:4">
-      <c r="A6387" t="s">
-        <v>17</v>
+      <c r="A6387">
+        <v>14</v>
       </c>
       <c r="B6387" s="2">
         <v>44577</v>
@@ -91006,8 +91009,8 @@
       </c>
     </row>
     <row r="6388" spans="1:4">
-      <c r="A6388" t="s">
-        <v>18</v>
+      <c r="A6388">
+        <v>15</v>
       </c>
       <c r="B6388" s="2">
         <v>44577</v>
@@ -91020,8 +91023,8 @@
       </c>
     </row>
     <row r="6389" spans="1:4">
-      <c r="A6389" t="s">
-        <v>19</v>
+      <c r="A6389">
+        <v>16</v>
       </c>
       <c r="B6389" s="2">
         <v>44577</v>
@@ -91034,8 +91037,8 @@
       </c>
     </row>
     <row r="6390" spans="1:4">
-      <c r="A6390" t="s">
-        <v>4</v>
+      <c r="A6390">
+        <v>1</v>
       </c>
       <c r="B6390" s="2">
         <v>44578</v>
@@ -91048,8 +91051,8 @@
       </c>
     </row>
     <row r="6391" spans="1:4">
-      <c r="A6391" t="s">
-        <v>5</v>
+      <c r="A6391">
+        <v>2</v>
       </c>
       <c r="B6391" s="2">
         <v>44578</v>
@@ -91062,8 +91065,8 @@
       </c>
     </row>
     <row r="6392" spans="1:4">
-      <c r="A6392" t="s">
-        <v>6</v>
+      <c r="A6392">
+        <v>3</v>
       </c>
       <c r="B6392" s="2">
         <v>44578</v>
@@ -91076,8 +91079,8 @@
       </c>
     </row>
     <row r="6393" spans="1:4">
-      <c r="A6393" t="s">
-        <v>7</v>
+      <c r="A6393">
+        <v>4</v>
       </c>
       <c r="B6393" s="2">
         <v>44578</v>
@@ -91090,8 +91093,8 @@
       </c>
     </row>
     <row r="6394" spans="1:4">
-      <c r="A6394" t="s">
-        <v>8</v>
+      <c r="A6394">
+        <v>5</v>
       </c>
       <c r="B6394" s="2">
         <v>44578</v>
@@ -91104,8 +91107,8 @@
       </c>
     </row>
     <row r="6395" spans="1:4">
-      <c r="A6395" t="s">
-        <v>9</v>
+      <c r="A6395">
+        <v>6</v>
       </c>
       <c r="B6395" s="2">
         <v>44578</v>
@@ -91118,8 +91121,8 @@
       </c>
     </row>
     <row r="6396" spans="1:4">
-      <c r="A6396" t="s">
-        <v>10</v>
+      <c r="A6396">
+        <v>7</v>
       </c>
       <c r="B6396" s="2">
         <v>44578</v>
@@ -91132,8 +91135,8 @@
       </c>
     </row>
     <row r="6397" spans="1:4">
-      <c r="A6397" t="s">
-        <v>11</v>
+      <c r="A6397">
+        <v>8</v>
       </c>
       <c r="B6397" s="2">
         <v>44578</v>
@@ -91146,8 +91149,8 @@
       </c>
     </row>
     <row r="6398" spans="1:4">
-      <c r="A6398" t="s">
-        <v>12</v>
+      <c r="A6398">
+        <v>9</v>
       </c>
       <c r="B6398" s="2">
         <v>44578</v>
@@ -91160,8 +91163,8 @@
       </c>
     </row>
     <row r="6399" spans="1:4">
-      <c r="A6399" t="s">
-        <v>13</v>
+      <c r="A6399">
+        <v>10</v>
       </c>
       <c r="B6399" s="2">
         <v>44578</v>
@@ -91174,8 +91177,8 @@
       </c>
     </row>
     <row r="6400" spans="1:4">
-      <c r="A6400" t="s">
-        <v>14</v>
+      <c r="A6400">
+        <v>11</v>
       </c>
       <c r="B6400" s="2">
         <v>44578</v>
@@ -91188,8 +91191,8 @@
       </c>
     </row>
     <row r="6401" spans="1:4">
-      <c r="A6401" t="s">
-        <v>15</v>
+      <c r="A6401">
+        <v>12</v>
       </c>
       <c r="B6401" s="2">
         <v>44578</v>
@@ -91202,8 +91205,8 @@
       </c>
     </row>
     <row r="6402" spans="1:4">
-      <c r="A6402" t="s">
-        <v>16</v>
+      <c r="A6402">
+        <v>13</v>
       </c>
       <c r="B6402" s="2">
         <v>44578</v>
@@ -91216,8 +91219,8 @@
       </c>
     </row>
     <row r="6403" spans="1:4">
-      <c r="A6403" t="s">
-        <v>17</v>
+      <c r="A6403">
+        <v>14</v>
       </c>
       <c r="B6403" s="2">
         <v>44578</v>
@@ -91230,8 +91233,8 @@
       </c>
     </row>
     <row r="6404" spans="1:4">
-      <c r="A6404" t="s">
-        <v>18</v>
+      <c r="A6404">
+        <v>15</v>
       </c>
       <c r="B6404" s="2">
         <v>44578</v>
@@ -91244,8 +91247,8 @@
       </c>
     </row>
     <row r="6405" spans="1:4">
-      <c r="A6405" t="s">
-        <v>19</v>
+      <c r="A6405">
+        <v>16</v>
       </c>
       <c r="B6405" s="2">
         <v>44578</v>
@@ -91254,6 +91257,454 @@
         <v>401</v>
       </c>
       <c r="D6405">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6406" spans="1:4">
+      <c r="A6406" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6406" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6406" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6406">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6407" spans="1:4">
+      <c r="A6407" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6407" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6407" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6407">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6408" spans="1:4">
+      <c r="A6408" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6408" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6408" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6408">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6409" spans="1:4">
+      <c r="A6409" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6409" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6409" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6409">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6410" spans="1:4">
+      <c r="A6410" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6410" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6410" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6410">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6411" spans="1:4">
+      <c r="A6411" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6411" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6411" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6411">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6412" spans="1:4">
+      <c r="A6412" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6412" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6412" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6412">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6413" spans="1:4">
+      <c r="A6413" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6413" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6413" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6413">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6414" spans="1:4">
+      <c r="A6414" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6414" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6414" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6414">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6415" spans="1:4">
+      <c r="A6415" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6415" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6415" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6415">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6416" spans="1:4">
+      <c r="A6416" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6416" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6416" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6416">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6417" spans="1:4">
+      <c r="A6417" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6417" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6417" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6417">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6418" spans="1:4">
+      <c r="A6418" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6418" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6418" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6418">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6419" spans="1:4">
+      <c r="A6419" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6419" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6419" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6419">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6420" spans="1:4">
+      <c r="A6420" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6420" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6420" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6420">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6421" spans="1:4">
+      <c r="A6421" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6421" s="2">
+        <v>44578</v>
+      </c>
+      <c r="C6421" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6421">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6422" spans="1:4">
+      <c r="A6422" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6422" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6422" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6422">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6423" spans="1:4">
+      <c r="A6423" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6423" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6423" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6423">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6424" spans="1:4">
+      <c r="A6424" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6424" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6424" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6424">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6425" spans="1:4">
+      <c r="A6425" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6425" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6425" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6425">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6426" spans="1:4">
+      <c r="A6426" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6426" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6426" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6426">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6427" spans="1:4">
+      <c r="A6427" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6427" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6427" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6427">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6428" spans="1:4">
+      <c r="A6428" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6428" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6428" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6428">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6429" spans="1:4">
+      <c r="A6429" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6429" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6429" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6429">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6430" spans="1:4">
+      <c r="A6430" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6430" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6430" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6430">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6431" spans="1:4">
+      <c r="A6431" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6431" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6431" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6431">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6432" spans="1:4">
+      <c r="A6432" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6432" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6432" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6432">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6433" spans="1:4">
+      <c r="A6433" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6433" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6433" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6433">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6434" spans="1:4">
+      <c r="A6434" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6434" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6434" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6434">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6435" spans="1:4">
+      <c r="A6435" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6435" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6435" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6435">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6436" spans="1:4">
+      <c r="A6436" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6436" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6436" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6436">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6437" spans="1:4">
+      <c r="A6437" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6437" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6437" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6437">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-21-2022 19-09-14
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11996" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12028" uniqueCount="404">
   <si>
     <t>Región</t>
   </si>
@@ -1224,6 +1224,9 @@
   <si>
     <t>2022-01-18</t>
   </si>
+  <si>
+    <t>2022-01-19</t>
+  </si>
 </sst>
 </file>
 
@@ -1584,7 +1587,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6437"/>
+  <dimension ref="A1:D6469"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -91261,8 +91264,8 @@
       </c>
     </row>
     <row r="6406" spans="1:4">
-      <c r="A6406" t="s">
-        <v>4</v>
+      <c r="A6406">
+        <v>1</v>
       </c>
       <c r="B6406" s="2">
         <v>44578</v>
@@ -91275,8 +91278,8 @@
       </c>
     </row>
     <row r="6407" spans="1:4">
-      <c r="A6407" t="s">
-        <v>5</v>
+      <c r="A6407">
+        <v>2</v>
       </c>
       <c r="B6407" s="2">
         <v>44578</v>
@@ -91289,8 +91292,8 @@
       </c>
     </row>
     <row r="6408" spans="1:4">
-      <c r="A6408" t="s">
-        <v>6</v>
+      <c r="A6408">
+        <v>3</v>
       </c>
       <c r="B6408" s="2">
         <v>44578</v>
@@ -91303,8 +91306,8 @@
       </c>
     </row>
     <row r="6409" spans="1:4">
-      <c r="A6409" t="s">
-        <v>7</v>
+      <c r="A6409">
+        <v>4</v>
       </c>
       <c r="B6409" s="2">
         <v>44578</v>
@@ -91317,8 +91320,8 @@
       </c>
     </row>
     <row r="6410" spans="1:4">
-      <c r="A6410" t="s">
-        <v>8</v>
+      <c r="A6410">
+        <v>5</v>
       </c>
       <c r="B6410" s="2">
         <v>44578</v>
@@ -91331,8 +91334,8 @@
       </c>
     </row>
     <row r="6411" spans="1:4">
-      <c r="A6411" t="s">
-        <v>9</v>
+      <c r="A6411">
+        <v>6</v>
       </c>
       <c r="B6411" s="2">
         <v>44578</v>
@@ -91345,8 +91348,8 @@
       </c>
     </row>
     <row r="6412" spans="1:4">
-      <c r="A6412" t="s">
-        <v>10</v>
+      <c r="A6412">
+        <v>7</v>
       </c>
       <c r="B6412" s="2">
         <v>44578</v>
@@ -91359,8 +91362,8 @@
       </c>
     </row>
     <row r="6413" spans="1:4">
-      <c r="A6413" t="s">
-        <v>11</v>
+      <c r="A6413">
+        <v>8</v>
       </c>
       <c r="B6413" s="2">
         <v>44578</v>
@@ -91373,8 +91376,8 @@
       </c>
     </row>
     <row r="6414" spans="1:4">
-      <c r="A6414" t="s">
-        <v>12</v>
+      <c r="A6414">
+        <v>9</v>
       </c>
       <c r="B6414" s="2">
         <v>44578</v>
@@ -91387,8 +91390,8 @@
       </c>
     </row>
     <row r="6415" spans="1:4">
-      <c r="A6415" t="s">
-        <v>13</v>
+      <c r="A6415">
+        <v>10</v>
       </c>
       <c r="B6415" s="2">
         <v>44578</v>
@@ -91401,8 +91404,8 @@
       </c>
     </row>
     <row r="6416" spans="1:4">
-      <c r="A6416" t="s">
-        <v>14</v>
+      <c r="A6416">
+        <v>11</v>
       </c>
       <c r="B6416" s="2">
         <v>44578</v>
@@ -91415,8 +91418,8 @@
       </c>
     </row>
     <row r="6417" spans="1:4">
-      <c r="A6417" t="s">
-        <v>15</v>
+      <c r="A6417">
+        <v>12</v>
       </c>
       <c r="B6417" s="2">
         <v>44578</v>
@@ -91429,8 +91432,8 @@
       </c>
     </row>
     <row r="6418" spans="1:4">
-      <c r="A6418" t="s">
-        <v>16</v>
+      <c r="A6418">
+        <v>13</v>
       </c>
       <c r="B6418" s="2">
         <v>44578</v>
@@ -91443,8 +91446,8 @@
       </c>
     </row>
     <row r="6419" spans="1:4">
-      <c r="A6419" t="s">
-        <v>17</v>
+      <c r="A6419">
+        <v>14</v>
       </c>
       <c r="B6419" s="2">
         <v>44578</v>
@@ -91457,8 +91460,8 @@
       </c>
     </row>
     <row r="6420" spans="1:4">
-      <c r="A6420" t="s">
-        <v>18</v>
+      <c r="A6420">
+        <v>15</v>
       </c>
       <c r="B6420" s="2">
         <v>44578</v>
@@ -91471,8 +91474,8 @@
       </c>
     </row>
     <row r="6421" spans="1:4">
-      <c r="A6421" t="s">
-        <v>19</v>
+      <c r="A6421">
+        <v>16</v>
       </c>
       <c r="B6421" s="2">
         <v>44578</v>
@@ -91485,8 +91488,8 @@
       </c>
     </row>
     <row r="6422" spans="1:4">
-      <c r="A6422" t="s">
-        <v>4</v>
+      <c r="A6422">
+        <v>1</v>
       </c>
       <c r="B6422" s="2">
         <v>44579</v>
@@ -91499,8 +91502,8 @@
       </c>
     </row>
     <row r="6423" spans="1:4">
-      <c r="A6423" t="s">
-        <v>5</v>
+      <c r="A6423">
+        <v>2</v>
       </c>
       <c r="B6423" s="2">
         <v>44579</v>
@@ -91513,8 +91516,8 @@
       </c>
     </row>
     <row r="6424" spans="1:4">
-      <c r="A6424" t="s">
-        <v>6</v>
+      <c r="A6424">
+        <v>3</v>
       </c>
       <c r="B6424" s="2">
         <v>44579</v>
@@ -91527,8 +91530,8 @@
       </c>
     </row>
     <row r="6425" spans="1:4">
-      <c r="A6425" t="s">
-        <v>7</v>
+      <c r="A6425">
+        <v>4</v>
       </c>
       <c r="B6425" s="2">
         <v>44579</v>
@@ -91541,8 +91544,8 @@
       </c>
     </row>
     <row r="6426" spans="1:4">
-      <c r="A6426" t="s">
-        <v>8</v>
+      <c r="A6426">
+        <v>5</v>
       </c>
       <c r="B6426" s="2">
         <v>44579</v>
@@ -91555,8 +91558,8 @@
       </c>
     </row>
     <row r="6427" spans="1:4">
-      <c r="A6427" t="s">
-        <v>9</v>
+      <c r="A6427">
+        <v>6</v>
       </c>
       <c r="B6427" s="2">
         <v>44579</v>
@@ -91569,8 +91572,8 @@
       </c>
     </row>
     <row r="6428" spans="1:4">
-      <c r="A6428" t="s">
-        <v>10</v>
+      <c r="A6428">
+        <v>7</v>
       </c>
       <c r="B6428" s="2">
         <v>44579</v>
@@ -91583,8 +91586,8 @@
       </c>
     </row>
     <row r="6429" spans="1:4">
-      <c r="A6429" t="s">
-        <v>11</v>
+      <c r="A6429">
+        <v>8</v>
       </c>
       <c r="B6429" s="2">
         <v>44579</v>
@@ -91597,8 +91600,8 @@
       </c>
     </row>
     <row r="6430" spans="1:4">
-      <c r="A6430" t="s">
-        <v>12</v>
+      <c r="A6430">
+        <v>9</v>
       </c>
       <c r="B6430" s="2">
         <v>44579</v>
@@ -91611,8 +91614,8 @@
       </c>
     </row>
     <row r="6431" spans="1:4">
-      <c r="A6431" t="s">
-        <v>13</v>
+      <c r="A6431">
+        <v>10</v>
       </c>
       <c r="B6431" s="2">
         <v>44579</v>
@@ -91625,8 +91628,8 @@
       </c>
     </row>
     <row r="6432" spans="1:4">
-      <c r="A6432" t="s">
-        <v>14</v>
+      <c r="A6432">
+        <v>11</v>
       </c>
       <c r="B6432" s="2">
         <v>44579</v>
@@ -91639,8 +91642,8 @@
       </c>
     </row>
     <row r="6433" spans="1:4">
-      <c r="A6433" t="s">
-        <v>15</v>
+      <c r="A6433">
+        <v>12</v>
       </c>
       <c r="B6433" s="2">
         <v>44579</v>
@@ -91653,8 +91656,8 @@
       </c>
     </row>
     <row r="6434" spans="1:4">
-      <c r="A6434" t="s">
-        <v>16</v>
+      <c r="A6434">
+        <v>13</v>
       </c>
       <c r="B6434" s="2">
         <v>44579</v>
@@ -91667,8 +91670,8 @@
       </c>
     </row>
     <row r="6435" spans="1:4">
-      <c r="A6435" t="s">
-        <v>17</v>
+      <c r="A6435">
+        <v>14</v>
       </c>
       <c r="B6435" s="2">
         <v>44579</v>
@@ -91681,8 +91684,8 @@
       </c>
     </row>
     <row r="6436" spans="1:4">
-      <c r="A6436" t="s">
-        <v>18</v>
+      <c r="A6436">
+        <v>15</v>
       </c>
       <c r="B6436" s="2">
         <v>44579</v>
@@ -91695,8 +91698,8 @@
       </c>
     </row>
     <row r="6437" spans="1:4">
-      <c r="A6437" t="s">
-        <v>19</v>
+      <c r="A6437">
+        <v>16</v>
       </c>
       <c r="B6437" s="2">
         <v>44579</v>
@@ -91705,6 +91708,454 @@
         <v>402</v>
       </c>
       <c r="D6437">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6438" spans="1:4">
+      <c r="A6438" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6438" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6438" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6438">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6439" spans="1:4">
+      <c r="A6439" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6439" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6439" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6439">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6440" spans="1:4">
+      <c r="A6440" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6440" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6440" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6440">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6441" spans="1:4">
+      <c r="A6441" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6441" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6441" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6441">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6442" spans="1:4">
+      <c r="A6442" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6442" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6442" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6442">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6443" spans="1:4">
+      <c r="A6443" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6443" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6443" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6443">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6444" spans="1:4">
+      <c r="A6444" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6444" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6444" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6444">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6445" spans="1:4">
+      <c r="A6445" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6445" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6445" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6445">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6446" spans="1:4">
+      <c r="A6446" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6446" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6446" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6446">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6447" spans="1:4">
+      <c r="A6447" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6447" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6447" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6447">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6448" spans="1:4">
+      <c r="A6448" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6448" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6448" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6448">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6449" spans="1:4">
+      <c r="A6449" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6449" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6449" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6449">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6450" spans="1:4">
+      <c r="A6450" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6450" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6450" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6450">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6451" spans="1:4">
+      <c r="A6451" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6451" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6451" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6451">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6452" spans="1:4">
+      <c r="A6452" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6452" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6452" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6452">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6453" spans="1:4">
+      <c r="A6453" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6453" s="2">
+        <v>44579</v>
+      </c>
+      <c r="C6453" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6453">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6454" spans="1:4">
+      <c r="A6454" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6454" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6454" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6454">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6455" spans="1:4">
+      <c r="A6455" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6455" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6455" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6455">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6456" spans="1:4">
+      <c r="A6456" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6456" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6456" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6456">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6457" spans="1:4">
+      <c r="A6457" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6457" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6457" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6457">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6458" spans="1:4">
+      <c r="A6458" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6458" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6458" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6458">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6459" spans="1:4">
+      <c r="A6459" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6459" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6459" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6459">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6460" spans="1:4">
+      <c r="A6460" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6460" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6460" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6460">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6461" spans="1:4">
+      <c r="A6461" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6461" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6461" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6461">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6462" spans="1:4">
+      <c r="A6462" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6462" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6462" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6462">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6463" spans="1:4">
+      <c r="A6463" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6463" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6463" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6463">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6464" spans="1:4">
+      <c r="A6464" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6464" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6464" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6464">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6465" spans="1:4">
+      <c r="A6465" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6465" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6465" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6465">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6466" spans="1:4">
+      <c r="A6466" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6466" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6466" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6466">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6467" spans="1:4">
+      <c r="A6467" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6467" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6467" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6467">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6468" spans="1:4">
+      <c r="A6468" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6468" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6468" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6468">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6469" spans="1:4">
+      <c r="A6469" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6469" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6469" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6469">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-22-2022 19-40-32
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12028" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12060" uniqueCount="405">
   <si>
     <t>Región</t>
   </si>
@@ -1227,6 +1227,9 @@
   <si>
     <t>2022-01-19</t>
   </si>
+  <si>
+    <t>2022-01-20</t>
+  </si>
 </sst>
 </file>
 
@@ -1587,7 +1590,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6469"/>
+  <dimension ref="A1:D6501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -91712,8 +91715,8 @@
       </c>
     </row>
     <row r="6438" spans="1:4">
-      <c r="A6438" t="s">
-        <v>4</v>
+      <c r="A6438">
+        <v>1</v>
       </c>
       <c r="B6438" s="2">
         <v>44579</v>
@@ -91726,8 +91729,8 @@
       </c>
     </row>
     <row r="6439" spans="1:4">
-      <c r="A6439" t="s">
-        <v>5</v>
+      <c r="A6439">
+        <v>2</v>
       </c>
       <c r="B6439" s="2">
         <v>44579</v>
@@ -91740,8 +91743,8 @@
       </c>
     </row>
     <row r="6440" spans="1:4">
-      <c r="A6440" t="s">
-        <v>6</v>
+      <c r="A6440">
+        <v>3</v>
       </c>
       <c r="B6440" s="2">
         <v>44579</v>
@@ -91754,8 +91757,8 @@
       </c>
     </row>
     <row r="6441" spans="1:4">
-      <c r="A6441" t="s">
-        <v>7</v>
+      <c r="A6441">
+        <v>4</v>
       </c>
       <c r="B6441" s="2">
         <v>44579</v>
@@ -91768,8 +91771,8 @@
       </c>
     </row>
     <row r="6442" spans="1:4">
-      <c r="A6442" t="s">
-        <v>8</v>
+      <c r="A6442">
+        <v>5</v>
       </c>
       <c r="B6442" s="2">
         <v>44579</v>
@@ -91782,8 +91785,8 @@
       </c>
     </row>
     <row r="6443" spans="1:4">
-      <c r="A6443" t="s">
-        <v>9</v>
+      <c r="A6443">
+        <v>6</v>
       </c>
       <c r="B6443" s="2">
         <v>44579</v>
@@ -91796,8 +91799,8 @@
       </c>
     </row>
     <row r="6444" spans="1:4">
-      <c r="A6444" t="s">
-        <v>10</v>
+      <c r="A6444">
+        <v>7</v>
       </c>
       <c r="B6444" s="2">
         <v>44579</v>
@@ -91810,8 +91813,8 @@
       </c>
     </row>
     <row r="6445" spans="1:4">
-      <c r="A6445" t="s">
-        <v>11</v>
+      <c r="A6445">
+        <v>8</v>
       </c>
       <c r="B6445" s="2">
         <v>44579</v>
@@ -91824,8 +91827,8 @@
       </c>
     </row>
     <row r="6446" spans="1:4">
-      <c r="A6446" t="s">
-        <v>12</v>
+      <c r="A6446">
+        <v>9</v>
       </c>
       <c r="B6446" s="2">
         <v>44579</v>
@@ -91838,8 +91841,8 @@
       </c>
     </row>
     <row r="6447" spans="1:4">
-      <c r="A6447" t="s">
-        <v>13</v>
+      <c r="A6447">
+        <v>10</v>
       </c>
       <c r="B6447" s="2">
         <v>44579</v>
@@ -91852,8 +91855,8 @@
       </c>
     </row>
     <row r="6448" spans="1:4">
-      <c r="A6448" t="s">
-        <v>14</v>
+      <c r="A6448">
+        <v>11</v>
       </c>
       <c r="B6448" s="2">
         <v>44579</v>
@@ -91866,8 +91869,8 @@
       </c>
     </row>
     <row r="6449" spans="1:4">
-      <c r="A6449" t="s">
-        <v>15</v>
+      <c r="A6449">
+        <v>12</v>
       </c>
       <c r="B6449" s="2">
         <v>44579</v>
@@ -91880,8 +91883,8 @@
       </c>
     </row>
     <row r="6450" spans="1:4">
-      <c r="A6450" t="s">
-        <v>16</v>
+      <c r="A6450">
+        <v>13</v>
       </c>
       <c r="B6450" s="2">
         <v>44579</v>
@@ -91894,8 +91897,8 @@
       </c>
     </row>
     <row r="6451" spans="1:4">
-      <c r="A6451" t="s">
-        <v>17</v>
+      <c r="A6451">
+        <v>14</v>
       </c>
       <c r="B6451" s="2">
         <v>44579</v>
@@ -91908,8 +91911,8 @@
       </c>
     </row>
     <row r="6452" spans="1:4">
-      <c r="A6452" t="s">
-        <v>18</v>
+      <c r="A6452">
+        <v>15</v>
       </c>
       <c r="B6452" s="2">
         <v>44579</v>
@@ -91922,8 +91925,8 @@
       </c>
     </row>
     <row r="6453" spans="1:4">
-      <c r="A6453" t="s">
-        <v>19</v>
+      <c r="A6453">
+        <v>16</v>
       </c>
       <c r="B6453" s="2">
         <v>44579</v>
@@ -91936,8 +91939,8 @@
       </c>
     </row>
     <row r="6454" spans="1:4">
-      <c r="A6454" t="s">
-        <v>4</v>
+      <c r="A6454">
+        <v>1</v>
       </c>
       <c r="B6454" s="2">
         <v>44580</v>
@@ -91950,8 +91953,8 @@
       </c>
     </row>
     <row r="6455" spans="1:4">
-      <c r="A6455" t="s">
-        <v>5</v>
+      <c r="A6455">
+        <v>2</v>
       </c>
       <c r="B6455" s="2">
         <v>44580</v>
@@ -91964,8 +91967,8 @@
       </c>
     </row>
     <row r="6456" spans="1:4">
-      <c r="A6456" t="s">
-        <v>6</v>
+      <c r="A6456">
+        <v>3</v>
       </c>
       <c r="B6456" s="2">
         <v>44580</v>
@@ -91978,8 +91981,8 @@
       </c>
     </row>
     <row r="6457" spans="1:4">
-      <c r="A6457" t="s">
-        <v>7</v>
+      <c r="A6457">
+        <v>4</v>
       </c>
       <c r="B6457" s="2">
         <v>44580</v>
@@ -91992,8 +91995,8 @@
       </c>
     </row>
     <row r="6458" spans="1:4">
-      <c r="A6458" t="s">
-        <v>8</v>
+      <c r="A6458">
+        <v>5</v>
       </c>
       <c r="B6458" s="2">
         <v>44580</v>
@@ -92006,8 +92009,8 @@
       </c>
     </row>
     <row r="6459" spans="1:4">
-      <c r="A6459" t="s">
-        <v>9</v>
+      <c r="A6459">
+        <v>6</v>
       </c>
       <c r="B6459" s="2">
         <v>44580</v>
@@ -92020,8 +92023,8 @@
       </c>
     </row>
     <row r="6460" spans="1:4">
-      <c r="A6460" t="s">
-        <v>10</v>
+      <c r="A6460">
+        <v>7</v>
       </c>
       <c r="B6460" s="2">
         <v>44580</v>
@@ -92034,8 +92037,8 @@
       </c>
     </row>
     <row r="6461" spans="1:4">
-      <c r="A6461" t="s">
-        <v>11</v>
+      <c r="A6461">
+        <v>8</v>
       </c>
       <c r="B6461" s="2">
         <v>44580</v>
@@ -92048,8 +92051,8 @@
       </c>
     </row>
     <row r="6462" spans="1:4">
-      <c r="A6462" t="s">
-        <v>12</v>
+      <c r="A6462">
+        <v>9</v>
       </c>
       <c r="B6462" s="2">
         <v>44580</v>
@@ -92062,8 +92065,8 @@
       </c>
     </row>
     <row r="6463" spans="1:4">
-      <c r="A6463" t="s">
-        <v>13</v>
+      <c r="A6463">
+        <v>10</v>
       </c>
       <c r="B6463" s="2">
         <v>44580</v>
@@ -92076,8 +92079,8 @@
       </c>
     </row>
     <row r="6464" spans="1:4">
-      <c r="A6464" t="s">
-        <v>14</v>
+      <c r="A6464">
+        <v>11</v>
       </c>
       <c r="B6464" s="2">
         <v>44580</v>
@@ -92090,8 +92093,8 @@
       </c>
     </row>
     <row r="6465" spans="1:4">
-      <c r="A6465" t="s">
-        <v>15</v>
+      <c r="A6465">
+        <v>12</v>
       </c>
       <c r="B6465" s="2">
         <v>44580</v>
@@ -92104,8 +92107,8 @@
       </c>
     </row>
     <row r="6466" spans="1:4">
-      <c r="A6466" t="s">
-        <v>16</v>
+      <c r="A6466">
+        <v>13</v>
       </c>
       <c r="B6466" s="2">
         <v>44580</v>
@@ -92118,8 +92121,8 @@
       </c>
     </row>
     <row r="6467" spans="1:4">
-      <c r="A6467" t="s">
-        <v>17</v>
+      <c r="A6467">
+        <v>14</v>
       </c>
       <c r="B6467" s="2">
         <v>44580</v>
@@ -92132,8 +92135,8 @@
       </c>
     </row>
     <row r="6468" spans="1:4">
-      <c r="A6468" t="s">
-        <v>18</v>
+      <c r="A6468">
+        <v>15</v>
       </c>
       <c r="B6468" s="2">
         <v>44580</v>
@@ -92146,8 +92149,8 @@
       </c>
     </row>
     <row r="6469" spans="1:4">
-      <c r="A6469" t="s">
-        <v>19</v>
+      <c r="A6469">
+        <v>16</v>
       </c>
       <c r="B6469" s="2">
         <v>44580</v>
@@ -92156,6 +92159,454 @@
         <v>403</v>
       </c>
       <c r="D6469">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6470" spans="1:4">
+      <c r="A6470" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6470" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6470" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6470">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6471" spans="1:4">
+      <c r="A6471" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6471" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6471" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6471">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6472" spans="1:4">
+      <c r="A6472" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6472" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6472" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6472">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6473" spans="1:4">
+      <c r="A6473" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6473" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6473" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6473">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6474" spans="1:4">
+      <c r="A6474" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6474" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6474" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6474">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6475" spans="1:4">
+      <c r="A6475" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6475" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6475" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6475">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6476" spans="1:4">
+      <c r="A6476" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6476" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6476" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6476">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6477" spans="1:4">
+      <c r="A6477" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6477" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6477" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6477">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6478" spans="1:4">
+      <c r="A6478" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6478" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6478" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6478">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6479" spans="1:4">
+      <c r="A6479" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6479" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6479" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6479">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6480" spans="1:4">
+      <c r="A6480" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6480" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6480" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6480">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6481" spans="1:4">
+      <c r="A6481" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6481" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6481" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6481">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6482" spans="1:4">
+      <c r="A6482" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6482" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6482" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6482">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6483" spans="1:4">
+      <c r="A6483" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6483" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6483" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6483">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6484" spans="1:4">
+      <c r="A6484" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6484" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6484" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6484">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6485" spans="1:4">
+      <c r="A6485" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6485" s="2">
+        <v>44580</v>
+      </c>
+      <c r="C6485" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6485">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6486" spans="1:4">
+      <c r="A6486" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6486" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6486" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6486">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6487" spans="1:4">
+      <c r="A6487" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6487" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6487" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6487">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6488" spans="1:4">
+      <c r="A6488" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6488" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6488" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6488">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6489" spans="1:4">
+      <c r="A6489" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6489" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6489" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6489">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6490" spans="1:4">
+      <c r="A6490" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6490" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6490" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6490">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6491" spans="1:4">
+      <c r="A6491" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6491" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6491" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6491">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6492" spans="1:4">
+      <c r="A6492" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6492" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6492" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6492">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6493" spans="1:4">
+      <c r="A6493" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6493" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6493" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6493">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6494" spans="1:4">
+      <c r="A6494" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6494" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6494" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6494">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6495" spans="1:4">
+      <c r="A6495" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6495" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6495" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6495">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6496" spans="1:4">
+      <c r="A6496" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6496" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6496" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6496">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6497" spans="1:4">
+      <c r="A6497" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6497" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6497" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6497">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6498" spans="1:4">
+      <c r="A6498" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6498" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6498" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6498">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6499" spans="1:4">
+      <c r="A6499" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6499" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6499" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6499">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6500" spans="1:4">
+      <c r="A6500" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6500" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6500" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6500">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6501" spans="1:4">
+      <c r="A6501" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6501" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6501" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6501">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-23-2022 20-10-00
</commit_message>
<xml_diff>
--- a/Data/ConsolidadoPuntosFuego.xlsx
+++ b/Data/ConsolidadoPuntosFuego.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12060" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12092" uniqueCount="406">
   <si>
     <t>Región</t>
   </si>
@@ -1230,6 +1230,9 @@
   <si>
     <t>2022-01-20</t>
   </si>
+  <si>
+    <t>2022-01-21</t>
+  </si>
 </sst>
 </file>
 
@@ -1590,7 +1593,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6501"/>
+  <dimension ref="A1:D6533"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -92163,8 +92166,8 @@
       </c>
     </row>
     <row r="6470" spans="1:4">
-      <c r="A6470" t="s">
-        <v>4</v>
+      <c r="A6470">
+        <v>1</v>
       </c>
       <c r="B6470" s="2">
         <v>44580</v>
@@ -92177,8 +92180,8 @@
       </c>
     </row>
     <row r="6471" spans="1:4">
-      <c r="A6471" t="s">
-        <v>5</v>
+      <c r="A6471">
+        <v>2</v>
       </c>
       <c r="B6471" s="2">
         <v>44580</v>
@@ -92191,8 +92194,8 @@
       </c>
     </row>
     <row r="6472" spans="1:4">
-      <c r="A6472" t="s">
-        <v>6</v>
+      <c r="A6472">
+        <v>3</v>
       </c>
       <c r="B6472" s="2">
         <v>44580</v>
@@ -92205,8 +92208,8 @@
       </c>
     </row>
     <row r="6473" spans="1:4">
-      <c r="A6473" t="s">
-        <v>7</v>
+      <c r="A6473">
+        <v>4</v>
       </c>
       <c r="B6473" s="2">
         <v>44580</v>
@@ -92219,8 +92222,8 @@
       </c>
     </row>
     <row r="6474" spans="1:4">
-      <c r="A6474" t="s">
-        <v>8</v>
+      <c r="A6474">
+        <v>5</v>
       </c>
       <c r="B6474" s="2">
         <v>44580</v>
@@ -92233,8 +92236,8 @@
       </c>
     </row>
     <row r="6475" spans="1:4">
-      <c r="A6475" t="s">
-        <v>9</v>
+      <c r="A6475">
+        <v>6</v>
       </c>
       <c r="B6475" s="2">
         <v>44580</v>
@@ -92247,8 +92250,8 @@
       </c>
     </row>
     <row r="6476" spans="1:4">
-      <c r="A6476" t="s">
-        <v>10</v>
+      <c r="A6476">
+        <v>7</v>
       </c>
       <c r="B6476" s="2">
         <v>44580</v>
@@ -92261,8 +92264,8 @@
       </c>
     </row>
     <row r="6477" spans="1:4">
-      <c r="A6477" t="s">
-        <v>11</v>
+      <c r="A6477">
+        <v>8</v>
       </c>
       <c r="B6477" s="2">
         <v>44580</v>
@@ -92275,8 +92278,8 @@
       </c>
     </row>
     <row r="6478" spans="1:4">
-      <c r="A6478" t="s">
-        <v>12</v>
+      <c r="A6478">
+        <v>9</v>
       </c>
       <c r="B6478" s="2">
         <v>44580</v>
@@ -92289,8 +92292,8 @@
       </c>
     </row>
     <row r="6479" spans="1:4">
-      <c r="A6479" t="s">
-        <v>13</v>
+      <c r="A6479">
+        <v>10</v>
       </c>
       <c r="B6479" s="2">
         <v>44580</v>
@@ -92303,8 +92306,8 @@
       </c>
     </row>
     <row r="6480" spans="1:4">
-      <c r="A6480" t="s">
-        <v>14</v>
+      <c r="A6480">
+        <v>11</v>
       </c>
       <c r="B6480" s="2">
         <v>44580</v>
@@ -92317,8 +92320,8 @@
       </c>
     </row>
     <row r="6481" spans="1:4">
-      <c r="A6481" t="s">
-        <v>15</v>
+      <c r="A6481">
+        <v>12</v>
       </c>
       <c r="B6481" s="2">
         <v>44580</v>
@@ -92331,8 +92334,8 @@
       </c>
     </row>
     <row r="6482" spans="1:4">
-      <c r="A6482" t="s">
-        <v>16</v>
+      <c r="A6482">
+        <v>13</v>
       </c>
       <c r="B6482" s="2">
         <v>44580</v>
@@ -92345,8 +92348,8 @@
       </c>
     </row>
     <row r="6483" spans="1:4">
-      <c r="A6483" t="s">
-        <v>17</v>
+      <c r="A6483">
+        <v>14</v>
       </c>
       <c r="B6483" s="2">
         <v>44580</v>
@@ -92359,8 +92362,8 @@
       </c>
     </row>
     <row r="6484" spans="1:4">
-      <c r="A6484" t="s">
-        <v>18</v>
+      <c r="A6484">
+        <v>15</v>
       </c>
       <c r="B6484" s="2">
         <v>44580</v>
@@ -92373,8 +92376,8 @@
       </c>
     </row>
     <row r="6485" spans="1:4">
-      <c r="A6485" t="s">
-        <v>19</v>
+      <c r="A6485">
+        <v>16</v>
       </c>
       <c r="B6485" s="2">
         <v>44580</v>
@@ -92387,8 +92390,8 @@
       </c>
     </row>
     <row r="6486" spans="1:4">
-      <c r="A6486" t="s">
-        <v>4</v>
+      <c r="A6486">
+        <v>1</v>
       </c>
       <c r="B6486" s="2">
         <v>44581</v>
@@ -92401,8 +92404,8 @@
       </c>
     </row>
     <row r="6487" spans="1:4">
-      <c r="A6487" t="s">
-        <v>5</v>
+      <c r="A6487">
+        <v>2</v>
       </c>
       <c r="B6487" s="2">
         <v>44581</v>
@@ -92415,8 +92418,8 @@
       </c>
     </row>
     <row r="6488" spans="1:4">
-      <c r="A6488" t="s">
-        <v>6</v>
+      <c r="A6488">
+        <v>3</v>
       </c>
       <c r="B6488" s="2">
         <v>44581</v>
@@ -92429,8 +92432,8 @@
       </c>
     </row>
     <row r="6489" spans="1:4">
-      <c r="A6489" t="s">
-        <v>7</v>
+      <c r="A6489">
+        <v>4</v>
       </c>
       <c r="B6489" s="2">
         <v>44581</v>
@@ -92443,8 +92446,8 @@
       </c>
     </row>
     <row r="6490" spans="1:4">
-      <c r="A6490" t="s">
-        <v>8</v>
+      <c r="A6490">
+        <v>5</v>
       </c>
       <c r="B6490" s="2">
         <v>44581</v>
@@ -92457,8 +92460,8 @@
       </c>
     </row>
     <row r="6491" spans="1:4">
-      <c r="A6491" t="s">
-        <v>9</v>
+      <c r="A6491">
+        <v>6</v>
       </c>
       <c r="B6491" s="2">
         <v>44581</v>
@@ -92471,8 +92474,8 @@
       </c>
     </row>
     <row r="6492" spans="1:4">
-      <c r="A6492" t="s">
-        <v>10</v>
+      <c r="A6492">
+        <v>7</v>
       </c>
       <c r="B6492" s="2">
         <v>44581</v>
@@ -92485,8 +92488,8 @@
       </c>
     </row>
     <row r="6493" spans="1:4">
-      <c r="A6493" t="s">
-        <v>11</v>
+      <c r="A6493">
+        <v>8</v>
       </c>
       <c r="B6493" s="2">
         <v>44581</v>
@@ -92499,8 +92502,8 @@
       </c>
     </row>
     <row r="6494" spans="1:4">
-      <c r="A6494" t="s">
-        <v>12</v>
+      <c r="A6494">
+        <v>9</v>
       </c>
       <c r="B6494" s="2">
         <v>44581</v>
@@ -92513,8 +92516,8 @@
       </c>
     </row>
     <row r="6495" spans="1:4">
-      <c r="A6495" t="s">
-        <v>13</v>
+      <c r="A6495">
+        <v>10</v>
       </c>
       <c r="B6495" s="2">
         <v>44581</v>
@@ -92527,8 +92530,8 @@
       </c>
     </row>
     <row r="6496" spans="1:4">
-      <c r="A6496" t="s">
-        <v>14</v>
+      <c r="A6496">
+        <v>11</v>
       </c>
       <c r="B6496" s="2">
         <v>44581</v>
@@ -92541,8 +92544,8 @@
       </c>
     </row>
     <row r="6497" spans="1:4">
-      <c r="A6497" t="s">
-        <v>15</v>
+      <c r="A6497">
+        <v>12</v>
       </c>
       <c r="B6497" s="2">
         <v>44581</v>
@@ -92555,8 +92558,8 @@
       </c>
     </row>
     <row r="6498" spans="1:4">
-      <c r="A6498" t="s">
-        <v>16</v>
+      <c r="A6498">
+        <v>13</v>
       </c>
       <c r="B6498" s="2">
         <v>44581</v>
@@ -92569,8 +92572,8 @@
       </c>
     </row>
     <row r="6499" spans="1:4">
-      <c r="A6499" t="s">
-        <v>17</v>
+      <c r="A6499">
+        <v>14</v>
       </c>
       <c r="B6499" s="2">
         <v>44581</v>
@@ -92583,8 +92586,8 @@
       </c>
     </row>
     <row r="6500" spans="1:4">
-      <c r="A6500" t="s">
-        <v>18</v>
+      <c r="A6500">
+        <v>15</v>
       </c>
       <c r="B6500" s="2">
         <v>44581</v>
@@ -92597,8 +92600,8 @@
       </c>
     </row>
     <row r="6501" spans="1:4">
-      <c r="A6501" t="s">
-        <v>19</v>
+      <c r="A6501">
+        <v>16</v>
       </c>
       <c r="B6501" s="2">
         <v>44581</v>
@@ -92608,6 +92611,454 @@
       </c>
       <c r="D6501">
         <v>0</v>
+      </c>
+    </row>
+    <row r="6502" spans="1:4">
+      <c r="A6502" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6502" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6502" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6502">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6503" spans="1:4">
+      <c r="A6503" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6503" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6503" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6503">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6504" spans="1:4">
+      <c r="A6504" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6504" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6504" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6504">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6505" spans="1:4">
+      <c r="A6505" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6505" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6505" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6505">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6506" spans="1:4">
+      <c r="A6506" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6506" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6506" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6506">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6507" spans="1:4">
+      <c r="A6507" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6507" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6507" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6507">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6508" spans="1:4">
+      <c r="A6508" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6508" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6508" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6508">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6509" spans="1:4">
+      <c r="A6509" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6509" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6509" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6509">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6510" spans="1:4">
+      <c r="A6510" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6510" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6510" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6510">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6511" spans="1:4">
+      <c r="A6511" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6511" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6511" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6511">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6512" spans="1:4">
+      <c r="A6512" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6512" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6512" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6512">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6513" spans="1:4">
+      <c r="A6513" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6513" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6513" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6513">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6514" spans="1:4">
+      <c r="A6514" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6514" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6514" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6514">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6515" spans="1:4">
+      <c r="A6515" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6515" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6515" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6515">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6516" spans="1:4">
+      <c r="A6516" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6516" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6516" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6516">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6517" spans="1:4">
+      <c r="A6517" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6517" s="2">
+        <v>44581</v>
+      </c>
+      <c r="C6517" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6517">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6518" spans="1:4">
+      <c r="A6518" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6518" s="2">
+        <v>44582</v>
+      </c>
+      <c r="C6518" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6518">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6519" spans="1:4">
+      <c r="A6519" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6519" s="2">
+        <v>44582</v>
+      </c>
+      <c r="C6519" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6519">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6520" spans="1:4">
+      <c r="A6520" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6520" s="2">
+        <v>44582</v>
+      </c>
+      <c r="C6520" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6520">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6521" spans="1:4">
+      <c r="A6521" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6521" s="2">
+        <v>44582</v>
+      </c>
+      <c r="C6521" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6521">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6522" spans="1:4">
+      <c r="A6522" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6522" s="2">
+        <v>44582</v>
+      </c>
+      <c r="C6522" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6522">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6523" spans="1:4">
+      <c r="A6523" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6523" s="2">
+        <v>44582</v>
+      </c>
+      <c r="C6523" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6523">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6524" spans="1:4">
+      <c r="A6524" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6524" s="2">
+        <v>44582</v>
+      </c>
+      <c r="C6524" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6524">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6525" spans="1:4">
+      <c r="A6525" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6525" s="2">
+        <v>44582</v>
+      </c>
+      <c r="C6525" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6525">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6526" spans="1:4">
+      <c r="A6526" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6526" s="2">
+        <v>44582</v>
+      </c>
+      <c r="C6526" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6526">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6527" spans="1:4">
+      <c r="A6527" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6527" s="2">
+        <v>44582</v>
+      </c>
+      <c r="C6527" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6527">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6528" spans="1:4">
+      <c r="A6528" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6528" s="2">
+        <v>44582</v>
+      </c>
+      <c r="C6528" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6528">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6529" spans="1:4">
+      <c r="A6529" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6529" s="2">
+        <v>44582</v>
+      </c>
+      <c r="C6529" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6529">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6530" spans="1:4">
+      <c r="A6530" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6530" s="2">
+        <v>44582</v>
+      </c>
+      <c r="C6530" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6530">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6531" spans="1:4">
+      <c r="A6531" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6531" s="2">
+        <v>44582</v>
+      </c>
+      <c r="C6531" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6531">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6532" spans="1:4">
+      <c r="A6532" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6532" s="2">
+        <v>44582</v>
+      </c>
+      <c r="C6532" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6532">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6533" spans="1:4">
+      <c r="A6533" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6533" s="2">
+        <v>44582</v>
+      </c>
+      <c r="C6533" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6533">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>